<commit_message>
WIP - adding PWM current support ot the diagnostics
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95CC1DB-D06A-4BFC-A9AA-E93FF3BBEE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53C2771-E259-4076-82A8-10FB9466EC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="527">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1621,6 +1621,9 @@
   </si>
   <si>
     <t>SPARE_OUT3001</t>
+  </si>
+  <si>
+    <t>PWM_CUR</t>
   </si>
 </sst>
 </file>
@@ -1764,7 +1767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1836,12 +1839,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2166,11 +2169,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA67"/>
+  <dimension ref="A1:T67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L30" sqref="L30"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2184,7 +2187,7 @@
     <col min="8" max="8" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.85546875" style="4" customWidth="1"/>
     <col min="14" max="14" width="44.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -2293,7 +2296,7 @@
         <f t="shared" ref="J2:J65" si="1">_xlfn.CONCAT(A2,".",D2)</f>
         <v>CHASSIS.IN0100</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="19" t="s">
         <v>356</v>
       </c>
       <c r="L2" s="19" t="str">
@@ -2310,7 +2313,7 @@
         <v>Machine_IO.Inputs.ESTOP_OK</v>
       </c>
       <c r="P2" s="20" t="str">
-        <f>_xlfn.CONCAT(O2,"(); // ",E2)</f>
+        <f t="shared" ref="P2:P33" si="2">_xlfn.CONCAT(O2,"(); // ",E2)</f>
         <v>Machine_IO.Inputs.ESTOP_OK(); // CR0709.IN0100</v>
       </c>
       <c r="Q2" s="20" t="str">
@@ -2318,15 +2321,15 @@
         <v>Machine_IO.Inputs.ESTOP_OK.Init('CHASSIS','ESTOP_OK','IN0100','a63',NVL_IO_CHASSIS.All_Inputs.IN0100,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R2" s="20" t="str">
-        <f>_xlfn.CONCAT(K2,": Mimic_Input_FB; // ",A2,":",D2)</f>
+        <f t="shared" ref="R2:R33" si="3">_xlfn.CONCAT(K2,": Mimic_Input_FB; // ",A2,":",D2)</f>
         <v>ESTOP_OK: Mimic_Input_FB; // CHASSIS:IN0100</v>
       </c>
       <c r="S2" s="20" t="str">
-        <f>_xlfn.CONCAT(A2,".",D2,"();")</f>
+        <f t="shared" ref="S2:S33" si="4">_xlfn.CONCAT(A2,".",D2,"();")</f>
         <v>CHASSIS.IN0100();</v>
       </c>
       <c r="T2" s="20" t="str">
-        <f>_xlfn.CONCAT(A2,".",D2,".Init(",O2,");")</f>
+        <f t="shared" ref="T2:T33" si="5">_xlfn.CONCAT(A2,".",D2,".Init(",O2,");")</f>
         <v>CHASSIS.IN0100.Init(Machine_IO.Inputs.ESTOP_OK);</v>
       </c>
     </row>
@@ -2344,7 +2347,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="17" t="str">
-        <f t="shared" ref="E3:E65" si="2">_xlfn.CONCAT(B3,".",D3)</f>
+        <f t="shared" ref="E3:E65" si="6">_xlfn.CONCAT(B3,".",D3)</f>
         <v>CR0709.IN0101</v>
       </c>
       <c r="F3" s="17" t="s">
@@ -2365,40 +2368,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0101</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="19" t="s">
         <v>357</v>
       </c>
       <c r="L3" s="19" t="str">
-        <f t="shared" ref="L3:L65" si="3">IF(K3&lt;&gt;"",UPPER(K3),_xlfn.CONCAT("SPARE_",D3))</f>
+        <f t="shared" ref="L3:L65" si="7">IF(K3&lt;&gt;"",UPPER(K3),_xlfn.CONCAT("SPARE_",D3))</f>
         <v>DRUM_PRESSURE</v>
       </c>
       <c r="M3" s="19"/>
       <c r="N3" s="20" t="str">
-        <f t="shared" ref="N3:N33" si="4">_xlfn.CONCAT(L3,":IpCom; // ",A3," ",D3)</f>
+        <f t="shared" ref="N3:N33" si="8">_xlfn.CONCAT(L3,":IpCom; // ",A3," ",D3)</f>
         <v>DRUM_PRESSURE:IpCom; // CHASSIS IN0101</v>
       </c>
       <c r="O3" s="20" t="str">
-        <f t="shared" ref="O3:O33" si="5">_xlfn.CONCAT("Machine_IO.","Inputs.",L3,"")</f>
+        <f t="shared" ref="O3:O33" si="9">_xlfn.CONCAT("Machine_IO.","Inputs.",L3,"")</f>
         <v>Machine_IO.Inputs.DRUM_PRESSURE</v>
       </c>
       <c r="P3" s="20" t="str">
-        <f>_xlfn.CONCAT(O3,"(); // ",E3)</f>
+        <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.DRUM_PRESSURE(); // CR0709.IN0101</v>
       </c>
       <c r="Q3" s="20" t="str">
-        <f t="shared" ref="Q3:Q33" si="6">_xlfn.CONCAT("Machine_IO.","Inputs.",K3,".Init('",A3,"','",K3,"','",D3,"','",G3,"',","NVL_IO_",A3,".All_Inputs.",D3,",Machine_IO.Node_",A3,");")</f>
+        <f t="shared" ref="Q3:Q33" si="10">_xlfn.CONCAT("Machine_IO.","Inputs.",K3,".Init('",A3,"','",K3,"','",D3,"','",G3,"',","NVL_IO_",A3,".All_Inputs.",D3,",Machine_IO.Node_",A3,");")</f>
         <v>Machine_IO.Inputs.DRUM_PRESSURE.Init('CHASSIS','DRUM_PRESSURE','IN0101','a64',NVL_IO_CHASSIS.All_Inputs.IN0101,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R3" s="20" t="str">
-        <f>_xlfn.CONCAT(K3,": Mimic_Input_FB; // ",A3,":",D3)</f>
+        <f t="shared" si="3"/>
         <v>DRUM_PRESSURE: Mimic_Input_FB; // CHASSIS:IN0101</v>
       </c>
       <c r="S3" s="20" t="str">
-        <f>_xlfn.CONCAT(A3,".",D3,"();")</f>
+        <f t="shared" si="4"/>
         <v>CHASSIS.IN0101();</v>
       </c>
       <c r="T3" s="20" t="str">
-        <f>_xlfn.CONCAT(A3,".",D3,".Init(",O3,");")</f>
+        <f t="shared" si="5"/>
         <v>CHASSIS.IN0101.Init(Machine_IO.Inputs.DRUM_PRESSURE);</v>
       </c>
     </row>
@@ -2416,7 +2419,7 @@
         <v>25</v>
       </c>
       <c r="E4" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0102</v>
       </c>
       <c r="F4" s="17" t="s">
@@ -2437,38 +2440,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0102</v>
       </c>
-      <c r="K4" s="30"/>
+      <c r="K4" s="19"/>
       <c r="L4" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0102</v>
       </c>
       <c r="M4" s="19"/>
       <c r="N4" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0102:IpCom; // CHASSIS IN0102</v>
+      </c>
+      <c r="O4" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0102</v>
+      </c>
+      <c r="P4" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0102(); // CR0709.IN0102</v>
+      </c>
+      <c r="Q4" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0102','a65',NVL_IO_CHASSIS.All_Inputs.IN0102,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R4" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0102</v>
+      </c>
+      <c r="S4" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0102:IpCom; // CHASSIS IN0102</v>
-      </c>
-      <c r="O4" s="20" t="str">
+        <v>CHASSIS.IN0102();</v>
+      </c>
+      <c r="T4" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0102</v>
-      </c>
-      <c r="P4" s="20" t="str">
-        <f>_xlfn.CONCAT(O4,"(); // ",E4)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0102(); // CR0709.IN0102</v>
-      </c>
-      <c r="Q4" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0102','a65',NVL_IO_CHASSIS.All_Inputs.IN0102,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R4" s="20" t="str">
-        <f>_xlfn.CONCAT(K4,": Mimic_Input_FB; // ",A4,":",D4)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0102</v>
-      </c>
-      <c r="S4" s="20" t="str">
-        <f>_xlfn.CONCAT(A4,".",D4,"();")</f>
-        <v>CHASSIS.IN0102();</v>
-      </c>
-      <c r="T4" s="20" t="str">
-        <f>_xlfn.CONCAT(A4,".",D4,".Init(",O4,");")</f>
         <v>CHASSIS.IN0102.Init(Machine_IO.Inputs.SPARE_IN0102);</v>
       </c>
     </row>
@@ -2486,7 +2489,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0103</v>
       </c>
       <c r="F5" s="17" t="s">
@@ -2507,38 +2510,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0103</v>
       </c>
-      <c r="K5" s="30"/>
+      <c r="K5" s="19"/>
       <c r="L5" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0103</v>
       </c>
       <c r="M5" s="19"/>
       <c r="N5" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0103:IpCom; // CHASSIS IN0103</v>
+      </c>
+      <c r="O5" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0103</v>
+      </c>
+      <c r="P5" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0103(); // CR0709.IN0103</v>
+      </c>
+      <c r="Q5" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0103','a66',NVL_IO_CHASSIS.All_Inputs.IN0103,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R5" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0103</v>
+      </c>
+      <c r="S5" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0103:IpCom; // CHASSIS IN0103</v>
-      </c>
-      <c r="O5" s="20" t="str">
+        <v>CHASSIS.IN0103();</v>
+      </c>
+      <c r="T5" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0103</v>
-      </c>
-      <c r="P5" s="20" t="str">
-        <f>_xlfn.CONCAT(O5,"(); // ",E5)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0103(); // CR0709.IN0103</v>
-      </c>
-      <c r="Q5" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0103','a66',NVL_IO_CHASSIS.All_Inputs.IN0103,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R5" s="20" t="str">
-        <f>_xlfn.CONCAT(K5,": Mimic_Input_FB; // ",A5,":",D5)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0103</v>
-      </c>
-      <c r="S5" s="20" t="str">
-        <f>_xlfn.CONCAT(A5,".",D5,"();")</f>
-        <v>CHASSIS.IN0103();</v>
-      </c>
-      <c r="T5" s="20" t="str">
-        <f>_xlfn.CONCAT(A5,".",D5,".Init(",O5,");")</f>
         <v>CHASSIS.IN0103.Init(Machine_IO.Inputs.SPARE_IN0103);</v>
       </c>
     </row>
@@ -2556,7 +2559,7 @@
         <v>27</v>
       </c>
       <c r="E6" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0200</v>
       </c>
       <c r="F6" s="17" t="s">
@@ -2577,38 +2580,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0200</v>
       </c>
-      <c r="K6" s="30"/>
+      <c r="K6" s="19"/>
       <c r="L6" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0200</v>
       </c>
       <c r="M6" s="19"/>
       <c r="N6" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0200:IpCom; // CHASSIS IN0200</v>
+      </c>
+      <c r="O6" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0200</v>
+      </c>
+      <c r="P6" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0200(); // CR0709.IN0200</v>
+      </c>
+      <c r="Q6" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0200','a67',NVL_IO_CHASSIS.All_Inputs.IN0200,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R6" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0200</v>
+      </c>
+      <c r="S6" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0200:IpCom; // CHASSIS IN0200</v>
-      </c>
-      <c r="O6" s="20" t="str">
+        <v>CHASSIS.IN0200();</v>
+      </c>
+      <c r="T6" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0200</v>
-      </c>
-      <c r="P6" s="20" t="str">
-        <f>_xlfn.CONCAT(O6,"(); // ",E6)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0200(); // CR0709.IN0200</v>
-      </c>
-      <c r="Q6" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0200','a67',NVL_IO_CHASSIS.All_Inputs.IN0200,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R6" s="20" t="str">
-        <f>_xlfn.CONCAT(K6,": Mimic_Input_FB; // ",A6,":",D6)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0200</v>
-      </c>
-      <c r="S6" s="20" t="str">
-        <f>_xlfn.CONCAT(A6,".",D6,"();")</f>
-        <v>CHASSIS.IN0200();</v>
-      </c>
-      <c r="T6" s="20" t="str">
-        <f>_xlfn.CONCAT(A6,".",D6,".Init(",O6,");")</f>
         <v>CHASSIS.IN0200.Init(Machine_IO.Inputs.SPARE_IN0200);</v>
       </c>
     </row>
@@ -2626,7 +2629,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0201</v>
       </c>
       <c r="F7" s="17" t="s">
@@ -2647,38 +2650,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0201</v>
       </c>
-      <c r="K7" s="30"/>
+      <c r="K7" s="19"/>
       <c r="L7" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0201</v>
       </c>
       <c r="M7" s="19"/>
       <c r="N7" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0201:IpCom; // CHASSIS IN0201</v>
+      </c>
+      <c r="O7" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0201</v>
+      </c>
+      <c r="P7" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0201(); // CR0709.IN0201</v>
+      </c>
+      <c r="Q7" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0201','a68',NVL_IO_CHASSIS.All_Inputs.IN0201,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R7" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0201</v>
+      </c>
+      <c r="S7" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0201:IpCom; // CHASSIS IN0201</v>
-      </c>
-      <c r="O7" s="20" t="str">
+        <v>CHASSIS.IN0201();</v>
+      </c>
+      <c r="T7" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0201</v>
-      </c>
-      <c r="P7" s="20" t="str">
-        <f>_xlfn.CONCAT(O7,"(); // ",E7)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0201(); // CR0709.IN0201</v>
-      </c>
-      <c r="Q7" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0201','a68',NVL_IO_CHASSIS.All_Inputs.IN0201,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R7" s="20" t="str">
-        <f>_xlfn.CONCAT(K7,": Mimic_Input_FB; // ",A7,":",D7)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0201</v>
-      </c>
-      <c r="S7" s="20" t="str">
-        <f>_xlfn.CONCAT(A7,".",D7,"();")</f>
-        <v>CHASSIS.IN0201();</v>
-      </c>
-      <c r="T7" s="20" t="str">
-        <f>_xlfn.CONCAT(A7,".",D7,".Init(",O7,");")</f>
         <v>CHASSIS.IN0201.Init(Machine_IO.Inputs.SPARE_IN0201);</v>
       </c>
     </row>
@@ -2696,7 +2699,7 @@
         <v>29</v>
       </c>
       <c r="E8" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0202</v>
       </c>
       <c r="F8" s="17" t="s">
@@ -2717,38 +2720,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0202</v>
       </c>
-      <c r="K8" s="30"/>
+      <c r="K8" s="19"/>
       <c r="L8" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0202</v>
       </c>
       <c r="M8" s="19"/>
       <c r="N8" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0202:IpCom; // CHASSIS IN0202</v>
+      </c>
+      <c r="O8" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0202</v>
+      </c>
+      <c r="P8" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0202(); // CR0709.IN0202</v>
+      </c>
+      <c r="Q8" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0202','a69',NVL_IO_CHASSIS.All_Inputs.IN0202,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R8" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0202</v>
+      </c>
+      <c r="S8" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0202:IpCom; // CHASSIS IN0202</v>
-      </c>
-      <c r="O8" s="20" t="str">
+        <v>CHASSIS.IN0202();</v>
+      </c>
+      <c r="T8" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0202</v>
-      </c>
-      <c r="P8" s="20" t="str">
-        <f>_xlfn.CONCAT(O8,"(); // ",E8)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0202(); // CR0709.IN0202</v>
-      </c>
-      <c r="Q8" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0202','a69',NVL_IO_CHASSIS.All_Inputs.IN0202,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R8" s="20" t="str">
-        <f>_xlfn.CONCAT(K8,": Mimic_Input_FB; // ",A8,":",D8)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0202</v>
-      </c>
-      <c r="S8" s="20" t="str">
-        <f>_xlfn.CONCAT(A8,".",D8,"();")</f>
-        <v>CHASSIS.IN0202();</v>
-      </c>
-      <c r="T8" s="20" t="str">
-        <f>_xlfn.CONCAT(A8,".",D8,".Init(",O8,");")</f>
         <v>CHASSIS.IN0202.Init(Machine_IO.Inputs.SPARE_IN0202);</v>
       </c>
     </row>
@@ -2766,7 +2769,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0203</v>
       </c>
       <c r="F9" s="17" t="s">
@@ -2787,38 +2790,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0203</v>
       </c>
-      <c r="K9" s="30"/>
+      <c r="K9" s="19"/>
       <c r="L9" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0203</v>
       </c>
       <c r="M9" s="19"/>
       <c r="N9" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0203:IpCom; // CHASSIS IN0203</v>
+      </c>
+      <c r="O9" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0203</v>
+      </c>
+      <c r="P9" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0203(); // CR0709.IN0203</v>
+      </c>
+      <c r="Q9" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0203','a70',NVL_IO_CHASSIS.All_Inputs.IN0203,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R9" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0203</v>
+      </c>
+      <c r="S9" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0203:IpCom; // CHASSIS IN0203</v>
-      </c>
-      <c r="O9" s="20" t="str">
+        <v>CHASSIS.IN0203();</v>
+      </c>
+      <c r="T9" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0203</v>
-      </c>
-      <c r="P9" s="20" t="str">
-        <f>_xlfn.CONCAT(O9,"(); // ",E9)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0203(); // CR0709.IN0203</v>
-      </c>
-      <c r="Q9" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0203','a70',NVL_IO_CHASSIS.All_Inputs.IN0203,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R9" s="20" t="str">
-        <f>_xlfn.CONCAT(K9,": Mimic_Input_FB; // ",A9,":",D9)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0203</v>
-      </c>
-      <c r="S9" s="20" t="str">
-        <f>_xlfn.CONCAT(A9,".",D9,"();")</f>
-        <v>CHASSIS.IN0203();</v>
-      </c>
-      <c r="T9" s="20" t="str">
-        <f>_xlfn.CONCAT(A9,".",D9,".Init(",O9,");")</f>
         <v>CHASSIS.IN0203.Init(Machine_IO.Inputs.SPARE_IN0203);</v>
       </c>
     </row>
@@ -2836,7 +2839,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0600</v>
       </c>
       <c r="F10" s="17" t="s">
@@ -2857,38 +2860,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0600</v>
       </c>
-      <c r="K10" s="30"/>
+      <c r="K10" s="19"/>
       <c r="L10" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0600</v>
       </c>
       <c r="M10" s="19"/>
       <c r="N10" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0600:IpCom; // CHASSIS IN0600</v>
+      </c>
+      <c r="O10" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0600</v>
+      </c>
+      <c r="P10" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0600(); // CR0709.IN0600</v>
+      </c>
+      <c r="Q10" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0600','a55',NVL_IO_CHASSIS.All_Inputs.IN0600,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R10" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0600</v>
+      </c>
+      <c r="S10" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0600:IpCom; // CHASSIS IN0600</v>
-      </c>
-      <c r="O10" s="20" t="str">
+        <v>CHASSIS.IN0600();</v>
+      </c>
+      <c r="T10" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0600</v>
-      </c>
-      <c r="P10" s="20" t="str">
-        <f>_xlfn.CONCAT(O10,"(); // ",E10)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0600(); // CR0709.IN0600</v>
-      </c>
-      <c r="Q10" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0600','a55',NVL_IO_CHASSIS.All_Inputs.IN0600,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R10" s="20" t="str">
-        <f>_xlfn.CONCAT(K10,": Mimic_Input_FB; // ",A10,":",D10)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0600</v>
-      </c>
-      <c r="S10" s="20" t="str">
-        <f>_xlfn.CONCAT(A10,".",D10,"();")</f>
-        <v>CHASSIS.IN0600();</v>
-      </c>
-      <c r="T10" s="20" t="str">
-        <f>_xlfn.CONCAT(A10,".",D10,".Init(",O10,");")</f>
         <v>CHASSIS.IN0600.Init(Machine_IO.Inputs.SPARE_IN0600);</v>
       </c>
     </row>
@@ -2906,7 +2909,7 @@
         <v>33</v>
       </c>
       <c r="E11" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0601</v>
       </c>
       <c r="F11" s="17" t="s">
@@ -2927,38 +2930,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0601</v>
       </c>
-      <c r="K11" s="30"/>
+      <c r="K11" s="19"/>
       <c r="L11" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0601</v>
       </c>
       <c r="M11" s="19"/>
       <c r="N11" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0601:IpCom; // CHASSIS IN0601</v>
+      </c>
+      <c r="O11" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0601</v>
+      </c>
+      <c r="P11" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0601(); // CR0709.IN0601</v>
+      </c>
+      <c r="Q11" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0601','a56',NVL_IO_CHASSIS.All_Inputs.IN0601,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R11" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0601</v>
+      </c>
+      <c r="S11" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0601:IpCom; // CHASSIS IN0601</v>
-      </c>
-      <c r="O11" s="20" t="str">
+        <v>CHASSIS.IN0601();</v>
+      </c>
+      <c r="T11" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0601</v>
-      </c>
-      <c r="P11" s="20" t="str">
-        <f>_xlfn.CONCAT(O11,"(); // ",E11)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0601(); // CR0709.IN0601</v>
-      </c>
-      <c r="Q11" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0601','a56',NVL_IO_CHASSIS.All_Inputs.IN0601,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R11" s="20" t="str">
-        <f>_xlfn.CONCAT(K11,": Mimic_Input_FB; // ",A11,":",D11)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0601</v>
-      </c>
-      <c r="S11" s="20" t="str">
-        <f>_xlfn.CONCAT(A11,".",D11,"();")</f>
-        <v>CHASSIS.IN0601();</v>
-      </c>
-      <c r="T11" s="20" t="str">
-        <f>_xlfn.CONCAT(A11,".",D11,".Init(",O11,");")</f>
         <v>CHASSIS.IN0601.Init(Machine_IO.Inputs.SPARE_IN0601);</v>
       </c>
     </row>
@@ -2976,7 +2979,7 @@
         <v>34</v>
       </c>
       <c r="E12" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0602</v>
       </c>
       <c r="F12" s="17" t="s">
@@ -2997,38 +3000,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0602</v>
       </c>
-      <c r="K12" s="30"/>
+      <c r="K12" s="19"/>
       <c r="L12" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0602</v>
       </c>
       <c r="M12" s="19"/>
       <c r="N12" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0602:IpCom; // CHASSIS IN0602</v>
+      </c>
+      <c r="O12" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0602</v>
+      </c>
+      <c r="P12" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0602(); // CR0709.IN0602</v>
+      </c>
+      <c r="Q12" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0602','a57',NVL_IO_CHASSIS.All_Inputs.IN0602,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R12" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0602</v>
+      </c>
+      <c r="S12" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0602:IpCom; // CHASSIS IN0602</v>
-      </c>
-      <c r="O12" s="20" t="str">
+        <v>CHASSIS.IN0602();</v>
+      </c>
+      <c r="T12" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0602</v>
-      </c>
-      <c r="P12" s="20" t="str">
-        <f>_xlfn.CONCAT(O12,"(); // ",E12)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0602(); // CR0709.IN0602</v>
-      </c>
-      <c r="Q12" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0602','a57',NVL_IO_CHASSIS.All_Inputs.IN0602,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R12" s="20" t="str">
-        <f>_xlfn.CONCAT(K12,": Mimic_Input_FB; // ",A12,":",D12)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0602</v>
-      </c>
-      <c r="S12" s="20" t="str">
-        <f>_xlfn.CONCAT(A12,".",D12,"();")</f>
-        <v>CHASSIS.IN0602();</v>
-      </c>
-      <c r="T12" s="20" t="str">
-        <f>_xlfn.CONCAT(A12,".",D12,".Init(",O12,");")</f>
         <v>CHASSIS.IN0602.Init(Machine_IO.Inputs.SPARE_IN0602);</v>
       </c>
     </row>
@@ -3046,7 +3049,7 @@
         <v>35</v>
       </c>
       <c r="E13" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0603</v>
       </c>
       <c r="F13" s="17" t="s">
@@ -3067,38 +3070,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0603</v>
       </c>
-      <c r="K13" s="30"/>
+      <c r="K13" s="19"/>
       <c r="L13" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0603</v>
       </c>
       <c r="M13" s="19"/>
       <c r="N13" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0603:IpCom; // CHASSIS IN0603</v>
+      </c>
+      <c r="O13" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0603</v>
+      </c>
+      <c r="P13" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0603(); // CR0709.IN0603</v>
+      </c>
+      <c r="Q13" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0603','a58',NVL_IO_CHASSIS.All_Inputs.IN0603,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R13" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0603</v>
+      </c>
+      <c r="S13" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0603:IpCom; // CHASSIS IN0603</v>
-      </c>
-      <c r="O13" s="20" t="str">
+        <v>CHASSIS.IN0603();</v>
+      </c>
+      <c r="T13" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0603</v>
-      </c>
-      <c r="P13" s="20" t="str">
-        <f>_xlfn.CONCAT(O13,"(); // ",E13)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0603(); // CR0709.IN0603</v>
-      </c>
-      <c r="Q13" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0603','a58',NVL_IO_CHASSIS.All_Inputs.IN0603,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R13" s="20" t="str">
-        <f>_xlfn.CONCAT(K13,": Mimic_Input_FB; // ",A13,":",D13)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0603</v>
-      </c>
-      <c r="S13" s="20" t="str">
-        <f>_xlfn.CONCAT(A13,".",D13,"();")</f>
-        <v>CHASSIS.IN0603();</v>
-      </c>
-      <c r="T13" s="20" t="str">
-        <f>_xlfn.CONCAT(A13,".",D13,".Init(",O13,");")</f>
         <v>CHASSIS.IN0603.Init(Machine_IO.Inputs.SPARE_IN0603);</v>
       </c>
     </row>
@@ -3116,7 +3119,7 @@
         <v>36</v>
       </c>
       <c r="E14" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0700</v>
       </c>
       <c r="F14" s="17" t="s">
@@ -3137,38 +3140,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0700</v>
       </c>
-      <c r="K14" s="30"/>
+      <c r="K14" s="19"/>
       <c r="L14" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0700</v>
       </c>
       <c r="M14" s="19"/>
       <c r="N14" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0700:IpCom; // CHASSIS IN0700</v>
+      </c>
+      <c r="O14" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0700</v>
+      </c>
+      <c r="P14" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0700(); // CR0709.IN0700</v>
+      </c>
+      <c r="Q14" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0700','a59',NVL_IO_CHASSIS.All_Inputs.IN0700,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R14" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0700</v>
+      </c>
+      <c r="S14" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0700:IpCom; // CHASSIS IN0700</v>
-      </c>
-      <c r="O14" s="20" t="str">
+        <v>CHASSIS.IN0700();</v>
+      </c>
+      <c r="T14" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0700</v>
-      </c>
-      <c r="P14" s="20" t="str">
-        <f>_xlfn.CONCAT(O14,"(); // ",E14)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0700(); // CR0709.IN0700</v>
-      </c>
-      <c r="Q14" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0700','a59',NVL_IO_CHASSIS.All_Inputs.IN0700,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R14" s="20" t="str">
-        <f>_xlfn.CONCAT(K14,": Mimic_Input_FB; // ",A14,":",D14)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0700</v>
-      </c>
-      <c r="S14" s="20" t="str">
-        <f>_xlfn.CONCAT(A14,".",D14,"();")</f>
-        <v>CHASSIS.IN0700();</v>
-      </c>
-      <c r="T14" s="20" t="str">
-        <f>_xlfn.CONCAT(A14,".",D14,".Init(",O14,");")</f>
         <v>CHASSIS.IN0700.Init(Machine_IO.Inputs.SPARE_IN0700);</v>
       </c>
     </row>
@@ -3186,7 +3189,7 @@
         <v>37</v>
       </c>
       <c r="E15" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0701</v>
       </c>
       <c r="F15" s="17" t="s">
@@ -3207,40 +3210,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0701</v>
       </c>
-      <c r="K15" s="30" t="s">
+      <c r="K15" s="19" t="s">
         <v>359</v>
       </c>
       <c r="L15" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RADIORHS_JACKLEGRAISE_REQ</v>
       </c>
       <c r="M15" s="19"/>
       <c r="N15" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>RADIORHS_JACKLEGRAISE_REQ:IpCom; // CHASSIS IN0701</v>
+      </c>
+      <c r="O15" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ</v>
+      </c>
+      <c r="P15" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ(); // CR0709.IN0701</v>
+      </c>
+      <c r="Q15" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RadioRHS_JackLegRaise_Req.Init('CHASSIS','RadioRHS_JackLegRaise_Req','IN0701','a60',NVL_IO_CHASSIS.All_Inputs.IN0701,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R15" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>RadioRHS_JackLegRaise_Req: Mimic_Input_FB; // CHASSIS:IN0701</v>
+      </c>
+      <c r="S15" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>RADIORHS_JACKLEGRAISE_REQ:IpCom; // CHASSIS IN0701</v>
-      </c>
-      <c r="O15" s="20" t="str">
+        <v>CHASSIS.IN0701();</v>
+      </c>
+      <c r="T15" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ</v>
-      </c>
-      <c r="P15" s="20" t="str">
-        <f>_xlfn.CONCAT(O15,"(); // ",E15)</f>
-        <v>Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ(); // CR0709.IN0701</v>
-      </c>
-      <c r="Q15" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.RadioRHS_JackLegRaise_Req.Init('CHASSIS','RadioRHS_JackLegRaise_Req','IN0701','a60',NVL_IO_CHASSIS.All_Inputs.IN0701,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R15" s="20" t="str">
-        <f>_xlfn.CONCAT(K15,": Mimic_Input_FB; // ",A15,":",D15)</f>
-        <v>RadioRHS_JackLegRaise_Req: Mimic_Input_FB; // CHASSIS:IN0701</v>
-      </c>
-      <c r="S15" s="20" t="str">
-        <f>_xlfn.CONCAT(A15,".",D15,"();")</f>
-        <v>CHASSIS.IN0701();</v>
-      </c>
-      <c r="T15" s="20" t="str">
-        <f>_xlfn.CONCAT(A15,".",D15,".Init(",O15,");")</f>
         <v>CHASSIS.IN0701.Init(Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ);</v>
       </c>
     </row>
@@ -3258,7 +3261,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0702</v>
       </c>
       <c r="F16" s="17" t="s">
@@ -3279,40 +3282,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0702</v>
       </c>
-      <c r="K16" s="30" t="s">
+      <c r="K16" s="19" t="s">
         <v>360</v>
       </c>
       <c r="L16" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RHS_TROMMELDOORSW</v>
       </c>
       <c r="M16" s="19"/>
       <c r="N16" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>RHS_TROMMELDOORSW:IpCom; // CHASSIS IN0702</v>
+      </c>
+      <c r="O16" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.RHS_TROMMELDOORSW</v>
+      </c>
+      <c r="P16" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.RHS_TROMMELDOORSW(); // CR0709.IN0702</v>
+      </c>
+      <c r="Q16" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RHS_TrommelDoorSw.Init('CHASSIS','RHS_TrommelDoorSw','IN0702','a61',NVL_IO_CHASSIS.All_Inputs.IN0702,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R16" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>RHS_TrommelDoorSw: Mimic_Input_FB; // CHASSIS:IN0702</v>
+      </c>
+      <c r="S16" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>RHS_TROMMELDOORSW:IpCom; // CHASSIS IN0702</v>
-      </c>
-      <c r="O16" s="20" t="str">
+        <v>CHASSIS.IN0702();</v>
+      </c>
+      <c r="T16" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.RHS_TROMMELDOORSW</v>
-      </c>
-      <c r="P16" s="20" t="str">
-        <f>_xlfn.CONCAT(O16,"(); // ",E16)</f>
-        <v>Machine_IO.Inputs.RHS_TROMMELDOORSW(); // CR0709.IN0702</v>
-      </c>
-      <c r="Q16" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.RHS_TrommelDoorSw.Init('CHASSIS','RHS_TrommelDoorSw','IN0702','a61',NVL_IO_CHASSIS.All_Inputs.IN0702,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R16" s="20" t="str">
-        <f>_xlfn.CONCAT(K16,": Mimic_Input_FB; // ",A16,":",D16)</f>
-        <v>RHS_TrommelDoorSw: Mimic_Input_FB; // CHASSIS:IN0702</v>
-      </c>
-      <c r="S16" s="20" t="str">
-        <f>_xlfn.CONCAT(A16,".",D16,"();")</f>
-        <v>CHASSIS.IN0702();</v>
-      </c>
-      <c r="T16" s="20" t="str">
-        <f>_xlfn.CONCAT(A16,".",D16,".Init(",O16,");")</f>
         <v>CHASSIS.IN0702.Init(Machine_IO.Inputs.RHS_TROMMELDOORSW);</v>
       </c>
     </row>
@@ -3330,7 +3333,7 @@
         <v>39</v>
       </c>
       <c r="E17" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0703</v>
       </c>
       <c r="F17" s="17" t="s">
@@ -3351,40 +3354,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0703</v>
       </c>
-      <c r="K17" s="30" t="s">
+      <c r="K17" s="19" t="s">
         <v>361</v>
       </c>
       <c r="L17" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>LHS_TROMMELDOORSW</v>
       </c>
       <c r="M17" s="19"/>
       <c r="N17" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>LHS_TROMMELDOORSW:IpCom; // CHASSIS IN0703</v>
+      </c>
+      <c r="O17" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.LHS_TROMMELDOORSW</v>
+      </c>
+      <c r="P17" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.LHS_TROMMELDOORSW(); // CR0709.IN0703</v>
+      </c>
+      <c r="Q17" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.LHS_TrommelDoorSw.Init('CHASSIS','LHS_TrommelDoorSw','IN0703','a62',NVL_IO_CHASSIS.All_Inputs.IN0703,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R17" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>LHS_TrommelDoorSw: Mimic_Input_FB; // CHASSIS:IN0703</v>
+      </c>
+      <c r="S17" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>LHS_TROMMELDOORSW:IpCom; // CHASSIS IN0703</v>
-      </c>
-      <c r="O17" s="20" t="str">
+        <v>CHASSIS.IN0703();</v>
+      </c>
+      <c r="T17" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.LHS_TROMMELDOORSW</v>
-      </c>
-      <c r="P17" s="20" t="str">
-        <f>_xlfn.CONCAT(O17,"(); // ",E17)</f>
-        <v>Machine_IO.Inputs.LHS_TROMMELDOORSW(); // CR0709.IN0703</v>
-      </c>
-      <c r="Q17" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.LHS_TrommelDoorSw.Init('CHASSIS','LHS_TrommelDoorSw','IN0703','a62',NVL_IO_CHASSIS.All_Inputs.IN0703,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R17" s="20" t="str">
-        <f>_xlfn.CONCAT(K17,": Mimic_Input_FB; // ",A17,":",D17)</f>
-        <v>LHS_TrommelDoorSw: Mimic_Input_FB; // CHASSIS:IN0703</v>
-      </c>
-      <c r="S17" s="20" t="str">
-        <f>_xlfn.CONCAT(A17,".",D17,"();")</f>
-        <v>CHASSIS.IN0703();</v>
-      </c>
-      <c r="T17" s="20" t="str">
-        <f>_xlfn.CONCAT(A17,".",D17,".Init(",O17,");")</f>
         <v>CHASSIS.IN0703.Init(Machine_IO.Inputs.LHS_TROMMELDOORSW);</v>
       </c>
     </row>
@@ -3402,7 +3405,7 @@
         <v>40</v>
       </c>
       <c r="E18" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0000</v>
       </c>
       <c r="F18" s="17" t="s">
@@ -3423,40 +3426,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0000</v>
       </c>
-      <c r="K18" s="30" t="s">
+      <c r="K18" s="19" t="s">
         <v>362</v>
       </c>
       <c r="L18" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>HYDOILTEMP_SW</v>
       </c>
       <c r="M18" s="19"/>
       <c r="N18" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>HYDOILTEMP_SW:IpCom; // CHASSIS IN0000</v>
+      </c>
+      <c r="O18" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.HYDOILTEMP_SW</v>
+      </c>
+      <c r="P18" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.HYDOILTEMP_SW(); // CR0709.IN0000</v>
+      </c>
+      <c r="Q18" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.HydOilTemp_Sw.Init('CHASSIS','HydOilTemp_Sw','IN0000','a25',NVL_IO_CHASSIS.All_Inputs.IN0000,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R18" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>HydOilTemp_Sw: Mimic_Input_FB; // CHASSIS:IN0000</v>
+      </c>
+      <c r="S18" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>HYDOILTEMP_SW:IpCom; // CHASSIS IN0000</v>
-      </c>
-      <c r="O18" s="20" t="str">
+        <v>CHASSIS.IN0000();</v>
+      </c>
+      <c r="T18" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.HYDOILTEMP_SW</v>
-      </c>
-      <c r="P18" s="20" t="str">
-        <f>_xlfn.CONCAT(O18,"(); // ",E18)</f>
-        <v>Machine_IO.Inputs.HYDOILTEMP_SW(); // CR0709.IN0000</v>
-      </c>
-      <c r="Q18" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.HydOilTemp_Sw.Init('CHASSIS','HydOilTemp_Sw','IN0000','a25',NVL_IO_CHASSIS.All_Inputs.IN0000,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R18" s="20" t="str">
-        <f>_xlfn.CONCAT(K18,": Mimic_Input_FB; // ",A18,":",D18)</f>
-        <v>HydOilTemp_Sw: Mimic_Input_FB; // CHASSIS:IN0000</v>
-      </c>
-      <c r="S18" s="20" t="str">
-        <f>_xlfn.CONCAT(A18,".",D18,"();")</f>
-        <v>CHASSIS.IN0000();</v>
-      </c>
-      <c r="T18" s="20" t="str">
-        <f>_xlfn.CONCAT(A18,".",D18,".Init(",O18,");")</f>
         <v>CHASSIS.IN0000.Init(Machine_IO.Inputs.HYDOILTEMP_SW);</v>
       </c>
     </row>
@@ -3474,7 +3477,7 @@
         <v>42</v>
       </c>
       <c r="E19" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0001</v>
       </c>
       <c r="F19" s="17" t="s">
@@ -3495,40 +3498,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0001</v>
       </c>
-      <c r="K19" s="30" t="s">
+      <c r="K19" s="19" t="s">
         <v>363</v>
       </c>
       <c r="L19" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>HYDOILLEVEL_SW</v>
       </c>
       <c r="M19" s="19"/>
       <c r="N19" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>HYDOILLEVEL_SW:IpCom; // CHASSIS IN0001</v>
+      </c>
+      <c r="O19" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.HYDOILLEVEL_SW</v>
+      </c>
+      <c r="P19" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.HYDOILLEVEL_SW(); // CR0709.IN0001</v>
+      </c>
+      <c r="Q19" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.HydOilLevel_Sw.Init('CHASSIS','HydOilLevel_Sw','IN0001','a26',NVL_IO_CHASSIS.All_Inputs.IN0001,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R19" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>HydOilLevel_Sw: Mimic_Input_FB; // CHASSIS:IN0001</v>
+      </c>
+      <c r="S19" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>HYDOILLEVEL_SW:IpCom; // CHASSIS IN0001</v>
-      </c>
-      <c r="O19" s="20" t="str">
+        <v>CHASSIS.IN0001();</v>
+      </c>
+      <c r="T19" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.HYDOILLEVEL_SW</v>
-      </c>
-      <c r="P19" s="20" t="str">
-        <f>_xlfn.CONCAT(O19,"(); // ",E19)</f>
-        <v>Machine_IO.Inputs.HYDOILLEVEL_SW(); // CR0709.IN0001</v>
-      </c>
-      <c r="Q19" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.HydOilLevel_Sw.Init('CHASSIS','HydOilLevel_Sw','IN0001','a26',NVL_IO_CHASSIS.All_Inputs.IN0001,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R19" s="20" t="str">
-        <f>_xlfn.CONCAT(K19,": Mimic_Input_FB; // ",A19,":",D19)</f>
-        <v>HydOilLevel_Sw: Mimic_Input_FB; // CHASSIS:IN0001</v>
-      </c>
-      <c r="S19" s="20" t="str">
-        <f>_xlfn.CONCAT(A19,".",D19,"();")</f>
-        <v>CHASSIS.IN0001();</v>
-      </c>
-      <c r="T19" s="20" t="str">
-        <f>_xlfn.CONCAT(A19,".",D19,".Init(",O19,");")</f>
         <v>CHASSIS.IN0001.Init(Machine_IO.Inputs.HYDOILLEVEL_SW);</v>
       </c>
     </row>
@@ -3546,7 +3549,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0002</v>
       </c>
       <c r="F20" s="17" t="s">
@@ -3567,40 +3570,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0002</v>
       </c>
-      <c r="K20" s="30" t="s">
+      <c r="K20" s="19" t="s">
         <v>364</v>
       </c>
       <c r="L20" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>THERMOSTAT</v>
       </c>
       <c r="M20" s="19"/>
       <c r="N20" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>THERMOSTAT:IpCom; // CHASSIS IN0002</v>
+      </c>
+      <c r="O20" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.THERMOSTAT</v>
+      </c>
+      <c r="P20" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.THERMOSTAT(); // CR0709.IN0002</v>
+      </c>
+      <c r="Q20" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.ThermoStat.Init('CHASSIS','ThermoStat','IN0002','a27',NVL_IO_CHASSIS.All_Inputs.IN0002,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R20" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>ThermoStat: Mimic_Input_FB; // CHASSIS:IN0002</v>
+      </c>
+      <c r="S20" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>THERMOSTAT:IpCom; // CHASSIS IN0002</v>
-      </c>
-      <c r="O20" s="20" t="str">
+        <v>CHASSIS.IN0002();</v>
+      </c>
+      <c r="T20" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.THERMOSTAT</v>
-      </c>
-      <c r="P20" s="20" t="str">
-        <f>_xlfn.CONCAT(O20,"(); // ",E20)</f>
-        <v>Machine_IO.Inputs.THERMOSTAT(); // CR0709.IN0002</v>
-      </c>
-      <c r="Q20" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.ThermoStat.Init('CHASSIS','ThermoStat','IN0002','a27',NVL_IO_CHASSIS.All_Inputs.IN0002,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R20" s="20" t="str">
-        <f>_xlfn.CONCAT(K20,": Mimic_Input_FB; // ",A20,":",D20)</f>
-        <v>ThermoStat: Mimic_Input_FB; // CHASSIS:IN0002</v>
-      </c>
-      <c r="S20" s="20" t="str">
-        <f>_xlfn.CONCAT(A20,".",D20,"();")</f>
-        <v>CHASSIS.IN0002();</v>
-      </c>
-      <c r="T20" s="20" t="str">
-        <f>_xlfn.CONCAT(A20,".",D20,".Init(",O20,");")</f>
         <v>CHASSIS.IN0002.Init(Machine_IO.Inputs.THERMOSTAT);</v>
       </c>
     </row>
@@ -3618,7 +3621,7 @@
         <v>44</v>
       </c>
       <c r="E21" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0003</v>
       </c>
       <c r="F21" s="17" t="s">
@@ -3639,40 +3642,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0003</v>
       </c>
-      <c r="K21" s="30" t="s">
+      <c r="K21" s="19" t="s">
         <v>365</v>
       </c>
       <c r="L21" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RADIORHS_JACKLEGLOWER_REQ</v>
       </c>
       <c r="M21" s="19"/>
       <c r="N21" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>RADIORHS_JACKLEGLOWER_REQ:IpCom; // CHASSIS IN0003</v>
+      </c>
+      <c r="O21" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ</v>
+      </c>
+      <c r="P21" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ(); // CR0709.IN0003</v>
+      </c>
+      <c r="Q21" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RadioRHS_JackLegLower_Req.Init('CHASSIS','RadioRHS_JackLegLower_Req','IN0003','a28',NVL_IO_CHASSIS.All_Inputs.IN0003,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R21" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>RadioRHS_JackLegLower_Req: Mimic_Input_FB; // CHASSIS:IN0003</v>
+      </c>
+      <c r="S21" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>RADIORHS_JACKLEGLOWER_REQ:IpCom; // CHASSIS IN0003</v>
-      </c>
-      <c r="O21" s="20" t="str">
+        <v>CHASSIS.IN0003();</v>
+      </c>
+      <c r="T21" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ</v>
-      </c>
-      <c r="P21" s="20" t="str">
-        <f>_xlfn.CONCAT(O21,"(); // ",E21)</f>
-        <v>Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ(); // CR0709.IN0003</v>
-      </c>
-      <c r="Q21" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.RadioRHS_JackLegLower_Req.Init('CHASSIS','RadioRHS_JackLegLower_Req','IN0003','a28',NVL_IO_CHASSIS.All_Inputs.IN0003,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R21" s="20" t="str">
-        <f>_xlfn.CONCAT(K21,": Mimic_Input_FB; // ",A21,":",D21)</f>
-        <v>RadioRHS_JackLegLower_Req: Mimic_Input_FB; // CHASSIS:IN0003</v>
-      </c>
-      <c r="S21" s="20" t="str">
-        <f>_xlfn.CONCAT(A21,".",D21,"();")</f>
-        <v>CHASSIS.IN0003();</v>
-      </c>
-      <c r="T21" s="20" t="str">
-        <f>_xlfn.CONCAT(A21,".",D21,".Init(",O21,");")</f>
         <v>CHASSIS.IN0003.Init(Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ);</v>
       </c>
     </row>
@@ -3690,7 +3693,7 @@
         <v>45</v>
       </c>
       <c r="E22" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0500</v>
       </c>
       <c r="F22" s="17" t="s">
@@ -3711,40 +3714,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0500</v>
       </c>
-      <c r="K22" s="30" t="s">
+      <c r="K22" s="19" t="s">
         <v>366</v>
       </c>
       <c r="L22" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RADIOLHS_JACKLEGRAISE_REQ</v>
       </c>
       <c r="M22" s="19"/>
       <c r="N22" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>RADIOLHS_JACKLEGRAISE_REQ:IpCom; // CHASSIS IN0500</v>
+      </c>
+      <c r="O22" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ</v>
+      </c>
+      <c r="P22" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ(); // CR0709.IN0500</v>
+      </c>
+      <c r="Q22" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RadioLHS_JackLegRaise_Req.Init('CHASSIS','RadioLHS_JackLegRaise_Req','IN0500','a40',NVL_IO_CHASSIS.All_Inputs.IN0500,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R22" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>RadioLHS_JackLegRaise_Req: Mimic_Input_FB; // CHASSIS:IN0500</v>
+      </c>
+      <c r="S22" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>RADIOLHS_JACKLEGRAISE_REQ:IpCom; // CHASSIS IN0500</v>
-      </c>
-      <c r="O22" s="20" t="str">
+        <v>CHASSIS.IN0500();</v>
+      </c>
+      <c r="T22" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ</v>
-      </c>
-      <c r="P22" s="20" t="str">
-        <f>_xlfn.CONCAT(O22,"(); // ",E22)</f>
-        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ(); // CR0709.IN0500</v>
-      </c>
-      <c r="Q22" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.RadioLHS_JackLegRaise_Req.Init('CHASSIS','RadioLHS_JackLegRaise_Req','IN0500','a40',NVL_IO_CHASSIS.All_Inputs.IN0500,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R22" s="20" t="str">
-        <f>_xlfn.CONCAT(K22,": Mimic_Input_FB; // ",A22,":",D22)</f>
-        <v>RadioLHS_JackLegRaise_Req: Mimic_Input_FB; // CHASSIS:IN0500</v>
-      </c>
-      <c r="S22" s="20" t="str">
-        <f>_xlfn.CONCAT(A22,".",D22,"();")</f>
-        <v>CHASSIS.IN0500();</v>
-      </c>
-      <c r="T22" s="20" t="str">
-        <f>_xlfn.CONCAT(A22,".",D22,".Init(",O22,");")</f>
         <v>CHASSIS.IN0500.Init(Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ);</v>
       </c>
     </row>
@@ -3762,7 +3765,7 @@
         <v>46</v>
       </c>
       <c r="E23" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0501</v>
       </c>
       <c r="F23" s="17" t="s">
@@ -3783,40 +3786,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0501</v>
       </c>
-      <c r="K23" s="30" t="s">
+      <c r="K23" s="19" t="s">
         <v>367</v>
       </c>
       <c r="L23" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RADIOLHS_JACKLEGLOWER_REQ</v>
       </c>
       <c r="M23" s="19"/>
       <c r="N23" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>RADIOLHS_JACKLEGLOWER_REQ:IpCom; // CHASSIS IN0501</v>
+      </c>
+      <c r="O23" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ</v>
+      </c>
+      <c r="P23" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ(); // CR0709.IN0501</v>
+      </c>
+      <c r="Q23" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RadioLHS_JackLegLower_Req.Init('CHASSIS','RadioLHS_JackLegLower_Req','IN0501','a41',NVL_IO_CHASSIS.All_Inputs.IN0501,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R23" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>RadioLHS_JackLegLower_Req: Mimic_Input_FB; // CHASSIS:IN0501</v>
+      </c>
+      <c r="S23" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>RADIOLHS_JACKLEGLOWER_REQ:IpCom; // CHASSIS IN0501</v>
-      </c>
-      <c r="O23" s="20" t="str">
+        <v>CHASSIS.IN0501();</v>
+      </c>
+      <c r="T23" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ</v>
-      </c>
-      <c r="P23" s="20" t="str">
-        <f>_xlfn.CONCAT(O23,"(); // ",E23)</f>
-        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ(); // CR0709.IN0501</v>
-      </c>
-      <c r="Q23" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.RadioLHS_JackLegLower_Req.Init('CHASSIS','RadioLHS_JackLegLower_Req','IN0501','a41',NVL_IO_CHASSIS.All_Inputs.IN0501,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R23" s="20" t="str">
-        <f>_xlfn.CONCAT(K23,": Mimic_Input_FB; // ",A23,":",D23)</f>
-        <v>RadioLHS_JackLegLower_Req: Mimic_Input_FB; // CHASSIS:IN0501</v>
-      </c>
-      <c r="S23" s="20" t="str">
-        <f>_xlfn.CONCAT(A23,".",D23,"();")</f>
-        <v>CHASSIS.IN0501();</v>
-      </c>
-      <c r="T23" s="20" t="str">
-        <f>_xlfn.CONCAT(A23,".",D23,".Init(",O23,");")</f>
         <v>CHASSIS.IN0501.Init(Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ);</v>
       </c>
     </row>
@@ -3834,7 +3837,7 @@
         <v>47</v>
       </c>
       <c r="E24" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0502</v>
       </c>
       <c r="F24" s="17" t="s">
@@ -3855,40 +3858,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0502</v>
       </c>
-      <c r="K24" s="30" t="s">
+      <c r="K24" s="19" t="s">
         <v>368</v>
       </c>
       <c r="L24" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RADIOSIDECONVRAISEREQ</v>
       </c>
       <c r="M24" s="19"/>
       <c r="N24" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>RADIOSIDECONVRAISEREQ:IpCom; // CHASSIS IN0502</v>
+      </c>
+      <c r="O24" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ</v>
+      </c>
+      <c r="P24" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ(); // CR0709.IN0502</v>
+      </c>
+      <c r="Q24" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RadioSideConvRaiseReq.Init('CHASSIS','RadioSideConvRaiseReq','IN0502','a42',NVL_IO_CHASSIS.All_Inputs.IN0502,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R24" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>RadioSideConvRaiseReq: Mimic_Input_FB; // CHASSIS:IN0502</v>
+      </c>
+      <c r="S24" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>RADIOSIDECONVRAISEREQ:IpCom; // CHASSIS IN0502</v>
-      </c>
-      <c r="O24" s="20" t="str">
+        <v>CHASSIS.IN0502();</v>
+      </c>
+      <c r="T24" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ</v>
-      </c>
-      <c r="P24" s="20" t="str">
-        <f>_xlfn.CONCAT(O24,"(); // ",E24)</f>
-        <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ(); // CR0709.IN0502</v>
-      </c>
-      <c r="Q24" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.RadioSideConvRaiseReq.Init('CHASSIS','RadioSideConvRaiseReq','IN0502','a42',NVL_IO_CHASSIS.All_Inputs.IN0502,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R24" s="20" t="str">
-        <f>_xlfn.CONCAT(K24,": Mimic_Input_FB; // ",A24,":",D24)</f>
-        <v>RadioSideConvRaiseReq: Mimic_Input_FB; // CHASSIS:IN0502</v>
-      </c>
-      <c r="S24" s="20" t="str">
-        <f>_xlfn.CONCAT(A24,".",D24,"();")</f>
-        <v>CHASSIS.IN0502();</v>
-      </c>
-      <c r="T24" s="20" t="str">
-        <f>_xlfn.CONCAT(A24,".",D24,".Init(",O24,");")</f>
         <v>CHASSIS.IN0502.Init(Machine_IO.Inputs.RADIOSIDECONVRAISEREQ);</v>
       </c>
     </row>
@@ -3906,7 +3909,7 @@
         <v>48</v>
       </c>
       <c r="E25" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0503</v>
       </c>
       <c r="F25" s="17" t="s">
@@ -3927,40 +3930,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0503</v>
       </c>
-      <c r="K25" s="30" t="s">
+      <c r="K25" s="19" t="s">
         <v>369</v>
       </c>
       <c r="L25" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RADIOSIDECONVLOWERREQ</v>
       </c>
       <c r="M25" s="19"/>
       <c r="N25" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>RADIOSIDECONVLOWERREQ:IpCom; // CHASSIS IN0503</v>
+      </c>
+      <c r="O25" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ</v>
+      </c>
+      <c r="P25" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ(); // CR0709.IN0503</v>
+      </c>
+      <c r="Q25" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RadioSideConvLowerReq.Init('CHASSIS','RadioSideConvLowerReq','IN0503','a43',NVL_IO_CHASSIS.All_Inputs.IN0503,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R25" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>RadioSideConvLowerReq: Mimic_Input_FB; // CHASSIS:IN0503</v>
+      </c>
+      <c r="S25" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>RADIOSIDECONVLOWERREQ:IpCom; // CHASSIS IN0503</v>
-      </c>
-      <c r="O25" s="20" t="str">
+        <v>CHASSIS.IN0503();</v>
+      </c>
+      <c r="T25" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ</v>
-      </c>
-      <c r="P25" s="20" t="str">
-        <f>_xlfn.CONCAT(O25,"(); // ",E25)</f>
-        <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ(); // CR0709.IN0503</v>
-      </c>
-      <c r="Q25" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.RadioSideConvLowerReq.Init('CHASSIS','RadioSideConvLowerReq','IN0503','a43',NVL_IO_CHASSIS.All_Inputs.IN0503,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R25" s="20" t="str">
-        <f>_xlfn.CONCAT(K25,": Mimic_Input_FB; // ",A25,":",D25)</f>
-        <v>RadioSideConvLowerReq: Mimic_Input_FB; // CHASSIS:IN0503</v>
-      </c>
-      <c r="S25" s="20" t="str">
-        <f>_xlfn.CONCAT(A25,".",D25,"();")</f>
-        <v>CHASSIS.IN0503();</v>
-      </c>
-      <c r="T25" s="20" t="str">
-        <f>_xlfn.CONCAT(A25,".",D25,".Init(",O25,");")</f>
         <v>CHASSIS.IN0503.Init(Machine_IO.Inputs.RADIOSIDECONVLOWERREQ);</v>
       </c>
     </row>
@@ -3978,7 +3981,7 @@
         <v>49</v>
       </c>
       <c r="E26" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0400</v>
       </c>
       <c r="F26" s="17" t="s">
@@ -3999,38 +4002,38 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0400</v>
       </c>
-      <c r="K26" s="30"/>
+      <c r="K26" s="19"/>
       <c r="L26" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_IN0400</v>
       </c>
       <c r="M26" s="19"/>
       <c r="N26" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>SPARE_IN0400:IpCom; // CHASSIS IN0400</v>
+      </c>
+      <c r="O26" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.SPARE_IN0400</v>
+      </c>
+      <c r="P26" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.SPARE_IN0400(); // CR0709.IN0400</v>
+      </c>
+      <c r="Q26" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0400','a46',NVL_IO_CHASSIS.All_Inputs.IN0400,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R26" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>: Mimic_Input_FB; // CHASSIS:IN0400</v>
+      </c>
+      <c r="S26" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>SPARE_IN0400:IpCom; // CHASSIS IN0400</v>
-      </c>
-      <c r="O26" s="20" t="str">
+        <v>CHASSIS.IN0400();</v>
+      </c>
+      <c r="T26" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.SPARE_IN0400</v>
-      </c>
-      <c r="P26" s="20" t="str">
-        <f>_xlfn.CONCAT(O26,"(); // ",E26)</f>
-        <v>Machine_IO.Inputs.SPARE_IN0400(); // CR0709.IN0400</v>
-      </c>
-      <c r="Q26" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0400','a46',NVL_IO_CHASSIS.All_Inputs.IN0400,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R26" s="20" t="str">
-        <f>_xlfn.CONCAT(K26,": Mimic_Input_FB; // ",A26,":",D26)</f>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0400</v>
-      </c>
-      <c r="S26" s="20" t="str">
-        <f>_xlfn.CONCAT(A26,".",D26,"();")</f>
-        <v>CHASSIS.IN0400();</v>
-      </c>
-      <c r="T26" s="20" t="str">
-        <f>_xlfn.CONCAT(A26,".",D26,".Init(",O26,");")</f>
         <v>CHASSIS.IN0400.Init(Machine_IO.Inputs.SPARE_IN0400);</v>
       </c>
     </row>
@@ -4048,7 +4051,7 @@
         <v>50</v>
       </c>
       <c r="E27" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0401</v>
       </c>
       <c r="F27" s="17" t="s">
@@ -4069,40 +4072,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0401</v>
       </c>
-      <c r="K27" s="30" t="s">
+      <c r="K27" s="19" t="s">
         <v>370</v>
       </c>
       <c r="L27" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>FUELLEVEL_PERCENT</v>
       </c>
       <c r="M27" s="19"/>
       <c r="N27" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>FUELLEVEL_PERCENT:IpCom; // CHASSIS IN0401</v>
+      </c>
+      <c r="O27" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.FUELLEVEL_PERCENT</v>
+      </c>
+      <c r="P27" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.FUELLEVEL_PERCENT(); // CR0709.IN0401</v>
+      </c>
+      <c r="Q27" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.FuelLevel_Percent.Init('CHASSIS','FuelLevel_Percent','IN0401','a47',NVL_IO_CHASSIS.All_Inputs.IN0401,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R27" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>FuelLevel_Percent: Mimic_Input_FB; // CHASSIS:IN0401</v>
+      </c>
+      <c r="S27" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>FUELLEVEL_PERCENT:IpCom; // CHASSIS IN0401</v>
-      </c>
-      <c r="O27" s="20" t="str">
+        <v>CHASSIS.IN0401();</v>
+      </c>
+      <c r="T27" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.FUELLEVEL_PERCENT</v>
-      </c>
-      <c r="P27" s="20" t="str">
-        <f>_xlfn.CONCAT(O27,"(); // ",E27)</f>
-        <v>Machine_IO.Inputs.FUELLEVEL_PERCENT(); // CR0709.IN0401</v>
-      </c>
-      <c r="Q27" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.FuelLevel_Percent.Init('CHASSIS','FuelLevel_Percent','IN0401','a47',NVL_IO_CHASSIS.All_Inputs.IN0401,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R27" s="20" t="str">
-        <f>_xlfn.CONCAT(K27,": Mimic_Input_FB; // ",A27,":",D27)</f>
-        <v>FuelLevel_Percent: Mimic_Input_FB; // CHASSIS:IN0401</v>
-      </c>
-      <c r="S27" s="20" t="str">
-        <f>_xlfn.CONCAT(A27,".",D27,"();")</f>
-        <v>CHASSIS.IN0401();</v>
-      </c>
-      <c r="T27" s="20" t="str">
-        <f>_xlfn.CONCAT(A27,".",D27,".Init(",O27,");")</f>
         <v>CHASSIS.IN0401.Init(Machine_IO.Inputs.FUELLEVEL_PERCENT);</v>
       </c>
     </row>
@@ -4120,7 +4123,7 @@
         <v>51</v>
       </c>
       <c r="E28" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0900</v>
       </c>
       <c r="F28" s="17" t="s">
@@ -4139,40 +4142,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0900</v>
       </c>
-      <c r="K28" s="30" t="s">
+      <c r="K28" s="19" t="s">
         <v>371</v>
       </c>
       <c r="L28" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>UMBTRACKREQ</v>
       </c>
       <c r="M28" s="19"/>
       <c r="N28" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>UMBTRACKREQ:IpCom; // CHASSIS IN0900</v>
+      </c>
+      <c r="O28" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.UMBTRACKREQ</v>
+      </c>
+      <c r="P28" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.UMBTRACKREQ(); // CR0709.IN0900</v>
+      </c>
+      <c r="Q28" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.UmbTrackReq.Init('CHASSIS','UmbTrackReq','IN0900','a38',NVL_IO_CHASSIS.All_Inputs.IN0900,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R28" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>UmbTrackReq: Mimic_Input_FB; // CHASSIS:IN0900</v>
+      </c>
+      <c r="S28" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>UMBTRACKREQ:IpCom; // CHASSIS IN0900</v>
-      </c>
-      <c r="O28" s="20" t="str">
+        <v>CHASSIS.IN0900();</v>
+      </c>
+      <c r="T28" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.UMBTRACKREQ</v>
-      </c>
-      <c r="P28" s="20" t="str">
-        <f>_xlfn.CONCAT(O28,"(); // ",E28)</f>
-        <v>Machine_IO.Inputs.UMBTRACKREQ(); // CR0709.IN0900</v>
-      </c>
-      <c r="Q28" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.UmbTrackReq.Init('CHASSIS','UmbTrackReq','IN0900','a38',NVL_IO_CHASSIS.All_Inputs.IN0900,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R28" s="20" t="str">
-        <f>_xlfn.CONCAT(K28,": Mimic_Input_FB; // ",A28,":",D28)</f>
-        <v>UmbTrackReq: Mimic_Input_FB; // CHASSIS:IN0900</v>
-      </c>
-      <c r="S28" s="20" t="str">
-        <f>_xlfn.CONCAT(A28,".",D28,"();")</f>
-        <v>CHASSIS.IN0900();</v>
-      </c>
-      <c r="T28" s="20" t="str">
-        <f>_xlfn.CONCAT(A28,".",D28,".Init(",O28,");")</f>
         <v>CHASSIS.IN0900.Init(Machine_IO.Inputs.UMBTRACKREQ);</v>
       </c>
     </row>
@@ -4190,7 +4193,7 @@
         <v>52</v>
       </c>
       <c r="E29" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0901</v>
       </c>
       <c r="F29" s="17" t="s">
@@ -4209,40 +4212,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0901</v>
       </c>
-      <c r="K29" s="30" t="s">
+      <c r="K29" s="19" t="s">
         <v>372</v>
       </c>
       <c r="L29" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>UMBMACHINESTOP</v>
       </c>
       <c r="M29" s="19"/>
       <c r="N29" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>UMBMACHINESTOP:IpCom; // CHASSIS IN0901</v>
+      </c>
+      <c r="O29" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.UMBMACHINESTOP</v>
+      </c>
+      <c r="P29" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.UMBMACHINESTOP(); // CR0709.IN0901</v>
+      </c>
+      <c r="Q29" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.UmbMachineStop.Init('CHASSIS','UmbMachineStop','IN0901','a39',NVL_IO_CHASSIS.All_Inputs.IN0901,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R29" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>UmbMachineStop: Mimic_Input_FB; // CHASSIS:IN0901</v>
+      </c>
+      <c r="S29" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>UMBMACHINESTOP:IpCom; // CHASSIS IN0901</v>
-      </c>
-      <c r="O29" s="20" t="str">
+        <v>CHASSIS.IN0901();</v>
+      </c>
+      <c r="T29" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.UMBMACHINESTOP</v>
-      </c>
-      <c r="P29" s="20" t="str">
-        <f>_xlfn.CONCAT(O29,"(); // ",E29)</f>
-        <v>Machine_IO.Inputs.UMBMACHINESTOP(); // CR0709.IN0901</v>
-      </c>
-      <c r="Q29" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.UmbMachineStop.Init('CHASSIS','UmbMachineStop','IN0901','a39',NVL_IO_CHASSIS.All_Inputs.IN0901,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R29" s="20" t="str">
-        <f>_xlfn.CONCAT(K29,": Mimic_Input_FB; // ",A29,":",D29)</f>
-        <v>UmbMachineStop: Mimic_Input_FB; // CHASSIS:IN0901</v>
-      </c>
-      <c r="S29" s="20" t="str">
-        <f>_xlfn.CONCAT(A29,".",D29,"();")</f>
-        <v>CHASSIS.IN0901();</v>
-      </c>
-      <c r="T29" s="20" t="str">
-        <f>_xlfn.CONCAT(A29,".",D29,".Init(",O29,");")</f>
         <v>CHASSIS.IN0901.Init(Machine_IO.Inputs.UMBMACHINESTOP);</v>
       </c>
     </row>
@@ -4260,7 +4263,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0300</v>
       </c>
       <c r="F30" s="17" t="s">
@@ -4279,40 +4282,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0300</v>
       </c>
-      <c r="K30" s="30" t="s">
+      <c r="K30" s="19" t="s">
         <v>373</v>
       </c>
       <c r="L30" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RTF_REQ</v>
       </c>
       <c r="M30" s="19"/>
       <c r="N30" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>RTF_REQ:IpCom; // CHASSIS IN0300</v>
+      </c>
+      <c r="O30" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.RTF_REQ</v>
+      </c>
+      <c r="P30" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.RTF_REQ(); // CR0709.IN0300</v>
+      </c>
+      <c r="Q30" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RTF_Req.Init('CHASSIS','RTF_Req','IN0300','a44',NVL_IO_CHASSIS.All_Inputs.IN0300,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R30" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>RTF_Req: Mimic_Input_FB; // CHASSIS:IN0300</v>
+      </c>
+      <c r="S30" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>RTF_REQ:IpCom; // CHASSIS IN0300</v>
-      </c>
-      <c r="O30" s="20" t="str">
+        <v>CHASSIS.IN0300();</v>
+      </c>
+      <c r="T30" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.RTF_REQ</v>
-      </c>
-      <c r="P30" s="20" t="str">
-        <f>_xlfn.CONCAT(O30,"(); // ",E30)</f>
-        <v>Machine_IO.Inputs.RTF_REQ(); // CR0709.IN0300</v>
-      </c>
-      <c r="Q30" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.RTF_Req.Init('CHASSIS','RTF_Req','IN0300','a44',NVL_IO_CHASSIS.All_Inputs.IN0300,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R30" s="20" t="str">
-        <f>_xlfn.CONCAT(K30,": Mimic_Input_FB; // ",A30,":",D30)</f>
-        <v>RTF_Req: Mimic_Input_FB; // CHASSIS:IN0300</v>
-      </c>
-      <c r="S30" s="20" t="str">
-        <f>_xlfn.CONCAT(A30,".",D30,"();")</f>
-        <v>CHASSIS.IN0300();</v>
-      </c>
-      <c r="T30" s="20" t="str">
-        <f>_xlfn.CONCAT(A30,".",D30,".Init(",O30,");")</f>
         <v>CHASSIS.IN0300.Init(Machine_IO.Inputs.RTF_REQ);</v>
       </c>
     </row>
@@ -4330,7 +4333,7 @@
         <v>54</v>
       </c>
       <c r="E31" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0301</v>
       </c>
       <c r="F31" s="17" t="s">
@@ -4349,40 +4352,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0301</v>
       </c>
-      <c r="K31" s="30" t="s">
+      <c r="K31" s="19" t="s">
         <v>374</v>
       </c>
       <c r="L31" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RTR_REQ</v>
       </c>
       <c r="M31" s="19"/>
       <c r="N31" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>RTR_REQ:IpCom; // CHASSIS IN0301</v>
+      </c>
+      <c r="O31" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.RTR_REQ</v>
+      </c>
+      <c r="P31" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.RTR_REQ(); // CR0709.IN0301</v>
+      </c>
+      <c r="Q31" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RTR_Req.Init('CHASSIS','RTR_Req','IN0301','a45',NVL_IO_CHASSIS.All_Inputs.IN0301,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R31" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>RTR_Req: Mimic_Input_FB; // CHASSIS:IN0301</v>
+      </c>
+      <c r="S31" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>RTR_REQ:IpCom; // CHASSIS IN0301</v>
-      </c>
-      <c r="O31" s="20" t="str">
+        <v>CHASSIS.IN0301();</v>
+      </c>
+      <c r="T31" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.RTR_REQ</v>
-      </c>
-      <c r="P31" s="20" t="str">
-        <f>_xlfn.CONCAT(O31,"(); // ",E31)</f>
-        <v>Machine_IO.Inputs.RTR_REQ(); // CR0709.IN0301</v>
-      </c>
-      <c r="Q31" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.RTR_Req.Init('CHASSIS','RTR_Req','IN0301','a45',NVL_IO_CHASSIS.All_Inputs.IN0301,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R31" s="20" t="str">
-        <f>_xlfn.CONCAT(K31,": Mimic_Input_FB; // ",A31,":",D31)</f>
-        <v>RTR_Req: Mimic_Input_FB; // CHASSIS:IN0301</v>
-      </c>
-      <c r="S31" s="20" t="str">
-        <f>_xlfn.CONCAT(A31,".",D31,"();")</f>
-        <v>CHASSIS.IN0301();</v>
-      </c>
-      <c r="T31" s="20" t="str">
-        <f>_xlfn.CONCAT(A31,".",D31,".Init(",O31,");")</f>
         <v>CHASSIS.IN0301.Init(Machine_IO.Inputs.RTR_REQ);</v>
       </c>
     </row>
@@ -4400,7 +4403,7 @@
         <v>55</v>
       </c>
       <c r="E32" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0800</v>
       </c>
       <c r="F32" s="17" t="s">
@@ -4419,40 +4422,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0800</v>
       </c>
-      <c r="K32" s="30" t="s">
+      <c r="K32" s="19" t="s">
         <v>375</v>
       </c>
       <c r="L32" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>LTF_REQ</v>
       </c>
       <c r="M32" s="19"/>
       <c r="N32" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>LTF_REQ:IpCom; // CHASSIS IN0800</v>
+      </c>
+      <c r="O32" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.LTF_REQ</v>
+      </c>
+      <c r="P32" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.LTF_REQ(); // CR0709.IN0800</v>
+      </c>
+      <c r="Q32" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.LTF_Req.Init('CHASSIS','LTF_Req','IN0800','a36',NVL_IO_CHASSIS.All_Inputs.IN0800,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R32" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>LTF_Req: Mimic_Input_FB; // CHASSIS:IN0800</v>
+      </c>
+      <c r="S32" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>LTF_REQ:IpCom; // CHASSIS IN0800</v>
-      </c>
-      <c r="O32" s="20" t="str">
+        <v>CHASSIS.IN0800();</v>
+      </c>
+      <c r="T32" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.LTF_REQ</v>
-      </c>
-      <c r="P32" s="20" t="str">
-        <f>_xlfn.CONCAT(O32,"(); // ",E32)</f>
-        <v>Machine_IO.Inputs.LTF_REQ(); // CR0709.IN0800</v>
-      </c>
-      <c r="Q32" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.LTF_Req.Init('CHASSIS','LTF_Req','IN0800','a36',NVL_IO_CHASSIS.All_Inputs.IN0800,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R32" s="20" t="str">
-        <f>_xlfn.CONCAT(K32,": Mimic_Input_FB; // ",A32,":",D32)</f>
-        <v>LTF_Req: Mimic_Input_FB; // CHASSIS:IN0800</v>
-      </c>
-      <c r="S32" s="20" t="str">
-        <f>_xlfn.CONCAT(A32,".",D32,"();")</f>
-        <v>CHASSIS.IN0800();</v>
-      </c>
-      <c r="T32" s="20" t="str">
-        <f>_xlfn.CONCAT(A32,".",D32,".Init(",O32,");")</f>
         <v>CHASSIS.IN0800.Init(Machine_IO.Inputs.LTF_REQ);</v>
       </c>
     </row>
@@ -4470,7 +4473,7 @@
         <v>56</v>
       </c>
       <c r="E33" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.IN0801</v>
       </c>
       <c r="F33" s="17" t="s">
@@ -4489,40 +4492,40 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0801</v>
       </c>
-      <c r="K33" s="30" t="s">
+      <c r="K33" s="19" t="s">
         <v>376</v>
       </c>
       <c r="L33" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>LTR_REQ</v>
       </c>
       <c r="M33" s="19"/>
       <c r="N33" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>LTR_REQ:IpCom; // CHASSIS IN0801</v>
+      </c>
+      <c r="O33" s="20" t="str">
+        <f t="shared" si="9"/>
+        <v>Machine_IO.Inputs.LTR_REQ</v>
+      </c>
+      <c r="P33" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Machine_IO.Inputs.LTR_REQ(); // CR0709.IN0801</v>
+      </c>
+      <c r="Q33" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.LTR_Req.Init('CHASSIS','LTR_Req','IN0801','a37',NVL_IO_CHASSIS.All_Inputs.IN0801,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R33" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>LTR_Req: Mimic_Input_FB; // CHASSIS:IN0801</v>
+      </c>
+      <c r="S33" s="20" t="str">
         <f t="shared" si="4"/>
-        <v>LTR_REQ:IpCom; // CHASSIS IN0801</v>
-      </c>
-      <c r="O33" s="20" t="str">
+        <v>CHASSIS.IN0801();</v>
+      </c>
+      <c r="T33" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>Machine_IO.Inputs.LTR_REQ</v>
-      </c>
-      <c r="P33" s="20" t="str">
-        <f>_xlfn.CONCAT(O33,"(); // ",E33)</f>
-        <v>Machine_IO.Inputs.LTR_REQ(); // CR0709.IN0801</v>
-      </c>
-      <c r="Q33" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>Machine_IO.Inputs.LTR_Req.Init('CHASSIS','LTR_Req','IN0801','a37',NVL_IO_CHASSIS.All_Inputs.IN0801,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R33" s="20" t="str">
-        <f>_xlfn.CONCAT(K33,": Mimic_Input_FB; // ",A33,":",D33)</f>
-        <v>LTR_Req: Mimic_Input_FB; // CHASSIS:IN0801</v>
-      </c>
-      <c r="S33" s="20" t="str">
-        <f>_xlfn.CONCAT(A33,".",D33,"();")</f>
-        <v>CHASSIS.IN0801();</v>
-      </c>
-      <c r="T33" s="20" t="str">
-        <f>_xlfn.CONCAT(A33,".",D33,".Init(",O33,");")</f>
         <v>CHASSIS.IN0801.Init(Machine_IO.Inputs.LTR_REQ);</v>
       </c>
     </row>
@@ -4540,7 +4543,7 @@
         <v>57</v>
       </c>
       <c r="E34" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0000</v>
       </c>
       <c r="F34" s="17" t="s">
@@ -4554,22 +4557,22 @@
         <f>_xlfn.XLOOKUP(E34,IfmPinRef!$B$2:$B$199,IfmPinRef!$I$2:$I$199)</f>
         <v>PWM 2.5A</v>
       </c>
-      <c r="I34" s="21" t="s">
-        <v>41</v>
+      <c r="I34" s="30" t="s">
+        <v>526</v>
       </c>
       <c r="J34" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0000</v>
       </c>
-      <c r="K34" s="30" t="s">
+      <c r="K34" s="19" t="s">
         <v>377</v>
       </c>
       <c r="L34" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>TAILCONVSPD_MA</v>
       </c>
       <c r="M34" s="19" t="str">
-        <f t="shared" ref="M34:M65" si="7">_xlfn.CONCAT(K34,":BOOL;")</f>
+        <f t="shared" ref="M34:M65" si="11">_xlfn.CONCAT(K34,":BOOL;")</f>
         <v>TailConvSpd_mA:BOOL;</v>
       </c>
       <c r="N34" s="20" t="str">
@@ -4581,23 +4584,23 @@
         <v>Machine_IO.Outputs.TAILCONVSPD_MA</v>
       </c>
       <c r="P34" s="20" t="str">
-        <f>_xlfn.CONCAT(O34,"(); // ",E34)</f>
+        <f t="shared" ref="P34:P65" si="12">_xlfn.CONCAT(O34,"(); // ",E34)</f>
         <v>Machine_IO.Outputs.TAILCONVSPD_MA(); // CR0709.OUT0000</v>
       </c>
       <c r="Q34" s="20" t="str">
-        <f>_xlfn.CONCAT(O34,".Init('",A34,"','",K34,"','",D34,"','",G34,"',NVL_Outputs_States_",A34,".All.",D34,",NVL_IO_",A2,".All_Outputs_Diag.",D34,",Machine_IO.Node_",A34,");")</f>
+        <f t="shared" ref="Q34:Q65" si="13">_xlfn.CONCAT(O34,".Init('",A34,"','",K34,"','",D34,"','",G34,"',NVL_Outputs_States_",A34,".All.",D34,",NVL_IO_",A2,".All_Outputs_Diag.",D34,",Machine_IO.Node_",A34,");")</f>
         <v>Machine_IO.Outputs.TAILCONVSPD_MA.Init('CHASSIS','TailConvSpd_mA','OUT0000','a16',NVL_Outputs_States_CHASSIS.All.OUT0000,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0000,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R34" s="20" t="str">
-        <f t="shared" ref="R34:R65" si="8">_xlfn.CONCAT(K34,": Mimic_Output_FB; // ",A34,":",D34)</f>
+        <f t="shared" ref="R34:R65" si="14">_xlfn.CONCAT(K34,": Mimic_Output_FB; // ",A34,":",D34)</f>
         <v>TailConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0000</v>
       </c>
       <c r="S34" s="20" t="str">
-        <f>_xlfn.CONCAT(A34,".",D34,"();")</f>
+        <f t="shared" ref="S34:S65" si="15">_xlfn.CONCAT(A34,".",D34,"();")</f>
         <v>CHASSIS.OUT0000();</v>
       </c>
       <c r="T34" s="20" t="str">
-        <f>_xlfn.CONCAT(A34,".",D34,".Init(",O34,");")</f>
+        <f t="shared" ref="T34:T65" si="16">_xlfn.CONCAT(A34,".",D34,".Init(",O34,");")</f>
         <v>CHASSIS.OUT0000.Init(Machine_IO.Outputs.TAILCONVSPD_MA);</v>
       </c>
     </row>
@@ -4615,7 +4618,7 @@
         <v>59</v>
       </c>
       <c r="E35" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0001</v>
       </c>
       <c r="F35" s="17" t="s">
@@ -4636,43 +4639,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0001</v>
       </c>
-      <c r="K35" s="30" t="s">
+      <c r="K35" s="19" t="s">
         <v>378</v>
       </c>
       <c r="L35" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RHS_JACKLEGLOWER_OP</v>
       </c>
       <c r="M35" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>RHS_JackLegLower_OP:BOOL;</v>
       </c>
       <c r="N35" s="20" t="str">
-        <f t="shared" ref="N35:N65" si="9">_xlfn.CONCAT(L35,":OpCom; // ",A35,".",D35)</f>
+        <f t="shared" ref="N35:N65" si="17">_xlfn.CONCAT(L35,":OpCom; // ",A35,".",D35)</f>
         <v>RHS_JACKLEGLOWER_OP:OpCom; // CHASSIS.OUT0001</v>
       </c>
       <c r="O35" s="20" t="str">
-        <f t="shared" ref="O35:O65" si="10">_xlfn.CONCAT("Machine_IO.","Outputs.",L35,"")</f>
+        <f t="shared" ref="O35:O65" si="18">_xlfn.CONCAT("Machine_IO.","Outputs.",L35,"")</f>
         <v>Machine_IO.Outputs.RHS_JACKLEGLOWER_OP</v>
       </c>
       <c r="P35" s="20" t="str">
-        <f>_xlfn.CONCAT(O35,"(); // ",E35)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.RHS_JACKLEGLOWER_OP(); // CR0709.OUT0001</v>
       </c>
       <c r="Q35" s="20" t="str">
-        <f>_xlfn.CONCAT(O35,".Init('",A35,"','",K35,"','",D35,"','",G35,"',NVL_Outputs_States_",A35,".All.",D35,",NVL_IO_",A3,".All_Outputs_Diag.",D35,",Machine_IO.Node_",A35,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.RHS_JACKLEGLOWER_OP.Init('CHASSIS','RHS_JackLegLower_OP','OUT0001','a17',NVL_Outputs_States_CHASSIS.All.OUT0001,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0001,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R35" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>RHS_JackLegLower_OP: Mimic_Output_FB; // CHASSIS:OUT0001</v>
       </c>
       <c r="S35" s="20" t="str">
-        <f>_xlfn.CONCAT(A35,".",D35,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0001();</v>
       </c>
       <c r="T35" s="20" t="str">
-        <f>_xlfn.CONCAT(A35,".",D35,".Init(",O35,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0001.Init(Machine_IO.Outputs.RHS_JACKLEGLOWER_OP);</v>
       </c>
     </row>
@@ -4690,7 +4693,7 @@
         <v>60</v>
       </c>
       <c r="E36" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0002</v>
       </c>
       <c r="F36" s="17" t="s">
@@ -4704,50 +4707,50 @@
         <f>_xlfn.XLOOKUP(E36,IfmPinRef!$B$2:$B$199,IfmPinRef!$I$2:$I$199)</f>
         <v>PWM 2.5A</v>
       </c>
-      <c r="I36" s="21" t="s">
-        <v>41</v>
+      <c r="I36" s="30" t="s">
+        <v>526</v>
       </c>
       <c r="J36" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0002</v>
       </c>
-      <c r="K36" s="30" t="s">
+      <c r="K36" s="19" t="s">
         <v>379</v>
       </c>
       <c r="L36" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SIDECONVSPD_MA</v>
       </c>
       <c r="M36" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SideConvSpd_mA:BOOL;</v>
       </c>
       <c r="N36" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>SIDECONVSPD_MA:OpCom; // CHASSIS.OUT0002</v>
       </c>
       <c r="O36" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDECONVSPD_MA</v>
       </c>
       <c r="P36" s="20" t="str">
-        <f>_xlfn.CONCAT(O36,"(); // ",E36)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.SIDECONVSPD_MA(); // CR0709.OUT0002</v>
       </c>
       <c r="Q36" s="20" t="str">
-        <f>_xlfn.CONCAT(O36,".Init('",A36,"','",K36,"','",D36,"','",G36,"',NVL_Outputs_States_",A36,".All.",D36,",NVL_IO_",A4,".All_Outputs_Diag.",D36,",Machine_IO.Node_",A36,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SIDECONVSPD_MA.Init('CHASSIS','SideConvSpd_mA','OUT0002','a18',NVL_Outputs_States_CHASSIS.All.OUT0002,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0002,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R36" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>SideConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0002</v>
       </c>
       <c r="S36" s="20" t="str">
-        <f>_xlfn.CONCAT(A36,".",D36,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0002();</v>
       </c>
       <c r="T36" s="20" t="str">
-        <f>_xlfn.CONCAT(A36,".",D36,".Init(",O36,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0002.Init(Machine_IO.Outputs.SIDECONVSPD_MA);</v>
       </c>
     </row>
@@ -4765,7 +4768,7 @@
         <v>61</v>
       </c>
       <c r="E37" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0003</v>
       </c>
       <c r="F37" s="17" t="s">
@@ -4786,43 +4789,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0003</v>
       </c>
-      <c r="K37" s="30" t="s">
+      <c r="K37" s="19" t="s">
         <v>380</v>
       </c>
       <c r="L37" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>LHS_JACKLEGRAISE_OP</v>
       </c>
       <c r="M37" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>LHS_JackLegRaise_OP:BOOL;</v>
       </c>
       <c r="N37" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>LHS_JACKLEGRAISE_OP:OpCom; // CHASSIS.OUT0003</v>
       </c>
       <c r="O37" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGRAISE_OP</v>
       </c>
       <c r="P37" s="20" t="str">
-        <f>_xlfn.CONCAT(O37,"(); // ",E37)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGRAISE_OP(); // CR0709.OUT0003</v>
       </c>
       <c r="Q37" s="20" t="str">
-        <f>_xlfn.CONCAT(O37,".Init('",A37,"','",K37,"','",D37,"','",G37,"',NVL_Outputs_States_",A37,".All.",D37,",NVL_IO_",A5,".All_Outputs_Diag.",D37,",Machine_IO.Node_",A37,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGRAISE_OP.Init('CHASSIS','LHS_JackLegRaise_OP','OUT0003','a19',NVL_Outputs_States_CHASSIS.All.OUT0003,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0003,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R37" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>LHS_JackLegRaise_OP: Mimic_Output_FB; // CHASSIS:OUT0003</v>
       </c>
       <c r="S37" s="20" t="str">
-        <f>_xlfn.CONCAT(A37,".",D37,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0003();</v>
       </c>
       <c r="T37" s="20" t="str">
-        <f>_xlfn.CONCAT(A37,".",D37,".Init(",O37,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0003.Init(Machine_IO.Outputs.LHS_JACKLEGRAISE_OP);</v>
       </c>
     </row>
@@ -4840,7 +4843,7 @@
         <v>62</v>
       </c>
       <c r="E38" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0004</v>
       </c>
       <c r="F38" s="17" t="s">
@@ -4854,50 +4857,50 @@
         <f>_xlfn.XLOOKUP(E38,IfmPinRef!$B$2:$B$199,IfmPinRef!$I$2:$I$199)</f>
         <v>PWM 2.5A</v>
       </c>
-      <c r="I38" s="21" t="s">
-        <v>41</v>
+      <c r="I38" s="30" t="s">
+        <v>526</v>
       </c>
       <c r="J38" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0004</v>
       </c>
-      <c r="K38" s="30" t="s">
+      <c r="K38" s="19" t="s">
         <v>381</v>
       </c>
       <c r="L38" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SIDETRANSFERSPD_MA</v>
       </c>
       <c r="M38" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SideTransferSpd_mA:BOOL;</v>
       </c>
       <c r="N38" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>SIDETRANSFERSPD_MA:OpCom; // CHASSIS.OUT0004</v>
       </c>
       <c r="O38" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDETRANSFERSPD_MA</v>
       </c>
       <c r="P38" s="20" t="str">
-        <f>_xlfn.CONCAT(O38,"(); // ",E38)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.SIDETRANSFERSPD_MA(); // CR0709.OUT0004</v>
       </c>
       <c r="Q38" s="20" t="str">
-        <f>_xlfn.CONCAT(O38,".Init('",A38,"','",K38,"','",D38,"','",G38,"',NVL_Outputs_States_",A38,".All.",D38,",NVL_IO_",A6,".All_Outputs_Diag.",D38,",Machine_IO.Node_",A38,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SIDETRANSFERSPD_MA.Init('CHASSIS','SideTransferSpd_mA','OUT0004','a20',NVL_Outputs_States_CHASSIS.All.OUT0004,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0004,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R38" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>SideTransferSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0004</v>
       </c>
       <c r="S38" s="20" t="str">
-        <f>_xlfn.CONCAT(A38,".",D38,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0004();</v>
       </c>
       <c r="T38" s="20" t="str">
-        <f>_xlfn.CONCAT(A38,".",D38,".Init(",O38,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0004.Init(Machine_IO.Outputs.SIDETRANSFERSPD_MA);</v>
       </c>
     </row>
@@ -4915,7 +4918,7 @@
         <v>63</v>
       </c>
       <c r="E39" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0005</v>
       </c>
       <c r="F39" s="17" t="s">
@@ -4936,43 +4939,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0005</v>
       </c>
-      <c r="K39" s="30" t="s">
+      <c r="K39" s="19" t="s">
         <v>382</v>
       </c>
       <c r="L39" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>LHS_JACKLEGLOWER_OP</v>
       </c>
       <c r="M39" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>LHS_JackLegLower_OP:BOOL;</v>
       </c>
       <c r="N39" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>LHS_JACKLEGLOWER_OP:OpCom; // CHASSIS.OUT0005</v>
       </c>
       <c r="O39" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGLOWER_OP</v>
       </c>
       <c r="P39" s="20" t="str">
-        <f>_xlfn.CONCAT(O39,"(); // ",E39)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGLOWER_OP(); // CR0709.OUT0005</v>
       </c>
       <c r="Q39" s="20" t="str">
-        <f>_xlfn.CONCAT(O39,".Init('",A39,"','",K39,"','",D39,"','",G39,"',NVL_Outputs_States_",A39,".All.",D39,",NVL_IO_",A7,".All_Outputs_Diag.",D39,",Machine_IO.Node_",A39,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGLOWER_OP.Init('CHASSIS','LHS_JackLegLower_OP','OUT0005','a21',NVL_Outputs_States_CHASSIS.All.OUT0005,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0005,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R39" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>LHS_JackLegLower_OP: Mimic_Output_FB; // CHASSIS:OUT0005</v>
       </c>
       <c r="S39" s="20" t="str">
-        <f>_xlfn.CONCAT(A39,".",D39,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0005();</v>
       </c>
       <c r="T39" s="20" t="str">
-        <f>_xlfn.CONCAT(A39,".",D39,".Init(",O39,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0005.Init(Machine_IO.Outputs.LHS_JACKLEGLOWER_OP);</v>
       </c>
     </row>
@@ -4990,7 +4993,7 @@
         <v>64</v>
       </c>
       <c r="E40" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0006</v>
       </c>
       <c r="F40" s="17" t="s">
@@ -5011,43 +5014,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0006</v>
       </c>
-      <c r="K40" s="30" t="s">
+      <c r="K40" s="19" t="s">
         <v>383</v>
       </c>
       <c r="L40" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SETUPDUMPVALVE_OP</v>
       </c>
       <c r="M40" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SetupDumpValve_OP:BOOL;</v>
       </c>
       <c r="N40" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>SETUPDUMPVALVE_OP:OpCom; // CHASSIS.OUT0006</v>
       </c>
       <c r="O40" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SETUPDUMPVALVE_OP</v>
       </c>
       <c r="P40" s="20" t="str">
-        <f>_xlfn.CONCAT(O40,"(); // ",E40)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.SETUPDUMPVALVE_OP(); // CR0709.OUT0006</v>
       </c>
       <c r="Q40" s="20" t="str">
-        <f>_xlfn.CONCAT(O40,".Init('",A40,"','",K40,"','",D40,"','",G40,"',NVL_Outputs_States_",A40,".All.",D40,",NVL_IO_",A8,".All_Outputs_Diag.",D40,",Machine_IO.Node_",A40,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SETUPDUMPVALVE_OP.Init('CHASSIS','SetupDumpValve_OP','OUT0006','a22',NVL_Outputs_States_CHASSIS.All.OUT0006,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0006,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R40" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>SetupDumpValve_OP: Mimic_Output_FB; // CHASSIS:OUT0006</v>
       </c>
       <c r="S40" s="20" t="str">
-        <f>_xlfn.CONCAT(A40,".",D40,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0006();</v>
       </c>
       <c r="T40" s="20" t="str">
-        <f>_xlfn.CONCAT(A40,".",D40,".Init(",O40,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0006.Init(Machine_IO.Outputs.SETUPDUMPVALVE_OP);</v>
       </c>
     </row>
@@ -5065,7 +5068,7 @@
         <v>65</v>
       </c>
       <c r="E41" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0007</v>
       </c>
       <c r="F41" s="17" t="s">
@@ -5079,50 +5082,50 @@
         <f>_xlfn.XLOOKUP(E41,IfmPinRef!$B$2:$B$199,IfmPinRef!$I$2:$I$199)</f>
         <v>PWM 4A</v>
       </c>
-      <c r="I41" s="21" t="s">
-        <v>41</v>
+      <c r="I41" s="30" t="s">
+        <v>526</v>
       </c>
       <c r="J41" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0007</v>
       </c>
-      <c r="K41" s="30" t="s">
+      <c r="K41" s="19" t="s">
         <v>384</v>
       </c>
       <c r="L41" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>COLLECTIONCONVSPD_MA</v>
       </c>
       <c r="M41" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CollectionConvSpd_mA:BOOL;</v>
       </c>
       <c r="N41" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>COLLECTIONCONVSPD_MA:OpCom; // CHASSIS.OUT0007</v>
       </c>
       <c r="O41" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVSPD_MA</v>
       </c>
       <c r="P41" s="20" t="str">
-        <f>_xlfn.CONCAT(O41,"(); // ",E41)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVSPD_MA(); // CR0709.OUT0007</v>
       </c>
       <c r="Q41" s="20" t="str">
-        <f>_xlfn.CONCAT(O41,".Init('",A41,"','",K41,"','",D41,"','",G41,"',NVL_Outputs_States_",A41,".All.",D41,",NVL_IO_",A9,".All_Outputs_Diag.",D41,",Machine_IO.Node_",A41,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVSPD_MA.Init('CHASSIS','CollectionConvSpd_mA','OUT0007','a23',NVL_Outputs_States_CHASSIS.All.OUT0007,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0007,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R41" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>CollectionConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0007</v>
       </c>
       <c r="S41" s="20" t="str">
-        <f>_xlfn.CONCAT(A41,".",D41,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0007();</v>
       </c>
       <c r="T41" s="20" t="str">
-        <f>_xlfn.CONCAT(A41,".",D41,".Init(",O41,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0007.Init(Machine_IO.Outputs.COLLECTIONCONVSPD_MA);</v>
       </c>
     </row>
@@ -5140,7 +5143,7 @@
         <v>66</v>
       </c>
       <c r="E42" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0008</v>
       </c>
       <c r="F42" s="17" t="s">
@@ -5161,43 +5164,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0008</v>
       </c>
-      <c r="K42" s="30" t="s">
+      <c r="K42" s="19" t="s">
         <v>385</v>
       </c>
       <c r="L42" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>COLLECTIONCONVON_OP</v>
       </c>
       <c r="M42" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CollectionConvOn_OP:BOOL;</v>
       </c>
       <c r="N42" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>COLLECTIONCONVON_OP:OpCom; // CHASSIS.OUT0008</v>
       </c>
       <c r="O42" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVON_OP</v>
       </c>
       <c r="P42" s="20" t="str">
-        <f>_xlfn.CONCAT(O42,"(); // ",E42)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVON_OP(); // CR0709.OUT0008</v>
       </c>
       <c r="Q42" s="20" t="str">
-        <f>_xlfn.CONCAT(O42,".Init('",A42,"','",K42,"','",D42,"','",G42,"',NVL_Outputs_States_",A42,".All.",D42,",NVL_IO_",A10,".All_Outputs_Diag.",D42,",Machine_IO.Node_",A42,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVON_OP.Init('CHASSIS','CollectionConvOn_OP','OUT0008','a24',NVL_Outputs_States_CHASSIS.All.OUT0008,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0008,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R42" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>CollectionConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0008</v>
       </c>
       <c r="S42" s="20" t="str">
-        <f>_xlfn.CONCAT(A42,".",D42,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0008();</v>
       </c>
       <c r="T42" s="20" t="str">
-        <f>_xlfn.CONCAT(A42,".",D42,".Init(",O42,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0008.Init(Machine_IO.Outputs.COLLECTIONCONVON_OP);</v>
       </c>
     </row>
@@ -5236,41 +5239,41 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.GROUP0</v>
       </c>
-      <c r="K43" s="30"/>
+      <c r="K43" s="19"/>
       <c r="L43" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_GROUP0</v>
       </c>
       <c r="M43" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>:BOOL;</v>
       </c>
       <c r="N43" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>SPARE_GROUP0:OpCom; // CHASSIS.GROUP0</v>
       </c>
       <c r="O43" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SPARE_GROUP0</v>
       </c>
       <c r="P43" s="20" t="str">
-        <f>_xlfn.CONCAT(O43,"(); // ",E43)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.SPARE_GROUP0(); // CR0709.GROUP0</v>
       </c>
       <c r="Q43" s="20" t="str">
-        <f>_xlfn.CONCAT(O43,".Init('",A43,"','",K43,"','",D43,"','",G43,"',NVL_Outputs_States_",A43,".All.",D43,",NVL_IO_",A11,".All_Outputs_Diag.",D43,",Machine_IO.Node_",A43,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SPARE_GROUP0.Init('CHASSIS','','GROUP0','a4',NVL_Outputs_States_CHASSIS.All.GROUP0,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP0,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R43" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>: Mimic_Output_FB; // CHASSIS:GROUP0</v>
       </c>
       <c r="S43" s="20" t="str">
-        <f>_xlfn.CONCAT(A43,".",D43,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.GROUP0();</v>
       </c>
       <c r="T43" s="20" t="str">
-        <f>_xlfn.CONCAT(A43,".",D43,".Init(",O43,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.GROUP0.Init(Machine_IO.Outputs.SPARE_GROUP0);</v>
       </c>
     </row>
@@ -5288,7 +5291,7 @@
         <v>70</v>
       </c>
       <c r="E44" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0100</v>
       </c>
       <c r="F44" s="17" t="s">
@@ -5302,50 +5305,50 @@
         <f>_xlfn.XLOOKUP(E44,IfmPinRef!$B$2:$B$199,IfmPinRef!$I$2:$I$199)</f>
         <v>PWM 2.5A</v>
       </c>
-      <c r="I44" s="21" t="s">
-        <v>41</v>
+      <c r="I44" s="30" t="s">
+        <v>526</v>
       </c>
       <c r="J44" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0100</v>
       </c>
-      <c r="K44" s="30" t="s">
+      <c r="K44" s="19" t="s">
         <v>386</v>
       </c>
       <c r="L44" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>DRUMSPD_MA_RAMP_LIMIT</v>
       </c>
       <c r="M44" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>DrumSpd_mA_RAMP_LIMIT:BOOL;</v>
       </c>
       <c r="N44" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>DRUMSPD_MA_RAMP_LIMIT:OpCom; // CHASSIS.OUT0100</v>
       </c>
       <c r="O44" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT</v>
       </c>
       <c r="P44" s="20" t="str">
-        <f>_xlfn.CONCAT(O44,"(); // ",E44)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT(); // CR0709.OUT0100</v>
       </c>
       <c r="Q44" s="20" t="str">
-        <f>_xlfn.CONCAT(O44,".Init('",A44,"','",K44,"','",D44,"','",G44,"',NVL_Outputs_States_",A44,".All.",D44,",NVL_IO_",A12,".All_Outputs_Diag.",D44,",Machine_IO.Node_",A44,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT.Init('CHASSIS','DrumSpd_mA_RAMP_LIMIT','OUT0100','a6',NVL_Outputs_States_CHASSIS.All.OUT0100,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0100,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R44" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>DrumSpd_mA_RAMP_LIMIT: Mimic_Output_FB; // CHASSIS:OUT0100</v>
       </c>
       <c r="S44" s="20" t="str">
-        <f>_xlfn.CONCAT(A44,".",D44,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0100();</v>
       </c>
       <c r="T44" s="20" t="str">
-        <f>_xlfn.CONCAT(A44,".",D44,".Init(",O44,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0100.Init(Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT);</v>
       </c>
     </row>
@@ -5363,7 +5366,7 @@
         <v>71</v>
       </c>
       <c r="E45" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0101</v>
       </c>
       <c r="F45" s="17" t="s">
@@ -5384,43 +5387,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0101</v>
       </c>
-      <c r="K45" s="30" t="s">
+      <c r="K45" s="19" t="s">
         <v>387</v>
       </c>
       <c r="L45" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>TRACKINGMODE</v>
       </c>
       <c r="M45" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>TrackingMode:BOOL;</v>
       </c>
       <c r="N45" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>TRACKINGMODE:OpCom; // CHASSIS.OUT0101</v>
       </c>
       <c r="O45" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.TRACKINGMODE</v>
       </c>
       <c r="P45" s="20" t="str">
-        <f>_xlfn.CONCAT(O45,"(); // ",E45)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.TRACKINGMODE(); // CR0709.OUT0101</v>
       </c>
       <c r="Q45" s="20" t="str">
-        <f>_xlfn.CONCAT(O45,".Init('",A45,"','",K45,"','",D45,"','",G45,"',NVL_Outputs_States_",A45,".All.",D45,",NVL_IO_",A13,".All_Outputs_Diag.",D45,",Machine_IO.Node_",A45,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.TRACKINGMODE.Init('CHASSIS','TrackingMode','OUT0101','a7',NVL_Outputs_States_CHASSIS.All.OUT0101,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0101,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R45" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>TrackingMode: Mimic_Output_FB; // CHASSIS:OUT0101</v>
       </c>
       <c r="S45" s="20" t="str">
-        <f>_xlfn.CONCAT(A45,".",D45,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0101();</v>
       </c>
       <c r="T45" s="20" t="str">
-        <f>_xlfn.CONCAT(A45,".",D45,".Init(",O45,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0101.Init(Machine_IO.Outputs.TRACKINGMODE);</v>
       </c>
     </row>
@@ -5438,7 +5441,7 @@
         <v>72</v>
       </c>
       <c r="E46" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0102</v>
       </c>
       <c r="F46" s="17" t="s">
@@ -5452,50 +5455,50 @@
         <f>_xlfn.XLOOKUP(E46,IfmPinRef!$B$2:$B$199,IfmPinRef!$I$2:$I$199)</f>
         <v>PWM 2.5A</v>
       </c>
-      <c r="I46" s="21" t="s">
-        <v>41</v>
+      <c r="I46" s="30" t="s">
+        <v>526</v>
       </c>
       <c r="J46" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0102</v>
       </c>
-      <c r="K46" s="30" t="s">
+      <c r="K46" s="19" t="s">
         <v>388</v>
       </c>
       <c r="L46" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>FEEDERSPD_MA</v>
       </c>
       <c r="M46" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FeederSpd_mA:BOOL;</v>
       </c>
       <c r="N46" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>FEEDERSPD_MA:OpCom; // CHASSIS.OUT0102</v>
       </c>
       <c r="O46" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.FEEDERSPD_MA</v>
       </c>
       <c r="P46" s="20" t="str">
-        <f>_xlfn.CONCAT(O46,"(); // ",E46)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.FEEDERSPD_MA(); // CR0709.OUT0102</v>
       </c>
       <c r="Q46" s="20" t="str">
-        <f>_xlfn.CONCAT(O46,".Init('",A46,"','",K46,"','",D46,"','",G46,"',NVL_Outputs_States_",A46,".All.",D46,",NVL_IO_",A14,".All_Outputs_Diag.",D46,",Machine_IO.Node_",A46,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.FEEDERSPD_MA.Init('CHASSIS','FeederSpd_mA','OUT0102','a8',NVL_Outputs_States_CHASSIS.All.OUT0102,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0102,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R46" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>FeederSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0102</v>
       </c>
       <c r="S46" s="20" t="str">
-        <f>_xlfn.CONCAT(A46,".",D46,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0102();</v>
       </c>
       <c r="T46" s="20" t="str">
-        <f>_xlfn.CONCAT(A46,".",D46,".Init(",O46,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0102.Init(Machine_IO.Outputs.FEEDERSPD_MA);</v>
       </c>
     </row>
@@ -5513,7 +5516,7 @@
         <v>73</v>
       </c>
       <c r="E47" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0103</v>
       </c>
       <c r="F47" s="17" t="s">
@@ -5534,43 +5537,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0103</v>
       </c>
-      <c r="K47" s="30" t="s">
+      <c r="K47" s="19" t="s">
         <v>389</v>
       </c>
       <c r="L47" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>CRANKENABLE</v>
       </c>
       <c r="M47" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>CrankEnable:BOOL;</v>
       </c>
       <c r="N47" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>CRANKENABLE:OpCom; // CHASSIS.OUT0103</v>
       </c>
       <c r="O47" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.CRANKENABLE</v>
       </c>
       <c r="P47" s="20" t="str">
-        <f>_xlfn.CONCAT(O47,"(); // ",E47)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.CRANKENABLE(); // CR0709.OUT0103</v>
       </c>
       <c r="Q47" s="20" t="str">
-        <f>_xlfn.CONCAT(O47,".Init('",A47,"','",K47,"','",D47,"','",G47,"',NVL_Outputs_States_",A47,".All.",D47,",NVL_IO_",A15,".All_Outputs_Diag.",D47,",Machine_IO.Node_",A47,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.CRANKENABLE.Init('CHASSIS','CrankEnable','OUT0103','a9',NVL_Outputs_States_CHASSIS.All.OUT0103,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0103,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R47" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>CrankEnable: Mimic_Output_FB; // CHASSIS:OUT0103</v>
       </c>
       <c r="S47" s="20" t="str">
-        <f>_xlfn.CONCAT(A47,".",D47,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0103();</v>
       </c>
       <c r="T47" s="20" t="str">
-        <f>_xlfn.CONCAT(A47,".",D47,".Init(",O47,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0103.Init(Machine_IO.Outputs.CRANKENABLE);</v>
       </c>
     </row>
@@ -5588,7 +5591,7 @@
         <v>74</v>
       </c>
       <c r="E48" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0104</v>
       </c>
       <c r="F48" s="17" t="s">
@@ -5609,43 +5612,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0104</v>
       </c>
-      <c r="K48" s="30" t="s">
+      <c r="K48" s="19" t="s">
         <v>390</v>
       </c>
       <c r="L48" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>DIVERTOILTOTRACK_OP</v>
       </c>
       <c r="M48" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>DivertOilToTrack_OP:BOOL;</v>
       </c>
       <c r="N48" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>DIVERTOILTOTRACK_OP:OpCom; // CHASSIS.OUT0104</v>
       </c>
       <c r="O48" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.DIVERTOILTOTRACK_OP</v>
       </c>
       <c r="P48" s="20" t="str">
-        <f>_xlfn.CONCAT(O48,"(); // ",E48)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.DIVERTOILTOTRACK_OP(); // CR0709.OUT0104</v>
       </c>
       <c r="Q48" s="20" t="str">
-        <f>_xlfn.CONCAT(O48,".Init('",A48,"','",K48,"','",D48,"','",G48,"',NVL_Outputs_States_",A48,".All.",D48,",NVL_IO_",A16,".All_Outputs_Diag.",D48,",Machine_IO.Node_",A48,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.DIVERTOILTOTRACK_OP.Init('CHASSIS','DivertOilToTrack_OP','OUT0104','a10',NVL_Outputs_States_CHASSIS.All.OUT0104,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0104,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R48" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>DivertOilToTrack_OP: Mimic_Output_FB; // CHASSIS:OUT0104</v>
       </c>
       <c r="S48" s="20" t="str">
-        <f>_xlfn.CONCAT(A48,".",D48,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0104();</v>
       </c>
       <c r="T48" s="20" t="str">
-        <f>_xlfn.CONCAT(A48,".",D48,".Init(",O48,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0104.Init(Machine_IO.Outputs.DIVERTOILTOTRACK_OP);</v>
       </c>
     </row>
@@ -5663,7 +5666,7 @@
         <v>75</v>
       </c>
       <c r="E49" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0105</v>
       </c>
       <c r="F49" s="17" t="s">
@@ -5684,43 +5687,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0105</v>
       </c>
-      <c r="K49" s="30" t="s">
+      <c r="K49" s="19" t="s">
         <v>391</v>
       </c>
       <c r="L49" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RHS_JACKLEGRAISE_OP</v>
       </c>
       <c r="M49" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>RHS_JackLegRaise_OP:BOOL;</v>
       </c>
       <c r="N49" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>RHS_JACKLEGRAISE_OP:OpCom; // CHASSIS.OUT0105</v>
       </c>
       <c r="O49" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RHS_JACKLEGRAISE_OP</v>
       </c>
       <c r="P49" s="20" t="str">
-        <f>_xlfn.CONCAT(O49,"(); // ",E49)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.RHS_JACKLEGRAISE_OP(); // CR0709.OUT0105</v>
       </c>
       <c r="Q49" s="20" t="str">
-        <f>_xlfn.CONCAT(O49,".Init('",A49,"','",K49,"','",D49,"','",G49,"',NVL_Outputs_States_",A49,".All.",D49,",NVL_IO_",A17,".All_Outputs_Diag.",D49,",Machine_IO.Node_",A49,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.RHS_JACKLEGRAISE_OP.Init('CHASSIS','RHS_JackLegRaise_OP','OUT0105','a11',NVL_Outputs_States_CHASSIS.All.OUT0105,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0105,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R49" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>RHS_JackLegRaise_OP: Mimic_Output_FB; // CHASSIS:OUT0105</v>
       </c>
       <c r="S49" s="20" t="str">
-        <f>_xlfn.CONCAT(A49,".",D49,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0105();</v>
       </c>
       <c r="T49" s="20" t="str">
-        <f>_xlfn.CONCAT(A49,".",D49,".Init(",O49,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0105.Init(Machine_IO.Outputs.RHS_JACKLEGRAISE_OP);</v>
       </c>
     </row>
@@ -5738,7 +5741,7 @@
         <v>76</v>
       </c>
       <c r="E50" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0106</v>
       </c>
       <c r="F50" s="17" t="s">
@@ -5759,43 +5762,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0106</v>
       </c>
-      <c r="K50" s="30" t="s">
+      <c r="K50" s="19" t="s">
         <v>392</v>
       </c>
       <c r="L50" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>TAILCONVON_OP</v>
       </c>
       <c r="M50" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>TailConvOn_OP:BOOL;</v>
       </c>
       <c r="N50" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>TAILCONVON_OP:OpCom; // CHASSIS.OUT0106</v>
       </c>
       <c r="O50" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.TAILCONVON_OP</v>
       </c>
       <c r="P50" s="20" t="str">
-        <f>_xlfn.CONCAT(O50,"(); // ",E50)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.TAILCONVON_OP(); // CR0709.OUT0106</v>
       </c>
       <c r="Q50" s="20" t="str">
-        <f>_xlfn.CONCAT(O50,".Init('",A50,"','",K50,"','",D50,"','",G50,"',NVL_Outputs_States_",A50,".All.",D50,",NVL_IO_",A18,".All_Outputs_Diag.",D50,",Machine_IO.Node_",A50,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.TAILCONVON_OP.Init('CHASSIS','TailConvOn_OP','OUT0106','a12',NVL_Outputs_States_CHASSIS.All.OUT0106,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0106,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R50" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>TailConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0106</v>
       </c>
       <c r="S50" s="20" t="str">
-        <f>_xlfn.CONCAT(A50,".",D50,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0106();</v>
       </c>
       <c r="T50" s="20" t="str">
-        <f>_xlfn.CONCAT(A50,".",D50,".Init(",O50,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0106.Init(Machine_IO.Outputs.TAILCONVON_OP);</v>
       </c>
     </row>
@@ -5813,7 +5816,7 @@
         <v>77</v>
       </c>
       <c r="E51" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0107</v>
       </c>
       <c r="F51" s="17" t="s">
@@ -5834,43 +5837,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0107</v>
       </c>
-      <c r="K51" s="30" t="s">
+      <c r="K51" s="19" t="s">
         <v>393</v>
       </c>
       <c r="L51" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SIDECONVON_OP</v>
       </c>
       <c r="M51" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SideConvOn_OP:BOOL;</v>
       </c>
       <c r="N51" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>SIDECONVON_OP:OpCom; // CHASSIS.OUT0107</v>
       </c>
       <c r="O51" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDECONVON_OP</v>
       </c>
       <c r="P51" s="20" t="str">
-        <f>_xlfn.CONCAT(O51,"(); // ",E51)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.SIDECONVON_OP(); // CR0709.OUT0107</v>
       </c>
       <c r="Q51" s="20" t="str">
-        <f>_xlfn.CONCAT(O51,".Init('",A51,"','",K51,"','",D51,"','",G51,"',NVL_Outputs_States_",A51,".All.",D51,",NVL_IO_",A19,".All_Outputs_Diag.",D51,",Machine_IO.Node_",A51,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SIDECONVON_OP.Init('CHASSIS','SideConvOn_OP','OUT0107','a13',NVL_Outputs_States_CHASSIS.All.OUT0107,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0107,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R51" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>SideConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0107</v>
       </c>
       <c r="S51" s="20" t="str">
-        <f>_xlfn.CONCAT(A51,".",D51,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0107();</v>
       </c>
       <c r="T51" s="20" t="str">
-        <f>_xlfn.CONCAT(A51,".",D51,".Init(",O51,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0107.Init(Machine_IO.Outputs.SIDECONVON_OP);</v>
       </c>
     </row>
@@ -5888,7 +5891,7 @@
         <v>78</v>
       </c>
       <c r="E52" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0108</v>
       </c>
       <c r="F52" s="17" t="s">
@@ -5909,43 +5912,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0108</v>
       </c>
-      <c r="K52" s="30" t="s">
+      <c r="K52" s="19" t="s">
         <v>394</v>
       </c>
       <c r="L52" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SIDETRANSFERON_OP</v>
       </c>
       <c r="M52" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>SideTransferOn_OP:BOOL;</v>
       </c>
       <c r="N52" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>SIDETRANSFERON_OP:OpCom; // CHASSIS.OUT0108</v>
       </c>
       <c r="O52" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDETRANSFERON_OP</v>
       </c>
       <c r="P52" s="20" t="str">
-        <f>_xlfn.CONCAT(O52,"(); // ",E52)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.SIDETRANSFERON_OP(); // CR0709.OUT0108</v>
       </c>
       <c r="Q52" s="20" t="str">
-        <f>_xlfn.CONCAT(O52,".Init('",A52,"','",K52,"','",D52,"','",G52,"',NVL_Outputs_States_",A52,".All.",D52,",NVL_IO_",A20,".All_Outputs_Diag.",D52,",Machine_IO.Node_",A52,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SIDETRANSFERON_OP.Init('CHASSIS','SideTransferOn_OP','OUT0108','a14',NVL_Outputs_States_CHASSIS.All.OUT0108,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0108,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R52" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>SideTransferOn_OP: Mimic_Output_FB; // CHASSIS:OUT0108</v>
       </c>
       <c r="S52" s="20" t="str">
-        <f>_xlfn.CONCAT(A52,".",D52,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0108();</v>
       </c>
       <c r="T52" s="20" t="str">
-        <f>_xlfn.CONCAT(A52,".",D52,".Init(",O52,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0108.Init(Machine_IO.Outputs.SIDETRANSFERON_OP);</v>
       </c>
     </row>
@@ -5984,41 +5987,41 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.GROUP1</v>
       </c>
-      <c r="K53" s="30"/>
+      <c r="K53" s="19"/>
       <c r="L53" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_GROUP1</v>
       </c>
       <c r="M53" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>:BOOL;</v>
       </c>
       <c r="N53" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>SPARE_GROUP1:OpCom; // CHASSIS.GROUP1</v>
       </c>
       <c r="O53" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SPARE_GROUP1</v>
       </c>
       <c r="P53" s="20" t="str">
-        <f>_xlfn.CONCAT(O53,"(); // ",E53)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.SPARE_GROUP1(); // CR0709.GROUP1</v>
       </c>
       <c r="Q53" s="20" t="str">
-        <f>_xlfn.CONCAT(O53,".Init('",A53,"','",K53,"','",D53,"','",G53,"',NVL_Outputs_States_",A53,".All.",D53,",NVL_IO_",A21,".All_Outputs_Diag.",D53,",Machine_IO.Node_",A53,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SPARE_GROUP1.Init('CHASSIS','','GROUP1','a3',NVL_Outputs_States_CHASSIS.All.GROUP1,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP1,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R53" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>: Mimic_Output_FB; // CHASSIS:GROUP1</v>
       </c>
       <c r="S53" s="20" t="str">
-        <f>_xlfn.CONCAT(A53,".",D53,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.GROUP1();</v>
       </c>
       <c r="T53" s="20" t="str">
-        <f>_xlfn.CONCAT(A53,".",D53,".Init(",O53,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.GROUP1.Init(Machine_IO.Outputs.SPARE_GROUP1);</v>
       </c>
     </row>
@@ -6036,7 +6039,7 @@
         <v>80</v>
       </c>
       <c r="E54" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0200</v>
       </c>
       <c r="F54" s="17" t="s">
@@ -6057,43 +6060,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0200</v>
       </c>
-      <c r="K54" s="30" t="s">
+      <c r="K54" s="19" t="s">
         <v>395</v>
       </c>
       <c r="L54" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>LEFTTRACKDIVERT_OP</v>
       </c>
       <c r="M54" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>LeftTrackDivert_OP:BOOL;</v>
       </c>
       <c r="N54" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>LEFTTRACKDIVERT_OP:OpCom; // CHASSIS.OUT0200</v>
       </c>
       <c r="O54" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LEFTTRACKDIVERT_OP</v>
       </c>
       <c r="P54" s="20" t="str">
-        <f>_xlfn.CONCAT(O54,"(); // ",E54)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.LEFTTRACKDIVERT_OP(); // CR0709.OUT0200</v>
       </c>
       <c r="Q54" s="20" t="str">
-        <f>_xlfn.CONCAT(O54,".Init('",A54,"','",K54,"','",D54,"','",G54,"',NVL_Outputs_States_",A54,".All.",D54,",NVL_IO_",A22,".All_Outputs_Diag.",D54,",Machine_IO.Node_",A54,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.LEFTTRACKDIVERT_OP.Init('CHASSIS','LeftTrackDivert_OP','OUT0200','a73',NVL_Outputs_States_CHASSIS.All.OUT0200,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0200,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R54" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>LeftTrackDivert_OP: Mimic_Output_FB; // CHASSIS:OUT0200</v>
       </c>
       <c r="S54" s="20" t="str">
-        <f>_xlfn.CONCAT(A54,".",D54,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0200();</v>
       </c>
       <c r="T54" s="20" t="str">
-        <f>_xlfn.CONCAT(A54,".",D54,".Init(",O54,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0200.Init(Machine_IO.Outputs.LEFTTRACKDIVERT_OP);</v>
       </c>
     </row>
@@ -6111,7 +6114,7 @@
         <v>81</v>
       </c>
       <c r="E55" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0201</v>
       </c>
       <c r="F55" s="17" t="s">
@@ -6132,43 +6135,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0201</v>
       </c>
-      <c r="K55" s="30" t="s">
+      <c r="K55" s="19" t="s">
         <v>396</v>
       </c>
       <c r="L55" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>LTF_OP</v>
       </c>
       <c r="M55" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>LTF_OP:BOOL;</v>
       </c>
       <c r="N55" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>LTF_OP:OpCom; // CHASSIS.OUT0201</v>
       </c>
       <c r="O55" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LTF_OP</v>
       </c>
       <c r="P55" s="20" t="str">
-        <f>_xlfn.CONCAT(O55,"(); // ",E55)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.LTF_OP(); // CR0709.OUT0201</v>
       </c>
       <c r="Q55" s="20" t="str">
-        <f>_xlfn.CONCAT(O55,".Init('",A55,"','",K55,"','",D55,"','",G55,"',NVL_Outputs_States_",A55,".All.",D55,",NVL_IO_",A23,".All_Outputs_Diag.",D55,",Machine_IO.Node_",A55,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.LTF_OP.Init('CHASSIS','LTF_OP','OUT0201','a74',NVL_Outputs_States_CHASSIS.All.OUT0201,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0201,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R55" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>LTF_OP: Mimic_Output_FB; // CHASSIS:OUT0201</v>
       </c>
       <c r="S55" s="20" t="str">
-        <f>_xlfn.CONCAT(A55,".",D55,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0201();</v>
       </c>
       <c r="T55" s="20" t="str">
-        <f>_xlfn.CONCAT(A55,".",D55,".Init(",O55,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0201.Init(Machine_IO.Outputs.LTF_OP);</v>
       </c>
     </row>
@@ -6186,7 +6189,7 @@
         <v>82</v>
       </c>
       <c r="E56" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0202</v>
       </c>
       <c r="F56" s="17" t="s">
@@ -6207,43 +6210,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0202</v>
       </c>
-      <c r="K56" s="30" t="s">
+      <c r="K56" s="19" t="s">
         <v>397</v>
       </c>
       <c r="L56" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>LTR_OP</v>
       </c>
       <c r="M56" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>LTR_OP:BOOL;</v>
       </c>
       <c r="N56" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>LTR_OP:OpCom; // CHASSIS.OUT0202</v>
       </c>
       <c r="O56" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LTR_OP</v>
       </c>
       <c r="P56" s="20" t="str">
-        <f>_xlfn.CONCAT(O56,"(); // ",E56)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.LTR_OP(); // CR0709.OUT0202</v>
       </c>
       <c r="Q56" s="20" t="str">
-        <f>_xlfn.CONCAT(O56,".Init('",A56,"','",K56,"','",D56,"','",G56,"',NVL_Outputs_States_",A56,".All.",D56,",NVL_IO_",A24,".All_Outputs_Diag.",D56,",Machine_IO.Node_",A56,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.LTR_OP.Init('CHASSIS','LTR_OP','OUT0202','a75',NVL_Outputs_States_CHASSIS.All.OUT0202,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0202,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R56" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>LTR_OP: Mimic_Output_FB; // CHASSIS:OUT0202</v>
       </c>
       <c r="S56" s="20" t="str">
-        <f>_xlfn.CONCAT(A56,".",D56,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0202();</v>
       </c>
       <c r="T56" s="20" t="str">
-        <f>_xlfn.CONCAT(A56,".",D56,".Init(",O56,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0202.Init(Machine_IO.Outputs.LTR_OP);</v>
       </c>
     </row>
@@ -6261,7 +6264,7 @@
         <v>83</v>
       </c>
       <c r="E57" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0203</v>
       </c>
       <c r="F57" s="17" t="s">
@@ -6282,43 +6285,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0203</v>
       </c>
-      <c r="K57" s="30" t="s">
+      <c r="K57" s="19" t="s">
         <v>398</v>
       </c>
       <c r="L57" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RIGHTTRACKDIVERT_OP</v>
       </c>
       <c r="M57" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>RightTrackDivert_OP:BOOL;</v>
       </c>
       <c r="N57" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>RIGHTTRACKDIVERT_OP:OpCom; // CHASSIS.OUT0203</v>
       </c>
       <c r="O57" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RIGHTTRACKDIVERT_OP</v>
       </c>
       <c r="P57" s="20" t="str">
-        <f>_xlfn.CONCAT(O57,"(); // ",E57)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.RIGHTTRACKDIVERT_OP(); // CR0709.OUT0203</v>
       </c>
       <c r="Q57" s="20" t="str">
-        <f>_xlfn.CONCAT(O57,".Init('",A57,"','",K57,"','",D57,"','",G57,"',NVL_Outputs_States_",A57,".All.",D57,",NVL_IO_",A25,".All_Outputs_Diag.",D57,",Machine_IO.Node_",A57,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.RIGHTTRACKDIVERT_OP.Init('CHASSIS','RightTrackDivert_OP','OUT0203','a76',NVL_Outputs_States_CHASSIS.All.OUT0203,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0203,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R57" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>RightTrackDivert_OP: Mimic_Output_FB; // CHASSIS:OUT0203</v>
       </c>
       <c r="S57" s="20" t="str">
-        <f>_xlfn.CONCAT(A57,".",D57,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0203();</v>
       </c>
       <c r="T57" s="20" t="str">
-        <f>_xlfn.CONCAT(A57,".",D57,".Init(",O57,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0203.Init(Machine_IO.Outputs.RIGHTTRACKDIVERT_OP);</v>
       </c>
     </row>
@@ -6336,7 +6339,7 @@
         <v>84</v>
       </c>
       <c r="E58" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0204</v>
       </c>
       <c r="F58" s="17" t="s">
@@ -6357,43 +6360,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0204</v>
       </c>
-      <c r="K58" s="30" t="s">
+      <c r="K58" s="19" t="s">
         <v>399</v>
       </c>
       <c r="L58" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RTF_OP</v>
       </c>
       <c r="M58" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>RTF_OP:BOOL;</v>
       </c>
       <c r="N58" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>RTF_OP:OpCom; // CHASSIS.OUT0204</v>
       </c>
       <c r="O58" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RTF_OP</v>
       </c>
       <c r="P58" s="20" t="str">
-        <f>_xlfn.CONCAT(O58,"(); // ",E58)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.RTF_OP(); // CR0709.OUT0204</v>
       </c>
       <c r="Q58" s="20" t="str">
-        <f>_xlfn.CONCAT(O58,".Init('",A58,"','",K58,"','",D58,"','",G58,"',NVL_Outputs_States_",A58,".All.",D58,",NVL_IO_",A26,".All_Outputs_Diag.",D58,",Machine_IO.Node_",A58,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.RTF_OP.Init('CHASSIS','RTF_OP','OUT0204','a77',NVL_Outputs_States_CHASSIS.All.OUT0204,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0204,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R58" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>RTF_OP: Mimic_Output_FB; // CHASSIS:OUT0204</v>
       </c>
       <c r="S58" s="20" t="str">
-        <f>_xlfn.CONCAT(A58,".",D58,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0204();</v>
       </c>
       <c r="T58" s="20" t="str">
-        <f>_xlfn.CONCAT(A58,".",D58,".Init(",O58,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0204.Init(Machine_IO.Outputs.RTF_OP);</v>
       </c>
     </row>
@@ -6411,7 +6414,7 @@
         <v>85</v>
       </c>
       <c r="E59" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0205</v>
       </c>
       <c r="F59" s="17" t="s">
@@ -6432,43 +6435,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0205</v>
       </c>
-      <c r="K59" s="30" t="s">
+      <c r="K59" s="19" t="s">
         <v>400</v>
       </c>
       <c r="L59" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>RTR_OP</v>
       </c>
       <c r="M59" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>RTR_OP:BOOL;</v>
       </c>
       <c r="N59" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>RTR_OP:OpCom; // CHASSIS.OUT0205</v>
       </c>
       <c r="O59" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RTR_OP</v>
       </c>
       <c r="P59" s="20" t="str">
-        <f>_xlfn.CONCAT(O59,"(); // ",E59)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.RTR_OP(); // CR0709.OUT0205</v>
       </c>
       <c r="Q59" s="20" t="str">
-        <f>_xlfn.CONCAT(O59,".Init('",A59,"','",K59,"','",D59,"','",G59,"',NVL_Outputs_States_",A59,".All.",D59,",NVL_IO_",A27,".All_Outputs_Diag.",D59,",Machine_IO.Node_",A59,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.RTR_OP.Init('CHASSIS','RTR_OP','OUT0205','a78',NVL_Outputs_States_CHASSIS.All.OUT0205,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0205,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R59" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>RTR_OP: Mimic_Output_FB; // CHASSIS:OUT0205</v>
       </c>
       <c r="S59" s="20" t="str">
-        <f>_xlfn.CONCAT(A59,".",D59,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0205();</v>
       </c>
       <c r="T59" s="20" t="str">
-        <f>_xlfn.CONCAT(A59,".",D59,".Init(",O59,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0205.Init(Machine_IO.Outputs.RTR_OP);</v>
       </c>
     </row>
@@ -6486,7 +6489,7 @@
         <v>86</v>
       </c>
       <c r="E60" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0206</v>
       </c>
       <c r="F60" s="17" t="s">
@@ -6507,43 +6510,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0206</v>
       </c>
-      <c r="K60" s="30" t="s">
+      <c r="K60" s="19" t="s">
         <v>401</v>
       </c>
       <c r="L60" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>DRUMONOFF_OP</v>
       </c>
       <c r="M60" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>DrumOnOff_OP:BOOL;</v>
       </c>
       <c r="N60" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>DRUMONOFF_OP:OpCom; // CHASSIS.OUT0206</v>
       </c>
       <c r="O60" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.DRUMONOFF_OP</v>
       </c>
       <c r="P60" s="20" t="str">
-        <f>_xlfn.CONCAT(O60,"(); // ",E60)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.DRUMONOFF_OP(); // CR0709.OUT0206</v>
       </c>
       <c r="Q60" s="20" t="str">
-        <f>_xlfn.CONCAT(O60,".Init('",A60,"','",K60,"','",D60,"','",G60,"',NVL_Outputs_States_",A60,".All.",D60,",NVL_IO_",A28,".All_Outputs_Diag.",D60,",Machine_IO.Node_",A60,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.DRUMONOFF_OP.Init('CHASSIS','DrumOnOff_OP','OUT0206','a79',NVL_Outputs_States_CHASSIS.All.OUT0206,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0206,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R60" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>DrumOnOff_OP: Mimic_Output_FB; // CHASSIS:OUT0206</v>
       </c>
       <c r="S60" s="20" t="str">
-        <f>_xlfn.CONCAT(A60,".",D60,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0206();</v>
       </c>
       <c r="T60" s="20" t="str">
-        <f>_xlfn.CONCAT(A60,".",D60,".Init(",O60,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0206.Init(Machine_IO.Outputs.DRUMONOFF_OP);</v>
       </c>
     </row>
@@ -6561,7 +6564,7 @@
         <v>87</v>
       </c>
       <c r="E61" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0207</v>
       </c>
       <c r="F61" s="17" t="s">
@@ -6582,43 +6585,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0207</v>
       </c>
-      <c r="K61" s="30" t="s">
+      <c r="K61" s="19" t="s">
         <v>402</v>
       </c>
       <c r="L61" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>FEEDERONOFF_OP</v>
       </c>
       <c r="M61" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>FeederOnOff_OP:BOOL;</v>
       </c>
       <c r="N61" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>FEEDERONOFF_OP:OpCom; // CHASSIS.OUT0207</v>
       </c>
       <c r="O61" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.FEEDERONOFF_OP</v>
       </c>
       <c r="P61" s="20" t="str">
-        <f>_xlfn.CONCAT(O61,"(); // ",E61)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.FEEDERONOFF_OP(); // CR0709.OUT0207</v>
       </c>
       <c r="Q61" s="20" t="str">
-        <f>_xlfn.CONCAT(O61,".Init('",A61,"','",K61,"','",D61,"','",G61,"',NVL_Outputs_States_",A61,".All.",D61,",NVL_IO_",A29,".All_Outputs_Diag.",D61,",Machine_IO.Node_",A61,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.FEEDERONOFF_OP.Init('CHASSIS','FeederOnOff_OP','OUT0207','a80',NVL_Outputs_States_CHASSIS.All.OUT0207,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0207,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R61" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>FeederOnOff_OP: Mimic_Output_FB; // CHASSIS:OUT0207</v>
       </c>
       <c r="S61" s="20" t="str">
-        <f>_xlfn.CONCAT(A61,".",D61,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0207();</v>
       </c>
       <c r="T61" s="20" t="str">
-        <f>_xlfn.CONCAT(A61,".",D61,".Init(",O61,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0207.Init(Machine_IO.Outputs.FEEDERONOFF_OP);</v>
       </c>
     </row>
@@ -6636,7 +6639,7 @@
         <v>88</v>
       </c>
       <c r="E62" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT0208</v>
       </c>
       <c r="F62" s="17" t="s">
@@ -6657,43 +6660,43 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0208</v>
       </c>
-      <c r="K62" s="30" t="s">
+      <c r="K62" s="19" t="s">
         <v>403</v>
       </c>
       <c r="L62" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>ECUENABLE</v>
       </c>
       <c r="M62" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>ECUenable:BOOL;</v>
       </c>
       <c r="N62" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>ECUENABLE:OpCom; // CHASSIS.OUT0208</v>
       </c>
       <c r="O62" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.ECUENABLE</v>
       </c>
       <c r="P62" s="20" t="str">
-        <f>_xlfn.CONCAT(O62,"(); // ",E62)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.ECUENABLE(); // CR0709.OUT0208</v>
       </c>
       <c r="Q62" s="20" t="str">
-        <f>_xlfn.CONCAT(O62,".Init('",A62,"','",K62,"','",D62,"','",G62,"',NVL_Outputs_States_",A62,".All.",D62,",NVL_IO_",A30,".All_Outputs_Diag.",D62,",Machine_IO.Node_",A62,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.ECUENABLE.Init('CHASSIS','ECUenable','OUT0208','a81',NVL_Outputs_States_CHASSIS.All.OUT0208,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0208,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R62" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>ECUenable: Mimic_Output_FB; // CHASSIS:OUT0208</v>
       </c>
       <c r="S62" s="20" t="str">
-        <f>_xlfn.CONCAT(A62,".",D62,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT0208();</v>
       </c>
       <c r="T62" s="20" t="str">
-        <f>_xlfn.CONCAT(A62,".",D62,".Init(",O62,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0208.Init(Machine_IO.Outputs.ECUENABLE);</v>
       </c>
     </row>
@@ -6732,41 +6735,41 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.GROUP2</v>
       </c>
-      <c r="K63" s="30"/>
+      <c r="K63" s="19"/>
       <c r="L63" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_GROUP2</v>
       </c>
       <c r="M63" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>:BOOL;</v>
       </c>
       <c r="N63" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>SPARE_GROUP2:OpCom; // CHASSIS.GROUP2</v>
       </c>
       <c r="O63" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SPARE_GROUP2</v>
       </c>
       <c r="P63" s="20" t="str">
-        <f>_xlfn.CONCAT(O63,"(); // ",E63)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.SPARE_GROUP2(); // CR0709.GROUP2</v>
       </c>
       <c r="Q63" s="20" t="str">
-        <f>_xlfn.CONCAT(O63,".Init('",A63,"','",K63,"','",D63,"','",G63,"',NVL_Outputs_States_",A63,".All.",D63,",NVL_IO_",A31,".All_Outputs_Diag.",D63,",Machine_IO.Node_",A63,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SPARE_GROUP2.Init('CHASSIS','','GROUP2','a1',NVL_Outputs_States_CHASSIS.All.GROUP2,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP2,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R63" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>: Mimic_Output_FB; // CHASSIS:GROUP2</v>
       </c>
       <c r="S63" s="20" t="str">
-        <f>_xlfn.CONCAT(A63,".",D63,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.GROUP2();</v>
       </c>
       <c r="T63" s="20" t="str">
-        <f>_xlfn.CONCAT(A63,".",D63,".Init(",O63,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.GROUP2.Init(Machine_IO.Outputs.SPARE_GROUP2);</v>
       </c>
     </row>
@@ -6784,7 +6787,7 @@
         <v>90</v>
       </c>
       <c r="E64" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT3000</v>
       </c>
       <c r="F64" s="17" t="s">
@@ -6803,41 +6806,41 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT3000</v>
       </c>
-      <c r="K64" s="30"/>
+      <c r="K64" s="19"/>
       <c r="L64" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_OUT3000</v>
       </c>
       <c r="M64" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>:BOOL;</v>
       </c>
       <c r="N64" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>SPARE_OUT3000:OpCom; // CHASSIS.OUT3000</v>
       </c>
       <c r="O64" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SPARE_OUT3000</v>
       </c>
       <c r="P64" s="20" t="str">
-        <f>_xlfn.CONCAT(O64,"(); // ",E64)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.SPARE_OUT3000(); // CR0709.OUT3000</v>
       </c>
       <c r="Q64" s="20" t="str">
-        <f>_xlfn.CONCAT(O64,".Init('",A64,"','",K64,"','",D64,"','",G64,"',NVL_Outputs_States_",A64,".All.",D64,",NVL_IO_",A32,".All_Outputs_Diag.",D64,",Machine_IO.Node_",A64,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SPARE_OUT3000.Init('CHASSIS','','OUT3000','a31',NVL_Outputs_States_CHASSIS.All.OUT3000,NVL_IO_CHASSIS.All_Outputs_Diag.OUT3000,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R64" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>: Mimic_Output_FB; // CHASSIS:OUT3000</v>
       </c>
       <c r="S64" s="20" t="str">
-        <f>_xlfn.CONCAT(A64,".",D64,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT3000();</v>
       </c>
       <c r="T64" s="20" t="str">
-        <f>_xlfn.CONCAT(A64,".",D64,".Init(",O64,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT3000.Init(Machine_IO.Outputs.SPARE_OUT3000);</v>
       </c>
     </row>
@@ -6855,7 +6858,7 @@
         <v>92</v>
       </c>
       <c r="E65" s="17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>CR0709.OUT3001</v>
       </c>
       <c r="F65" s="17" t="s">
@@ -6874,41 +6877,41 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT3001</v>
       </c>
-      <c r="K65" s="30"/>
+      <c r="K65" s="19"/>
       <c r="L65" s="19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>SPARE_OUT3001</v>
       </c>
       <c r="M65" s="19" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>:BOOL;</v>
       </c>
       <c r="N65" s="20" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>SPARE_OUT3001:OpCom; // CHASSIS.OUT3001</v>
       </c>
       <c r="O65" s="20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SPARE_OUT3001</v>
       </c>
       <c r="P65" s="20" t="str">
-        <f>_xlfn.CONCAT(O65,"(); // ",E65)</f>
+        <f t="shared" si="12"/>
         <v>Machine_IO.Outputs.SPARE_OUT3001(); // CR0709.OUT3001</v>
       </c>
       <c r="Q65" s="20" t="str">
-        <f>_xlfn.CONCAT(O65,".Init('",A65,"','",K65,"','",D65,"','",G65,"',NVL_Outputs_States_",A65,".All.",D65,",NVL_IO_",A33,".All_Outputs_Diag.",D65,",Machine_IO.Node_",A65,");")</f>
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SPARE_OUT3001.Init('CHASSIS','','OUT3001','a32',NVL_Outputs_States_CHASSIS.All.OUT3001,NVL_IO_CHASSIS.All_Outputs_Diag.OUT3001,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R65" s="20" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>: Mimic_Output_FB; // CHASSIS:OUT3001</v>
       </c>
       <c r="S65" s="20" t="str">
-        <f>_xlfn.CONCAT(A65,".",D65,"();")</f>
+        <f t="shared" si="15"/>
         <v>CHASSIS.OUT3001();</v>
       </c>
       <c r="T65" s="20" t="str">
-        <f>_xlfn.CONCAT(A65,".",D65,".Init(",O65,");")</f>
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT3001.Init(Machine_IO.Outputs.SPARE_OUT3001);</v>
       </c>
     </row>
@@ -6923,7 +6926,6 @@
       <c r="H66" s="23"/>
       <c r="I66" s="23"/>
       <c r="J66" s="23"/>
-      <c r="K66" s="31"/>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
@@ -6943,7 +6945,6 @@
       <c r="H67" s="23"/>
       <c r="I67" s="23"/>
       <c r="J67" s="23"/>
-      <c r="K67" s="31"/>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
@@ -15235,22 +15236,22 @@
         <v>356</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H28" si="3">_xlfn.CONCAT(G2," {",B2,".",C2,"}")</f>
+        <f t="shared" ref="H2:H25" si="3">_xlfn.CONCAT(G2," {",B2,".",C2,"}")</f>
         <v>ESTOP_OK {CHASSIS.CHASSIS.IN0100}</v>
       </c>
       <c r="I2" s="26">
-        <f t="shared" ref="I2:I28" si="4">LEN(H2)</f>
+        <f t="shared" ref="I2:I25" si="4">LEN(H2)</f>
         <v>33</v>
       </c>
       <c r="J2" t="s">
         <v>296</v>
       </c>
       <c r="K2" t="str">
-        <f t="shared" ref="K2:K28" si="5">_xlfn.CONCAT(G2,"(Bit_Input:=",J2,".Alarm_Active",",ID:=",A2,",Description:='",H2,"',Add_Info:=",J2,".AlmLog.Buffer",");")</f>
+        <f t="shared" ref="K2:K25" si="5">_xlfn.CONCAT(G2,"(Bit_Input:=",J2,".Alarm_Active",",ID:=",A2,",Description:='",H2,"',Add_Info:=",J2,".AlmLog.Buffer",");")</f>
         <v>ESTOP_OK(Bit_Input:=Machine_IO.CHASSIS_Inputs.EStop_Safety_Relay_Signal.Alarm_Active,ID:=2000,Description:='ESTOP_OK {CHASSIS.CHASSIS.IN0100}',Add_Info:=Machine_IO.CHASSIS_Inputs.EStop_Safety_Relay_Signal.AlmLog.Buffer);</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:L28" si="6">_xlfn.CONCAT(G2,": MGSE_AlarmBit;")</f>
+        <f t="shared" ref="L2:L25" si="6">_xlfn.CONCAT(G2,": MGSE_AlarmBit;")</f>
         <v>ESTOP_OK: MGSE_AlarmBit;</v>
       </c>
     </row>
@@ -16675,22 +16676,22 @@
         <v>422</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" ref="H29:H48" si="14">_xlfn.CONCAT(G34," {",B34,".",C34,"}")</f>
+        <f t="shared" ref="H34" si="14">_xlfn.CONCAT(G34," {",B34,".",C34,"}")</f>
         <v>TAILCONVSPD_MA {CHASSIS.CHASSIS.OUT0000}</v>
       </c>
       <c r="I34" s="26">
-        <f t="shared" ref="I29:I48" si="15">LEN(H34)</f>
+        <f t="shared" ref="I34" si="15">LEN(H34)</f>
         <v>40</v>
       </c>
       <c r="J34" t="s">
         <v>320</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" ref="K29:K48" si="16">_xlfn.CONCAT(G34,"(Bit_Input:=",J34,".Alarm_Active",",ID:=",A34,",Description:='",H34,"',Add_Info:=",J34,".AlmLog.Buffer",");")</f>
+        <f t="shared" ref="K34" si="16">_xlfn.CONCAT(G34,"(Bit_Input:=",J34,".Alarm_Active",",ID:=",A34,",Description:='",H34,"',Add_Info:=",J34,".AlmLog.Buffer",");")</f>
         <v>TAILCONVSPD_MA(Bit_Input:=Machine_IO.CHASSIS_Outputs.Cabin_Panel_Active_LED.Alarm_Active,ID:=2032,Description:='TAILCONVSPD_MA {CHASSIS.CHASSIS.OUT0000}',Add_Info:=Machine_IO.CHASSIS_Outputs.Cabin_Panel_Active_LED.AlmLog.Buffer);</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" ref="L29:L48" si="17">_xlfn.CONCAT(G34,": MGSE_AlarmBit;")</f>
+        <f t="shared" ref="L34" si="17">_xlfn.CONCAT(G34,": MGSE_AlarmBit;")</f>
         <v>TAILCONVSPD_MA: MGSE_AlarmBit;</v>
       </c>
     </row>
@@ -18105,6 +18106,24 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
+    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
+      <UserInfo>
+        <DisplayName>Noel Loughran</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9F7729ADF49144A01A6175DD599202" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f00ebe7287476f312414df31db46304">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c96d9849-7071-4555-8535-ee11c374d0f7" xmlns:ns3="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f2e969a0d0c60cbdf6bd0d859a86451" ns2:_="" ns3:_="">
     <xsd:import namespace="c96d9849-7071-4555-8535-ee11c374d0f7"/>
@@ -18327,24 +18346,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
-    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
-      <UserInfo>
-        <DisplayName>Noel Loughran</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
   <ds:schemaRefs>
@@ -18354,6 +18355,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6596B7D1-B3E6-40CB-B05E-2E959D1A2B6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18370,21 +18388,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
IO now correct in the dianostics screens
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53C2771-E259-4076-82A8-10FB9466EC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8915D6B6-E630-4487-8700-A6FB902527C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="530">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1624,6 +1624,15 @@
   </si>
   <si>
     <t>PWM_CUR</t>
+  </si>
+  <si>
+    <t>SUPPLY_GROUP0</t>
+  </si>
+  <si>
+    <t>SUPPLY_GROUP1</t>
+  </si>
+  <si>
+    <t>SUPPLY_GROUP2</t>
   </si>
 </sst>
 </file>
@@ -2171,9 +2180,9 @@
   </sheetPr>
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2317,7 +2326,7 @@
         <v>Machine_IO.Inputs.ESTOP_OK(); // CR0709.IN0100</v>
       </c>
       <c r="Q2" s="20" t="str">
-        <f>_xlfn.CONCAT("Machine_IO.","Inputs.",K2,".Init('",A2,"','",K2,"','",D2,"','",G2,"',","NVL_IO_",A2,".All_Inputs.",D2,",Machine_IO.Node_",A2,");")</f>
+        <f>_xlfn.CONCAT("Machine_IO.","Inputs.",L2,".Init('",A2,"','",L2,"','",D2,"','",G2,"',","NVL_IO_",A2,".All_Inputs.",D2,",Machine_IO.Node_",A2,");")</f>
         <v>Machine_IO.Inputs.ESTOP_OK.Init('CHASSIS','ESTOP_OK','IN0100','a63',NVL_IO_CHASSIS.All_Inputs.IN0100,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R2" s="20" t="str">
@@ -2389,7 +2398,7 @@
         <v>Machine_IO.Inputs.DRUM_PRESSURE(); // CR0709.IN0101</v>
       </c>
       <c r="Q3" s="20" t="str">
-        <f t="shared" ref="Q3:Q33" si="10">_xlfn.CONCAT("Machine_IO.","Inputs.",K3,".Init('",A3,"','",K3,"','",D3,"','",G3,"',","NVL_IO_",A3,".All_Inputs.",D3,",Machine_IO.Node_",A3,");")</f>
+        <f t="shared" ref="Q3:Q33" si="10">_xlfn.CONCAT("Machine_IO.","Inputs.",L3,".Init('",A3,"','",L3,"','",D3,"','",G3,"',","NVL_IO_",A3,".All_Inputs.",D3,",Machine_IO.Node_",A3,");")</f>
         <v>Machine_IO.Inputs.DRUM_PRESSURE.Init('CHASSIS','DRUM_PRESSURE','IN0101','a64',NVL_IO_CHASSIS.All_Inputs.IN0101,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R3" s="20" t="str">
@@ -2460,7 +2469,7 @@
       </c>
       <c r="Q4" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0102','a65',NVL_IO_CHASSIS.All_Inputs.IN0102,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0102.Init('CHASSIS','SPARE_IN0102','IN0102','a65',NVL_IO_CHASSIS.All_Inputs.IN0102,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R4" s="20" t="str">
         <f t="shared" si="3"/>
@@ -2530,7 +2539,7 @@
       </c>
       <c r="Q5" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0103','a66',NVL_IO_CHASSIS.All_Inputs.IN0103,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0103.Init('CHASSIS','SPARE_IN0103','IN0103','a66',NVL_IO_CHASSIS.All_Inputs.IN0103,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R5" s="20" t="str">
         <f t="shared" si="3"/>
@@ -2600,7 +2609,7 @@
       </c>
       <c r="Q6" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0200','a67',NVL_IO_CHASSIS.All_Inputs.IN0200,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0200.Init('CHASSIS','SPARE_IN0200','IN0200','a67',NVL_IO_CHASSIS.All_Inputs.IN0200,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R6" s="20" t="str">
         <f t="shared" si="3"/>
@@ -2670,7 +2679,7 @@
       </c>
       <c r="Q7" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0201','a68',NVL_IO_CHASSIS.All_Inputs.IN0201,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0201.Init('CHASSIS','SPARE_IN0201','IN0201','a68',NVL_IO_CHASSIS.All_Inputs.IN0201,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R7" s="20" t="str">
         <f t="shared" si="3"/>
@@ -2740,7 +2749,7 @@
       </c>
       <c r="Q8" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0202','a69',NVL_IO_CHASSIS.All_Inputs.IN0202,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0202.Init('CHASSIS','SPARE_IN0202','IN0202','a69',NVL_IO_CHASSIS.All_Inputs.IN0202,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R8" s="20" t="str">
         <f t="shared" si="3"/>
@@ -2810,7 +2819,7 @@
       </c>
       <c r="Q9" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0203','a70',NVL_IO_CHASSIS.All_Inputs.IN0203,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0203.Init('CHASSIS','SPARE_IN0203','IN0203','a70',NVL_IO_CHASSIS.All_Inputs.IN0203,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R9" s="20" t="str">
         <f t="shared" si="3"/>
@@ -2880,7 +2889,7 @@
       </c>
       <c r="Q10" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0600','a55',NVL_IO_CHASSIS.All_Inputs.IN0600,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0600.Init('CHASSIS','SPARE_IN0600','IN0600','a55',NVL_IO_CHASSIS.All_Inputs.IN0600,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R10" s="20" t="str">
         <f t="shared" si="3"/>
@@ -2950,7 +2959,7 @@
       </c>
       <c r="Q11" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0601','a56',NVL_IO_CHASSIS.All_Inputs.IN0601,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0601.Init('CHASSIS','SPARE_IN0601','IN0601','a56',NVL_IO_CHASSIS.All_Inputs.IN0601,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R11" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3020,7 +3029,7 @@
       </c>
       <c r="Q12" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0602','a57',NVL_IO_CHASSIS.All_Inputs.IN0602,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0602.Init('CHASSIS','SPARE_IN0602','IN0602','a57',NVL_IO_CHASSIS.All_Inputs.IN0602,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R12" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3090,7 +3099,7 @@
       </c>
       <c r="Q13" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0603','a58',NVL_IO_CHASSIS.All_Inputs.IN0603,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0603.Init('CHASSIS','SPARE_IN0603','IN0603','a58',NVL_IO_CHASSIS.All_Inputs.IN0603,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R13" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3160,7 +3169,7 @@
       </c>
       <c r="Q14" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0700','a59',NVL_IO_CHASSIS.All_Inputs.IN0700,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0700.Init('CHASSIS','SPARE_IN0700','IN0700','a59',NVL_IO_CHASSIS.All_Inputs.IN0700,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R14" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3232,7 +3241,7 @@
       </c>
       <c r="Q15" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.RadioRHS_JackLegRaise_Req.Init('CHASSIS','RadioRHS_JackLegRaise_Req','IN0701','a60',NVL_IO_CHASSIS.All_Inputs.IN0701,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ.Init('CHASSIS','RADIORHS_JACKLEGRAISE_REQ','IN0701','a60',NVL_IO_CHASSIS.All_Inputs.IN0701,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R15" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3304,7 +3313,7 @@
       </c>
       <c r="Q16" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.RHS_TrommelDoorSw.Init('CHASSIS','RHS_TrommelDoorSw','IN0702','a61',NVL_IO_CHASSIS.All_Inputs.IN0702,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.RHS_TROMMELDOORSW.Init('CHASSIS','RHS_TROMMELDOORSW','IN0702','a61',NVL_IO_CHASSIS.All_Inputs.IN0702,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R16" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3376,7 +3385,7 @@
       </c>
       <c r="Q17" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.LHS_TrommelDoorSw.Init('CHASSIS','LHS_TrommelDoorSw','IN0703','a62',NVL_IO_CHASSIS.All_Inputs.IN0703,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.LHS_TROMMELDOORSW.Init('CHASSIS','LHS_TROMMELDOORSW','IN0703','a62',NVL_IO_CHASSIS.All_Inputs.IN0703,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R17" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3448,7 +3457,7 @@
       </c>
       <c r="Q18" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.HydOilTemp_Sw.Init('CHASSIS','HydOilTemp_Sw','IN0000','a25',NVL_IO_CHASSIS.All_Inputs.IN0000,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.HYDOILTEMP_SW.Init('CHASSIS','HYDOILTEMP_SW','IN0000','a25',NVL_IO_CHASSIS.All_Inputs.IN0000,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R18" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3520,7 +3529,7 @@
       </c>
       <c r="Q19" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.HydOilLevel_Sw.Init('CHASSIS','HydOilLevel_Sw','IN0001','a26',NVL_IO_CHASSIS.All_Inputs.IN0001,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.HYDOILLEVEL_SW.Init('CHASSIS','HYDOILLEVEL_SW','IN0001','a26',NVL_IO_CHASSIS.All_Inputs.IN0001,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R19" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3592,7 +3601,7 @@
       </c>
       <c r="Q20" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.ThermoStat.Init('CHASSIS','ThermoStat','IN0002','a27',NVL_IO_CHASSIS.All_Inputs.IN0002,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.THERMOSTAT.Init('CHASSIS','THERMOSTAT','IN0002','a27',NVL_IO_CHASSIS.All_Inputs.IN0002,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R20" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3664,7 +3673,7 @@
       </c>
       <c r="Q21" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.RadioRHS_JackLegLower_Req.Init('CHASSIS','RadioRHS_JackLegLower_Req','IN0003','a28',NVL_IO_CHASSIS.All_Inputs.IN0003,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ.Init('CHASSIS','RADIORHS_JACKLEGLOWER_REQ','IN0003','a28',NVL_IO_CHASSIS.All_Inputs.IN0003,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R21" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3736,7 +3745,7 @@
       </c>
       <c r="Q22" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.RadioLHS_JackLegRaise_Req.Init('CHASSIS','RadioLHS_JackLegRaise_Req','IN0500','a40',NVL_IO_CHASSIS.All_Inputs.IN0500,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ.Init('CHASSIS','RADIOLHS_JACKLEGRAISE_REQ','IN0500','a40',NVL_IO_CHASSIS.All_Inputs.IN0500,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R22" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3808,7 +3817,7 @@
       </c>
       <c r="Q23" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.RadioLHS_JackLegLower_Req.Init('CHASSIS','RadioLHS_JackLegLower_Req','IN0501','a41',NVL_IO_CHASSIS.All_Inputs.IN0501,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ.Init('CHASSIS','RADIOLHS_JACKLEGLOWER_REQ','IN0501','a41',NVL_IO_CHASSIS.All_Inputs.IN0501,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R23" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3880,7 +3889,7 @@
       </c>
       <c r="Q24" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.RadioSideConvRaiseReq.Init('CHASSIS','RadioSideConvRaiseReq','IN0502','a42',NVL_IO_CHASSIS.All_Inputs.IN0502,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ.Init('CHASSIS','RADIOSIDECONVRAISEREQ','IN0502','a42',NVL_IO_CHASSIS.All_Inputs.IN0502,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R24" s="20" t="str">
         <f t="shared" si="3"/>
@@ -3952,7 +3961,7 @@
       </c>
       <c r="Q25" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.RadioSideConvLowerReq.Init('CHASSIS','RadioSideConvLowerReq','IN0503','a43',NVL_IO_CHASSIS.All_Inputs.IN0503,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ.Init('CHASSIS','RADIOSIDECONVLOWERREQ','IN0503','a43',NVL_IO_CHASSIS.All_Inputs.IN0503,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R25" s="20" t="str">
         <f t="shared" si="3"/>
@@ -4022,7 +4031,7 @@
       </c>
       <c r="Q26" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs..Init('CHASSIS','','IN0400','a46',NVL_IO_CHASSIS.All_Inputs.IN0400,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SPARE_IN0400.Init('CHASSIS','SPARE_IN0400','IN0400','a46',NVL_IO_CHASSIS.All_Inputs.IN0400,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R26" s="20" t="str">
         <f t="shared" si="3"/>
@@ -4094,7 +4103,7 @@
       </c>
       <c r="Q27" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.FuelLevel_Percent.Init('CHASSIS','FuelLevel_Percent','IN0401','a47',NVL_IO_CHASSIS.All_Inputs.IN0401,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.FUELLEVEL_PERCENT.Init('CHASSIS','FUELLEVEL_PERCENT','IN0401','a47',NVL_IO_CHASSIS.All_Inputs.IN0401,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R27" s="20" t="str">
         <f t="shared" si="3"/>
@@ -4164,7 +4173,7 @@
       </c>
       <c r="Q28" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.UmbTrackReq.Init('CHASSIS','UmbTrackReq','IN0900','a38',NVL_IO_CHASSIS.All_Inputs.IN0900,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.UMBTRACKREQ.Init('CHASSIS','UMBTRACKREQ','IN0900','a38',NVL_IO_CHASSIS.All_Inputs.IN0900,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R28" s="20" t="str">
         <f t="shared" si="3"/>
@@ -4234,7 +4243,7 @@
       </c>
       <c r="Q29" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.UmbMachineStop.Init('CHASSIS','UmbMachineStop','IN0901','a39',NVL_IO_CHASSIS.All_Inputs.IN0901,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.UMBMACHINESTOP.Init('CHASSIS','UMBMACHINESTOP','IN0901','a39',NVL_IO_CHASSIS.All_Inputs.IN0901,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R29" s="20" t="str">
         <f t="shared" si="3"/>
@@ -4304,7 +4313,7 @@
       </c>
       <c r="Q30" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.RTF_Req.Init('CHASSIS','RTF_Req','IN0300','a44',NVL_IO_CHASSIS.All_Inputs.IN0300,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.RTF_REQ.Init('CHASSIS','RTF_REQ','IN0300','a44',NVL_IO_CHASSIS.All_Inputs.IN0300,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R30" s="20" t="str">
         <f t="shared" si="3"/>
@@ -4374,7 +4383,7 @@
       </c>
       <c r="Q31" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.RTR_Req.Init('CHASSIS','RTR_Req','IN0301','a45',NVL_IO_CHASSIS.All_Inputs.IN0301,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.RTR_REQ.Init('CHASSIS','RTR_REQ','IN0301','a45',NVL_IO_CHASSIS.All_Inputs.IN0301,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R31" s="20" t="str">
         <f t="shared" si="3"/>
@@ -4444,7 +4453,7 @@
       </c>
       <c r="Q32" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.LTF_Req.Init('CHASSIS','LTF_Req','IN0800','a36',NVL_IO_CHASSIS.All_Inputs.IN0800,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.LTF_REQ.Init('CHASSIS','LTF_REQ','IN0800','a36',NVL_IO_CHASSIS.All_Inputs.IN0800,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R32" s="20" t="str">
         <f t="shared" si="3"/>
@@ -4514,7 +4523,7 @@
       </c>
       <c r="Q33" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.LTR_Req.Init('CHASSIS','LTR_Req','IN0801','a37',NVL_IO_CHASSIS.All_Inputs.IN0801,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.LTR_REQ.Init('CHASSIS','LTR_REQ','IN0801','a37',NVL_IO_CHASSIS.All_Inputs.IN0801,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R33" s="20" t="str">
         <f t="shared" si="3"/>
@@ -4588,19 +4597,19 @@
         <v>Machine_IO.Outputs.TAILCONVSPD_MA(); // CR0709.OUT0000</v>
       </c>
       <c r="Q34" s="20" t="str">
-        <f t="shared" ref="Q34:Q65" si="13">_xlfn.CONCAT(O34,".Init('",A34,"','",K34,"','",D34,"','",G34,"',NVL_Outputs_States_",A34,".All.",D34,",NVL_IO_",A2,".All_Outputs_Diag.",D34,",Machine_IO.Node_",A34,");")</f>
-        <v>Machine_IO.Outputs.TAILCONVSPD_MA.Init('CHASSIS','TailConvSpd_mA','OUT0000','a16',NVL_Outputs_States_CHASSIS.All.OUT0000,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0000,Machine_IO.Node_CHASSIS);</v>
+        <f>_xlfn.CONCAT(O34,".Init('",A34,"','",L34,"','",D34,"','",G34,"',NVL_Outputs_States_",A34,".All.",D34,",NVL_IO_",A2,".All_Outputs_Diag.",D34,",Machine_IO.Node_",A34,");")</f>
+        <v>Machine_IO.Outputs.TAILCONVSPD_MA.Init('CHASSIS','TAILCONVSPD_MA','OUT0000','a16',NVL_Outputs_States_CHASSIS.All.OUT0000,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0000,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="R34" s="20" t="str">
-        <f t="shared" ref="R34:R65" si="14">_xlfn.CONCAT(K34,": Mimic_Output_FB; // ",A34,":",D34)</f>
+        <f t="shared" ref="R34:R65" si="13">_xlfn.CONCAT(K34,": Mimic_Output_FB; // ",A34,":",D34)</f>
         <v>TailConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0000</v>
       </c>
       <c r="S34" s="20" t="str">
-        <f t="shared" ref="S34:S65" si="15">_xlfn.CONCAT(A34,".",D34,"();")</f>
+        <f t="shared" ref="S34:S65" si="14">_xlfn.CONCAT(A34,".",D34,"();")</f>
         <v>CHASSIS.OUT0000();</v>
       </c>
       <c r="T34" s="20" t="str">
-        <f t="shared" ref="T34:T65" si="16">_xlfn.CONCAT(A34,".",D34,".Init(",O34,");")</f>
+        <f t="shared" ref="T34:T65" si="15">_xlfn.CONCAT(A34,".",D34,".Init(",O34,");")</f>
         <v>CHASSIS.OUT0000.Init(Machine_IO.Outputs.TAILCONVSPD_MA);</v>
       </c>
     </row>
@@ -4651,11 +4660,11 @@
         <v>RHS_JackLegLower_OP:BOOL;</v>
       </c>
       <c r="N35" s="20" t="str">
-        <f t="shared" ref="N35:N65" si="17">_xlfn.CONCAT(L35,":OpCom; // ",A35,".",D35)</f>
+        <f t="shared" ref="N35:N65" si="16">_xlfn.CONCAT(L35,":OpCom; // ",A35,".",D35)</f>
         <v>RHS_JACKLEGLOWER_OP:OpCom; // CHASSIS.OUT0001</v>
       </c>
       <c r="O35" s="20" t="str">
-        <f t="shared" ref="O35:O65" si="18">_xlfn.CONCAT("Machine_IO.","Outputs.",L35,"")</f>
+        <f t="shared" ref="O35:O65" si="17">_xlfn.CONCAT("Machine_IO.","Outputs.",L35,"")</f>
         <v>Machine_IO.Outputs.RHS_JACKLEGLOWER_OP</v>
       </c>
       <c r="P35" s="20" t="str">
@@ -4663,19 +4672,19 @@
         <v>Machine_IO.Outputs.RHS_JACKLEGLOWER_OP(); // CR0709.OUT0001</v>
       </c>
       <c r="Q35" s="20" t="str">
+        <f t="shared" ref="Q35:Q65" si="18">_xlfn.CONCAT(O35,".Init('",A35,"','",L35,"','",D35,"','",G35,"',NVL_Outputs_States_",A35,".All.",D35,",NVL_IO_",A3,".All_Outputs_Diag.",D35,",Machine_IO.Node_",A35,");")</f>
+        <v>Machine_IO.Outputs.RHS_JACKLEGLOWER_OP.Init('CHASSIS','RHS_JACKLEGLOWER_OP','OUT0001','a17',NVL_Outputs_States_CHASSIS.All.OUT0001,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0001,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R35" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.RHS_JACKLEGLOWER_OP.Init('CHASSIS','RHS_JackLegLower_OP','OUT0001','a17',NVL_Outputs_States_CHASSIS.All.OUT0001,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0001,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R35" s="20" t="str">
+        <v>RHS_JackLegLower_OP: Mimic_Output_FB; // CHASSIS:OUT0001</v>
+      </c>
+      <c r="S35" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>RHS_JackLegLower_OP: Mimic_Output_FB; // CHASSIS:OUT0001</v>
-      </c>
-      <c r="S35" s="20" t="str">
+        <v>CHASSIS.OUT0001();</v>
+      </c>
+      <c r="T35" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0001();</v>
-      </c>
-      <c r="T35" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0001.Init(Machine_IO.Outputs.RHS_JACKLEGLOWER_OP);</v>
       </c>
     </row>
@@ -4726,11 +4735,11 @@
         <v>SideConvSpd_mA:BOOL;</v>
       </c>
       <c r="N36" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>SIDECONVSPD_MA:OpCom; // CHASSIS.OUT0002</v>
+      </c>
+      <c r="O36" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>SIDECONVSPD_MA:OpCom; // CHASSIS.OUT0002</v>
-      </c>
-      <c r="O36" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDECONVSPD_MA</v>
       </c>
       <c r="P36" s="20" t="str">
@@ -4738,19 +4747,19 @@
         <v>Machine_IO.Outputs.SIDECONVSPD_MA(); // CR0709.OUT0002</v>
       </c>
       <c r="Q36" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.SIDECONVSPD_MA.Init('CHASSIS','SIDECONVSPD_MA','OUT0002','a18',NVL_Outputs_States_CHASSIS.All.OUT0002,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0002,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R36" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.SIDECONVSPD_MA.Init('CHASSIS','SideConvSpd_mA','OUT0002','a18',NVL_Outputs_States_CHASSIS.All.OUT0002,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0002,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R36" s="20" t="str">
+        <v>SideConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0002</v>
+      </c>
+      <c r="S36" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>SideConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0002</v>
-      </c>
-      <c r="S36" s="20" t="str">
+        <v>CHASSIS.OUT0002();</v>
+      </c>
+      <c r="T36" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0002();</v>
-      </c>
-      <c r="T36" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0002.Init(Machine_IO.Outputs.SIDECONVSPD_MA);</v>
       </c>
     </row>
@@ -4801,11 +4810,11 @@
         <v>LHS_JackLegRaise_OP:BOOL;</v>
       </c>
       <c r="N37" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>LHS_JACKLEGRAISE_OP:OpCom; // CHASSIS.OUT0003</v>
+      </c>
+      <c r="O37" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>LHS_JACKLEGRAISE_OP:OpCom; // CHASSIS.OUT0003</v>
-      </c>
-      <c r="O37" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGRAISE_OP</v>
       </c>
       <c r="P37" s="20" t="str">
@@ -4813,19 +4822,19 @@
         <v>Machine_IO.Outputs.LHS_JACKLEGRAISE_OP(); // CR0709.OUT0003</v>
       </c>
       <c r="Q37" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.LHS_JACKLEGRAISE_OP.Init('CHASSIS','LHS_JACKLEGRAISE_OP','OUT0003','a19',NVL_Outputs_States_CHASSIS.All.OUT0003,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0003,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R37" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.LHS_JACKLEGRAISE_OP.Init('CHASSIS','LHS_JackLegRaise_OP','OUT0003','a19',NVL_Outputs_States_CHASSIS.All.OUT0003,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0003,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R37" s="20" t="str">
+        <v>LHS_JackLegRaise_OP: Mimic_Output_FB; // CHASSIS:OUT0003</v>
+      </c>
+      <c r="S37" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>LHS_JackLegRaise_OP: Mimic_Output_FB; // CHASSIS:OUT0003</v>
-      </c>
-      <c r="S37" s="20" t="str">
+        <v>CHASSIS.OUT0003();</v>
+      </c>
+      <c r="T37" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0003();</v>
-      </c>
-      <c r="T37" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0003.Init(Machine_IO.Outputs.LHS_JACKLEGRAISE_OP);</v>
       </c>
     </row>
@@ -4876,11 +4885,11 @@
         <v>SideTransferSpd_mA:BOOL;</v>
       </c>
       <c r="N38" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>SIDETRANSFERSPD_MA:OpCom; // CHASSIS.OUT0004</v>
+      </c>
+      <c r="O38" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>SIDETRANSFERSPD_MA:OpCom; // CHASSIS.OUT0004</v>
-      </c>
-      <c r="O38" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDETRANSFERSPD_MA</v>
       </c>
       <c r="P38" s="20" t="str">
@@ -4888,19 +4897,19 @@
         <v>Machine_IO.Outputs.SIDETRANSFERSPD_MA(); // CR0709.OUT0004</v>
       </c>
       <c r="Q38" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.SIDETRANSFERSPD_MA.Init('CHASSIS','SIDETRANSFERSPD_MA','OUT0004','a20',NVL_Outputs_States_CHASSIS.All.OUT0004,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0004,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R38" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.SIDETRANSFERSPD_MA.Init('CHASSIS','SideTransferSpd_mA','OUT0004','a20',NVL_Outputs_States_CHASSIS.All.OUT0004,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0004,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R38" s="20" t="str">
+        <v>SideTransferSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0004</v>
+      </c>
+      <c r="S38" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>SideTransferSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0004</v>
-      </c>
-      <c r="S38" s="20" t="str">
+        <v>CHASSIS.OUT0004();</v>
+      </c>
+      <c r="T38" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0004();</v>
-      </c>
-      <c r="T38" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0004.Init(Machine_IO.Outputs.SIDETRANSFERSPD_MA);</v>
       </c>
     </row>
@@ -4951,11 +4960,11 @@
         <v>LHS_JackLegLower_OP:BOOL;</v>
       </c>
       <c r="N39" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>LHS_JACKLEGLOWER_OP:OpCom; // CHASSIS.OUT0005</v>
+      </c>
+      <c r="O39" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>LHS_JACKLEGLOWER_OP:OpCom; // CHASSIS.OUT0005</v>
-      </c>
-      <c r="O39" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGLOWER_OP</v>
       </c>
       <c r="P39" s="20" t="str">
@@ -4963,19 +4972,19 @@
         <v>Machine_IO.Outputs.LHS_JACKLEGLOWER_OP(); // CR0709.OUT0005</v>
       </c>
       <c r="Q39" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.LHS_JACKLEGLOWER_OP.Init('CHASSIS','LHS_JACKLEGLOWER_OP','OUT0005','a21',NVL_Outputs_States_CHASSIS.All.OUT0005,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0005,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R39" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.LHS_JACKLEGLOWER_OP.Init('CHASSIS','LHS_JackLegLower_OP','OUT0005','a21',NVL_Outputs_States_CHASSIS.All.OUT0005,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0005,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R39" s="20" t="str">
+        <v>LHS_JackLegLower_OP: Mimic_Output_FB; // CHASSIS:OUT0005</v>
+      </c>
+      <c r="S39" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>LHS_JackLegLower_OP: Mimic_Output_FB; // CHASSIS:OUT0005</v>
-      </c>
-      <c r="S39" s="20" t="str">
+        <v>CHASSIS.OUT0005();</v>
+      </c>
+      <c r="T39" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0005();</v>
-      </c>
-      <c r="T39" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0005.Init(Machine_IO.Outputs.LHS_JACKLEGLOWER_OP);</v>
       </c>
     </row>
@@ -5026,11 +5035,11 @@
         <v>SetupDumpValve_OP:BOOL;</v>
       </c>
       <c r="N40" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>SETUPDUMPVALVE_OP:OpCom; // CHASSIS.OUT0006</v>
+      </c>
+      <c r="O40" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>SETUPDUMPVALVE_OP:OpCom; // CHASSIS.OUT0006</v>
-      </c>
-      <c r="O40" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SETUPDUMPVALVE_OP</v>
       </c>
       <c r="P40" s="20" t="str">
@@ -5038,19 +5047,19 @@
         <v>Machine_IO.Outputs.SETUPDUMPVALVE_OP(); // CR0709.OUT0006</v>
       </c>
       <c r="Q40" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.SETUPDUMPVALVE_OP.Init('CHASSIS','SETUPDUMPVALVE_OP','OUT0006','a22',NVL_Outputs_States_CHASSIS.All.OUT0006,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0006,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R40" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.SETUPDUMPVALVE_OP.Init('CHASSIS','SetupDumpValve_OP','OUT0006','a22',NVL_Outputs_States_CHASSIS.All.OUT0006,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0006,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R40" s="20" t="str">
+        <v>SetupDumpValve_OP: Mimic_Output_FB; // CHASSIS:OUT0006</v>
+      </c>
+      <c r="S40" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>SetupDumpValve_OP: Mimic_Output_FB; // CHASSIS:OUT0006</v>
-      </c>
-      <c r="S40" s="20" t="str">
+        <v>CHASSIS.OUT0006();</v>
+      </c>
+      <c r="T40" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0006();</v>
-      </c>
-      <c r="T40" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0006.Init(Machine_IO.Outputs.SETUPDUMPVALVE_OP);</v>
       </c>
     </row>
@@ -5101,11 +5110,11 @@
         <v>CollectionConvSpd_mA:BOOL;</v>
       </c>
       <c r="N41" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>COLLECTIONCONVSPD_MA:OpCom; // CHASSIS.OUT0007</v>
+      </c>
+      <c r="O41" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>COLLECTIONCONVSPD_MA:OpCom; // CHASSIS.OUT0007</v>
-      </c>
-      <c r="O41" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVSPD_MA</v>
       </c>
       <c r="P41" s="20" t="str">
@@ -5113,19 +5122,19 @@
         <v>Machine_IO.Outputs.COLLECTIONCONVSPD_MA(); // CR0709.OUT0007</v>
       </c>
       <c r="Q41" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.COLLECTIONCONVSPD_MA.Init('CHASSIS','COLLECTIONCONVSPD_MA','OUT0007','a23',NVL_Outputs_States_CHASSIS.All.OUT0007,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0007,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R41" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.COLLECTIONCONVSPD_MA.Init('CHASSIS','CollectionConvSpd_mA','OUT0007','a23',NVL_Outputs_States_CHASSIS.All.OUT0007,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0007,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R41" s="20" t="str">
+        <v>CollectionConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0007</v>
+      </c>
+      <c r="S41" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CollectionConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0007</v>
-      </c>
-      <c r="S41" s="20" t="str">
+        <v>CHASSIS.OUT0007();</v>
+      </c>
+      <c r="T41" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0007();</v>
-      </c>
-      <c r="T41" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0007.Init(Machine_IO.Outputs.COLLECTIONCONVSPD_MA);</v>
       </c>
     </row>
@@ -5176,11 +5185,11 @@
         <v>CollectionConvOn_OP:BOOL;</v>
       </c>
       <c r="N42" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>COLLECTIONCONVON_OP:OpCom; // CHASSIS.OUT0008</v>
+      </c>
+      <c r="O42" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>COLLECTIONCONVON_OP:OpCom; // CHASSIS.OUT0008</v>
-      </c>
-      <c r="O42" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVON_OP</v>
       </c>
       <c r="P42" s="20" t="str">
@@ -5188,19 +5197,19 @@
         <v>Machine_IO.Outputs.COLLECTIONCONVON_OP(); // CR0709.OUT0008</v>
       </c>
       <c r="Q42" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.COLLECTIONCONVON_OP.Init('CHASSIS','COLLECTIONCONVON_OP','OUT0008','a24',NVL_Outputs_States_CHASSIS.All.OUT0008,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0008,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R42" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.COLLECTIONCONVON_OP.Init('CHASSIS','CollectionConvOn_OP','OUT0008','a24',NVL_Outputs_States_CHASSIS.All.OUT0008,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0008,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R42" s="20" t="str">
+        <v>CollectionConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0008</v>
+      </c>
+      <c r="S42" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CollectionConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0008</v>
-      </c>
-      <c r="S42" s="20" t="str">
+        <v>CHASSIS.OUT0008();</v>
+      </c>
+      <c r="T42" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0008();</v>
-      </c>
-      <c r="T42" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0008.Init(Machine_IO.Outputs.COLLECTIONCONVON_OP);</v>
       </c>
     </row>
@@ -5239,42 +5248,44 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.GROUP0</v>
       </c>
-      <c r="K43" s="19"/>
+      <c r="K43" s="19" t="s">
+        <v>527</v>
+      </c>
       <c r="L43" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>SPARE_GROUP0</v>
+        <v>SUPPLY_GROUP0</v>
       </c>
       <c r="M43" s="19" t="str">
         <f t="shared" si="11"/>
-        <v>:BOOL;</v>
+        <v>SUPPLY_GROUP0:BOOL;</v>
       </c>
       <c r="N43" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>SUPPLY_GROUP0:OpCom; // CHASSIS.GROUP0</v>
+      </c>
+      <c r="O43" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>SPARE_GROUP0:OpCom; // CHASSIS.GROUP0</v>
-      </c>
-      <c r="O43" s="20" t="str">
-        <f t="shared" si="18"/>
-        <v>Machine_IO.Outputs.SPARE_GROUP0</v>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP0</v>
       </c>
       <c r="P43" s="20" t="str">
         <f t="shared" si="12"/>
-        <v>Machine_IO.Outputs.SPARE_GROUP0(); // CR0709.GROUP0</v>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP0(); // CR0709.GROUP0</v>
       </c>
       <c r="Q43" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP0.Init('CHASSIS','SUPPLY_GROUP0','GROUP0','a4',NVL_Outputs_States_CHASSIS.All.GROUP0,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP0,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R43" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.SPARE_GROUP0.Init('CHASSIS','','GROUP0','a4',NVL_Outputs_States_CHASSIS.All.GROUP0,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP0,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R43" s="20" t="str">
+        <v>SUPPLY_GROUP0: Mimic_Output_FB; // CHASSIS:GROUP0</v>
+      </c>
+      <c r="S43" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>: Mimic_Output_FB; // CHASSIS:GROUP0</v>
-      </c>
-      <c r="S43" s="20" t="str">
+        <v>CHASSIS.GROUP0();</v>
+      </c>
+      <c r="T43" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.GROUP0();</v>
-      </c>
-      <c r="T43" s="20" t="str">
-        <f t="shared" si="16"/>
-        <v>CHASSIS.GROUP0.Init(Machine_IO.Outputs.SPARE_GROUP0);</v>
+        <v>CHASSIS.GROUP0.Init(Machine_IO.Outputs.SUPPLY_GROUP0);</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
@@ -5324,11 +5335,11 @@
         <v>DrumSpd_mA_RAMP_LIMIT:BOOL;</v>
       </c>
       <c r="N44" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>DRUMSPD_MA_RAMP_LIMIT:OpCom; // CHASSIS.OUT0100</v>
+      </c>
+      <c r="O44" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>DRUMSPD_MA_RAMP_LIMIT:OpCom; // CHASSIS.OUT0100</v>
-      </c>
-      <c r="O44" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT</v>
       </c>
       <c r="P44" s="20" t="str">
@@ -5336,19 +5347,19 @@
         <v>Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT(); // CR0709.OUT0100</v>
       </c>
       <c r="Q44" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT.Init('CHASSIS','DRUMSPD_MA_RAMP_LIMIT','OUT0100','a6',NVL_Outputs_States_CHASSIS.All.OUT0100,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0100,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R44" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT.Init('CHASSIS','DrumSpd_mA_RAMP_LIMIT','OUT0100','a6',NVL_Outputs_States_CHASSIS.All.OUT0100,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0100,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R44" s="20" t="str">
+        <v>DrumSpd_mA_RAMP_LIMIT: Mimic_Output_FB; // CHASSIS:OUT0100</v>
+      </c>
+      <c r="S44" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>DrumSpd_mA_RAMP_LIMIT: Mimic_Output_FB; // CHASSIS:OUT0100</v>
-      </c>
-      <c r="S44" s="20" t="str">
+        <v>CHASSIS.OUT0100();</v>
+      </c>
+      <c r="T44" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0100();</v>
-      </c>
-      <c r="T44" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0100.Init(Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT);</v>
       </c>
     </row>
@@ -5399,11 +5410,11 @@
         <v>TrackingMode:BOOL;</v>
       </c>
       <c r="N45" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>TRACKINGMODE:OpCom; // CHASSIS.OUT0101</v>
+      </c>
+      <c r="O45" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>TRACKINGMODE:OpCom; // CHASSIS.OUT0101</v>
-      </c>
-      <c r="O45" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.TRACKINGMODE</v>
       </c>
       <c r="P45" s="20" t="str">
@@ -5411,19 +5422,19 @@
         <v>Machine_IO.Outputs.TRACKINGMODE(); // CR0709.OUT0101</v>
       </c>
       <c r="Q45" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.TRACKINGMODE.Init('CHASSIS','TRACKINGMODE','OUT0101','a7',NVL_Outputs_States_CHASSIS.All.OUT0101,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0101,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R45" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.TRACKINGMODE.Init('CHASSIS','TrackingMode','OUT0101','a7',NVL_Outputs_States_CHASSIS.All.OUT0101,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0101,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R45" s="20" t="str">
+        <v>TrackingMode: Mimic_Output_FB; // CHASSIS:OUT0101</v>
+      </c>
+      <c r="S45" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>TrackingMode: Mimic_Output_FB; // CHASSIS:OUT0101</v>
-      </c>
-      <c r="S45" s="20" t="str">
+        <v>CHASSIS.OUT0101();</v>
+      </c>
+      <c r="T45" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0101();</v>
-      </c>
-      <c r="T45" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0101.Init(Machine_IO.Outputs.TRACKINGMODE);</v>
       </c>
     </row>
@@ -5474,11 +5485,11 @@
         <v>FeederSpd_mA:BOOL;</v>
       </c>
       <c r="N46" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>FEEDERSPD_MA:OpCom; // CHASSIS.OUT0102</v>
+      </c>
+      <c r="O46" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>FEEDERSPD_MA:OpCom; // CHASSIS.OUT0102</v>
-      </c>
-      <c r="O46" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.FEEDERSPD_MA</v>
       </c>
       <c r="P46" s="20" t="str">
@@ -5486,19 +5497,19 @@
         <v>Machine_IO.Outputs.FEEDERSPD_MA(); // CR0709.OUT0102</v>
       </c>
       <c r="Q46" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.FEEDERSPD_MA.Init('CHASSIS','FEEDERSPD_MA','OUT0102','a8',NVL_Outputs_States_CHASSIS.All.OUT0102,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0102,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R46" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.FEEDERSPD_MA.Init('CHASSIS','FeederSpd_mA','OUT0102','a8',NVL_Outputs_States_CHASSIS.All.OUT0102,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0102,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R46" s="20" t="str">
+        <v>FeederSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0102</v>
+      </c>
+      <c r="S46" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>FeederSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0102</v>
-      </c>
-      <c r="S46" s="20" t="str">
+        <v>CHASSIS.OUT0102();</v>
+      </c>
+      <c r="T46" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0102();</v>
-      </c>
-      <c r="T46" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0102.Init(Machine_IO.Outputs.FEEDERSPD_MA);</v>
       </c>
     </row>
@@ -5549,11 +5560,11 @@
         <v>CrankEnable:BOOL;</v>
       </c>
       <c r="N47" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>CRANKENABLE:OpCom; // CHASSIS.OUT0103</v>
+      </c>
+      <c r="O47" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>CRANKENABLE:OpCom; // CHASSIS.OUT0103</v>
-      </c>
-      <c r="O47" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.CRANKENABLE</v>
       </c>
       <c r="P47" s="20" t="str">
@@ -5561,19 +5572,19 @@
         <v>Machine_IO.Outputs.CRANKENABLE(); // CR0709.OUT0103</v>
       </c>
       <c r="Q47" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.CRANKENABLE.Init('CHASSIS','CRANKENABLE','OUT0103','a9',NVL_Outputs_States_CHASSIS.All.OUT0103,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0103,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R47" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.CRANKENABLE.Init('CHASSIS','CrankEnable','OUT0103','a9',NVL_Outputs_States_CHASSIS.All.OUT0103,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0103,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R47" s="20" t="str">
+        <v>CrankEnable: Mimic_Output_FB; // CHASSIS:OUT0103</v>
+      </c>
+      <c r="S47" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CrankEnable: Mimic_Output_FB; // CHASSIS:OUT0103</v>
-      </c>
-      <c r="S47" s="20" t="str">
+        <v>CHASSIS.OUT0103();</v>
+      </c>
+      <c r="T47" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0103();</v>
-      </c>
-      <c r="T47" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0103.Init(Machine_IO.Outputs.CRANKENABLE);</v>
       </c>
     </row>
@@ -5624,11 +5635,11 @@
         <v>DivertOilToTrack_OP:BOOL;</v>
       </c>
       <c r="N48" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>DIVERTOILTOTRACK_OP:OpCom; // CHASSIS.OUT0104</v>
+      </c>
+      <c r="O48" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>DIVERTOILTOTRACK_OP:OpCom; // CHASSIS.OUT0104</v>
-      </c>
-      <c r="O48" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.DIVERTOILTOTRACK_OP</v>
       </c>
       <c r="P48" s="20" t="str">
@@ -5636,19 +5647,19 @@
         <v>Machine_IO.Outputs.DIVERTOILTOTRACK_OP(); // CR0709.OUT0104</v>
       </c>
       <c r="Q48" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.DIVERTOILTOTRACK_OP.Init('CHASSIS','DIVERTOILTOTRACK_OP','OUT0104','a10',NVL_Outputs_States_CHASSIS.All.OUT0104,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0104,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R48" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.DIVERTOILTOTRACK_OP.Init('CHASSIS','DivertOilToTrack_OP','OUT0104','a10',NVL_Outputs_States_CHASSIS.All.OUT0104,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0104,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R48" s="20" t="str">
+        <v>DivertOilToTrack_OP: Mimic_Output_FB; // CHASSIS:OUT0104</v>
+      </c>
+      <c r="S48" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>DivertOilToTrack_OP: Mimic_Output_FB; // CHASSIS:OUT0104</v>
-      </c>
-      <c r="S48" s="20" t="str">
+        <v>CHASSIS.OUT0104();</v>
+      </c>
+      <c r="T48" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0104();</v>
-      </c>
-      <c r="T48" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0104.Init(Machine_IO.Outputs.DIVERTOILTOTRACK_OP);</v>
       </c>
     </row>
@@ -5699,11 +5710,11 @@
         <v>RHS_JackLegRaise_OP:BOOL;</v>
       </c>
       <c r="N49" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>RHS_JACKLEGRAISE_OP:OpCom; // CHASSIS.OUT0105</v>
+      </c>
+      <c r="O49" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>RHS_JACKLEGRAISE_OP:OpCom; // CHASSIS.OUT0105</v>
-      </c>
-      <c r="O49" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RHS_JACKLEGRAISE_OP</v>
       </c>
       <c r="P49" s="20" t="str">
@@ -5711,19 +5722,19 @@
         <v>Machine_IO.Outputs.RHS_JACKLEGRAISE_OP(); // CR0709.OUT0105</v>
       </c>
       <c r="Q49" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.RHS_JACKLEGRAISE_OP.Init('CHASSIS','RHS_JACKLEGRAISE_OP','OUT0105','a11',NVL_Outputs_States_CHASSIS.All.OUT0105,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0105,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R49" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.RHS_JACKLEGRAISE_OP.Init('CHASSIS','RHS_JackLegRaise_OP','OUT0105','a11',NVL_Outputs_States_CHASSIS.All.OUT0105,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0105,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R49" s="20" t="str">
+        <v>RHS_JackLegRaise_OP: Mimic_Output_FB; // CHASSIS:OUT0105</v>
+      </c>
+      <c r="S49" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>RHS_JackLegRaise_OP: Mimic_Output_FB; // CHASSIS:OUT0105</v>
-      </c>
-      <c r="S49" s="20" t="str">
+        <v>CHASSIS.OUT0105();</v>
+      </c>
+      <c r="T49" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0105();</v>
-      </c>
-      <c r="T49" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0105.Init(Machine_IO.Outputs.RHS_JACKLEGRAISE_OP);</v>
       </c>
     </row>
@@ -5774,11 +5785,11 @@
         <v>TailConvOn_OP:BOOL;</v>
       </c>
       <c r="N50" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>TAILCONVON_OP:OpCom; // CHASSIS.OUT0106</v>
+      </c>
+      <c r="O50" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>TAILCONVON_OP:OpCom; // CHASSIS.OUT0106</v>
-      </c>
-      <c r="O50" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.TAILCONVON_OP</v>
       </c>
       <c r="P50" s="20" t="str">
@@ -5786,19 +5797,19 @@
         <v>Machine_IO.Outputs.TAILCONVON_OP(); // CR0709.OUT0106</v>
       </c>
       <c r="Q50" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.TAILCONVON_OP.Init('CHASSIS','TAILCONVON_OP','OUT0106','a12',NVL_Outputs_States_CHASSIS.All.OUT0106,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0106,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R50" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.TAILCONVON_OP.Init('CHASSIS','TailConvOn_OP','OUT0106','a12',NVL_Outputs_States_CHASSIS.All.OUT0106,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0106,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R50" s="20" t="str">
+        <v>TailConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0106</v>
+      </c>
+      <c r="S50" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>TailConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0106</v>
-      </c>
-      <c r="S50" s="20" t="str">
+        <v>CHASSIS.OUT0106();</v>
+      </c>
+      <c r="T50" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0106();</v>
-      </c>
-      <c r="T50" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0106.Init(Machine_IO.Outputs.TAILCONVON_OP);</v>
       </c>
     </row>
@@ -5849,11 +5860,11 @@
         <v>SideConvOn_OP:BOOL;</v>
       </c>
       <c r="N51" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>SIDECONVON_OP:OpCom; // CHASSIS.OUT0107</v>
+      </c>
+      <c r="O51" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>SIDECONVON_OP:OpCom; // CHASSIS.OUT0107</v>
-      </c>
-      <c r="O51" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDECONVON_OP</v>
       </c>
       <c r="P51" s="20" t="str">
@@ -5861,19 +5872,19 @@
         <v>Machine_IO.Outputs.SIDECONVON_OP(); // CR0709.OUT0107</v>
       </c>
       <c r="Q51" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.SIDECONVON_OP.Init('CHASSIS','SIDECONVON_OP','OUT0107','a13',NVL_Outputs_States_CHASSIS.All.OUT0107,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0107,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R51" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.SIDECONVON_OP.Init('CHASSIS','SideConvOn_OP','OUT0107','a13',NVL_Outputs_States_CHASSIS.All.OUT0107,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0107,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R51" s="20" t="str">
+        <v>SideConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0107</v>
+      </c>
+      <c r="S51" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>SideConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0107</v>
-      </c>
-      <c r="S51" s="20" t="str">
+        <v>CHASSIS.OUT0107();</v>
+      </c>
+      <c r="T51" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0107();</v>
-      </c>
-      <c r="T51" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0107.Init(Machine_IO.Outputs.SIDECONVON_OP);</v>
       </c>
     </row>
@@ -5924,11 +5935,11 @@
         <v>SideTransferOn_OP:BOOL;</v>
       </c>
       <c r="N52" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>SIDETRANSFERON_OP:OpCom; // CHASSIS.OUT0108</v>
+      </c>
+      <c r="O52" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>SIDETRANSFERON_OP:OpCom; // CHASSIS.OUT0108</v>
-      </c>
-      <c r="O52" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDETRANSFERON_OP</v>
       </c>
       <c r="P52" s="20" t="str">
@@ -5936,19 +5947,19 @@
         <v>Machine_IO.Outputs.SIDETRANSFERON_OP(); // CR0709.OUT0108</v>
       </c>
       <c r="Q52" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.SIDETRANSFERON_OP.Init('CHASSIS','SIDETRANSFERON_OP','OUT0108','a14',NVL_Outputs_States_CHASSIS.All.OUT0108,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0108,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R52" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.SIDETRANSFERON_OP.Init('CHASSIS','SideTransferOn_OP','OUT0108','a14',NVL_Outputs_States_CHASSIS.All.OUT0108,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0108,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R52" s="20" t="str">
+        <v>SideTransferOn_OP: Mimic_Output_FB; // CHASSIS:OUT0108</v>
+      </c>
+      <c r="S52" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>SideTransferOn_OP: Mimic_Output_FB; // CHASSIS:OUT0108</v>
-      </c>
-      <c r="S52" s="20" t="str">
+        <v>CHASSIS.OUT0108();</v>
+      </c>
+      <c r="T52" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0108();</v>
-      </c>
-      <c r="T52" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0108.Init(Machine_IO.Outputs.SIDETRANSFERON_OP);</v>
       </c>
     </row>
@@ -5987,42 +5998,44 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.GROUP1</v>
       </c>
-      <c r="K53" s="19"/>
+      <c r="K53" s="19" t="s">
+        <v>528</v>
+      </c>
       <c r="L53" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>SPARE_GROUP1</v>
+        <v>SUPPLY_GROUP1</v>
       </c>
       <c r="M53" s="19" t="str">
         <f t="shared" si="11"/>
-        <v>:BOOL;</v>
+        <v>SUPPLY_GROUP1:BOOL;</v>
       </c>
       <c r="N53" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>SUPPLY_GROUP1:OpCom; // CHASSIS.GROUP1</v>
+      </c>
+      <c r="O53" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>SPARE_GROUP1:OpCom; // CHASSIS.GROUP1</v>
-      </c>
-      <c r="O53" s="20" t="str">
-        <f t="shared" si="18"/>
-        <v>Machine_IO.Outputs.SPARE_GROUP1</v>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP1</v>
       </c>
       <c r="P53" s="20" t="str">
         <f t="shared" si="12"/>
-        <v>Machine_IO.Outputs.SPARE_GROUP1(); // CR0709.GROUP1</v>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP1(); // CR0709.GROUP1</v>
       </c>
       <c r="Q53" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP1.Init('CHASSIS','SUPPLY_GROUP1','GROUP1','a3',NVL_Outputs_States_CHASSIS.All.GROUP1,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP1,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R53" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.SPARE_GROUP1.Init('CHASSIS','','GROUP1','a3',NVL_Outputs_States_CHASSIS.All.GROUP1,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP1,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R53" s="20" t="str">
+        <v>SUPPLY_GROUP1: Mimic_Output_FB; // CHASSIS:GROUP1</v>
+      </c>
+      <c r="S53" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>: Mimic_Output_FB; // CHASSIS:GROUP1</v>
-      </c>
-      <c r="S53" s="20" t="str">
+        <v>CHASSIS.GROUP1();</v>
+      </c>
+      <c r="T53" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.GROUP1();</v>
-      </c>
-      <c r="T53" s="20" t="str">
-        <f t="shared" si="16"/>
-        <v>CHASSIS.GROUP1.Init(Machine_IO.Outputs.SPARE_GROUP1);</v>
+        <v>CHASSIS.GROUP1.Init(Machine_IO.Outputs.SUPPLY_GROUP1);</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
@@ -6072,11 +6085,11 @@
         <v>LeftTrackDivert_OP:BOOL;</v>
       </c>
       <c r="N54" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>LEFTTRACKDIVERT_OP:OpCom; // CHASSIS.OUT0200</v>
+      </c>
+      <c r="O54" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>LEFTTRACKDIVERT_OP:OpCom; // CHASSIS.OUT0200</v>
-      </c>
-      <c r="O54" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LEFTTRACKDIVERT_OP</v>
       </c>
       <c r="P54" s="20" t="str">
@@ -6084,19 +6097,19 @@
         <v>Machine_IO.Outputs.LEFTTRACKDIVERT_OP(); // CR0709.OUT0200</v>
       </c>
       <c r="Q54" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.LEFTTRACKDIVERT_OP.Init('CHASSIS','LEFTTRACKDIVERT_OP','OUT0200','a73',NVL_Outputs_States_CHASSIS.All.OUT0200,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0200,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R54" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.LEFTTRACKDIVERT_OP.Init('CHASSIS','LeftTrackDivert_OP','OUT0200','a73',NVL_Outputs_States_CHASSIS.All.OUT0200,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0200,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R54" s="20" t="str">
+        <v>LeftTrackDivert_OP: Mimic_Output_FB; // CHASSIS:OUT0200</v>
+      </c>
+      <c r="S54" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>LeftTrackDivert_OP: Mimic_Output_FB; // CHASSIS:OUT0200</v>
-      </c>
-      <c r="S54" s="20" t="str">
+        <v>CHASSIS.OUT0200();</v>
+      </c>
+      <c r="T54" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0200();</v>
-      </c>
-      <c r="T54" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0200.Init(Machine_IO.Outputs.LEFTTRACKDIVERT_OP);</v>
       </c>
     </row>
@@ -6147,11 +6160,11 @@
         <v>LTF_OP:BOOL;</v>
       </c>
       <c r="N55" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>LTF_OP:OpCom; // CHASSIS.OUT0201</v>
+      </c>
+      <c r="O55" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>LTF_OP:OpCom; // CHASSIS.OUT0201</v>
-      </c>
-      <c r="O55" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LTF_OP</v>
       </c>
       <c r="P55" s="20" t="str">
@@ -6159,19 +6172,19 @@
         <v>Machine_IO.Outputs.LTF_OP(); // CR0709.OUT0201</v>
       </c>
       <c r="Q55" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.LTF_OP.Init('CHASSIS','LTF_OP','OUT0201','a74',NVL_Outputs_States_CHASSIS.All.OUT0201,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0201,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R55" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.LTF_OP.Init('CHASSIS','LTF_OP','OUT0201','a74',NVL_Outputs_States_CHASSIS.All.OUT0201,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0201,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R55" s="20" t="str">
+        <v>LTF_OP: Mimic_Output_FB; // CHASSIS:OUT0201</v>
+      </c>
+      <c r="S55" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>LTF_OP: Mimic_Output_FB; // CHASSIS:OUT0201</v>
-      </c>
-      <c r="S55" s="20" t="str">
+        <v>CHASSIS.OUT0201();</v>
+      </c>
+      <c r="T55" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0201();</v>
-      </c>
-      <c r="T55" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0201.Init(Machine_IO.Outputs.LTF_OP);</v>
       </c>
     </row>
@@ -6222,11 +6235,11 @@
         <v>LTR_OP:BOOL;</v>
       </c>
       <c r="N56" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>LTR_OP:OpCom; // CHASSIS.OUT0202</v>
+      </c>
+      <c r="O56" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>LTR_OP:OpCom; // CHASSIS.OUT0202</v>
-      </c>
-      <c r="O56" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LTR_OP</v>
       </c>
       <c r="P56" s="20" t="str">
@@ -6234,19 +6247,19 @@
         <v>Machine_IO.Outputs.LTR_OP(); // CR0709.OUT0202</v>
       </c>
       <c r="Q56" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.LTR_OP.Init('CHASSIS','LTR_OP','OUT0202','a75',NVL_Outputs_States_CHASSIS.All.OUT0202,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0202,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R56" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.LTR_OP.Init('CHASSIS','LTR_OP','OUT0202','a75',NVL_Outputs_States_CHASSIS.All.OUT0202,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0202,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R56" s="20" t="str">
+        <v>LTR_OP: Mimic_Output_FB; // CHASSIS:OUT0202</v>
+      </c>
+      <c r="S56" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>LTR_OP: Mimic_Output_FB; // CHASSIS:OUT0202</v>
-      </c>
-      <c r="S56" s="20" t="str">
+        <v>CHASSIS.OUT0202();</v>
+      </c>
+      <c r="T56" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0202();</v>
-      </c>
-      <c r="T56" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0202.Init(Machine_IO.Outputs.LTR_OP);</v>
       </c>
     </row>
@@ -6297,11 +6310,11 @@
         <v>RightTrackDivert_OP:BOOL;</v>
       </c>
       <c r="N57" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>RIGHTTRACKDIVERT_OP:OpCom; // CHASSIS.OUT0203</v>
+      </c>
+      <c r="O57" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>RIGHTTRACKDIVERT_OP:OpCom; // CHASSIS.OUT0203</v>
-      </c>
-      <c r="O57" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RIGHTTRACKDIVERT_OP</v>
       </c>
       <c r="P57" s="20" t="str">
@@ -6309,19 +6322,19 @@
         <v>Machine_IO.Outputs.RIGHTTRACKDIVERT_OP(); // CR0709.OUT0203</v>
       </c>
       <c r="Q57" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.RIGHTTRACKDIVERT_OP.Init('CHASSIS','RIGHTTRACKDIVERT_OP','OUT0203','a76',NVL_Outputs_States_CHASSIS.All.OUT0203,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0203,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R57" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.RIGHTTRACKDIVERT_OP.Init('CHASSIS','RightTrackDivert_OP','OUT0203','a76',NVL_Outputs_States_CHASSIS.All.OUT0203,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0203,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R57" s="20" t="str">
+        <v>RightTrackDivert_OP: Mimic_Output_FB; // CHASSIS:OUT0203</v>
+      </c>
+      <c r="S57" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>RightTrackDivert_OP: Mimic_Output_FB; // CHASSIS:OUT0203</v>
-      </c>
-      <c r="S57" s="20" t="str">
+        <v>CHASSIS.OUT0203();</v>
+      </c>
+      <c r="T57" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0203();</v>
-      </c>
-      <c r="T57" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0203.Init(Machine_IO.Outputs.RIGHTTRACKDIVERT_OP);</v>
       </c>
     </row>
@@ -6372,11 +6385,11 @@
         <v>RTF_OP:BOOL;</v>
       </c>
       <c r="N58" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>RTF_OP:OpCom; // CHASSIS.OUT0204</v>
+      </c>
+      <c r="O58" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>RTF_OP:OpCom; // CHASSIS.OUT0204</v>
-      </c>
-      <c r="O58" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RTF_OP</v>
       </c>
       <c r="P58" s="20" t="str">
@@ -6384,19 +6397,19 @@
         <v>Machine_IO.Outputs.RTF_OP(); // CR0709.OUT0204</v>
       </c>
       <c r="Q58" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.RTF_OP.Init('CHASSIS','RTF_OP','OUT0204','a77',NVL_Outputs_States_CHASSIS.All.OUT0204,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0204,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R58" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.RTF_OP.Init('CHASSIS','RTF_OP','OUT0204','a77',NVL_Outputs_States_CHASSIS.All.OUT0204,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0204,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R58" s="20" t="str">
+        <v>RTF_OP: Mimic_Output_FB; // CHASSIS:OUT0204</v>
+      </c>
+      <c r="S58" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>RTF_OP: Mimic_Output_FB; // CHASSIS:OUT0204</v>
-      </c>
-      <c r="S58" s="20" t="str">
+        <v>CHASSIS.OUT0204();</v>
+      </c>
+      <c r="T58" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0204();</v>
-      </c>
-      <c r="T58" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0204.Init(Machine_IO.Outputs.RTF_OP);</v>
       </c>
     </row>
@@ -6447,11 +6460,11 @@
         <v>RTR_OP:BOOL;</v>
       </c>
       <c r="N59" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>RTR_OP:OpCom; // CHASSIS.OUT0205</v>
+      </c>
+      <c r="O59" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>RTR_OP:OpCom; // CHASSIS.OUT0205</v>
-      </c>
-      <c r="O59" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RTR_OP</v>
       </c>
       <c r="P59" s="20" t="str">
@@ -6459,19 +6472,19 @@
         <v>Machine_IO.Outputs.RTR_OP(); // CR0709.OUT0205</v>
       </c>
       <c r="Q59" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.RTR_OP.Init('CHASSIS','RTR_OP','OUT0205','a78',NVL_Outputs_States_CHASSIS.All.OUT0205,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0205,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R59" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.RTR_OP.Init('CHASSIS','RTR_OP','OUT0205','a78',NVL_Outputs_States_CHASSIS.All.OUT0205,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0205,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R59" s="20" t="str">
+        <v>RTR_OP: Mimic_Output_FB; // CHASSIS:OUT0205</v>
+      </c>
+      <c r="S59" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>RTR_OP: Mimic_Output_FB; // CHASSIS:OUT0205</v>
-      </c>
-      <c r="S59" s="20" t="str">
+        <v>CHASSIS.OUT0205();</v>
+      </c>
+      <c r="T59" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0205();</v>
-      </c>
-      <c r="T59" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0205.Init(Machine_IO.Outputs.RTR_OP);</v>
       </c>
     </row>
@@ -6522,11 +6535,11 @@
         <v>DrumOnOff_OP:BOOL;</v>
       </c>
       <c r="N60" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>DRUMONOFF_OP:OpCom; // CHASSIS.OUT0206</v>
+      </c>
+      <c r="O60" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>DRUMONOFF_OP:OpCom; // CHASSIS.OUT0206</v>
-      </c>
-      <c r="O60" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.DRUMONOFF_OP</v>
       </c>
       <c r="P60" s="20" t="str">
@@ -6534,19 +6547,19 @@
         <v>Machine_IO.Outputs.DRUMONOFF_OP(); // CR0709.OUT0206</v>
       </c>
       <c r="Q60" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.DRUMONOFF_OP.Init('CHASSIS','DRUMONOFF_OP','OUT0206','a79',NVL_Outputs_States_CHASSIS.All.OUT0206,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0206,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R60" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.DRUMONOFF_OP.Init('CHASSIS','DrumOnOff_OP','OUT0206','a79',NVL_Outputs_States_CHASSIS.All.OUT0206,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0206,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R60" s="20" t="str">
+        <v>DrumOnOff_OP: Mimic_Output_FB; // CHASSIS:OUT0206</v>
+      </c>
+      <c r="S60" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>DrumOnOff_OP: Mimic_Output_FB; // CHASSIS:OUT0206</v>
-      </c>
-      <c r="S60" s="20" t="str">
+        <v>CHASSIS.OUT0206();</v>
+      </c>
+      <c r="T60" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0206();</v>
-      </c>
-      <c r="T60" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0206.Init(Machine_IO.Outputs.DRUMONOFF_OP);</v>
       </c>
     </row>
@@ -6597,11 +6610,11 @@
         <v>FeederOnOff_OP:BOOL;</v>
       </c>
       <c r="N61" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>FEEDERONOFF_OP:OpCom; // CHASSIS.OUT0207</v>
+      </c>
+      <c r="O61" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>FEEDERONOFF_OP:OpCom; // CHASSIS.OUT0207</v>
-      </c>
-      <c r="O61" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.FEEDERONOFF_OP</v>
       </c>
       <c r="P61" s="20" t="str">
@@ -6609,19 +6622,19 @@
         <v>Machine_IO.Outputs.FEEDERONOFF_OP(); // CR0709.OUT0207</v>
       </c>
       <c r="Q61" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.FEEDERONOFF_OP.Init('CHASSIS','FEEDERONOFF_OP','OUT0207','a80',NVL_Outputs_States_CHASSIS.All.OUT0207,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0207,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R61" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.FEEDERONOFF_OP.Init('CHASSIS','FeederOnOff_OP','OUT0207','a80',NVL_Outputs_States_CHASSIS.All.OUT0207,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0207,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R61" s="20" t="str">
+        <v>FeederOnOff_OP: Mimic_Output_FB; // CHASSIS:OUT0207</v>
+      </c>
+      <c r="S61" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>FeederOnOff_OP: Mimic_Output_FB; // CHASSIS:OUT0207</v>
-      </c>
-      <c r="S61" s="20" t="str">
+        <v>CHASSIS.OUT0207();</v>
+      </c>
+      <c r="T61" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0207();</v>
-      </c>
-      <c r="T61" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0207.Init(Machine_IO.Outputs.FEEDERONOFF_OP);</v>
       </c>
     </row>
@@ -6672,11 +6685,11 @@
         <v>ECUenable:BOOL;</v>
       </c>
       <c r="N62" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>ECUENABLE:OpCom; // CHASSIS.OUT0208</v>
+      </c>
+      <c r="O62" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>ECUENABLE:OpCom; // CHASSIS.OUT0208</v>
-      </c>
-      <c r="O62" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.ECUENABLE</v>
       </c>
       <c r="P62" s="20" t="str">
@@ -6684,19 +6697,19 @@
         <v>Machine_IO.Outputs.ECUENABLE(); // CR0709.OUT0208</v>
       </c>
       <c r="Q62" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.ECUENABLE.Init('CHASSIS','ECUENABLE','OUT0208','a81',NVL_Outputs_States_CHASSIS.All.OUT0208,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0208,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R62" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.ECUENABLE.Init('CHASSIS','ECUenable','OUT0208','a81',NVL_Outputs_States_CHASSIS.All.OUT0208,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0208,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R62" s="20" t="str">
+        <v>ECUenable: Mimic_Output_FB; // CHASSIS:OUT0208</v>
+      </c>
+      <c r="S62" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>ECUenable: Mimic_Output_FB; // CHASSIS:OUT0208</v>
-      </c>
-      <c r="S62" s="20" t="str">
+        <v>CHASSIS.OUT0208();</v>
+      </c>
+      <c r="T62" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT0208();</v>
-      </c>
-      <c r="T62" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0208.Init(Machine_IO.Outputs.ECUENABLE);</v>
       </c>
     </row>
@@ -6735,42 +6748,44 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.GROUP2</v>
       </c>
-      <c r="K63" s="19"/>
+      <c r="K63" s="19" t="s">
+        <v>529</v>
+      </c>
       <c r="L63" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>SPARE_GROUP2</v>
+        <v>SUPPLY_GROUP2</v>
       </c>
       <c r="M63" s="19" t="str">
         <f t="shared" si="11"/>
-        <v>:BOOL;</v>
+        <v>SUPPLY_GROUP2:BOOL;</v>
       </c>
       <c r="N63" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>SUPPLY_GROUP2:OpCom; // CHASSIS.GROUP2</v>
+      </c>
+      <c r="O63" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>SPARE_GROUP2:OpCom; // CHASSIS.GROUP2</v>
-      </c>
-      <c r="O63" s="20" t="str">
-        <f t="shared" si="18"/>
-        <v>Machine_IO.Outputs.SPARE_GROUP2</v>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP2</v>
       </c>
       <c r="P63" s="20" t="str">
         <f t="shared" si="12"/>
-        <v>Machine_IO.Outputs.SPARE_GROUP2(); // CR0709.GROUP2</v>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP2(); // CR0709.GROUP2</v>
       </c>
       <c r="Q63" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP2.Init('CHASSIS','SUPPLY_GROUP2','GROUP2','a1',NVL_Outputs_States_CHASSIS.All.GROUP2,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP2,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R63" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.SPARE_GROUP2.Init('CHASSIS','','GROUP2','a1',NVL_Outputs_States_CHASSIS.All.GROUP2,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP2,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R63" s="20" t="str">
+        <v>SUPPLY_GROUP2: Mimic_Output_FB; // CHASSIS:GROUP2</v>
+      </c>
+      <c r="S63" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>: Mimic_Output_FB; // CHASSIS:GROUP2</v>
-      </c>
-      <c r="S63" s="20" t="str">
+        <v>CHASSIS.GROUP2();</v>
+      </c>
+      <c r="T63" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.GROUP2();</v>
-      </c>
-      <c r="T63" s="20" t="str">
-        <f t="shared" si="16"/>
-        <v>CHASSIS.GROUP2.Init(Machine_IO.Outputs.SPARE_GROUP2);</v>
+        <v>CHASSIS.GROUP2.Init(Machine_IO.Outputs.SUPPLY_GROUP2);</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
@@ -6816,11 +6831,11 @@
         <v>:BOOL;</v>
       </c>
       <c r="N64" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>SPARE_OUT3000:OpCom; // CHASSIS.OUT3000</v>
+      </c>
+      <c r="O64" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>SPARE_OUT3000:OpCom; // CHASSIS.OUT3000</v>
-      </c>
-      <c r="O64" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SPARE_OUT3000</v>
       </c>
       <c r="P64" s="20" t="str">
@@ -6828,19 +6843,19 @@
         <v>Machine_IO.Outputs.SPARE_OUT3000(); // CR0709.OUT3000</v>
       </c>
       <c r="Q64" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.SPARE_OUT3000.Init('CHASSIS','SPARE_OUT3000','OUT3000','a31',NVL_Outputs_States_CHASSIS.All.OUT3000,NVL_IO_CHASSIS.All_Outputs_Diag.OUT3000,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R64" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.SPARE_OUT3000.Init('CHASSIS','','OUT3000','a31',NVL_Outputs_States_CHASSIS.All.OUT3000,NVL_IO_CHASSIS.All_Outputs_Diag.OUT3000,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R64" s="20" t="str">
+        <v>: Mimic_Output_FB; // CHASSIS:OUT3000</v>
+      </c>
+      <c r="S64" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>: Mimic_Output_FB; // CHASSIS:OUT3000</v>
-      </c>
-      <c r="S64" s="20" t="str">
+        <v>CHASSIS.OUT3000();</v>
+      </c>
+      <c r="T64" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT3000();</v>
-      </c>
-      <c r="T64" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT3000.Init(Machine_IO.Outputs.SPARE_OUT3000);</v>
       </c>
     </row>
@@ -6887,11 +6902,11 @@
         <v>:BOOL;</v>
       </c>
       <c r="N65" s="20" t="str">
+        <f t="shared" si="16"/>
+        <v>SPARE_OUT3001:OpCom; // CHASSIS.OUT3001</v>
+      </c>
+      <c r="O65" s="20" t="str">
         <f t="shared" si="17"/>
-        <v>SPARE_OUT3001:OpCom; // CHASSIS.OUT3001</v>
-      </c>
-      <c r="O65" s="20" t="str">
-        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SPARE_OUT3001</v>
       </c>
       <c r="P65" s="20" t="str">
@@ -6899,19 +6914,19 @@
         <v>Machine_IO.Outputs.SPARE_OUT3001(); // CR0709.OUT3001</v>
       </c>
       <c r="Q65" s="20" t="str">
+        <f t="shared" si="18"/>
+        <v>Machine_IO.Outputs.SPARE_OUT3001.Init('CHASSIS','SPARE_OUT3001','OUT3001','a32',NVL_Outputs_States_CHASSIS.All.OUT3001,NVL_IO_CHASSIS.All_Outputs_Diag.OUT3001,Machine_IO.Node_CHASSIS);</v>
+      </c>
+      <c r="R65" s="20" t="str">
         <f t="shared" si="13"/>
-        <v>Machine_IO.Outputs.SPARE_OUT3001.Init('CHASSIS','','OUT3001','a32',NVL_Outputs_States_CHASSIS.All.OUT3001,NVL_IO_CHASSIS.All_Outputs_Diag.OUT3001,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R65" s="20" t="str">
+        <v>: Mimic_Output_FB; // CHASSIS:OUT3001</v>
+      </c>
+      <c r="S65" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>: Mimic_Output_FB; // CHASSIS:OUT3001</v>
-      </c>
-      <c r="S65" s="20" t="str">
+        <v>CHASSIS.OUT3001();</v>
+      </c>
+      <c r="T65" s="20" t="str">
         <f t="shared" si="15"/>
-        <v>CHASSIS.OUT3001();</v>
-      </c>
-      <c r="T65" s="20" t="str">
-        <f t="shared" si="16"/>
         <v>CHASSIS.OUT3001.Init(Machine_IO.Outputs.SPARE_OUT3001);</v>
       </c>
     </row>
@@ -18106,24 +18121,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
-    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
-      <UserInfo>
-        <DisplayName>Noel Loughran</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9F7729ADF49144A01A6175DD599202" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f00ebe7287476f312414df31db46304">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c96d9849-7071-4555-8535-ee11c374d0f7" xmlns:ns3="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f2e969a0d0c60cbdf6bd0d859a86451" ns2:_="" ns3:_="">
     <xsd:import namespace="c96d9849-7071-4555-8535-ee11c374d0f7"/>
@@ -18346,6 +18343,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
+    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
+      <UserInfo>
+        <DisplayName>Noel Loughran</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
   <ds:schemaRefs>
@@ -18355,23 +18370,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6596B7D1-B3E6-40CB-B05E-2E959D1A2B6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18388,4 +18386,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cleaned out the old navigation
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8915D6B6-E630-4487-8700-A6FB902527C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960FD73E-28F6-4D6E-AC23-175DC5D6BE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="4" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
-    <sheet name="IfmPinRef" sheetId="21" r:id="rId2"/>
-    <sheet name="ALARMS" sheetId="24" r:id="rId3"/>
-    <sheet name="ALARMS_IO" sheetId="31" r:id="rId4"/>
+    <sheet name="Settings" sheetId="32" r:id="rId2"/>
+    <sheet name="IfmPinRef" sheetId="21" r:id="rId3"/>
+    <sheet name="ALARMS" sheetId="24" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="33" r:id="rId5"/>
+    <sheet name="ALARMS_IO" sheetId="31" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AO$71</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1898" uniqueCount="561">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1633,6 +1635,99 @@
   </si>
   <si>
     <t>SUPPLY_GROUP2</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.TailConvSpd_Min_mA</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.TailConvSpd_Max_mA</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.SideTransferConvSpd_Min_mA</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.SideTransferConvSpd_Max_mA</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.DrumSpd_Min_mA</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.CollectConvSpd_Min_mA</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.CollectConvSpd_Max_mA</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.DrumSpd_Max_mA</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.FeederSpd_Min_mA</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.FeederSpd_Max_mA</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.EnableDrumPressCutOut</t>
+  </si>
+  <si>
+    <t>Siren Beacon</t>
+  </si>
+  <si>
+    <t>oil Cooker</t>
+  </si>
+  <si>
+    <t>oil cooler for/rev</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.DrumPressHiHi_SP_bar</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.DrumPressReset_SP_bar</t>
+  </si>
+  <si>
+    <t>NVL_UDP_RX.App_Settings.DrumPressHi_SP_bar</t>
+  </si>
+  <si>
+    <t>Pin code has system</t>
+  </si>
+  <si>
+    <t>Scale fuel sender for Diag</t>
+  </si>
+  <si>
+    <t>Scale pressure sensor for Diag</t>
+  </si>
+  <si>
+    <t>Siren/Beacon Blip for Alarm</t>
+  </si>
+  <si>
+    <t>Check DM1 decoding</t>
+  </si>
+  <si>
+    <t>DM1 text list? (SPN)</t>
+  </si>
+  <si>
+    <t>consolidate radio program</t>
+  </si>
+  <si>
+    <t>consolidate all to the HMI</t>
+  </si>
+  <si>
+    <t>NVL_UDP_TX.App_Settings.CollectConvSpd_Percent</t>
+  </si>
+  <si>
+    <t>NVL_UDP_TX.App_Settings.SideTransferConvSpd_Percent</t>
+  </si>
+  <si>
+    <t>NVL_UDP_TX.App_Settings.SideConvSpd_Percent</t>
+  </si>
+  <si>
+    <t>NVL_UDP_TX.App_Settings.TailConvSpd_Percent</t>
+  </si>
+  <si>
+    <t>NVL_UDP_TX.App_Settings.FeederSpd_Percent</t>
+  </si>
+  <si>
+    <t>NVL_UDP_TX.App_Settings.DrumSpd_Percent</t>
   </si>
 </sst>
 </file>
@@ -2178,11 +2273,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T67"/>
+  <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K64" sqref="K64"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -6960,6 +7055,9 @@
       <c r="H67" s="23"/>
       <c r="I67" s="23"/>
       <c r="J67" s="23"/>
+      <c r="K67" s="24" t="s">
+        <v>541</v>
+      </c>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
@@ -6967,6 +7065,16 @@
       <c r="R67" s="2"/>
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K68" s="4" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="K69" s="4" t="s">
+        <v>543</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AO71" xr:uid="{1E4EBF08-015A-4388-B8C8-8A07CE5EF3C7}"/>
@@ -6977,6 +7085,218 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C712512B-3394-456F-A3A8-618A03016890}">
+  <dimension ref="B2:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="54.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>530</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>530</v>
+      </c>
+      <c r="D3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>530</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>531</v>
+      </c>
+      <c r="D6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>532</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>533</v>
+      </c>
+      <c r="D9">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>535</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>536</v>
+      </c>
+      <c r="D12">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>534</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>537</v>
+      </c>
+      <c r="D15">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>538</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>539</v>
+      </c>
+      <c r="D18">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>540</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>544</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>545</v>
+      </c>
+      <c r="D24">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>559</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>560</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>555</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>556</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>557</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>558</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E538D0C9-5DB1-4DD2-BFB3-B509B6A8D4D3}">
   <dimension ref="A1:Q196"/>
   <sheetViews>
@@ -13211,11 +13531,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D6A96C-314C-4D0F-A31C-2D0C36E8E519}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -15172,7 +15492,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
+  <dimension ref="B3:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>554</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B17012-44D7-48B2-87FC-FA2A9133EF8D}">
   <dimension ref="A1:L65"/>
   <sheetViews>
@@ -18121,6 +18499,24 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
+    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
+      <UserInfo>
+        <DisplayName>Noel Loughran</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9F7729ADF49144A01A6175DD599202" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f00ebe7287476f312414df31db46304">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c96d9849-7071-4555-8535-ee11c374d0f7" xmlns:ns3="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f2e969a0d0c60cbdf6bd0d859a86451" ns2:_="" ns3:_="">
     <xsd:import namespace="c96d9849-7071-4555-8535-ee11c374d0f7"/>
@@ -18343,24 +18739,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
-    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
-      <UserInfo>
-        <DisplayName>Noel Loughran</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
   <ds:schemaRefs>
@@ -18370,6 +18748,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6596B7D1-B3E6-40CB-B05E-2E959D1A2B6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18386,21 +18781,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
WIP - moving machine logic to the HM!
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960FD73E-28F6-4D6E-AC23-175DC5D6BE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA9DB45-1D46-4E6E-A53F-D3F79AD947E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="4" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AO$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$71</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -2273,11 +2273,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T69"/>
+  <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K70" sqref="K70"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2293,19 +2293,20 @@
     <col min="10" max="10" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="44.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="54" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="70.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="200" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="61.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="57.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="14.140625" style="4" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="4"/>
+    <col min="13" max="13" width="26.85546875" style="4" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="44.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="54" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="54" style="2" customWidth="1"/>
+    <col min="17" max="17" width="70.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="200" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="61.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="57.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="14.140625" style="4" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="9" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="9" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -2349,23 +2350,24 @@
       <c r="O1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="R1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="S1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="T1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="U1" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>93</v>
       </c>
@@ -2417,27 +2419,31 @@
         <v>Machine_IO.Inputs.ESTOP_OK</v>
       </c>
       <c r="P2" s="20" t="str">
-        <f t="shared" ref="P2:P33" si="2">_xlfn.CONCAT(O2,"(); // ",E2)</f>
+        <f>_xlfn.CONCAT(O2,".Dig")</f>
+        <v>Machine_IO.Inputs.ESTOP_OK.Dig</v>
+      </c>
+      <c r="Q2" s="20" t="str">
+        <f t="shared" ref="Q2:Q33" si="2">_xlfn.CONCAT(O2,"(); // ",E2)</f>
         <v>Machine_IO.Inputs.ESTOP_OK(); // CR0709.IN0100</v>
       </c>
-      <c r="Q2" s="20" t="str">
+      <c r="R2" s="20" t="str">
         <f>_xlfn.CONCAT("Machine_IO.","Inputs.",L2,".Init('",A2,"','",L2,"','",D2,"','",G2,"',","NVL_IO_",A2,".All_Inputs.",D2,",Machine_IO.Node_",A2,");")</f>
         <v>Machine_IO.Inputs.ESTOP_OK.Init('CHASSIS','ESTOP_OK','IN0100','a63',NVL_IO_CHASSIS.All_Inputs.IN0100,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R2" s="20" t="str">
-        <f t="shared" ref="R2:R33" si="3">_xlfn.CONCAT(K2,": Mimic_Input_FB; // ",A2,":",D2)</f>
+      <c r="S2" s="20" t="str">
+        <f t="shared" ref="S2:S33" si="3">_xlfn.CONCAT(K2,": Mimic_Input_FB; // ",A2,":",D2)</f>
         <v>ESTOP_OK: Mimic_Input_FB; // CHASSIS:IN0100</v>
       </c>
-      <c r="S2" s="20" t="str">
-        <f t="shared" ref="S2:S33" si="4">_xlfn.CONCAT(A2,".",D2,"();")</f>
+      <c r="T2" s="20" t="str">
+        <f t="shared" ref="T2:T33" si="4">_xlfn.CONCAT(A2,".",D2,"();")</f>
         <v>CHASSIS.IN0100();</v>
       </c>
-      <c r="T2" s="20" t="str">
-        <f t="shared" ref="T2:T33" si="5">_xlfn.CONCAT(A2,".",D2,".Init(",O2,");")</f>
+      <c r="U2" s="20" t="str">
+        <f t="shared" ref="U2:U33" si="5">_xlfn.CONCAT(A2,".",D2,".Init(",O2,");")</f>
         <v>CHASSIS.IN0100.Init(Machine_IO.Inputs.ESTOP_OK);</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>93</v>
       </c>
@@ -2489,27 +2495,31 @@
         <v>Machine_IO.Inputs.DRUM_PRESSURE</v>
       </c>
       <c r="P3" s="20" t="str">
+        <f t="shared" ref="P3:P65" si="10">_xlfn.CONCAT(O3,".Dig")</f>
+        <v>Machine_IO.Inputs.DRUM_PRESSURE.Dig</v>
+      </c>
+      <c r="Q3" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.DRUM_PRESSURE(); // CR0709.IN0101</v>
       </c>
-      <c r="Q3" s="20" t="str">
-        <f t="shared" ref="Q3:Q33" si="10">_xlfn.CONCAT("Machine_IO.","Inputs.",L3,".Init('",A3,"','",L3,"','",D3,"','",G3,"',","NVL_IO_",A3,".All_Inputs.",D3,",Machine_IO.Node_",A3,");")</f>
+      <c r="R3" s="20" t="str">
+        <f t="shared" ref="R3:R33" si="11">_xlfn.CONCAT("Machine_IO.","Inputs.",L3,".Init('",A3,"','",L3,"','",D3,"','",G3,"',","NVL_IO_",A3,".All_Inputs.",D3,",Machine_IO.Node_",A3,");")</f>
         <v>Machine_IO.Inputs.DRUM_PRESSURE.Init('CHASSIS','DRUM_PRESSURE','IN0101','a64',NVL_IO_CHASSIS.All_Inputs.IN0101,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R3" s="20" t="str">
+      <c r="S3" s="20" t="str">
         <f t="shared" si="3"/>
         <v>DRUM_PRESSURE: Mimic_Input_FB; // CHASSIS:IN0101</v>
       </c>
-      <c r="S3" s="20" t="str">
+      <c r="T3" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0101();</v>
       </c>
-      <c r="T3" s="20" t="str">
+      <c r="U3" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0101.Init(Machine_IO.Inputs.DRUM_PRESSURE);</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>93</v>
       </c>
@@ -2559,27 +2569,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0102</v>
       </c>
       <c r="P4" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0102.Dig</v>
+      </c>
+      <c r="Q4" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0102(); // CR0709.IN0102</v>
       </c>
-      <c r="Q4" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R4" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0102.Init('CHASSIS','SPARE_IN0102','IN0102','a65',NVL_IO_CHASSIS.All_Inputs.IN0102,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R4" s="20" t="str">
+      <c r="S4" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0102</v>
       </c>
-      <c r="S4" s="20" t="str">
+      <c r="T4" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0102();</v>
       </c>
-      <c r="T4" s="20" t="str">
+      <c r="U4" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0102.Init(Machine_IO.Inputs.SPARE_IN0102);</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>93</v>
       </c>
@@ -2629,27 +2643,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0103</v>
       </c>
       <c r="P5" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0103.Dig</v>
+      </c>
+      <c r="Q5" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0103(); // CR0709.IN0103</v>
       </c>
-      <c r="Q5" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R5" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0103.Init('CHASSIS','SPARE_IN0103','IN0103','a66',NVL_IO_CHASSIS.All_Inputs.IN0103,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R5" s="20" t="str">
+      <c r="S5" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0103</v>
       </c>
-      <c r="S5" s="20" t="str">
+      <c r="T5" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0103();</v>
       </c>
-      <c r="T5" s="20" t="str">
+      <c r="U5" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0103.Init(Machine_IO.Inputs.SPARE_IN0103);</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>93</v>
       </c>
@@ -2699,27 +2717,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0200</v>
       </c>
       <c r="P6" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0200.Dig</v>
+      </c>
+      <c r="Q6" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0200(); // CR0709.IN0200</v>
       </c>
-      <c r="Q6" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R6" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0200.Init('CHASSIS','SPARE_IN0200','IN0200','a67',NVL_IO_CHASSIS.All_Inputs.IN0200,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R6" s="20" t="str">
+      <c r="S6" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0200</v>
       </c>
-      <c r="S6" s="20" t="str">
+      <c r="T6" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0200();</v>
       </c>
-      <c r="T6" s="20" t="str">
+      <c r="U6" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0200.Init(Machine_IO.Inputs.SPARE_IN0200);</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>93</v>
       </c>
@@ -2769,27 +2791,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0201</v>
       </c>
       <c r="P7" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0201.Dig</v>
+      </c>
+      <c r="Q7" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0201(); // CR0709.IN0201</v>
       </c>
-      <c r="Q7" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R7" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0201.Init('CHASSIS','SPARE_IN0201','IN0201','a68',NVL_IO_CHASSIS.All_Inputs.IN0201,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R7" s="20" t="str">
+      <c r="S7" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0201</v>
       </c>
-      <c r="S7" s="20" t="str">
+      <c r="T7" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0201();</v>
       </c>
-      <c r="T7" s="20" t="str">
+      <c r="U7" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0201.Init(Machine_IO.Inputs.SPARE_IN0201);</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>93</v>
       </c>
@@ -2839,27 +2865,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0202</v>
       </c>
       <c r="P8" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0202.Dig</v>
+      </c>
+      <c r="Q8" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0202(); // CR0709.IN0202</v>
       </c>
-      <c r="Q8" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R8" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0202.Init('CHASSIS','SPARE_IN0202','IN0202','a69',NVL_IO_CHASSIS.All_Inputs.IN0202,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R8" s="20" t="str">
+      <c r="S8" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0202</v>
       </c>
-      <c r="S8" s="20" t="str">
+      <c r="T8" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0202();</v>
       </c>
-      <c r="T8" s="20" t="str">
+      <c r="U8" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0202.Init(Machine_IO.Inputs.SPARE_IN0202);</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>93</v>
       </c>
@@ -2909,27 +2939,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0203</v>
       </c>
       <c r="P9" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0203.Dig</v>
+      </c>
+      <c r="Q9" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0203(); // CR0709.IN0203</v>
       </c>
-      <c r="Q9" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R9" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0203.Init('CHASSIS','SPARE_IN0203','IN0203','a70',NVL_IO_CHASSIS.All_Inputs.IN0203,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R9" s="20" t="str">
+      <c r="S9" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0203</v>
       </c>
-      <c r="S9" s="20" t="str">
+      <c r="T9" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0203();</v>
       </c>
-      <c r="T9" s="20" t="str">
+      <c r="U9" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0203.Init(Machine_IO.Inputs.SPARE_IN0203);</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>93</v>
       </c>
@@ -2979,27 +3013,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0600</v>
       </c>
       <c r="P10" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0600.Dig</v>
+      </c>
+      <c r="Q10" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0600(); // CR0709.IN0600</v>
       </c>
-      <c r="Q10" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R10" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0600.Init('CHASSIS','SPARE_IN0600','IN0600','a55',NVL_IO_CHASSIS.All_Inputs.IN0600,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R10" s="20" t="str">
+      <c r="S10" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0600</v>
       </c>
-      <c r="S10" s="20" t="str">
+      <c r="T10" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0600();</v>
       </c>
-      <c r="T10" s="20" t="str">
+      <c r="U10" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0600.Init(Machine_IO.Inputs.SPARE_IN0600);</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>93</v>
       </c>
@@ -3049,27 +3087,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0601</v>
       </c>
       <c r="P11" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0601.Dig</v>
+      </c>
+      <c r="Q11" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0601(); // CR0709.IN0601</v>
       </c>
-      <c r="Q11" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R11" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0601.Init('CHASSIS','SPARE_IN0601','IN0601','a56',NVL_IO_CHASSIS.All_Inputs.IN0601,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R11" s="20" t="str">
+      <c r="S11" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0601</v>
       </c>
-      <c r="S11" s="20" t="str">
+      <c r="T11" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0601();</v>
       </c>
-      <c r="T11" s="20" t="str">
+      <c r="U11" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0601.Init(Machine_IO.Inputs.SPARE_IN0601);</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>93</v>
       </c>
@@ -3119,27 +3161,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0602</v>
       </c>
       <c r="P12" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0602.Dig</v>
+      </c>
+      <c r="Q12" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0602(); // CR0709.IN0602</v>
       </c>
-      <c r="Q12" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R12" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0602.Init('CHASSIS','SPARE_IN0602','IN0602','a57',NVL_IO_CHASSIS.All_Inputs.IN0602,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R12" s="20" t="str">
+      <c r="S12" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0602</v>
       </c>
-      <c r="S12" s="20" t="str">
+      <c r="T12" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0602();</v>
       </c>
-      <c r="T12" s="20" t="str">
+      <c r="U12" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0602.Init(Machine_IO.Inputs.SPARE_IN0602);</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>93</v>
       </c>
@@ -3189,27 +3235,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0603</v>
       </c>
       <c r="P13" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0603.Dig</v>
+      </c>
+      <c r="Q13" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0603(); // CR0709.IN0603</v>
       </c>
-      <c r="Q13" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R13" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0603.Init('CHASSIS','SPARE_IN0603','IN0603','a58',NVL_IO_CHASSIS.All_Inputs.IN0603,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R13" s="20" t="str">
+      <c r="S13" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0603</v>
       </c>
-      <c r="S13" s="20" t="str">
+      <c r="T13" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0603();</v>
       </c>
-      <c r="T13" s="20" t="str">
+      <c r="U13" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0603.Init(Machine_IO.Inputs.SPARE_IN0603);</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>93</v>
       </c>
@@ -3259,27 +3309,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0700</v>
       </c>
       <c r="P14" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0700.Dig</v>
+      </c>
+      <c r="Q14" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0700(); // CR0709.IN0700</v>
       </c>
-      <c r="Q14" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R14" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0700.Init('CHASSIS','SPARE_IN0700','IN0700','a59',NVL_IO_CHASSIS.All_Inputs.IN0700,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R14" s="20" t="str">
+      <c r="S14" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0700</v>
       </c>
-      <c r="S14" s="20" t="str">
+      <c r="T14" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0700();</v>
       </c>
-      <c r="T14" s="20" t="str">
+      <c r="U14" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0700.Init(Machine_IO.Inputs.SPARE_IN0700);</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>93</v>
       </c>
@@ -3331,27 +3385,31 @@
         <v>Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ</v>
       </c>
       <c r="P15" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ.Dig</v>
+      </c>
+      <c r="Q15" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ(); // CR0709.IN0701</v>
       </c>
-      <c r="Q15" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R15" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ.Init('CHASSIS','RADIORHS_JACKLEGRAISE_REQ','IN0701','a60',NVL_IO_CHASSIS.All_Inputs.IN0701,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R15" s="20" t="str">
+      <c r="S15" s="20" t="str">
         <f t="shared" si="3"/>
         <v>RadioRHS_JackLegRaise_Req: Mimic_Input_FB; // CHASSIS:IN0701</v>
       </c>
-      <c r="S15" s="20" t="str">
+      <c r="T15" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0701();</v>
       </c>
-      <c r="T15" s="20" t="str">
+      <c r="U15" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0701.Init(Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ);</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>93</v>
       </c>
@@ -3403,27 +3461,31 @@
         <v>Machine_IO.Inputs.RHS_TROMMELDOORSW</v>
       </c>
       <c r="P16" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RHS_TROMMELDOORSW.Dig</v>
+      </c>
+      <c r="Q16" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.RHS_TROMMELDOORSW(); // CR0709.IN0702</v>
       </c>
-      <c r="Q16" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R16" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.RHS_TROMMELDOORSW.Init('CHASSIS','RHS_TROMMELDOORSW','IN0702','a61',NVL_IO_CHASSIS.All_Inputs.IN0702,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R16" s="20" t="str">
+      <c r="S16" s="20" t="str">
         <f t="shared" si="3"/>
         <v>RHS_TrommelDoorSw: Mimic_Input_FB; // CHASSIS:IN0702</v>
       </c>
-      <c r="S16" s="20" t="str">
+      <c r="T16" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0702();</v>
       </c>
-      <c r="T16" s="20" t="str">
+      <c r="U16" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0702.Init(Machine_IO.Inputs.RHS_TROMMELDOORSW);</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>93</v>
       </c>
@@ -3475,27 +3537,31 @@
         <v>Machine_IO.Inputs.LHS_TROMMELDOORSW</v>
       </c>
       <c r="P17" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.LHS_TROMMELDOORSW.Dig</v>
+      </c>
+      <c r="Q17" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.LHS_TROMMELDOORSW(); // CR0709.IN0703</v>
       </c>
-      <c r="Q17" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R17" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.LHS_TROMMELDOORSW.Init('CHASSIS','LHS_TROMMELDOORSW','IN0703','a62',NVL_IO_CHASSIS.All_Inputs.IN0703,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R17" s="20" t="str">
+      <c r="S17" s="20" t="str">
         <f t="shared" si="3"/>
         <v>LHS_TrommelDoorSw: Mimic_Input_FB; // CHASSIS:IN0703</v>
       </c>
-      <c r="S17" s="20" t="str">
+      <c r="T17" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0703();</v>
       </c>
-      <c r="T17" s="20" t="str">
+      <c r="U17" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0703.Init(Machine_IO.Inputs.LHS_TROMMELDOORSW);</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>93</v>
       </c>
@@ -3547,27 +3613,31 @@
         <v>Machine_IO.Inputs.HYDOILTEMP_SW</v>
       </c>
       <c r="P18" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.HYDOILTEMP_SW.Dig</v>
+      </c>
+      <c r="Q18" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.HYDOILTEMP_SW(); // CR0709.IN0000</v>
       </c>
-      <c r="Q18" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R18" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.HYDOILTEMP_SW.Init('CHASSIS','HYDOILTEMP_SW','IN0000','a25',NVL_IO_CHASSIS.All_Inputs.IN0000,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R18" s="20" t="str">
+      <c r="S18" s="20" t="str">
         <f t="shared" si="3"/>
         <v>HydOilTemp_Sw: Mimic_Input_FB; // CHASSIS:IN0000</v>
       </c>
-      <c r="S18" s="20" t="str">
+      <c r="T18" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0000();</v>
       </c>
-      <c r="T18" s="20" t="str">
+      <c r="U18" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0000.Init(Machine_IO.Inputs.HYDOILTEMP_SW);</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>93</v>
       </c>
@@ -3619,27 +3689,31 @@
         <v>Machine_IO.Inputs.HYDOILLEVEL_SW</v>
       </c>
       <c r="P19" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.HYDOILLEVEL_SW.Dig</v>
+      </c>
+      <c r="Q19" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.HYDOILLEVEL_SW(); // CR0709.IN0001</v>
       </c>
-      <c r="Q19" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R19" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.HYDOILLEVEL_SW.Init('CHASSIS','HYDOILLEVEL_SW','IN0001','a26',NVL_IO_CHASSIS.All_Inputs.IN0001,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R19" s="20" t="str">
+      <c r="S19" s="20" t="str">
         <f t="shared" si="3"/>
         <v>HydOilLevel_Sw: Mimic_Input_FB; // CHASSIS:IN0001</v>
       </c>
-      <c r="S19" s="20" t="str">
+      <c r="T19" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0001();</v>
       </c>
-      <c r="T19" s="20" t="str">
+      <c r="U19" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0001.Init(Machine_IO.Inputs.HYDOILLEVEL_SW);</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>93</v>
       </c>
@@ -3691,27 +3765,31 @@
         <v>Machine_IO.Inputs.THERMOSTAT</v>
       </c>
       <c r="P20" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.THERMOSTAT.Dig</v>
+      </c>
+      <c r="Q20" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.THERMOSTAT(); // CR0709.IN0002</v>
       </c>
-      <c r="Q20" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R20" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.THERMOSTAT.Init('CHASSIS','THERMOSTAT','IN0002','a27',NVL_IO_CHASSIS.All_Inputs.IN0002,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R20" s="20" t="str">
+      <c r="S20" s="20" t="str">
         <f t="shared" si="3"/>
         <v>ThermoStat: Mimic_Input_FB; // CHASSIS:IN0002</v>
       </c>
-      <c r="S20" s="20" t="str">
+      <c r="T20" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0002();</v>
       </c>
-      <c r="T20" s="20" t="str">
+      <c r="U20" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0002.Init(Machine_IO.Inputs.THERMOSTAT);</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>93</v>
       </c>
@@ -3763,27 +3841,31 @@
         <v>Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ</v>
       </c>
       <c r="P21" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ.Dig</v>
+      </c>
+      <c r="Q21" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ(); // CR0709.IN0003</v>
       </c>
-      <c r="Q21" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R21" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ.Init('CHASSIS','RADIORHS_JACKLEGLOWER_REQ','IN0003','a28',NVL_IO_CHASSIS.All_Inputs.IN0003,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R21" s="20" t="str">
+      <c r="S21" s="20" t="str">
         <f t="shared" si="3"/>
         <v>RadioRHS_JackLegLower_Req: Mimic_Input_FB; // CHASSIS:IN0003</v>
       </c>
-      <c r="S21" s="20" t="str">
+      <c r="T21" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0003();</v>
       </c>
-      <c r="T21" s="20" t="str">
+      <c r="U21" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0003.Init(Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ);</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>93</v>
       </c>
@@ -3835,27 +3917,31 @@
         <v>Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ</v>
       </c>
       <c r="P22" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ.Dig</v>
+      </c>
+      <c r="Q22" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ(); // CR0709.IN0500</v>
       </c>
-      <c r="Q22" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R22" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ.Init('CHASSIS','RADIOLHS_JACKLEGRAISE_REQ','IN0500','a40',NVL_IO_CHASSIS.All_Inputs.IN0500,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R22" s="20" t="str">
+      <c r="S22" s="20" t="str">
         <f t="shared" si="3"/>
         <v>RadioLHS_JackLegRaise_Req: Mimic_Input_FB; // CHASSIS:IN0500</v>
       </c>
-      <c r="S22" s="20" t="str">
+      <c r="T22" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0500();</v>
       </c>
-      <c r="T22" s="20" t="str">
+      <c r="U22" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0500.Init(Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ);</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>93</v>
       </c>
@@ -3907,27 +3993,31 @@
         <v>Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ</v>
       </c>
       <c r="P23" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ.Dig</v>
+      </c>
+      <c r="Q23" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ(); // CR0709.IN0501</v>
       </c>
-      <c r="Q23" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R23" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ.Init('CHASSIS','RADIOLHS_JACKLEGLOWER_REQ','IN0501','a41',NVL_IO_CHASSIS.All_Inputs.IN0501,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R23" s="20" t="str">
+      <c r="S23" s="20" t="str">
         <f t="shared" si="3"/>
         <v>RadioLHS_JackLegLower_Req: Mimic_Input_FB; // CHASSIS:IN0501</v>
       </c>
-      <c r="S23" s="20" t="str">
+      <c r="T23" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0501();</v>
       </c>
-      <c r="T23" s="20" t="str">
+      <c r="U23" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0501.Init(Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ);</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>93</v>
       </c>
@@ -3979,27 +4069,31 @@
         <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ</v>
       </c>
       <c r="P24" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ.Dig</v>
+      </c>
+      <c r="Q24" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ(); // CR0709.IN0502</v>
       </c>
-      <c r="Q24" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R24" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ.Init('CHASSIS','RADIOSIDECONVRAISEREQ','IN0502','a42',NVL_IO_CHASSIS.All_Inputs.IN0502,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R24" s="20" t="str">
+      <c r="S24" s="20" t="str">
         <f t="shared" si="3"/>
         <v>RadioSideConvRaiseReq: Mimic_Input_FB; // CHASSIS:IN0502</v>
       </c>
-      <c r="S24" s="20" t="str">
+      <c r="T24" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0502();</v>
       </c>
-      <c r="T24" s="20" t="str">
+      <c r="U24" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0502.Init(Machine_IO.Inputs.RADIOSIDECONVRAISEREQ);</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>93</v>
       </c>
@@ -4051,27 +4145,31 @@
         <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ</v>
       </c>
       <c r="P25" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ.Dig</v>
+      </c>
+      <c r="Q25" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ(); // CR0709.IN0503</v>
       </c>
-      <c r="Q25" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R25" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ.Init('CHASSIS','RADIOSIDECONVLOWERREQ','IN0503','a43',NVL_IO_CHASSIS.All_Inputs.IN0503,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R25" s="20" t="str">
+      <c r="S25" s="20" t="str">
         <f t="shared" si="3"/>
         <v>RadioSideConvLowerReq: Mimic_Input_FB; // CHASSIS:IN0503</v>
       </c>
-      <c r="S25" s="20" t="str">
+      <c r="T25" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0503();</v>
       </c>
-      <c r="T25" s="20" t="str">
+      <c r="U25" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0503.Init(Machine_IO.Inputs.RADIOSIDECONVLOWERREQ);</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>93</v>
       </c>
@@ -4121,27 +4219,31 @@
         <v>Machine_IO.Inputs.SPARE_IN0400</v>
       </c>
       <c r="P26" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.SPARE_IN0400.Dig</v>
+      </c>
+      <c r="Q26" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.SPARE_IN0400(); // CR0709.IN0400</v>
       </c>
-      <c r="Q26" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R26" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.SPARE_IN0400.Init('CHASSIS','SPARE_IN0400','IN0400','a46',NVL_IO_CHASSIS.All_Inputs.IN0400,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R26" s="20" t="str">
+      <c r="S26" s="20" t="str">
         <f t="shared" si="3"/>
         <v>: Mimic_Input_FB; // CHASSIS:IN0400</v>
       </c>
-      <c r="S26" s="20" t="str">
+      <c r="T26" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0400();</v>
       </c>
-      <c r="T26" s="20" t="str">
+      <c r="U26" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0400.Init(Machine_IO.Inputs.SPARE_IN0400);</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>93</v>
       </c>
@@ -4193,27 +4295,31 @@
         <v>Machine_IO.Inputs.FUELLEVEL_PERCENT</v>
       </c>
       <c r="P27" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.FUELLEVEL_PERCENT.Dig</v>
+      </c>
+      <c r="Q27" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.FUELLEVEL_PERCENT(); // CR0709.IN0401</v>
       </c>
-      <c r="Q27" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R27" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.FUELLEVEL_PERCENT.Init('CHASSIS','FUELLEVEL_PERCENT','IN0401','a47',NVL_IO_CHASSIS.All_Inputs.IN0401,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R27" s="20" t="str">
+      <c r="S27" s="20" t="str">
         <f t="shared" si="3"/>
         <v>FuelLevel_Percent: Mimic_Input_FB; // CHASSIS:IN0401</v>
       </c>
-      <c r="S27" s="20" t="str">
+      <c r="T27" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0401();</v>
       </c>
-      <c r="T27" s="20" t="str">
+      <c r="U27" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0401.Init(Machine_IO.Inputs.FUELLEVEL_PERCENT);</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>93</v>
       </c>
@@ -4263,27 +4369,31 @@
         <v>Machine_IO.Inputs.UMBTRACKREQ</v>
       </c>
       <c r="P28" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.UMBTRACKREQ.Dig</v>
+      </c>
+      <c r="Q28" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.UMBTRACKREQ(); // CR0709.IN0900</v>
       </c>
-      <c r="Q28" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R28" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.UMBTRACKREQ.Init('CHASSIS','UMBTRACKREQ','IN0900','a38',NVL_IO_CHASSIS.All_Inputs.IN0900,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R28" s="20" t="str">
+      <c r="S28" s="20" t="str">
         <f t="shared" si="3"/>
         <v>UmbTrackReq: Mimic_Input_FB; // CHASSIS:IN0900</v>
       </c>
-      <c r="S28" s="20" t="str">
+      <c r="T28" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0900();</v>
       </c>
-      <c r="T28" s="20" t="str">
+      <c r="U28" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0900.Init(Machine_IO.Inputs.UMBTRACKREQ);</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>93</v>
       </c>
@@ -4333,27 +4443,31 @@
         <v>Machine_IO.Inputs.UMBMACHINESTOP</v>
       </c>
       <c r="P29" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.UMBMACHINESTOP.Dig</v>
+      </c>
+      <c r="Q29" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.UMBMACHINESTOP(); // CR0709.IN0901</v>
       </c>
-      <c r="Q29" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R29" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.UMBMACHINESTOP.Init('CHASSIS','UMBMACHINESTOP','IN0901','a39',NVL_IO_CHASSIS.All_Inputs.IN0901,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R29" s="20" t="str">
+      <c r="S29" s="20" t="str">
         <f t="shared" si="3"/>
         <v>UmbMachineStop: Mimic_Input_FB; // CHASSIS:IN0901</v>
       </c>
-      <c r="S29" s="20" t="str">
+      <c r="T29" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0901();</v>
       </c>
-      <c r="T29" s="20" t="str">
+      <c r="U29" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0901.Init(Machine_IO.Inputs.UMBMACHINESTOP);</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>93</v>
       </c>
@@ -4403,27 +4517,31 @@
         <v>Machine_IO.Inputs.RTF_REQ</v>
       </c>
       <c r="P30" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RTF_REQ.Dig</v>
+      </c>
+      <c r="Q30" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.RTF_REQ(); // CR0709.IN0300</v>
       </c>
-      <c r="Q30" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R30" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.RTF_REQ.Init('CHASSIS','RTF_REQ','IN0300','a44',NVL_IO_CHASSIS.All_Inputs.IN0300,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R30" s="20" t="str">
+      <c r="S30" s="20" t="str">
         <f t="shared" si="3"/>
         <v>RTF_Req: Mimic_Input_FB; // CHASSIS:IN0300</v>
       </c>
-      <c r="S30" s="20" t="str">
+      <c r="T30" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0300();</v>
       </c>
-      <c r="T30" s="20" t="str">
+      <c r="U30" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0300.Init(Machine_IO.Inputs.RTF_REQ);</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>93</v>
       </c>
@@ -4473,27 +4591,31 @@
         <v>Machine_IO.Inputs.RTR_REQ</v>
       </c>
       <c r="P31" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.RTR_REQ.Dig</v>
+      </c>
+      <c r="Q31" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.RTR_REQ(); // CR0709.IN0301</v>
       </c>
-      <c r="Q31" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R31" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.RTR_REQ.Init('CHASSIS','RTR_REQ','IN0301','a45',NVL_IO_CHASSIS.All_Inputs.IN0301,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R31" s="20" t="str">
+      <c r="S31" s="20" t="str">
         <f t="shared" si="3"/>
         <v>RTR_Req: Mimic_Input_FB; // CHASSIS:IN0301</v>
       </c>
-      <c r="S31" s="20" t="str">
+      <c r="T31" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0301();</v>
       </c>
-      <c r="T31" s="20" t="str">
+      <c r="U31" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0301.Init(Machine_IO.Inputs.RTR_REQ);</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>93</v>
       </c>
@@ -4543,27 +4665,31 @@
         <v>Machine_IO.Inputs.LTF_REQ</v>
       </c>
       <c r="P32" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.LTF_REQ.Dig</v>
+      </c>
+      <c r="Q32" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.LTF_REQ(); // CR0709.IN0800</v>
       </c>
-      <c r="Q32" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R32" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.LTF_REQ.Init('CHASSIS','LTF_REQ','IN0800','a36',NVL_IO_CHASSIS.All_Inputs.IN0800,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R32" s="20" t="str">
+      <c r="S32" s="20" t="str">
         <f t="shared" si="3"/>
         <v>LTF_Req: Mimic_Input_FB; // CHASSIS:IN0800</v>
       </c>
-      <c r="S32" s="20" t="str">
+      <c r="T32" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0800();</v>
       </c>
-      <c r="T32" s="20" t="str">
+      <c r="U32" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0800.Init(Machine_IO.Inputs.LTF_REQ);</v>
       </c>
     </row>
-    <row r="33" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>93</v>
       </c>
@@ -4613,27 +4739,31 @@
         <v>Machine_IO.Inputs.LTR_REQ</v>
       </c>
       <c r="P33" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Inputs.LTR_REQ.Dig</v>
+      </c>
+      <c r="Q33" s="20" t="str">
         <f t="shared" si="2"/>
         <v>Machine_IO.Inputs.LTR_REQ(); // CR0709.IN0801</v>
       </c>
-      <c r="Q33" s="20" t="str">
-        <f t="shared" si="10"/>
+      <c r="R33" s="20" t="str">
+        <f t="shared" si="11"/>
         <v>Machine_IO.Inputs.LTR_REQ.Init('CHASSIS','LTR_REQ','IN0801','a37',NVL_IO_CHASSIS.All_Inputs.IN0801,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R33" s="20" t="str">
+      <c r="S33" s="20" t="str">
         <f t="shared" si="3"/>
         <v>LTR_Req: Mimic_Input_FB; // CHASSIS:IN0801</v>
       </c>
-      <c r="S33" s="20" t="str">
+      <c r="T33" s="20" t="str">
         <f t="shared" si="4"/>
         <v>CHASSIS.IN0801();</v>
       </c>
-      <c r="T33" s="20" t="str">
+      <c r="U33" s="20" t="str">
         <f t="shared" si="5"/>
         <v>CHASSIS.IN0801.Init(Machine_IO.Inputs.LTR_REQ);</v>
       </c>
     </row>
-    <row r="34" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>93</v>
       </c>
@@ -4676,7 +4806,7 @@
         <v>TAILCONVSPD_MA</v>
       </c>
       <c r="M34" s="19" t="str">
-        <f t="shared" ref="M34:M65" si="11">_xlfn.CONCAT(K34,":BOOL;")</f>
+        <f t="shared" ref="M34:M65" si="12">_xlfn.CONCAT(K34,":BOOL;")</f>
         <v>TailConvSpd_mA:BOOL;</v>
       </c>
       <c r="N34" s="20" t="str">
@@ -4688,27 +4818,31 @@
         <v>Machine_IO.Outputs.TAILCONVSPD_MA</v>
       </c>
       <c r="P34" s="20" t="str">
-        <f t="shared" ref="P34:P65" si="12">_xlfn.CONCAT(O34,"(); // ",E34)</f>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.TAILCONVSPD_MA.Dig</v>
+      </c>
+      <c r="Q34" s="20" t="str">
+        <f t="shared" ref="Q34:Q65" si="13">_xlfn.CONCAT(O34,"(); // ",E34)</f>
         <v>Machine_IO.Outputs.TAILCONVSPD_MA(); // CR0709.OUT0000</v>
       </c>
-      <c r="Q34" s="20" t="str">
+      <c r="R34" s="20" t="str">
         <f>_xlfn.CONCAT(O34,".Init('",A34,"','",L34,"','",D34,"','",G34,"',NVL_Outputs_States_",A34,".All.",D34,",NVL_IO_",A2,".All_Outputs_Diag.",D34,",Machine_IO.Node_",A34,");")</f>
         <v>Machine_IO.Outputs.TAILCONVSPD_MA.Init('CHASSIS','TAILCONVSPD_MA','OUT0000','a16',NVL_Outputs_States_CHASSIS.All.OUT0000,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0000,Machine_IO.Node_CHASSIS);</v>
       </c>
-      <c r="R34" s="20" t="str">
-        <f t="shared" ref="R34:R65" si="13">_xlfn.CONCAT(K34,": Mimic_Output_FB; // ",A34,":",D34)</f>
+      <c r="S34" s="20" t="str">
+        <f t="shared" ref="S34:S65" si="14">_xlfn.CONCAT(K34,": Mimic_Output_FB; // ",A34,":",D34)</f>
         <v>TailConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0000</v>
       </c>
-      <c r="S34" s="20" t="str">
-        <f t="shared" ref="S34:S65" si="14">_xlfn.CONCAT(A34,".",D34,"();")</f>
+      <c r="T34" s="20" t="str">
+        <f t="shared" ref="T34:T65" si="15">_xlfn.CONCAT(A34,".",D34,"();")</f>
         <v>CHASSIS.OUT0000();</v>
       </c>
-      <c r="T34" s="20" t="str">
-        <f t="shared" ref="T34:T65" si="15">_xlfn.CONCAT(A34,".",D34,".Init(",O34,");")</f>
+      <c r="U34" s="20" t="str">
+        <f t="shared" ref="U34:U65" si="16">_xlfn.CONCAT(A34,".",D34,".Init(",O34,");")</f>
         <v>CHASSIS.OUT0000.Init(Machine_IO.Outputs.TAILCONVSPD_MA);</v>
       </c>
     </row>
-    <row r="35" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>93</v>
       </c>
@@ -4751,39 +4885,43 @@
         <v>RHS_JACKLEGLOWER_OP</v>
       </c>
       <c r="M35" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>RHS_JackLegLower_OP:BOOL;</v>
       </c>
       <c r="N35" s="20" t="str">
-        <f t="shared" ref="N35:N65" si="16">_xlfn.CONCAT(L35,":OpCom; // ",A35,".",D35)</f>
+        <f t="shared" ref="N35:N65" si="17">_xlfn.CONCAT(L35,":OpCom; // ",A35,".",D35)</f>
         <v>RHS_JACKLEGLOWER_OP:OpCom; // CHASSIS.OUT0001</v>
       </c>
       <c r="O35" s="20" t="str">
-        <f t="shared" ref="O35:O65" si="17">_xlfn.CONCAT("Machine_IO.","Outputs.",L35,"")</f>
+        <f t="shared" ref="O35:O65" si="18">_xlfn.CONCAT("Machine_IO.","Outputs.",L35,"")</f>
         <v>Machine_IO.Outputs.RHS_JACKLEGLOWER_OP</v>
       </c>
       <c r="P35" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.RHS_JACKLEGLOWER_OP.Dig</v>
+      </c>
+      <c r="Q35" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.RHS_JACKLEGLOWER_OP(); // CR0709.OUT0001</v>
       </c>
-      <c r="Q35" s="20" t="str">
-        <f t="shared" ref="Q35:Q65" si="18">_xlfn.CONCAT(O35,".Init('",A35,"','",L35,"','",D35,"','",G35,"',NVL_Outputs_States_",A35,".All.",D35,",NVL_IO_",A3,".All_Outputs_Diag.",D35,",Machine_IO.Node_",A35,");")</f>
+      <c r="R35" s="20" t="str">
+        <f t="shared" ref="R35:R65" si="19">_xlfn.CONCAT(O35,".Init('",A35,"','",L35,"','",D35,"','",G35,"',NVL_Outputs_States_",A35,".All.",D35,",NVL_IO_",A3,".All_Outputs_Diag.",D35,",Machine_IO.Node_",A35,");")</f>
         <v>Machine_IO.Outputs.RHS_JACKLEGLOWER_OP.Init('CHASSIS','RHS_JACKLEGLOWER_OP','OUT0001','a17',NVL_Outputs_States_CHASSIS.All.OUT0001,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0001,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R35" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>RHS_JackLegLower_OP: Mimic_Output_FB; // CHASSIS:OUT0001</v>
       </c>
       <c r="S35" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0001();</v>
+        <v>RHS_JackLegLower_OP: Mimic_Output_FB; // CHASSIS:OUT0001</v>
       </c>
       <c r="T35" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0001();</v>
+      </c>
+      <c r="U35" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0001.Init(Machine_IO.Outputs.RHS_JACKLEGLOWER_OP);</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>93</v>
       </c>
@@ -4826,39 +4964,43 @@
         <v>SIDECONVSPD_MA</v>
       </c>
       <c r="M36" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SideConvSpd_mA:BOOL;</v>
       </c>
       <c r="N36" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>SIDECONVSPD_MA:OpCom; // CHASSIS.OUT0002</v>
       </c>
       <c r="O36" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDECONVSPD_MA</v>
       </c>
       <c r="P36" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.SIDECONVSPD_MA.Dig</v>
+      </c>
+      <c r="Q36" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SIDECONVSPD_MA(); // CR0709.OUT0002</v>
       </c>
-      <c r="Q36" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R36" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.SIDECONVSPD_MA.Init('CHASSIS','SIDECONVSPD_MA','OUT0002','a18',NVL_Outputs_States_CHASSIS.All.OUT0002,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0002,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R36" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>SideConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0002</v>
       </c>
       <c r="S36" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0002();</v>
+        <v>SideConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0002</v>
       </c>
       <c r="T36" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0002();</v>
+      </c>
+      <c r="U36" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0002.Init(Machine_IO.Outputs.SIDECONVSPD_MA);</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>93</v>
       </c>
@@ -4901,39 +5043,43 @@
         <v>LHS_JACKLEGRAISE_OP</v>
       </c>
       <c r="M37" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>LHS_JackLegRaise_OP:BOOL;</v>
       </c>
       <c r="N37" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>LHS_JACKLEGRAISE_OP:OpCom; // CHASSIS.OUT0003</v>
       </c>
       <c r="O37" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGRAISE_OP</v>
       </c>
       <c r="P37" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.LHS_JACKLEGRAISE_OP.Dig</v>
+      </c>
+      <c r="Q37" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGRAISE_OP(); // CR0709.OUT0003</v>
       </c>
-      <c r="Q37" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R37" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGRAISE_OP.Init('CHASSIS','LHS_JACKLEGRAISE_OP','OUT0003','a19',NVL_Outputs_States_CHASSIS.All.OUT0003,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0003,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R37" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>LHS_JackLegRaise_OP: Mimic_Output_FB; // CHASSIS:OUT0003</v>
       </c>
       <c r="S37" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0003();</v>
+        <v>LHS_JackLegRaise_OP: Mimic_Output_FB; // CHASSIS:OUT0003</v>
       </c>
       <c r="T37" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0003();</v>
+      </c>
+      <c r="U37" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0003.Init(Machine_IO.Outputs.LHS_JACKLEGRAISE_OP);</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>93</v>
       </c>
@@ -4976,39 +5122,43 @@
         <v>SIDETRANSFERSPD_MA</v>
       </c>
       <c r="M38" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SideTransferSpd_mA:BOOL;</v>
       </c>
       <c r="N38" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>SIDETRANSFERSPD_MA:OpCom; // CHASSIS.OUT0004</v>
       </c>
       <c r="O38" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDETRANSFERSPD_MA</v>
       </c>
       <c r="P38" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.SIDETRANSFERSPD_MA.Dig</v>
+      </c>
+      <c r="Q38" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SIDETRANSFERSPD_MA(); // CR0709.OUT0004</v>
       </c>
-      <c r="Q38" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R38" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.SIDETRANSFERSPD_MA.Init('CHASSIS','SIDETRANSFERSPD_MA','OUT0004','a20',NVL_Outputs_States_CHASSIS.All.OUT0004,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0004,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R38" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>SideTransferSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0004</v>
       </c>
       <c r="S38" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0004();</v>
+        <v>SideTransferSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0004</v>
       </c>
       <c r="T38" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0004();</v>
+      </c>
+      <c r="U38" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0004.Init(Machine_IO.Outputs.SIDETRANSFERSPD_MA);</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>93</v>
       </c>
@@ -5051,39 +5201,43 @@
         <v>LHS_JACKLEGLOWER_OP</v>
       </c>
       <c r="M39" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>LHS_JackLegLower_OP:BOOL;</v>
       </c>
       <c r="N39" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>LHS_JACKLEGLOWER_OP:OpCom; // CHASSIS.OUT0005</v>
       </c>
       <c r="O39" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGLOWER_OP</v>
       </c>
       <c r="P39" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.LHS_JACKLEGLOWER_OP.Dig</v>
+      </c>
+      <c r="Q39" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGLOWER_OP(); // CR0709.OUT0005</v>
       </c>
-      <c r="Q39" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R39" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.LHS_JACKLEGLOWER_OP.Init('CHASSIS','LHS_JACKLEGLOWER_OP','OUT0005','a21',NVL_Outputs_States_CHASSIS.All.OUT0005,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0005,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R39" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>LHS_JackLegLower_OP: Mimic_Output_FB; // CHASSIS:OUT0005</v>
       </c>
       <c r="S39" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0005();</v>
+        <v>LHS_JackLegLower_OP: Mimic_Output_FB; // CHASSIS:OUT0005</v>
       </c>
       <c r="T39" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0005();</v>
+      </c>
+      <c r="U39" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0005.Init(Machine_IO.Outputs.LHS_JACKLEGLOWER_OP);</v>
       </c>
     </row>
-    <row r="40" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>93</v>
       </c>
@@ -5126,39 +5280,43 @@
         <v>SETUPDUMPVALVE_OP</v>
       </c>
       <c r="M40" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SetupDumpValve_OP:BOOL;</v>
       </c>
       <c r="N40" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>SETUPDUMPVALVE_OP:OpCom; // CHASSIS.OUT0006</v>
       </c>
       <c r="O40" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SETUPDUMPVALVE_OP</v>
       </c>
       <c r="P40" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.SETUPDUMPVALVE_OP.Dig</v>
+      </c>
+      <c r="Q40" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SETUPDUMPVALVE_OP(); // CR0709.OUT0006</v>
       </c>
-      <c r="Q40" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R40" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.SETUPDUMPVALVE_OP.Init('CHASSIS','SETUPDUMPVALVE_OP','OUT0006','a22',NVL_Outputs_States_CHASSIS.All.OUT0006,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0006,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R40" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>SetupDumpValve_OP: Mimic_Output_FB; // CHASSIS:OUT0006</v>
       </c>
       <c r="S40" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0006();</v>
+        <v>SetupDumpValve_OP: Mimic_Output_FB; // CHASSIS:OUT0006</v>
       </c>
       <c r="T40" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0006();</v>
+      </c>
+      <c r="U40" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0006.Init(Machine_IO.Outputs.SETUPDUMPVALVE_OP);</v>
       </c>
     </row>
-    <row r="41" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
         <v>93</v>
       </c>
@@ -5201,39 +5359,43 @@
         <v>COLLECTIONCONVSPD_MA</v>
       </c>
       <c r="M41" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>CollectionConvSpd_mA:BOOL;</v>
       </c>
       <c r="N41" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>COLLECTIONCONVSPD_MA:OpCom; // CHASSIS.OUT0007</v>
       </c>
       <c r="O41" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVSPD_MA</v>
       </c>
       <c r="P41" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.COLLECTIONCONVSPD_MA.Dig</v>
+      </c>
+      <c r="Q41" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVSPD_MA(); // CR0709.OUT0007</v>
       </c>
-      <c r="Q41" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R41" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVSPD_MA.Init('CHASSIS','COLLECTIONCONVSPD_MA','OUT0007','a23',NVL_Outputs_States_CHASSIS.All.OUT0007,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0007,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R41" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>CollectionConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0007</v>
       </c>
       <c r="S41" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0007();</v>
+        <v>CollectionConvSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0007</v>
       </c>
       <c r="T41" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0007();</v>
+      </c>
+      <c r="U41" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0007.Init(Machine_IO.Outputs.COLLECTIONCONVSPD_MA);</v>
       </c>
     </row>
-    <row r="42" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
         <v>93</v>
       </c>
@@ -5276,39 +5438,43 @@
         <v>COLLECTIONCONVON_OP</v>
       </c>
       <c r="M42" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>CollectionConvOn_OP:BOOL;</v>
       </c>
       <c r="N42" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>COLLECTIONCONVON_OP:OpCom; // CHASSIS.OUT0008</v>
       </c>
       <c r="O42" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVON_OP</v>
       </c>
       <c r="P42" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.COLLECTIONCONVON_OP.Dig</v>
+      </c>
+      <c r="Q42" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVON_OP(); // CR0709.OUT0008</v>
       </c>
-      <c r="Q42" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R42" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.COLLECTIONCONVON_OP.Init('CHASSIS','COLLECTIONCONVON_OP','OUT0008','a24',NVL_Outputs_States_CHASSIS.All.OUT0008,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0008,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R42" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>CollectionConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0008</v>
       </c>
       <c r="S42" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0008();</v>
+        <v>CollectionConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0008</v>
       </c>
       <c r="T42" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0008();</v>
+      </c>
+      <c r="U42" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0008.Init(Machine_IO.Outputs.COLLECTIONCONVON_OP);</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>93</v>
       </c>
@@ -5351,39 +5517,43 @@
         <v>SUPPLY_GROUP0</v>
       </c>
       <c r="M43" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SUPPLY_GROUP0:BOOL;</v>
       </c>
       <c r="N43" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>SUPPLY_GROUP0:OpCom; // CHASSIS.GROUP0</v>
       </c>
       <c r="O43" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SUPPLY_GROUP0</v>
       </c>
       <c r="P43" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP0.Dig</v>
+      </c>
+      <c r="Q43" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SUPPLY_GROUP0(); // CR0709.GROUP0</v>
       </c>
-      <c r="Q43" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R43" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.SUPPLY_GROUP0.Init('CHASSIS','SUPPLY_GROUP0','GROUP0','a4',NVL_Outputs_States_CHASSIS.All.GROUP0,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP0,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R43" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>SUPPLY_GROUP0: Mimic_Output_FB; // CHASSIS:GROUP0</v>
       </c>
       <c r="S43" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.GROUP0();</v>
+        <v>SUPPLY_GROUP0: Mimic_Output_FB; // CHASSIS:GROUP0</v>
       </c>
       <c r="T43" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.GROUP0();</v>
+      </c>
+      <c r="U43" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.GROUP0.Init(Machine_IO.Outputs.SUPPLY_GROUP0);</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>93</v>
       </c>
@@ -5426,39 +5596,43 @@
         <v>DRUMSPD_MA_RAMP_LIMIT</v>
       </c>
       <c r="M44" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>DrumSpd_mA_RAMP_LIMIT:BOOL;</v>
       </c>
       <c r="N44" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>DRUMSPD_MA_RAMP_LIMIT:OpCom; // CHASSIS.OUT0100</v>
       </c>
       <c r="O44" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT</v>
       </c>
       <c r="P44" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT.Dig</v>
+      </c>
+      <c r="Q44" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT(); // CR0709.OUT0100</v>
       </c>
-      <c r="Q44" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R44" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT.Init('CHASSIS','DRUMSPD_MA_RAMP_LIMIT','OUT0100','a6',NVL_Outputs_States_CHASSIS.All.OUT0100,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0100,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R44" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>DrumSpd_mA_RAMP_LIMIT: Mimic_Output_FB; // CHASSIS:OUT0100</v>
       </c>
       <c r="S44" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0100();</v>
+        <v>DrumSpd_mA_RAMP_LIMIT: Mimic_Output_FB; // CHASSIS:OUT0100</v>
       </c>
       <c r="T44" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0100();</v>
+      </c>
+      <c r="U44" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0100.Init(Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT);</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
         <v>93</v>
       </c>
@@ -5501,39 +5675,43 @@
         <v>TRACKINGMODE</v>
       </c>
       <c r="M45" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>TrackingMode:BOOL;</v>
       </c>
       <c r="N45" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>TRACKINGMODE:OpCom; // CHASSIS.OUT0101</v>
       </c>
       <c r="O45" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.TRACKINGMODE</v>
       </c>
       <c r="P45" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.TRACKINGMODE.Dig</v>
+      </c>
+      <c r="Q45" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.TRACKINGMODE(); // CR0709.OUT0101</v>
       </c>
-      <c r="Q45" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R45" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.TRACKINGMODE.Init('CHASSIS','TRACKINGMODE','OUT0101','a7',NVL_Outputs_States_CHASSIS.All.OUT0101,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0101,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R45" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>TrackingMode: Mimic_Output_FB; // CHASSIS:OUT0101</v>
       </c>
       <c r="S45" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0101();</v>
+        <v>TrackingMode: Mimic_Output_FB; // CHASSIS:OUT0101</v>
       </c>
       <c r="T45" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0101();</v>
+      </c>
+      <c r="U45" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0101.Init(Machine_IO.Outputs.TRACKINGMODE);</v>
       </c>
     </row>
-    <row r="46" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>93</v>
       </c>
@@ -5576,39 +5754,43 @@
         <v>FEEDERSPD_MA</v>
       </c>
       <c r="M46" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>FeederSpd_mA:BOOL;</v>
       </c>
       <c r="N46" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>FEEDERSPD_MA:OpCom; // CHASSIS.OUT0102</v>
       </c>
       <c r="O46" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.FEEDERSPD_MA</v>
       </c>
       <c r="P46" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.FEEDERSPD_MA.Dig</v>
+      </c>
+      <c r="Q46" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.FEEDERSPD_MA(); // CR0709.OUT0102</v>
       </c>
-      <c r="Q46" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R46" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.FEEDERSPD_MA.Init('CHASSIS','FEEDERSPD_MA','OUT0102','a8',NVL_Outputs_States_CHASSIS.All.OUT0102,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0102,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R46" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>FeederSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0102</v>
       </c>
       <c r="S46" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0102();</v>
+        <v>FeederSpd_mA: Mimic_Output_FB; // CHASSIS:OUT0102</v>
       </c>
       <c r="T46" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0102();</v>
+      </c>
+      <c r="U46" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0102.Init(Machine_IO.Outputs.FEEDERSPD_MA);</v>
       </c>
     </row>
-    <row r="47" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>93</v>
       </c>
@@ -5651,39 +5833,43 @@
         <v>CRANKENABLE</v>
       </c>
       <c r="M47" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>CrankEnable:BOOL;</v>
       </c>
       <c r="N47" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>CRANKENABLE:OpCom; // CHASSIS.OUT0103</v>
       </c>
       <c r="O47" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.CRANKENABLE</v>
       </c>
       <c r="P47" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.CRANKENABLE.Dig</v>
+      </c>
+      <c r="Q47" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.CRANKENABLE(); // CR0709.OUT0103</v>
       </c>
-      <c r="Q47" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R47" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.CRANKENABLE.Init('CHASSIS','CRANKENABLE','OUT0103','a9',NVL_Outputs_States_CHASSIS.All.OUT0103,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0103,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R47" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>CrankEnable: Mimic_Output_FB; // CHASSIS:OUT0103</v>
       </c>
       <c r="S47" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0103();</v>
+        <v>CrankEnable: Mimic_Output_FB; // CHASSIS:OUT0103</v>
       </c>
       <c r="T47" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0103();</v>
+      </c>
+      <c r="U47" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0103.Init(Machine_IO.Outputs.CRANKENABLE);</v>
       </c>
     </row>
-    <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>93</v>
       </c>
@@ -5726,39 +5912,43 @@
         <v>DIVERTOILTOTRACK_OP</v>
       </c>
       <c r="M48" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>DivertOilToTrack_OP:BOOL;</v>
       </c>
       <c r="N48" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>DIVERTOILTOTRACK_OP:OpCom; // CHASSIS.OUT0104</v>
       </c>
       <c r="O48" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.DIVERTOILTOTRACK_OP</v>
       </c>
       <c r="P48" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.DIVERTOILTOTRACK_OP.Dig</v>
+      </c>
+      <c r="Q48" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.DIVERTOILTOTRACK_OP(); // CR0709.OUT0104</v>
       </c>
-      <c r="Q48" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R48" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.DIVERTOILTOTRACK_OP.Init('CHASSIS','DIVERTOILTOTRACK_OP','OUT0104','a10',NVL_Outputs_States_CHASSIS.All.OUT0104,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0104,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R48" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>DivertOilToTrack_OP: Mimic_Output_FB; // CHASSIS:OUT0104</v>
       </c>
       <c r="S48" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0104();</v>
+        <v>DivertOilToTrack_OP: Mimic_Output_FB; // CHASSIS:OUT0104</v>
       </c>
       <c r="T48" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0104();</v>
+      </c>
+      <c r="U48" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0104.Init(Machine_IO.Outputs.DIVERTOILTOTRACK_OP);</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
         <v>93</v>
       </c>
@@ -5801,39 +5991,43 @@
         <v>RHS_JACKLEGRAISE_OP</v>
       </c>
       <c r="M49" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>RHS_JackLegRaise_OP:BOOL;</v>
       </c>
       <c r="N49" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>RHS_JACKLEGRAISE_OP:OpCom; // CHASSIS.OUT0105</v>
       </c>
       <c r="O49" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RHS_JACKLEGRAISE_OP</v>
       </c>
       <c r="P49" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.RHS_JACKLEGRAISE_OP.Dig</v>
+      </c>
+      <c r="Q49" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.RHS_JACKLEGRAISE_OP(); // CR0709.OUT0105</v>
       </c>
-      <c r="Q49" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R49" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.RHS_JACKLEGRAISE_OP.Init('CHASSIS','RHS_JACKLEGRAISE_OP','OUT0105','a11',NVL_Outputs_States_CHASSIS.All.OUT0105,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0105,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R49" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>RHS_JackLegRaise_OP: Mimic_Output_FB; // CHASSIS:OUT0105</v>
       </c>
       <c r="S49" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0105();</v>
+        <v>RHS_JackLegRaise_OP: Mimic_Output_FB; // CHASSIS:OUT0105</v>
       </c>
       <c r="T49" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0105();</v>
+      </c>
+      <c r="U49" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0105.Init(Machine_IO.Outputs.RHS_JACKLEGRAISE_OP);</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
         <v>93</v>
       </c>
@@ -5876,39 +6070,43 @@
         <v>TAILCONVON_OP</v>
       </c>
       <c r="M50" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>TailConvOn_OP:BOOL;</v>
       </c>
       <c r="N50" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>TAILCONVON_OP:OpCom; // CHASSIS.OUT0106</v>
       </c>
       <c r="O50" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.TAILCONVON_OP</v>
       </c>
       <c r="P50" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.TAILCONVON_OP.Dig</v>
+      </c>
+      <c r="Q50" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.TAILCONVON_OP(); // CR0709.OUT0106</v>
       </c>
-      <c r="Q50" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R50" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.TAILCONVON_OP.Init('CHASSIS','TAILCONVON_OP','OUT0106','a12',NVL_Outputs_States_CHASSIS.All.OUT0106,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0106,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R50" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>TailConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0106</v>
       </c>
       <c r="S50" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0106();</v>
+        <v>TailConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0106</v>
       </c>
       <c r="T50" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0106();</v>
+      </c>
+      <c r="U50" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0106.Init(Machine_IO.Outputs.TAILCONVON_OP);</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>93</v>
       </c>
@@ -5951,39 +6149,43 @@
         <v>SIDECONVON_OP</v>
       </c>
       <c r="M51" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SideConvOn_OP:BOOL;</v>
       </c>
       <c r="N51" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>SIDECONVON_OP:OpCom; // CHASSIS.OUT0107</v>
       </c>
       <c r="O51" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDECONVON_OP</v>
       </c>
       <c r="P51" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.SIDECONVON_OP.Dig</v>
+      </c>
+      <c r="Q51" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SIDECONVON_OP(); // CR0709.OUT0107</v>
       </c>
-      <c r="Q51" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R51" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.SIDECONVON_OP.Init('CHASSIS','SIDECONVON_OP','OUT0107','a13',NVL_Outputs_States_CHASSIS.All.OUT0107,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0107,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R51" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>SideConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0107</v>
       </c>
       <c r="S51" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0107();</v>
+        <v>SideConvOn_OP: Mimic_Output_FB; // CHASSIS:OUT0107</v>
       </c>
       <c r="T51" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0107();</v>
+      </c>
+      <c r="U51" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0107.Init(Machine_IO.Outputs.SIDECONVON_OP);</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
         <v>93</v>
       </c>
@@ -6026,39 +6228,43 @@
         <v>SIDETRANSFERON_OP</v>
       </c>
       <c r="M52" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SideTransferOn_OP:BOOL;</v>
       </c>
       <c r="N52" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>SIDETRANSFERON_OP:OpCom; // CHASSIS.OUT0108</v>
       </c>
       <c r="O52" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SIDETRANSFERON_OP</v>
       </c>
       <c r="P52" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.SIDETRANSFERON_OP.Dig</v>
+      </c>
+      <c r="Q52" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SIDETRANSFERON_OP(); // CR0709.OUT0108</v>
       </c>
-      <c r="Q52" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R52" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.SIDETRANSFERON_OP.Init('CHASSIS','SIDETRANSFERON_OP','OUT0108','a14',NVL_Outputs_States_CHASSIS.All.OUT0108,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0108,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R52" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>SideTransferOn_OP: Mimic_Output_FB; // CHASSIS:OUT0108</v>
       </c>
       <c r="S52" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0108();</v>
+        <v>SideTransferOn_OP: Mimic_Output_FB; // CHASSIS:OUT0108</v>
       </c>
       <c r="T52" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0108();</v>
+      </c>
+      <c r="U52" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0108.Init(Machine_IO.Outputs.SIDETRANSFERON_OP);</v>
       </c>
     </row>
-    <row r="53" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>93</v>
       </c>
@@ -6101,39 +6307,43 @@
         <v>SUPPLY_GROUP1</v>
       </c>
       <c r="M53" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SUPPLY_GROUP1:BOOL;</v>
       </c>
       <c r="N53" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>SUPPLY_GROUP1:OpCom; // CHASSIS.GROUP1</v>
       </c>
       <c r="O53" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SUPPLY_GROUP1</v>
       </c>
       <c r="P53" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP1.Dig</v>
+      </c>
+      <c r="Q53" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SUPPLY_GROUP1(); // CR0709.GROUP1</v>
       </c>
-      <c r="Q53" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R53" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.SUPPLY_GROUP1.Init('CHASSIS','SUPPLY_GROUP1','GROUP1','a3',NVL_Outputs_States_CHASSIS.All.GROUP1,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP1,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R53" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>SUPPLY_GROUP1: Mimic_Output_FB; // CHASSIS:GROUP1</v>
       </c>
       <c r="S53" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.GROUP1();</v>
+        <v>SUPPLY_GROUP1: Mimic_Output_FB; // CHASSIS:GROUP1</v>
       </c>
       <c r="T53" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.GROUP1();</v>
+      </c>
+      <c r="U53" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.GROUP1.Init(Machine_IO.Outputs.SUPPLY_GROUP1);</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
         <v>93</v>
       </c>
@@ -6176,39 +6386,43 @@
         <v>LEFTTRACKDIVERT_OP</v>
       </c>
       <c r="M54" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>LeftTrackDivert_OP:BOOL;</v>
       </c>
       <c r="N54" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>LEFTTRACKDIVERT_OP:OpCom; // CHASSIS.OUT0200</v>
       </c>
       <c r="O54" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LEFTTRACKDIVERT_OP</v>
       </c>
       <c r="P54" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.LEFTTRACKDIVERT_OP.Dig</v>
+      </c>
+      <c r="Q54" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.LEFTTRACKDIVERT_OP(); // CR0709.OUT0200</v>
       </c>
-      <c r="Q54" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R54" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.LEFTTRACKDIVERT_OP.Init('CHASSIS','LEFTTRACKDIVERT_OP','OUT0200','a73',NVL_Outputs_States_CHASSIS.All.OUT0200,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0200,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R54" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>LeftTrackDivert_OP: Mimic_Output_FB; // CHASSIS:OUT0200</v>
       </c>
       <c r="S54" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0200();</v>
+        <v>LeftTrackDivert_OP: Mimic_Output_FB; // CHASSIS:OUT0200</v>
       </c>
       <c r="T54" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0200();</v>
+      </c>
+      <c r="U54" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0200.Init(Machine_IO.Outputs.LEFTTRACKDIVERT_OP);</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>93</v>
       </c>
@@ -6251,39 +6465,43 @@
         <v>LTF_OP</v>
       </c>
       <c r="M55" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>LTF_OP:BOOL;</v>
       </c>
       <c r="N55" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>LTF_OP:OpCom; // CHASSIS.OUT0201</v>
       </c>
       <c r="O55" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LTF_OP</v>
       </c>
       <c r="P55" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.LTF_OP.Dig</v>
+      </c>
+      <c r="Q55" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.LTF_OP(); // CR0709.OUT0201</v>
       </c>
-      <c r="Q55" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R55" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.LTF_OP.Init('CHASSIS','LTF_OP','OUT0201','a74',NVL_Outputs_States_CHASSIS.All.OUT0201,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0201,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R55" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>LTF_OP: Mimic_Output_FB; // CHASSIS:OUT0201</v>
       </c>
       <c r="S55" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0201();</v>
+        <v>LTF_OP: Mimic_Output_FB; // CHASSIS:OUT0201</v>
       </c>
       <c r="T55" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0201();</v>
+      </c>
+      <c r="U55" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0201.Init(Machine_IO.Outputs.LTF_OP);</v>
       </c>
     </row>
-    <row r="56" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
         <v>93</v>
       </c>
@@ -6326,39 +6544,43 @@
         <v>LTR_OP</v>
       </c>
       <c r="M56" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>LTR_OP:BOOL;</v>
       </c>
       <c r="N56" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>LTR_OP:OpCom; // CHASSIS.OUT0202</v>
       </c>
       <c r="O56" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.LTR_OP</v>
       </c>
       <c r="P56" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.LTR_OP.Dig</v>
+      </c>
+      <c r="Q56" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.LTR_OP(); // CR0709.OUT0202</v>
       </c>
-      <c r="Q56" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R56" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.LTR_OP.Init('CHASSIS','LTR_OP','OUT0202','a75',NVL_Outputs_States_CHASSIS.All.OUT0202,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0202,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R56" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>LTR_OP: Mimic_Output_FB; // CHASSIS:OUT0202</v>
       </c>
       <c r="S56" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0202();</v>
+        <v>LTR_OP: Mimic_Output_FB; // CHASSIS:OUT0202</v>
       </c>
       <c r="T56" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0202();</v>
+      </c>
+      <c r="U56" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0202.Init(Machine_IO.Outputs.LTR_OP);</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
         <v>93</v>
       </c>
@@ -6401,39 +6623,43 @@
         <v>RIGHTTRACKDIVERT_OP</v>
       </c>
       <c r="M57" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>RightTrackDivert_OP:BOOL;</v>
       </c>
       <c r="N57" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>RIGHTTRACKDIVERT_OP:OpCom; // CHASSIS.OUT0203</v>
       </c>
       <c r="O57" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RIGHTTRACKDIVERT_OP</v>
       </c>
       <c r="P57" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.RIGHTTRACKDIVERT_OP.Dig</v>
+      </c>
+      <c r="Q57" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.RIGHTTRACKDIVERT_OP(); // CR0709.OUT0203</v>
       </c>
-      <c r="Q57" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R57" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.RIGHTTRACKDIVERT_OP.Init('CHASSIS','RIGHTTRACKDIVERT_OP','OUT0203','a76',NVL_Outputs_States_CHASSIS.All.OUT0203,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0203,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R57" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>RightTrackDivert_OP: Mimic_Output_FB; // CHASSIS:OUT0203</v>
       </c>
       <c r="S57" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0203();</v>
+        <v>RightTrackDivert_OP: Mimic_Output_FB; // CHASSIS:OUT0203</v>
       </c>
       <c r="T57" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0203();</v>
+      </c>
+      <c r="U57" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0203.Init(Machine_IO.Outputs.RIGHTTRACKDIVERT_OP);</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
         <v>93</v>
       </c>
@@ -6476,39 +6702,43 @@
         <v>RTF_OP</v>
       </c>
       <c r="M58" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>RTF_OP:BOOL;</v>
       </c>
       <c r="N58" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>RTF_OP:OpCom; // CHASSIS.OUT0204</v>
       </c>
       <c r="O58" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RTF_OP</v>
       </c>
       <c r="P58" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.RTF_OP.Dig</v>
+      </c>
+      <c r="Q58" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.RTF_OP(); // CR0709.OUT0204</v>
       </c>
-      <c r="Q58" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R58" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.RTF_OP.Init('CHASSIS','RTF_OP','OUT0204','a77',NVL_Outputs_States_CHASSIS.All.OUT0204,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0204,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R58" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>RTF_OP: Mimic_Output_FB; // CHASSIS:OUT0204</v>
       </c>
       <c r="S58" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0204();</v>
+        <v>RTF_OP: Mimic_Output_FB; // CHASSIS:OUT0204</v>
       </c>
       <c r="T58" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0204();</v>
+      </c>
+      <c r="U58" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0204.Init(Machine_IO.Outputs.RTF_OP);</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
         <v>93</v>
       </c>
@@ -6551,39 +6781,43 @@
         <v>RTR_OP</v>
       </c>
       <c r="M59" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>RTR_OP:BOOL;</v>
       </c>
       <c r="N59" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>RTR_OP:OpCom; // CHASSIS.OUT0205</v>
       </c>
       <c r="O59" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.RTR_OP</v>
       </c>
       <c r="P59" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.RTR_OP.Dig</v>
+      </c>
+      <c r="Q59" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.RTR_OP(); // CR0709.OUT0205</v>
       </c>
-      <c r="Q59" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R59" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.RTR_OP.Init('CHASSIS','RTR_OP','OUT0205','a78',NVL_Outputs_States_CHASSIS.All.OUT0205,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0205,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R59" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>RTR_OP: Mimic_Output_FB; // CHASSIS:OUT0205</v>
       </c>
       <c r="S59" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0205();</v>
+        <v>RTR_OP: Mimic_Output_FB; // CHASSIS:OUT0205</v>
       </c>
       <c r="T59" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0205();</v>
+      </c>
+      <c r="U59" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0205.Init(Machine_IO.Outputs.RTR_OP);</v>
       </c>
     </row>
-    <row r="60" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>93</v>
       </c>
@@ -6626,39 +6860,43 @@
         <v>DRUMONOFF_OP</v>
       </c>
       <c r="M60" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>DrumOnOff_OP:BOOL;</v>
       </c>
       <c r="N60" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>DRUMONOFF_OP:OpCom; // CHASSIS.OUT0206</v>
       </c>
       <c r="O60" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.DRUMONOFF_OP</v>
       </c>
       <c r="P60" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.DRUMONOFF_OP.Dig</v>
+      </c>
+      <c r="Q60" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.DRUMONOFF_OP(); // CR0709.OUT0206</v>
       </c>
-      <c r="Q60" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R60" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.DRUMONOFF_OP.Init('CHASSIS','DRUMONOFF_OP','OUT0206','a79',NVL_Outputs_States_CHASSIS.All.OUT0206,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0206,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R60" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>DrumOnOff_OP: Mimic_Output_FB; // CHASSIS:OUT0206</v>
       </c>
       <c r="S60" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0206();</v>
+        <v>DrumOnOff_OP: Mimic_Output_FB; // CHASSIS:OUT0206</v>
       </c>
       <c r="T60" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0206();</v>
+      </c>
+      <c r="U60" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0206.Init(Machine_IO.Outputs.DRUMONOFF_OP);</v>
       </c>
     </row>
-    <row r="61" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
         <v>93</v>
       </c>
@@ -6701,39 +6939,43 @@
         <v>FEEDERONOFF_OP</v>
       </c>
       <c r="M61" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>FeederOnOff_OP:BOOL;</v>
       </c>
       <c r="N61" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>FEEDERONOFF_OP:OpCom; // CHASSIS.OUT0207</v>
       </c>
       <c r="O61" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.FEEDERONOFF_OP</v>
       </c>
       <c r="P61" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.FEEDERONOFF_OP.Dig</v>
+      </c>
+      <c r="Q61" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.FEEDERONOFF_OP(); // CR0709.OUT0207</v>
       </c>
-      <c r="Q61" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R61" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.FEEDERONOFF_OP.Init('CHASSIS','FEEDERONOFF_OP','OUT0207','a80',NVL_Outputs_States_CHASSIS.All.OUT0207,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0207,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R61" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>FeederOnOff_OP: Mimic_Output_FB; // CHASSIS:OUT0207</v>
       </c>
       <c r="S61" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0207();</v>
+        <v>FeederOnOff_OP: Mimic_Output_FB; // CHASSIS:OUT0207</v>
       </c>
       <c r="T61" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0207();</v>
+      </c>
+      <c r="U61" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0207.Init(Machine_IO.Outputs.FEEDERONOFF_OP);</v>
       </c>
     </row>
-    <row r="62" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
         <v>93</v>
       </c>
@@ -6776,39 +7018,43 @@
         <v>ECUENABLE</v>
       </c>
       <c r="M62" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>ECUenable:BOOL;</v>
       </c>
       <c r="N62" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ECUENABLE:OpCom; // CHASSIS.OUT0208</v>
       </c>
       <c r="O62" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.ECUENABLE</v>
       </c>
       <c r="P62" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.ECUENABLE.Dig</v>
+      </c>
+      <c r="Q62" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.ECUENABLE(); // CR0709.OUT0208</v>
       </c>
-      <c r="Q62" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R62" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.ECUENABLE.Init('CHASSIS','ECUENABLE','OUT0208','a81',NVL_Outputs_States_CHASSIS.All.OUT0208,NVL_IO_CHASSIS.All_Outputs_Diag.OUT0208,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R62" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>ECUenable: Mimic_Output_FB; // CHASSIS:OUT0208</v>
       </c>
       <c r="S62" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT0208();</v>
+        <v>ECUenable: Mimic_Output_FB; // CHASSIS:OUT0208</v>
       </c>
       <c r="T62" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT0208();</v>
+      </c>
+      <c r="U62" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT0208.Init(Machine_IO.Outputs.ECUENABLE);</v>
       </c>
     </row>
-    <row r="63" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
         <v>93</v>
       </c>
@@ -6851,39 +7097,43 @@
         <v>SUPPLY_GROUP2</v>
       </c>
       <c r="M63" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SUPPLY_GROUP2:BOOL;</v>
       </c>
       <c r="N63" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>SUPPLY_GROUP2:OpCom; // CHASSIS.GROUP2</v>
       </c>
       <c r="O63" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SUPPLY_GROUP2</v>
       </c>
       <c r="P63" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.SUPPLY_GROUP2.Dig</v>
+      </c>
+      <c r="Q63" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SUPPLY_GROUP2(); // CR0709.GROUP2</v>
       </c>
-      <c r="Q63" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R63" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.SUPPLY_GROUP2.Init('CHASSIS','SUPPLY_GROUP2','GROUP2','a1',NVL_Outputs_States_CHASSIS.All.GROUP2,NVL_IO_CHASSIS.All_Outputs_Diag.GROUP2,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R63" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>SUPPLY_GROUP2: Mimic_Output_FB; // CHASSIS:GROUP2</v>
       </c>
       <c r="S63" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.GROUP2();</v>
+        <v>SUPPLY_GROUP2: Mimic_Output_FB; // CHASSIS:GROUP2</v>
       </c>
       <c r="T63" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.GROUP2();</v>
+      </c>
+      <c r="U63" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.GROUP2.Init(Machine_IO.Outputs.SUPPLY_GROUP2);</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="17" t="s">
         <v>93</v>
       </c>
@@ -6922,39 +7172,43 @@
         <v>SPARE_OUT3000</v>
       </c>
       <c r="M64" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>:BOOL;</v>
       </c>
       <c r="N64" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>SPARE_OUT3000:OpCom; // CHASSIS.OUT3000</v>
       </c>
       <c r="O64" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SPARE_OUT3000</v>
       </c>
       <c r="P64" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.SPARE_OUT3000.Dig</v>
+      </c>
+      <c r="Q64" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SPARE_OUT3000(); // CR0709.OUT3000</v>
       </c>
-      <c r="Q64" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R64" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.SPARE_OUT3000.Init('CHASSIS','SPARE_OUT3000','OUT3000','a31',NVL_Outputs_States_CHASSIS.All.OUT3000,NVL_IO_CHASSIS.All_Outputs_Diag.OUT3000,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R64" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>: Mimic_Output_FB; // CHASSIS:OUT3000</v>
       </c>
       <c r="S64" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT3000();</v>
+        <v>: Mimic_Output_FB; // CHASSIS:OUT3000</v>
       </c>
       <c r="T64" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT3000();</v>
+      </c>
+      <c r="U64" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT3000.Init(Machine_IO.Outputs.SPARE_OUT3000);</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="17" t="s">
         <v>93</v>
       </c>
@@ -6993,39 +7247,43 @@
         <v>SPARE_OUT3001</v>
       </c>
       <c r="M65" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>:BOOL;</v>
       </c>
       <c r="N65" s="20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>SPARE_OUT3001:OpCom; // CHASSIS.OUT3001</v>
       </c>
       <c r="O65" s="20" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Machine_IO.Outputs.SPARE_OUT3001</v>
       </c>
       <c r="P65" s="20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
+        <v>Machine_IO.Outputs.SPARE_OUT3001.Dig</v>
+      </c>
+      <c r="Q65" s="20" t="str">
+        <f t="shared" si="13"/>
         <v>Machine_IO.Outputs.SPARE_OUT3001(); // CR0709.OUT3001</v>
       </c>
-      <c r="Q65" s="20" t="str">
-        <f t="shared" si="18"/>
+      <c r="R65" s="20" t="str">
+        <f t="shared" si="19"/>
         <v>Machine_IO.Outputs.SPARE_OUT3001.Init('CHASSIS','SPARE_OUT3001','OUT3001','a32',NVL_Outputs_States_CHASSIS.All.OUT3001,NVL_IO_CHASSIS.All_Outputs_Diag.OUT3001,Machine_IO.Node_CHASSIS);</v>
-      </c>
-      <c r="R65" s="20" t="str">
-        <f t="shared" si="13"/>
-        <v>: Mimic_Output_FB; // CHASSIS:OUT3001</v>
       </c>
       <c r="S65" s="20" t="str">
         <f t="shared" si="14"/>
-        <v>CHASSIS.OUT3001();</v>
+        <v>: Mimic_Output_FB; // CHASSIS:OUT3001</v>
       </c>
       <c r="T65" s="20" t="str">
         <f t="shared" si="15"/>
+        <v>CHASSIS.OUT3001();</v>
+      </c>
+      <c r="U65" s="20" t="str">
+        <f t="shared" si="16"/>
         <v>CHASSIS.OUT3001.Init(Machine_IO.Outputs.SPARE_OUT3001);</v>
       </c>
     </row>
-    <row r="66" spans="1:20" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="23"/>
       <c r="B66" s="23"/>
       <c r="C66" s="4"/>
@@ -7043,8 +7301,9 @@
       <c r="R66" s="2"/>
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
-    </row>
-    <row r="67" spans="1:20" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="U66" s="2"/>
+    </row>
+    <row r="67" spans="1:21" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="23"/>
       <c r="B67" s="23"/>
       <c r="C67" s="4"/>
@@ -7065,19 +7324,20 @@
       <c r="R67" s="2"/>
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U67" s="2"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="K68" s="4" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="K69" s="4" t="s">
         <v>543</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO71" xr:uid="{1E4EBF08-015A-4388-B8C8-8A07CE5EF3C7}"/>
+  <autoFilter ref="A1:AP71" xr:uid="{1E4EBF08-015A-4388-B8C8-8A07CE5EF3C7}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.23622047244094488" right="0.23622047244094488" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="71" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -15496,7 +15756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <dimension ref="B3:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B14"/>
     </sheetView>
   </sheetViews>
@@ -18490,15 +18750,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -18514,6 +18765,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18740,14 +19000,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -18760,6 +19012,14 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
PLC is now just local control with interlocks for tracks and engine
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA9DB45-1D46-4E6E-A53F-D3F79AD947E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1ABA9F-8E1E-4B88-9BC6-F07A8C203B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1898" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="579">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1688,9 +1688,6 @@
     <t>NVL_UDP_RX.App_Settings.DrumPressHi_SP_bar</t>
   </si>
   <si>
-    <t>Pin code has system</t>
-  </si>
-  <si>
     <t>Scale fuel sender for Diag</t>
   </si>
   <si>
@@ -1728,13 +1725,70 @@
   </si>
   <si>
     <t>NVL_UDP_TX.App_Settings.DrumSpd_Percent</t>
+  </si>
+  <si>
+    <t>Move DM1 to the screen</t>
+  </si>
+  <si>
+    <t>J1939 Task</t>
+  </si>
+  <si>
+    <t>INPUTS</t>
+  </si>
+  <si>
+    <t>pressure transduscer test all the way through</t>
+  </si>
+  <si>
+    <t>check the diagnostics on the analog inputs</t>
+  </si>
+  <si>
+    <t>check the estop button feeback on each screen</t>
+  </si>
+  <si>
+    <t>CR0403 Inputs</t>
+  </si>
+  <si>
+    <t>OUTPUTS</t>
+  </si>
+  <si>
+    <t>POWER UP</t>
+  </si>
+  <si>
+    <t>DM1</t>
+  </si>
+  <si>
+    <t>J1939</t>
+  </si>
+  <si>
+    <t>EDS for the Engine</t>
+  </si>
+  <si>
+    <t>SETTINGS</t>
+  </si>
+  <si>
+    <t>mode to bypass engine started for manual testing (resets on power up)</t>
+  </si>
+  <si>
+    <t>MIMICS</t>
+  </si>
+  <si>
+    <t>main mimic graphic switching between models</t>
+  </si>
+  <si>
+    <t>side conveyor graphic not good</t>
+  </si>
+  <si>
+    <t>feedback of the mA for each function on the main screen</t>
+  </si>
+  <si>
+    <t>MACHINE_APP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1835,6 +1889,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1871,7 +1932,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1949,6 +2010,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2275,9 +2337,9 @@
   </sheetPr>
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2402,7 +2464,7 @@
         <f t="shared" ref="J2:J65" si="1">_xlfn.CONCAT(A2,".",D2)</f>
         <v>CHASSIS.IN0100</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="31" t="s">
         <v>356</v>
       </c>
       <c r="L2" s="19" t="str">
@@ -3844,9 +3906,8 @@
         <f t="shared" si="10"/>
         <v>Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ.Dig</v>
       </c>
-      <c r="Q21" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ(); // CR0709.IN0003</v>
+      <c r="Q21" s="20">
+        <v>43</v>
       </c>
       <c r="R21" s="20" t="str">
         <f t="shared" si="11"/>
@@ -4352,7 +4413,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0900</v>
       </c>
-      <c r="K28" s="19" t="s">
+      <c r="K28" s="31" t="s">
         <v>371</v>
       </c>
       <c r="L28" s="19" t="str">
@@ -4426,7 +4487,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0901</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="31" t="s">
         <v>372</v>
       </c>
       <c r="L29" s="19" t="str">
@@ -4500,7 +4561,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0300</v>
       </c>
-      <c r="K30" s="19" t="s">
+      <c r="K30" s="31" t="s">
         <v>373</v>
       </c>
       <c r="L30" s="19" t="str">
@@ -4574,7 +4635,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0301</v>
       </c>
-      <c r="K31" s="19" t="s">
+      <c r="K31" s="31" t="s">
         <v>374</v>
       </c>
       <c r="L31" s="19" t="str">
@@ -4648,7 +4709,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0800</v>
       </c>
-      <c r="K32" s="19" t="s">
+      <c r="K32" s="31" t="s">
         <v>375</v>
       </c>
       <c r="L32" s="19" t="str">
@@ -4722,7 +4783,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0801</v>
       </c>
-      <c r="K33" s="19" t="s">
+      <c r="K33" s="31" t="s">
         <v>376</v>
       </c>
       <c r="L33" s="19" t="str">
@@ -5667,7 +5728,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0101</v>
       </c>
-      <c r="K45" s="19" t="s">
+      <c r="K45" s="31" t="s">
         <v>387</v>
       </c>
       <c r="L45" s="19" t="str">
@@ -5825,7 +5886,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0103</v>
       </c>
-      <c r="K47" s="19" t="s">
+      <c r="K47" s="31" t="s">
         <v>389</v>
       </c>
       <c r="L47" s="19" t="str">
@@ -6378,7 +6439,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0200</v>
       </c>
-      <c r="K54" s="19" t="s">
+      <c r="K54" s="31" t="s">
         <v>395</v>
       </c>
       <c r="L54" s="19" t="str">
@@ -6457,7 +6518,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0201</v>
       </c>
-      <c r="K55" s="19" t="s">
+      <c r="K55" s="31" t="s">
         <v>396</v>
       </c>
       <c r="L55" s="19" t="str">
@@ -6536,7 +6597,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0202</v>
       </c>
-      <c r="K56" s="19" t="s">
+      <c r="K56" s="31" t="s">
         <v>397</v>
       </c>
       <c r="L56" s="19" t="str">
@@ -6615,7 +6676,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0203</v>
       </c>
-      <c r="K57" s="19" t="s">
+      <c r="K57" s="31" t="s">
         <v>398</v>
       </c>
       <c r="L57" s="19" t="str">
@@ -6694,7 +6755,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0204</v>
       </c>
-      <c r="K58" s="19" t="s">
+      <c r="K58" s="31" t="s">
         <v>399</v>
       </c>
       <c r="L58" s="19" t="str">
@@ -6773,7 +6834,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0205</v>
       </c>
-      <c r="K59" s="19" t="s">
+      <c r="K59" s="31" t="s">
         <v>400</v>
       </c>
       <c r="L59" s="19" t="str">
@@ -7010,7 +7071,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0208</v>
       </c>
-      <c r="K62" s="19" t="s">
+      <c r="K62" s="31" t="s">
         <v>403</v>
       </c>
       <c r="L62" s="19" t="str">
@@ -7487,7 +7548,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -7498,7 +7559,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -7509,7 +7570,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -7520,7 +7581,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -7531,7 +7592,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -7542,7 +7603,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -15754,55 +15815,168 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
-  <dimension ref="B3:B14"/>
+  <dimension ref="A3:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B14"/>
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>562</v>
+      </c>
       <c r="B3" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>562</v>
+      </c>
+      <c r="B4" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>562</v>
+      </c>
+      <c r="B5" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>562</v>
+      </c>
+      <c r="B6" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>562</v>
+      </c>
+      <c r="B7" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>562</v>
+      </c>
+      <c r="B8" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>567</v>
+      </c>
+      <c r="B10" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>568</v>
+      </c>
+      <c r="B12" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>569</v>
+      </c>
+      <c r="B14" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>569</v>
+      </c>
+      <c r="B15" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>569</v>
+      </c>
+      <c r="B16" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>570</v>
+      </c>
+      <c r="B18" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>570</v>
+      </c>
+      <c r="B19" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>578</v>
+      </c>
+      <c r="B21" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>578</v>
+      </c>
+      <c r="B22" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>554</v>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>572</v>
+      </c>
+      <c r="B24" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>574</v>
+      </c>
+      <c r="B26" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>574</v>
+      </c>
+      <c r="B27" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>574</v>
+      </c>
+      <c r="B28" t="s">
+        <v>577</v>
       </c>
     </row>
   </sheetData>
@@ -18750,6 +18924,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -18765,15 +18948,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19000,6 +19174,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -19012,14 +19194,6 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fixes for the tracking IO - PLC OUT0101 tags!
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1ABA9F-8E1E-4B88-9BC6-F07A8C203B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26DA70A-468F-44E8-A726-263493F6403C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
     <sheet name="Settings" sheetId="32" r:id="rId2"/>
     <sheet name="IfmPinRef" sheetId="21" r:id="rId3"/>
     <sheet name="ALARMS" sheetId="24" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="33" r:id="rId5"/>
-    <sheet name="ALARMS_IO" sheetId="31" r:id="rId6"/>
+    <sheet name="ALARMS_IO" sheetId="31" r:id="rId5"/>
+    <sheet name="SNAGS" sheetId="33" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$71</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="585">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1782,13 +1782,31 @@
   </si>
   <si>
     <t>MACHINE_APP</t>
+  </si>
+  <si>
+    <t>TRACKS</t>
+  </si>
+  <si>
+    <t>Umbilical Stop - does it do much? Is it the estop feedback from teleradio?</t>
+  </si>
+  <si>
+    <t>Interlock in PLC with the Siren?</t>
+  </si>
+  <si>
+    <t>Fuel Sender - scale for diagnostics</t>
+  </si>
+  <si>
+    <t>Drum Pressure - scale</t>
+  </si>
+  <si>
+    <t>Check for stuck signals on power up (directions / req / stop)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1896,6 +1914,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1932,7 +1958,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2011,6 +2037,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2337,8 +2364,8 @@
   </sheetPr>
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
@@ -3430,7 +3457,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0701</v>
       </c>
-      <c r="K15" s="19" t="s">
+      <c r="K15" s="32" t="s">
         <v>359</v>
       </c>
       <c r="L15" s="19" t="str">
@@ -3886,7 +3913,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0003</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="K21" s="32" t="s">
         <v>365</v>
       </c>
       <c r="L21" s="19" t="str">
@@ -3961,7 +3988,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0500</v>
       </c>
-      <c r="K22" s="19" t="s">
+      <c r="K22" s="32" t="s">
         <v>366</v>
       </c>
       <c r="L22" s="19" t="str">
@@ -4037,7 +4064,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0501</v>
       </c>
-      <c r="K23" s="19" t="s">
+      <c r="K23" s="32" t="s">
         <v>367</v>
       </c>
       <c r="L23" s="19" t="str">
@@ -4113,7 +4140,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0502</v>
       </c>
-      <c r="K24" s="19" t="s">
+      <c r="K24" s="32" t="s">
         <v>368</v>
       </c>
       <c r="L24" s="19" t="str">
@@ -4189,7 +4216,7 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0503</v>
       </c>
-      <c r="K25" s="19" t="s">
+      <c r="K25" s="32" t="s">
         <v>369</v>
       </c>
       <c r="L25" s="19" t="str">
@@ -15814,177 +15841,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
-  <dimension ref="A3:B28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>562</v>
-      </c>
-      <c r="B3" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>562</v>
-      </c>
-      <c r="B4" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>562</v>
-      </c>
-      <c r="B5" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>562</v>
-      </c>
-      <c r="B6" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>562</v>
-      </c>
-      <c r="B7" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>562</v>
-      </c>
-      <c r="B8" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>567</v>
-      </c>
-      <c r="B10" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>568</v>
-      </c>
-      <c r="B12" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>569</v>
-      </c>
-      <c r="B14" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>569</v>
-      </c>
-      <c r="B15" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>569</v>
-      </c>
-      <c r="B16" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>570</v>
-      </c>
-      <c r="B18" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>570</v>
-      </c>
-      <c r="B19" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>578</v>
-      </c>
-      <c r="B21" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>578</v>
-      </c>
-      <c r="B22" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>572</v>
-      </c>
-      <c r="B24" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>574</v>
-      </c>
-      <c r="B26" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>574</v>
-      </c>
-      <c r="B27" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>574</v>
-      </c>
-      <c r="B28" t="s">
-        <v>577</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B17012-44D7-48B2-87FC-FA2A9133EF8D}">
   <dimension ref="A1:L65"/>
   <sheetViews>
@@ -18923,16 +18779,218 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
+  <dimension ref="A2:B33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>579</v>
+      </c>
+      <c r="B2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>579</v>
+      </c>
+      <c r="B3" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>579</v>
+      </c>
+      <c r="B4" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>562</v>
+      </c>
+      <c r="B6" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>562</v>
+      </c>
+      <c r="B7" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>562</v>
+      </c>
+      <c r="B8" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>562</v>
+      </c>
+      <c r="B9" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>562</v>
+      </c>
+      <c r="B10" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>562</v>
+      </c>
+      <c r="B11" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>562</v>
+      </c>
+      <c r="B12" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>562</v>
+      </c>
+      <c r="B13" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>567</v>
+      </c>
+      <c r="B15" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>568</v>
+      </c>
+      <c r="B17" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>569</v>
+      </c>
+      <c r="B19" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>569</v>
+      </c>
+      <c r="B20" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>569</v>
+      </c>
+      <c r="B21" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>570</v>
+      </c>
+      <c r="B23" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>570</v>
+      </c>
+      <c r="B24" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>578</v>
+      </c>
+      <c r="B26" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>578</v>
+      </c>
+      <c r="B27" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>572</v>
+      </c>
+      <c r="B29" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>574</v>
+      </c>
+      <c r="B31" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>574</v>
+      </c>
+      <c r="B32" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>574</v>
+      </c>
+      <c r="B33" t="s">
+        <v>577</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -18948,6 +19006,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19174,14 +19241,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -19194,6 +19253,14 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
HMI - check the estop logic - TBC
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26DA70A-468F-44E8-A726-263493F6403C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FE7035-6A4F-4286-9308-F6DF537DD095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -2364,9 +2364,9 @@
   </sheetPr>
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -18781,207 +18781,207 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
-  <dimension ref="A2:B33"/>
+  <dimension ref="B2:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="65.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>579</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>579</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>579</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>562</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>562</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>562</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>562</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>562</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>562</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>562</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>562</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>567</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>568</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>569</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>569</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>569</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>570</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>570</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>578</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>578</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>572</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>574</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>574</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>574</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>577</v>
       </c>
     </row>
@@ -18991,6 +18991,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -19006,15 +19015,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19241,6 +19241,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -19253,14 +19261,6 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
WIP sonsite small plc hmi fix ups
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FE7035-6A4F-4286-9308-F6DF537DD095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D944C8A-3F53-4B92-8690-9181F7FE8D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1972" uniqueCount="607">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1800,6 +1800,72 @@
   </si>
   <si>
     <t>Check for stuck signals on power up (directions / req / stop)</t>
+  </si>
+  <si>
+    <t>PINCODE</t>
+  </si>
+  <si>
+    <t>4 digits message instead of 6</t>
+  </si>
+  <si>
+    <t>UDP</t>
+  </si>
+  <si>
+    <t>PLC warning and error timeouts</t>
+  </si>
+  <si>
+    <t>machine mimic psi or bar?</t>
+  </si>
+  <si>
+    <t>HYD_SETUP</t>
+  </si>
+  <si>
+    <t>radio stop pressed - engine still runs</t>
+  </si>
+  <si>
+    <t>RADIO</t>
+  </si>
+  <si>
+    <t>DM1 's not added to the fault logger</t>
+  </si>
+  <si>
+    <t>FAULTS</t>
+  </si>
+  <si>
+    <t>ECU</t>
+  </si>
+  <si>
+    <t>oil pressure not showing</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>psi!</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>indication that setup mode is on / starting</t>
+  </si>
+  <si>
+    <t>very slow interlock on jacks/side - long delay?</t>
+  </si>
+  <si>
+    <t>NAV</t>
+  </si>
+  <si>
+    <t>IO first page entry index issue</t>
+  </si>
+  <si>
+    <t>engine first page entry index issue</t>
+  </si>
+  <si>
+    <t>left / right arrows</t>
   </si>
 </sst>
 </file>
@@ -2364,7 +2430,7 @@
   </sheetPr>
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
@@ -18781,19 +18847,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
-  <dimension ref="B2:C33"/>
+  <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>579</v>
       </c>
@@ -18801,7 +18867,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>579</v>
       </c>
@@ -18809,7 +18875,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>579</v>
       </c>
@@ -18817,7 +18883,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>562</v>
       </c>
@@ -18825,55 +18891,73 @@
         <v>565</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>562</v>
       </c>
       <c r="C7" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>562</v>
       </c>
       <c r="C8" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>562</v>
       </c>
       <c r="C9" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>562</v>
       </c>
       <c r="C10" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>562</v>
       </c>
       <c r="C11" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>562</v>
       </c>
       <c r="C12" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>562</v>
       </c>
@@ -18881,108 +18965,212 @@
         <v>566</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>562</v>
+      </c>
+      <c r="C14" t="s">
+        <v>589</v>
+      </c>
+      <c r="D14" t="s">
+        <v>598</v>
+      </c>
+      <c r="E14" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>567</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>568</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>569</v>
-      </c>
-      <c r="C19" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>569</v>
       </c>
       <c r="C20" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+      <c r="D20" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>569</v>
       </c>
       <c r="C21" t="s">
+        <v>550</v>
+      </c>
+      <c r="D21" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>569</v>
+      </c>
+      <c r="C22" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>570</v>
-      </c>
-      <c r="C23" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>570</v>
       </c>
       <c r="C24" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>570</v>
+      </c>
+      <c r="C25" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>578</v>
-      </c>
-      <c r="C26" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>578</v>
       </c>
       <c r="C27" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>578</v>
+      </c>
+      <c r="C28" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>572</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>574</v>
-      </c>
-      <c r="C31" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>574</v>
       </c>
       <c r="C32" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>574</v>
       </c>
       <c r="C33" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>574</v>
+      </c>
+      <c r="C34" t="s">
         <v>577</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>585</v>
+      </c>
+      <c r="C37" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>587</v>
+      </c>
+      <c r="C40" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>590</v>
+      </c>
+      <c r="C42" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>579</v>
+      </c>
+      <c r="C44" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>592</v>
+      </c>
+      <c r="C45" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>594</v>
+      </c>
+      <c r="C46" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>595</v>
+      </c>
+      <c r="C48" t="s">
+        <v>596</v>
+      </c>
+      <c r="D48" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>603</v>
+      </c>
+      <c r="C50" t="s">
+        <v>604</v>
+      </c>
+      <c r="E50" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>603</v>
+      </c>
+      <c r="C51" t="s">
+        <v>605</v>
+      </c>
+      <c r="E51" t="s">
+        <v>606</v>
       </c>
     </row>
   </sheetData>
@@ -18991,15 +19179,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -19015,6 +19194,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19241,14 +19429,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -19261,6 +19441,14 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
WIP leaving site PLC - fixes for the ouputs fault on the low voltage from cranking - added IN0102 to monitor if cranking (keyswitch) is active
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D944C8A-3F53-4B92-8690-9181F7FE8D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1073266A-D9F6-4B33-9BF4-B54DBE3A7EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="17145" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1972" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="609">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1844,9 +1844,6 @@
     <t>DONE</t>
   </si>
   <si>
-    <t>psi!</t>
-  </si>
-  <si>
     <t>SKIP</t>
   </si>
   <si>
@@ -1866,6 +1863,15 @@
   </si>
   <si>
     <t>left / right arrows</t>
+  </si>
+  <si>
+    <t>VIZ</t>
+  </si>
+  <si>
+    <t>chassis plc name clipped in PLC_Status</t>
+  </si>
+  <si>
+    <t>KEYSWITCH_CRANKING</t>
   </si>
 </sst>
 </file>
@@ -2430,9 +2436,9 @@
   </sheetPr>
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2709,35 +2715,37 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0102</v>
       </c>
-      <c r="K4" s="19"/>
+      <c r="K4" s="19" t="s">
+        <v>608</v>
+      </c>
       <c r="L4" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>SPARE_IN0102</v>
+        <v>KEYSWITCH_CRANKING</v>
       </c>
       <c r="M4" s="19"/>
       <c r="N4" s="20" t="str">
         <f t="shared" si="8"/>
-        <v>SPARE_IN0102:IpCom; // CHASSIS IN0102</v>
+        <v>KEYSWITCH_CRANKING:IpCom; // CHASSIS IN0102</v>
       </c>
       <c r="O4" s="20" t="str">
         <f t="shared" si="9"/>
-        <v>Machine_IO.Inputs.SPARE_IN0102</v>
+        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING</v>
       </c>
       <c r="P4" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.SPARE_IN0102.Dig</v>
+        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING.Dig</v>
       </c>
       <c r="Q4" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>Machine_IO.Inputs.SPARE_IN0102(); // CR0709.IN0102</v>
+        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING(); // CR0709.IN0102</v>
       </c>
       <c r="R4" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>Machine_IO.Inputs.SPARE_IN0102.Init('CHASSIS','SPARE_IN0102','IN0102','a65',NVL_IO_CHASSIS.All_Inputs.IN0102,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING.Init('CHASSIS','KEYSWITCH_CRANKING','IN0102','a65',NVL_IO_CHASSIS.All_Inputs.IN0102,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="S4" s="20" t="str">
         <f t="shared" si="3"/>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0102</v>
+        <v>KEYSWITCH_CRANKING: Mimic_Input_FB; // CHASSIS:IN0102</v>
       </c>
       <c r="T4" s="20" t="str">
         <f t="shared" si="4"/>
@@ -2745,7 +2753,7 @@
       </c>
       <c r="U4" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>CHASSIS.IN0102.Init(Machine_IO.Inputs.SPARE_IN0102);</v>
+        <v>CHASSIS.IN0102.Init(Machine_IO.Inputs.KEYSWITCH_CRANKING);</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -18847,19 +18855,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
-  <dimension ref="B2:E51"/>
+  <dimension ref="B2:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="67.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>579</v>
       </c>
@@ -18867,7 +18876,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>579</v>
       </c>
@@ -18875,7 +18884,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>579</v>
       </c>
@@ -18883,7 +18892,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>562</v>
       </c>
@@ -18891,7 +18900,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>562</v>
       </c>
@@ -18902,7 +18911,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>562</v>
       </c>
@@ -18913,7 +18922,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>562</v>
       </c>
@@ -18924,7 +18933,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>562</v>
       </c>
@@ -18935,7 +18944,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>562</v>
       </c>
@@ -18946,7 +18955,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>562</v>
       </c>
@@ -18957,7 +18966,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>562</v>
       </c>
@@ -18965,7 +18974,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>562</v>
       </c>
@@ -18975,11 +18984,8 @@
       <c r="D14" t="s">
         <v>598</v>
       </c>
-      <c r="E14" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>567</v>
       </c>
@@ -19025,7 +19031,7 @@
         <v>551</v>
       </c>
       <c r="D22" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -19113,7 +19119,7 @@
         <v>590</v>
       </c>
       <c r="C42" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
@@ -19129,7 +19135,7 @@
         <v>592</v>
       </c>
       <c r="C45" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
@@ -19153,24 +19159,32 @@
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>602</v>
+      </c>
+      <c r="C50" t="s">
         <v>603</v>
       </c>
-      <c r="C50" t="s">
-        <v>604</v>
-      </c>
       <c r="E50" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C51" t="s">
+        <v>604</v>
+      </c>
+      <c r="E51" t="s">
         <v>605</v>
       </c>
-      <c r="E51" t="s">
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>606</v>
+      </c>
+      <c r="C53" t="s">
+        <v>607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the CR0403 outputs page
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1073266A-D9F6-4B33-9BF4-B54DBE3A7EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA445A5-747E-451D-A730-AD803DF1D9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="17145" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -23,6 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SNAGS!$B$1:$E$53</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="628">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1670,15 +1671,6 @@
     <t>NVL_UDP_RX.App_Settings.EnableDrumPressCutOut</t>
   </si>
   <si>
-    <t>Siren Beacon</t>
-  </si>
-  <si>
-    <t>oil Cooker</t>
-  </si>
-  <si>
-    <t>oil cooler for/rev</t>
-  </si>
-  <si>
     <t>NVL_UDP_RX.App_Settings.DrumPressHiHi_SP_bar</t>
   </si>
   <si>
@@ -1838,9 +1830,6 @@
     <t>oil pressure not showing</t>
   </si>
   <si>
-    <t>FIXED</t>
-  </si>
-  <si>
     <t>DONE</t>
   </si>
   <si>
@@ -1872,6 +1861,75 @@
   </si>
   <si>
     <t>KEYSWITCH_CRANKING</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>SECTION</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>AUX</t>
+  </si>
+  <si>
+    <t>CR0403</t>
+  </si>
+  <si>
+    <t>OP0</t>
+  </si>
+  <si>
+    <t>SIREN</t>
+  </si>
+  <si>
+    <t>OP1</t>
+  </si>
+  <si>
+    <t>OP2</t>
+  </si>
+  <si>
+    <t>OP3</t>
+  </si>
+  <si>
+    <t>OP4</t>
+  </si>
+  <si>
+    <t>OP5</t>
+  </si>
+  <si>
+    <t>OP6</t>
+  </si>
+  <si>
+    <t>OP7</t>
+  </si>
+  <si>
+    <t>OP8</t>
+  </si>
+  <si>
+    <t>OP9</t>
+  </si>
+  <si>
+    <t>OP10</t>
+  </si>
+  <si>
+    <t>OP11</t>
+  </si>
+  <si>
+    <t>DIVERT_VALVE</t>
+  </si>
+  <si>
+    <t>FAN_FORWARD</t>
+  </si>
+  <si>
+    <t>FAN_REVERSE</t>
+  </si>
+  <si>
+    <t>SIDE_CONV_RAISE</t>
+  </si>
+  <si>
+    <t>SIDE_CONV_LOWER</t>
   </si>
 </sst>
 </file>
@@ -2434,11 +2492,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U69"/>
+  <dimension ref="A1:U78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2716,7 +2774,7 @@
         <v>CHASSIS.IN0102</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="L4" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7465,37 +7523,820 @@
       <c r="T66" s="2"/>
       <c r="U66" s="2"/>
     </row>
-    <row r="67" spans="1:21" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
-      <c r="B67" s="23"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
-      <c r="H67" s="23"/>
-      <c r="I67" s="23"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="24" t="s">
-        <v>541</v>
-      </c>
-      <c r="N67" s="2"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="2"/>
-      <c r="Q67" s="2"/>
-      <c r="R67" s="2"/>
-      <c r="S67" s="2"/>
-      <c r="T67" s="2"/>
-      <c r="U67" s="2"/>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A67" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C67" s="19"/>
+      <c r="D67" s="17" t="s">
+        <v>610</v>
+      </c>
+      <c r="E67" s="17" t="str">
+        <f t="shared" ref="E67:E74" si="20">_xlfn.CONCAT(B67,".",D67)</f>
+        <v>CR0403.OP0</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21" t="str">
+        <f t="shared" ref="J67" si="21">_xlfn.CONCAT(A67,".",D67)</f>
+        <v>AUX.OP0</v>
+      </c>
+      <c r="K67" s="19" t="s">
+        <v>611</v>
+      </c>
+      <c r="L67" s="19" t="str">
+        <f t="shared" ref="L67" si="22">IF(K67&lt;&gt;"",UPPER(K67),_xlfn.CONCAT("SPARE_",D67))</f>
+        <v>SIREN</v>
+      </c>
+      <c r="M67" s="19" t="str">
+        <f t="shared" ref="M67" si="23">_xlfn.CONCAT(K67,":BOOL;")</f>
+        <v>SIREN:BOOL;</v>
+      </c>
+      <c r="N67" s="20" t="str">
+        <f t="shared" ref="N67" si="24">_xlfn.CONCAT(L67,":OpCom; // ",A67,".",D67)</f>
+        <v>SIREN:OpCom; // AUX.OP0</v>
+      </c>
+      <c r="O67" s="20" t="str">
+        <f t="shared" ref="O67" si="25">_xlfn.CONCAT("Machine_IO.","Outputs.",L67,"")</f>
+        <v>Machine_IO.Outputs.SIREN</v>
+      </c>
+      <c r="P67" s="20" t="str">
+        <f t="shared" ref="P67" si="26">_xlfn.CONCAT(O67,".Dig")</f>
+        <v>Machine_IO.Outputs.SIREN.Dig</v>
+      </c>
+      <c r="Q67" s="20" t="str">
+        <f t="shared" ref="Q67" si="27">_xlfn.CONCAT(O67,"(); // ",E67)</f>
+        <v>Machine_IO.Outputs.SIREN(); // CR0403.OP0</v>
+      </c>
+      <c r="R67" s="20" t="str">
+        <f t="shared" ref="R67" si="28">_xlfn.CONCAT(O67,".Init('",A67,"','",L67,"','",D67,"','",G67,"',NVL_Outputs_States_",A67,".All.",D67,",NVL_IO_",A35,".All_Outputs_Diag.",D67,",Machine_IO.Node_",A67,");")</f>
+        <v>Machine_IO.Outputs.SIREN.Init('AUX','SIREN','OP0','',NVL_Outputs_States_AUX.All.OP0,NVL_IO_CHASSIS.All_Outputs_Diag.OP0,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S67" s="20" t="str">
+        <f t="shared" ref="S67" si="29">_xlfn.CONCAT(K67,": Mimic_Output_FB; // ",A67,":",D67)</f>
+        <v>SIREN: Mimic_Output_FB; // AUX:OP0</v>
+      </c>
+      <c r="T67" s="20" t="str">
+        <f t="shared" ref="T67" si="30">_xlfn.CONCAT(A67,".",D67,"();")</f>
+        <v>AUX.OP0();</v>
+      </c>
+      <c r="U67" s="20" t="str">
+        <f t="shared" ref="U67" si="31">_xlfn.CONCAT(A67,".",D67,".Init(",O67,");")</f>
+        <v>AUX.OP0.Init(Machine_IO.Outputs.SIREN);</v>
+      </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="K68" s="4" t="s">
-        <v>542</v>
+      <c r="A68" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C68" s="19"/>
+      <c r="D68" s="17" t="s">
+        <v>612</v>
+      </c>
+      <c r="E68" s="17" t="str">
+        <f t="shared" si="20"/>
+        <v>CR0403.OP1</v>
+      </c>
+      <c r="F68" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21" t="str">
+        <f t="shared" ref="J68:J71" si="32">_xlfn.CONCAT(A68,".",D68)</f>
+        <v>AUX.OP1</v>
+      </c>
+      <c r="K68" s="19"/>
+      <c r="L68" s="19" t="str">
+        <f t="shared" ref="L68:L71" si="33">IF(K68&lt;&gt;"",UPPER(K68),_xlfn.CONCAT("SPARE_",D68))</f>
+        <v>SPARE_OP1</v>
+      </c>
+      <c r="M68" s="19" t="str">
+        <f t="shared" ref="M68:M71" si="34">_xlfn.CONCAT(K68,":BOOL;")</f>
+        <v>:BOOL;</v>
+      </c>
+      <c r="N68" s="20" t="str">
+        <f t="shared" ref="N68:N71" si="35">_xlfn.CONCAT(L68,":OpCom; // ",A68,".",D68)</f>
+        <v>SPARE_OP1:OpCom; // AUX.OP1</v>
+      </c>
+      <c r="O68" s="20" t="str">
+        <f t="shared" ref="O68:O71" si="36">_xlfn.CONCAT("Machine_IO.","Outputs.",L68,"")</f>
+        <v>Machine_IO.Outputs.SPARE_OP1</v>
+      </c>
+      <c r="P68" s="20" t="str">
+        <f t="shared" ref="P68:P71" si="37">_xlfn.CONCAT(O68,".Dig")</f>
+        <v>Machine_IO.Outputs.SPARE_OP1.Dig</v>
+      </c>
+      <c r="Q68" s="20" t="str">
+        <f t="shared" ref="Q68:Q71" si="38">_xlfn.CONCAT(O68,"(); // ",E68)</f>
+        <v>Machine_IO.Outputs.SPARE_OP1(); // CR0403.OP1</v>
+      </c>
+      <c r="R68" s="20" t="str">
+        <f t="shared" ref="R68:R71" si="39">_xlfn.CONCAT(O68,".Init('",A68,"','",L68,"','",D68,"','",G68,"',NVL_Outputs_States_",A68,".All.",D68,",NVL_IO_",A36,".All_Outputs_Diag.",D68,",Machine_IO.Node_",A68,");")</f>
+        <v>Machine_IO.Outputs.SPARE_OP1.Init('AUX','SPARE_OP1','OP1','',NVL_Outputs_States_AUX.All.OP1,NVL_IO_CHASSIS.All_Outputs_Diag.OP1,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S68" s="20" t="str">
+        <f t="shared" ref="S68:S71" si="40">_xlfn.CONCAT(K68,": Mimic_Output_FB; // ",A68,":",D68)</f>
+        <v>: Mimic_Output_FB; // AUX:OP1</v>
+      </c>
+      <c r="T68" s="20" t="str">
+        <f t="shared" ref="T68:T71" si="41">_xlfn.CONCAT(A68,".",D68,"();")</f>
+        <v>AUX.OP1();</v>
+      </c>
+      <c r="U68" s="20" t="str">
+        <f t="shared" ref="U68:U71" si="42">_xlfn.CONCAT(A68,".",D68,".Init(",O68,");")</f>
+        <v>AUX.OP1.Init(Machine_IO.Outputs.SPARE_OP1);</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="K69" s="4" t="s">
-        <v>543</v>
+      <c r="A69" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C69" s="19"/>
+      <c r="D69" s="17" t="s">
+        <v>613</v>
+      </c>
+      <c r="E69" s="17" t="str">
+        <f t="shared" si="20"/>
+        <v>CR0403.OP2</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21" t="str">
+        <f t="shared" si="32"/>
+        <v>AUX.OP2</v>
+      </c>
+      <c r="K69" s="19"/>
+      <c r="L69" s="19" t="str">
+        <f t="shared" si="33"/>
+        <v>SPARE_OP2</v>
+      </c>
+      <c r="M69" s="19" t="str">
+        <f t="shared" si="34"/>
+        <v>:BOOL;</v>
+      </c>
+      <c r="N69" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v>SPARE_OP2:OpCom; // AUX.OP2</v>
+      </c>
+      <c r="O69" s="20" t="str">
+        <f t="shared" si="36"/>
+        <v>Machine_IO.Outputs.SPARE_OP2</v>
+      </c>
+      <c r="P69" s="20" t="str">
+        <f t="shared" si="37"/>
+        <v>Machine_IO.Outputs.SPARE_OP2.Dig</v>
+      </c>
+      <c r="Q69" s="20" t="str">
+        <f t="shared" si="38"/>
+        <v>Machine_IO.Outputs.SPARE_OP2(); // CR0403.OP2</v>
+      </c>
+      <c r="R69" s="20" t="str">
+        <f t="shared" si="39"/>
+        <v>Machine_IO.Outputs.SPARE_OP2.Init('AUX','SPARE_OP2','OP2','',NVL_Outputs_States_AUX.All.OP2,NVL_IO_CHASSIS.All_Outputs_Diag.OP2,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S69" s="20" t="str">
+        <f t="shared" si="40"/>
+        <v>: Mimic_Output_FB; // AUX:OP2</v>
+      </c>
+      <c r="T69" s="20" t="str">
+        <f t="shared" si="41"/>
+        <v>AUX.OP2();</v>
+      </c>
+      <c r="U69" s="20" t="str">
+        <f t="shared" si="42"/>
+        <v>AUX.OP2.Init(Machine_IO.Outputs.SPARE_OP2);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A70" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C70" s="19"/>
+      <c r="D70" s="17" t="s">
+        <v>614</v>
+      </c>
+      <c r="E70" s="17" t="str">
+        <f t="shared" si="20"/>
+        <v>CR0403.OP3</v>
+      </c>
+      <c r="F70" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21" t="str">
+        <f t="shared" si="32"/>
+        <v>AUX.OP3</v>
+      </c>
+      <c r="K70" s="19" t="s">
+        <v>623</v>
+      </c>
+      <c r="L70" s="19" t="str">
+        <f t="shared" si="33"/>
+        <v>DIVERT_VALVE</v>
+      </c>
+      <c r="M70" s="19" t="str">
+        <f t="shared" si="34"/>
+        <v>DIVERT_VALVE:BOOL;</v>
+      </c>
+      <c r="N70" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v>DIVERT_VALVE:OpCom; // AUX.OP3</v>
+      </c>
+      <c r="O70" s="20" t="str">
+        <f t="shared" si="36"/>
+        <v>Machine_IO.Outputs.DIVERT_VALVE</v>
+      </c>
+      <c r="P70" s="20" t="str">
+        <f t="shared" si="37"/>
+        <v>Machine_IO.Outputs.DIVERT_VALVE.Dig</v>
+      </c>
+      <c r="Q70" s="20" t="str">
+        <f t="shared" si="38"/>
+        <v>Machine_IO.Outputs.DIVERT_VALVE(); // CR0403.OP3</v>
+      </c>
+      <c r="R70" s="20" t="str">
+        <f t="shared" si="39"/>
+        <v>Machine_IO.Outputs.DIVERT_VALVE.Init('AUX','DIVERT_VALVE','OP3','',NVL_Outputs_States_AUX.All.OP3,NVL_IO_CHASSIS.All_Outputs_Diag.OP3,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S70" s="20" t="str">
+        <f t="shared" si="40"/>
+        <v>DIVERT_VALVE: Mimic_Output_FB; // AUX:OP3</v>
+      </c>
+      <c r="T70" s="20" t="str">
+        <f t="shared" si="41"/>
+        <v>AUX.OP3();</v>
+      </c>
+      <c r="U70" s="20" t="str">
+        <f t="shared" si="42"/>
+        <v>AUX.OP3.Init(Machine_IO.Outputs.DIVERT_VALVE);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A71" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C71" s="19"/>
+      <c r="D71" s="17" t="s">
+        <v>615</v>
+      </c>
+      <c r="E71" s="17" t="str">
+        <f t="shared" si="20"/>
+        <v>CR0403.OP4</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="21" t="str">
+        <f t="shared" si="32"/>
+        <v>AUX.OP4</v>
+      </c>
+      <c r="K71" s="19" t="s">
+        <v>624</v>
+      </c>
+      <c r="L71" s="19" t="str">
+        <f t="shared" si="33"/>
+        <v>FAN_FORWARD</v>
+      </c>
+      <c r="M71" s="19" t="str">
+        <f t="shared" si="34"/>
+        <v>FAN_FORWARD:BOOL;</v>
+      </c>
+      <c r="N71" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v>FAN_FORWARD:OpCom; // AUX.OP4</v>
+      </c>
+      <c r="O71" s="20" t="str">
+        <f t="shared" si="36"/>
+        <v>Machine_IO.Outputs.FAN_FORWARD</v>
+      </c>
+      <c r="P71" s="20" t="str">
+        <f t="shared" si="37"/>
+        <v>Machine_IO.Outputs.FAN_FORWARD.Dig</v>
+      </c>
+      <c r="Q71" s="20" t="str">
+        <f t="shared" si="38"/>
+        <v>Machine_IO.Outputs.FAN_FORWARD(); // CR0403.OP4</v>
+      </c>
+      <c r="R71" s="20" t="str">
+        <f t="shared" si="39"/>
+        <v>Machine_IO.Outputs.FAN_FORWARD.Init('AUX','FAN_FORWARD','OP4','',NVL_Outputs_States_AUX.All.OP4,NVL_IO_CHASSIS.All_Outputs_Diag.OP4,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S71" s="20" t="str">
+        <f t="shared" si="40"/>
+        <v>FAN_FORWARD: Mimic_Output_FB; // AUX:OP4</v>
+      </c>
+      <c r="T71" s="20" t="str">
+        <f t="shared" si="41"/>
+        <v>AUX.OP4();</v>
+      </c>
+      <c r="U71" s="20" t="str">
+        <f t="shared" si="42"/>
+        <v>AUX.OP4.Init(Machine_IO.Outputs.FAN_FORWARD);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A72" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C72" s="19"/>
+      <c r="D72" s="17" t="s">
+        <v>616</v>
+      </c>
+      <c r="E72" s="17" t="str">
+        <f t="shared" si="20"/>
+        <v>CR0403.OP5</v>
+      </c>
+      <c r="F72" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
+      <c r="J72" s="21" t="str">
+        <f t="shared" ref="J72:J75" si="43">_xlfn.CONCAT(A72,".",D72)</f>
+        <v>AUX.OP5</v>
+      </c>
+      <c r="K72" s="19" t="s">
+        <v>625</v>
+      </c>
+      <c r="L72" s="19" t="str">
+        <f t="shared" ref="L72:L75" si="44">IF(K72&lt;&gt;"",UPPER(K72),_xlfn.CONCAT("SPARE_",D72))</f>
+        <v>FAN_REVERSE</v>
+      </c>
+      <c r="M72" s="19" t="str">
+        <f t="shared" ref="M72:M75" si="45">_xlfn.CONCAT(K72,":BOOL;")</f>
+        <v>FAN_REVERSE:BOOL;</v>
+      </c>
+      <c r="N72" s="20" t="str">
+        <f t="shared" ref="N72:N75" si="46">_xlfn.CONCAT(L72,":OpCom; // ",A72,".",D72)</f>
+        <v>FAN_REVERSE:OpCom; // AUX.OP5</v>
+      </c>
+      <c r="O72" s="20" t="str">
+        <f t="shared" ref="O72:O75" si="47">_xlfn.CONCAT("Machine_IO.","Outputs.",L72,"")</f>
+        <v>Machine_IO.Outputs.FAN_REVERSE</v>
+      </c>
+      <c r="P72" s="20" t="str">
+        <f t="shared" ref="P72:P75" si="48">_xlfn.CONCAT(O72,".Dig")</f>
+        <v>Machine_IO.Outputs.FAN_REVERSE.Dig</v>
+      </c>
+      <c r="Q72" s="20" t="str">
+        <f t="shared" ref="Q72:Q75" si="49">_xlfn.CONCAT(O72,"(); // ",E72)</f>
+        <v>Machine_IO.Outputs.FAN_REVERSE(); // CR0403.OP5</v>
+      </c>
+      <c r="R72" s="20" t="str">
+        <f t="shared" ref="R72:R75" si="50">_xlfn.CONCAT(O72,".Init('",A72,"','",L72,"','",D72,"','",G72,"',NVL_Outputs_States_",A72,".All.",D72,",NVL_IO_",A40,".All_Outputs_Diag.",D72,",Machine_IO.Node_",A72,");")</f>
+        <v>Machine_IO.Outputs.FAN_REVERSE.Init('AUX','FAN_REVERSE','OP5','',NVL_Outputs_States_AUX.All.OP5,NVL_IO_CHASSIS.All_Outputs_Diag.OP5,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S72" s="20" t="str">
+        <f t="shared" ref="S72:S75" si="51">_xlfn.CONCAT(K72,": Mimic_Output_FB; // ",A72,":",D72)</f>
+        <v>FAN_REVERSE: Mimic_Output_FB; // AUX:OP5</v>
+      </c>
+      <c r="T72" s="20" t="str">
+        <f t="shared" ref="T72:T75" si="52">_xlfn.CONCAT(A72,".",D72,"();")</f>
+        <v>AUX.OP5();</v>
+      </c>
+      <c r="U72" s="20" t="str">
+        <f t="shared" ref="U72:U75" si="53">_xlfn.CONCAT(A72,".",D72,".Init(",O72,");")</f>
+        <v>AUX.OP5.Init(Machine_IO.Outputs.FAN_REVERSE);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A73" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C73" s="19"/>
+      <c r="D73" s="17" t="s">
+        <v>617</v>
+      </c>
+      <c r="E73" s="17" t="str">
+        <f t="shared" si="20"/>
+        <v>CR0403.OP6</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
+      <c r="J73" s="21" t="str">
+        <f t="shared" si="43"/>
+        <v>AUX.OP6</v>
+      </c>
+      <c r="K73" s="19" t="s">
+        <v>626</v>
+      </c>
+      <c r="L73" s="19" t="str">
+        <f t="shared" si="44"/>
+        <v>SIDE_CONV_RAISE</v>
+      </c>
+      <c r="M73" s="19" t="str">
+        <f t="shared" si="45"/>
+        <v>SIDE_CONV_RAISE:BOOL;</v>
+      </c>
+      <c r="N73" s="20" t="str">
+        <f t="shared" si="46"/>
+        <v>SIDE_CONV_RAISE:OpCom; // AUX.OP6</v>
+      </c>
+      <c r="O73" s="20" t="str">
+        <f t="shared" si="47"/>
+        <v>Machine_IO.Outputs.SIDE_CONV_RAISE</v>
+      </c>
+      <c r="P73" s="20" t="str">
+        <f t="shared" si="48"/>
+        <v>Machine_IO.Outputs.SIDE_CONV_RAISE.Dig</v>
+      </c>
+      <c r="Q73" s="20" t="str">
+        <f t="shared" si="49"/>
+        <v>Machine_IO.Outputs.SIDE_CONV_RAISE(); // CR0403.OP6</v>
+      </c>
+      <c r="R73" s="20" t="str">
+        <f t="shared" si="50"/>
+        <v>Machine_IO.Outputs.SIDE_CONV_RAISE.Init('AUX','SIDE_CONV_RAISE','OP6','',NVL_Outputs_States_AUX.All.OP6,NVL_IO_CHASSIS.All_Outputs_Diag.OP6,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S73" s="20" t="str">
+        <f t="shared" si="51"/>
+        <v>SIDE_CONV_RAISE: Mimic_Output_FB; // AUX:OP6</v>
+      </c>
+      <c r="T73" s="20" t="str">
+        <f t="shared" si="52"/>
+        <v>AUX.OP6();</v>
+      </c>
+      <c r="U73" s="20" t="str">
+        <f t="shared" si="53"/>
+        <v>AUX.OP6.Init(Machine_IO.Outputs.SIDE_CONV_RAISE);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A74" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C74" s="19"/>
+      <c r="D74" s="17" t="s">
+        <v>618</v>
+      </c>
+      <c r="E74" s="17" t="str">
+        <f t="shared" si="20"/>
+        <v>CR0403.OP7</v>
+      </c>
+      <c r="F74" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21" t="str">
+        <f t="shared" si="43"/>
+        <v>AUX.OP7</v>
+      </c>
+      <c r="K74" s="19" t="s">
+        <v>627</v>
+      </c>
+      <c r="L74" s="19" t="str">
+        <f t="shared" si="44"/>
+        <v>SIDE_CONV_LOWER</v>
+      </c>
+      <c r="M74" s="19" t="str">
+        <f t="shared" si="45"/>
+        <v>SIDE_CONV_LOWER:BOOL;</v>
+      </c>
+      <c r="N74" s="20" t="str">
+        <f t="shared" si="46"/>
+        <v>SIDE_CONV_LOWER:OpCom; // AUX.OP7</v>
+      </c>
+      <c r="O74" s="20" t="str">
+        <f t="shared" si="47"/>
+        <v>Machine_IO.Outputs.SIDE_CONV_LOWER</v>
+      </c>
+      <c r="P74" s="20" t="str">
+        <f t="shared" si="48"/>
+        <v>Machine_IO.Outputs.SIDE_CONV_LOWER.Dig</v>
+      </c>
+      <c r="Q74" s="20" t="str">
+        <f t="shared" si="49"/>
+        <v>Machine_IO.Outputs.SIDE_CONV_LOWER(); // CR0403.OP7</v>
+      </c>
+      <c r="R74" s="20" t="str">
+        <f t="shared" si="50"/>
+        <v>Machine_IO.Outputs.SIDE_CONV_LOWER.Init('AUX','SIDE_CONV_LOWER','OP7','',NVL_Outputs_States_AUX.All.OP7,NVL_IO_CHASSIS.All_Outputs_Diag.OP7,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S74" s="20" t="str">
+        <f t="shared" si="51"/>
+        <v>SIDE_CONV_LOWER: Mimic_Output_FB; // AUX:OP7</v>
+      </c>
+      <c r="T74" s="20" t="str">
+        <f t="shared" si="52"/>
+        <v>AUX.OP7();</v>
+      </c>
+      <c r="U74" s="20" t="str">
+        <f t="shared" si="53"/>
+        <v>AUX.OP7.Init(Machine_IO.Outputs.SIDE_CONV_LOWER);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A75" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C75" s="19"/>
+      <c r="D75" s="17" t="s">
+        <v>619</v>
+      </c>
+      <c r="E75" s="17" t="str">
+        <f t="shared" ref="E75:E78" si="54">_xlfn.CONCAT(B75,".",D75)</f>
+        <v>CR0403.OP8</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G75" s="21"/>
+      <c r="H75" s="21"/>
+      <c r="I75" s="21"/>
+      <c r="J75" s="21" t="str">
+        <f t="shared" si="43"/>
+        <v>AUX.OP8</v>
+      </c>
+      <c r="K75" s="19"/>
+      <c r="L75" s="19" t="str">
+        <f t="shared" si="44"/>
+        <v>SPARE_OP8</v>
+      </c>
+      <c r="M75" s="19" t="str">
+        <f t="shared" si="45"/>
+        <v>:BOOL;</v>
+      </c>
+      <c r="N75" s="20" t="str">
+        <f t="shared" si="46"/>
+        <v>SPARE_OP8:OpCom; // AUX.OP8</v>
+      </c>
+      <c r="O75" s="20" t="str">
+        <f t="shared" si="47"/>
+        <v>Machine_IO.Outputs.SPARE_OP8</v>
+      </c>
+      <c r="P75" s="20" t="str">
+        <f t="shared" si="48"/>
+        <v>Machine_IO.Outputs.SPARE_OP8.Dig</v>
+      </c>
+      <c r="Q75" s="20" t="str">
+        <f t="shared" si="49"/>
+        <v>Machine_IO.Outputs.SPARE_OP8(); // CR0403.OP8</v>
+      </c>
+      <c r="R75" s="20" t="str">
+        <f t="shared" si="50"/>
+        <v>Machine_IO.Outputs.SPARE_OP8.Init('AUX','SPARE_OP8','OP8','',NVL_Outputs_States_AUX.All.OP8,NVL_IO_CHASSIS.All_Outputs_Diag.OP8,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S75" s="20" t="str">
+        <f t="shared" si="51"/>
+        <v>: Mimic_Output_FB; // AUX:OP8</v>
+      </c>
+      <c r="T75" s="20" t="str">
+        <f t="shared" si="52"/>
+        <v>AUX.OP8();</v>
+      </c>
+      <c r="U75" s="20" t="str">
+        <f t="shared" si="53"/>
+        <v>AUX.OP8.Init(Machine_IO.Outputs.SPARE_OP8);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A76" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C76" s="19"/>
+      <c r="D76" s="17" t="s">
+        <v>620</v>
+      </c>
+      <c r="E76" s="17" t="str">
+        <f t="shared" si="54"/>
+        <v>CR0403.OP9</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G76" s="21"/>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
+      <c r="J76" s="21" t="str">
+        <f t="shared" ref="J76:J78" si="55">_xlfn.CONCAT(A76,".",D76)</f>
+        <v>AUX.OP9</v>
+      </c>
+      <c r="K76" s="19"/>
+      <c r="L76" s="19" t="str">
+        <f t="shared" ref="L76:L78" si="56">IF(K76&lt;&gt;"",UPPER(K76),_xlfn.CONCAT("SPARE_",D76))</f>
+        <v>SPARE_OP9</v>
+      </c>
+      <c r="M76" s="19" t="str">
+        <f t="shared" ref="M76:M78" si="57">_xlfn.CONCAT(K76,":BOOL;")</f>
+        <v>:BOOL;</v>
+      </c>
+      <c r="N76" s="20" t="str">
+        <f t="shared" ref="N76:N78" si="58">_xlfn.CONCAT(L76,":OpCom; // ",A76,".",D76)</f>
+        <v>SPARE_OP9:OpCom; // AUX.OP9</v>
+      </c>
+      <c r="O76" s="20" t="str">
+        <f t="shared" ref="O76:O78" si="59">_xlfn.CONCAT("Machine_IO.","Outputs.",L76,"")</f>
+        <v>Machine_IO.Outputs.SPARE_OP9</v>
+      </c>
+      <c r="P76" s="20" t="str">
+        <f t="shared" ref="P76:P78" si="60">_xlfn.CONCAT(O76,".Dig")</f>
+        <v>Machine_IO.Outputs.SPARE_OP9.Dig</v>
+      </c>
+      <c r="Q76" s="20" t="str">
+        <f t="shared" ref="Q76:Q78" si="61">_xlfn.CONCAT(O76,"(); // ",E76)</f>
+        <v>Machine_IO.Outputs.SPARE_OP9(); // CR0403.OP9</v>
+      </c>
+      <c r="R76" s="20" t="str">
+        <f t="shared" ref="R76:R78" si="62">_xlfn.CONCAT(O76,".Init('",A76,"','",L76,"','",D76,"','",G76,"',NVL_Outputs_States_",A76,".All.",D76,",NVL_IO_",A44,".All_Outputs_Diag.",D76,",Machine_IO.Node_",A76,");")</f>
+        <v>Machine_IO.Outputs.SPARE_OP9.Init('AUX','SPARE_OP9','OP9','',NVL_Outputs_States_AUX.All.OP9,NVL_IO_CHASSIS.All_Outputs_Diag.OP9,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S76" s="20" t="str">
+        <f t="shared" ref="S76:S78" si="63">_xlfn.CONCAT(K76,": Mimic_Output_FB; // ",A76,":",D76)</f>
+        <v>: Mimic_Output_FB; // AUX:OP9</v>
+      </c>
+      <c r="T76" s="20" t="str">
+        <f t="shared" ref="T76:T78" si="64">_xlfn.CONCAT(A76,".",D76,"();")</f>
+        <v>AUX.OP9();</v>
+      </c>
+      <c r="U76" s="20" t="str">
+        <f t="shared" ref="U76:U78" si="65">_xlfn.CONCAT(A76,".",D76,".Init(",O76,");")</f>
+        <v>AUX.OP9.Init(Machine_IO.Outputs.SPARE_OP9);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A77" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C77" s="19"/>
+      <c r="D77" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="E77" s="17" t="str">
+        <f t="shared" si="54"/>
+        <v>CR0403.OP10</v>
+      </c>
+      <c r="F77" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="21"/>
+      <c r="J77" s="21" t="str">
+        <f t="shared" si="55"/>
+        <v>AUX.OP10</v>
+      </c>
+      <c r="K77" s="19"/>
+      <c r="L77" s="19" t="str">
+        <f t="shared" si="56"/>
+        <v>SPARE_OP10</v>
+      </c>
+      <c r="M77" s="19" t="str">
+        <f t="shared" si="57"/>
+        <v>:BOOL;</v>
+      </c>
+      <c r="N77" s="20" t="str">
+        <f t="shared" si="58"/>
+        <v>SPARE_OP10:OpCom; // AUX.OP10</v>
+      </c>
+      <c r="O77" s="20" t="str">
+        <f t="shared" si="59"/>
+        <v>Machine_IO.Outputs.SPARE_OP10</v>
+      </c>
+      <c r="P77" s="20" t="str">
+        <f t="shared" si="60"/>
+        <v>Machine_IO.Outputs.SPARE_OP10.Dig</v>
+      </c>
+      <c r="Q77" s="20" t="str">
+        <f t="shared" si="61"/>
+        <v>Machine_IO.Outputs.SPARE_OP10(); // CR0403.OP10</v>
+      </c>
+      <c r="R77" s="20" t="str">
+        <f t="shared" si="62"/>
+        <v>Machine_IO.Outputs.SPARE_OP10.Init('AUX','SPARE_OP10','OP10','',NVL_Outputs_States_AUX.All.OP10,NVL_IO_CHASSIS.All_Outputs_Diag.OP10,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S77" s="20" t="str">
+        <f t="shared" si="63"/>
+        <v>: Mimic_Output_FB; // AUX:OP10</v>
+      </c>
+      <c r="T77" s="20" t="str">
+        <f t="shared" si="64"/>
+        <v>AUX.OP10();</v>
+      </c>
+      <c r="U77" s="20" t="str">
+        <f t="shared" si="65"/>
+        <v>AUX.OP10.Init(Machine_IO.Outputs.SPARE_OP10);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A78" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B78" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C78" s="19"/>
+      <c r="D78" s="17" t="s">
+        <v>622</v>
+      </c>
+      <c r="E78" s="17" t="str">
+        <f t="shared" si="54"/>
+        <v>CR0403.OP11</v>
+      </c>
+      <c r="F78" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G78" s="21"/>
+      <c r="H78" s="21"/>
+      <c r="I78" s="21"/>
+      <c r="J78" s="21" t="str">
+        <f t="shared" si="55"/>
+        <v>AUX.OP11</v>
+      </c>
+      <c r="K78" s="19"/>
+      <c r="L78" s="19" t="str">
+        <f t="shared" si="56"/>
+        <v>SPARE_OP11</v>
+      </c>
+      <c r="M78" s="19" t="str">
+        <f t="shared" si="57"/>
+        <v>:BOOL;</v>
+      </c>
+      <c r="N78" s="20" t="str">
+        <f t="shared" si="58"/>
+        <v>SPARE_OP11:OpCom; // AUX.OP11</v>
+      </c>
+      <c r="O78" s="20" t="str">
+        <f t="shared" si="59"/>
+        <v>Machine_IO.Outputs.SPARE_OP11</v>
+      </c>
+      <c r="P78" s="20" t="str">
+        <f t="shared" si="60"/>
+        <v>Machine_IO.Outputs.SPARE_OP11.Dig</v>
+      </c>
+      <c r="Q78" s="20" t="str">
+        <f t="shared" si="61"/>
+        <v>Machine_IO.Outputs.SPARE_OP11(); // CR0403.OP11</v>
+      </c>
+      <c r="R78" s="20" t="str">
+        <f t="shared" si="62"/>
+        <v>Machine_IO.Outputs.SPARE_OP11.Init('AUX','SPARE_OP11','OP11','',NVL_Outputs_States_AUX.All.OP11,NVL_IO_CHASSIS.All_Outputs_Diag.OP11,Machine_IO.Node_AUX);</v>
+      </c>
+      <c r="S78" s="20" t="str">
+        <f t="shared" si="63"/>
+        <v>: Mimic_Output_FB; // AUX:OP11</v>
+      </c>
+      <c r="T78" s="20" t="str">
+        <f t="shared" si="64"/>
+        <v>AUX.OP11();</v>
+      </c>
+      <c r="U78" s="20" t="str">
+        <f t="shared" si="65"/>
+        <v>AUX.OP11.Init(Machine_IO.Outputs.SPARE_OP11);</v>
       </c>
     </row>
   </sheetData>
@@ -7628,7 +8469,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -7636,12 +8477,12 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D24">
         <v>250</v>
@@ -7649,7 +8490,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -7660,7 +8501,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -7671,7 +8512,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -7682,7 +8523,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -7693,7 +8534,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -7704,7 +8545,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -18855,344 +19696,402 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
-  <dimension ref="B2:E53"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="B1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="67.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>606</v>
+      </c>
+      <c r="C1" t="s">
+        <v>607</v>
+      </c>
+      <c r="D1" t="s">
+        <v>605</v>
+      </c>
+    </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C2" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C4" t="s">
-        <v>584</v>
-      </c>
-    </row>
+        <v>581</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>559</v>
+      </c>
+      <c r="C6" t="s">
         <v>562</v>
       </c>
-      <c r="C6" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C7" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="D7" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C8" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="D8" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C9" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D9" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C10" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D10" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C11" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="D11" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C12" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D12" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C13" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C14" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D14" t="s">
-        <v>598</v>
-      </c>
-    </row>
+        <v>594</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C16" t="s">
-        <v>566</v>
-      </c>
-    </row>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>565</v>
+      </c>
+      <c r="C18" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>566</v>
+      </c>
+      <c r="C20" t="s">
+        <v>557</v>
+      </c>
+      <c r="D20" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>566</v>
+      </c>
+      <c r="C21" t="s">
+        <v>547</v>
+      </c>
+      <c r="D21" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>566</v>
+      </c>
+      <c r="C22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D22" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>567</v>
+      </c>
+      <c r="C24" t="s">
+        <v>558</v>
+      </c>
+      <c r="D24" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>567</v>
+      </c>
+      <c r="C25" t="s">
         <v>568</v>
       </c>
-      <c r="C18" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>569</v>
-      </c>
-      <c r="C20" t="s">
-        <v>560</v>
-      </c>
-      <c r="D20" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>569</v>
-      </c>
-      <c r="C21" t="s">
-        <v>550</v>
-      </c>
-      <c r="D21" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>569</v>
-      </c>
-      <c r="C22" t="s">
-        <v>551</v>
-      </c>
-      <c r="D22" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>570</v>
-      </c>
-      <c r="C24" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>570</v>
-      </c>
-      <c r="C25" t="s">
-        <v>571</v>
-      </c>
-    </row>
+      <c r="D25" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C27" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C28" t="s">
-        <v>553</v>
-      </c>
-    </row>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C30" t="s">
-        <v>573</v>
-      </c>
-    </row>
+        <v>570</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C32" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C33" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>571</v>
+      </c>
+      <c r="C34" t="s">
         <v>574</v>
       </c>
-      <c r="C34" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C37" t="s">
-        <v>586</v>
-      </c>
-    </row>
+        <v>583</v>
+      </c>
+      <c r="D37" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C40" t="s">
-        <v>588</v>
-      </c>
-    </row>
+        <v>585</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C42" t="s">
-        <v>600</v>
-      </c>
-    </row>
+        <v>596</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C44" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="C45" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>591</v>
+      </c>
+      <c r="C46" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>592</v>
+      </c>
+      <c r="C48" t="s">
+        <v>593</v>
+      </c>
+      <c r="D48" t="s">
         <v>594</v>
       </c>
-      <c r="C46" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>595</v>
-      </c>
-      <c r="C48" t="s">
-        <v>596</v>
-      </c>
-      <c r="D48" t="s">
-        <v>597</v>
-      </c>
-    </row>
+    </row>
+    <row r="49" spans="2:5" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C50" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="E50" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C51" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="E51" t="s">
-        <v>605</v>
-      </c>
-    </row>
+        <v>601</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C53" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:E53" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -19208,15 +20107,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19443,6 +20333,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -19455,14 +20353,6 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
HMI - viz snags fix fo rhe plc info
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA445A5-747E-451D-A730-AD803DF1D9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF27BBAB-A99B-481F-9D0E-77F6FD82181D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="629">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1930,6 +1930,9 @@
   </si>
   <si>
     <t>SIDE_CONV_LOWER</t>
+  </si>
+  <si>
+    <t>CR0403 8 outputs</t>
   </si>
 </sst>
 </file>
@@ -2494,7 +2497,7 @@
   </sheetPr>
   <dimension ref="A1:U78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K70" sqref="K70"/>
     </sheetView>
@@ -19699,14 +19702,14 @@
   <sheetPr filterMode="1"/>
   <dimension ref="B1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" customWidth="1"/>
+    <col min="3" max="3" width="71.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
   </cols>
@@ -19821,12 +19824,15 @@
         <v>594</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>559</v>
       </c>
       <c r="C13" t="s">
         <v>563</v>
+      </c>
+      <c r="D13" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="14" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -19841,21 +19847,27 @@
       </c>
     </row>
     <row r="15" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>564</v>
       </c>
       <c r="C16" t="s">
-        <v>563</v>
+        <v>628</v>
+      </c>
+      <c r="D16" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="17" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>565</v>
       </c>
       <c r="C18" t="s">
         <v>546</v>
+      </c>
+      <c r="D18" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="19" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
@@ -20036,35 +20048,44 @@
       </c>
     </row>
     <row r="49" spans="2:5" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>598</v>
       </c>
       <c r="C50" t="s">
         <v>599</v>
       </c>
+      <c r="D50" t="s">
+        <v>594</v>
+      </c>
       <c r="E50" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>598</v>
       </c>
       <c r="C51" t="s">
         <v>600</v>
       </c>
+      <c r="D51" t="s">
+        <v>594</v>
+      </c>
       <c r="E51" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="52" spans="2:5" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>602</v>
       </c>
       <c r="C53" t="s">
         <v>603</v>
+      </c>
+      <c r="D53" t="s">
+        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -20083,15 +20104,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -20107,6 +20119,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20333,14 +20354,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -20353,6 +20366,14 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
WIP - tracking and sim fixups
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF27BBAB-A99B-481F-9D0E-77F6FD82181D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88580305-ED33-4CB7-B259-BB69784F133D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$71</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SNAGS!$B$1:$E$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SNAGS!$B$1:$E$54</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2041" uniqueCount="631">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1933,6 +1933,12 @@
   </si>
   <si>
     <t>CR0403 8 outputs</t>
+  </si>
+  <si>
+    <t>check for disconencted valves?</t>
+  </si>
+  <si>
+    <t>Check direction buttons not active during presiren</t>
   </si>
 </sst>
 </file>
@@ -19700,10 +19706,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="B1:E53"/>
+  <dimension ref="B1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19749,24 +19755,28 @@
         <v>581</v>
       </c>
     </row>
-    <row r="5" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>576</v>
+      </c>
+      <c r="C5" t="s">
+        <v>629</v>
+      </c>
+    </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>559</v>
+        <v>576</v>
       </c>
       <c r="C6" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>559</v>
       </c>
       <c r="C7" t="s">
-        <v>544</v>
-      </c>
-      <c r="D7" t="s">
-        <v>594</v>
+        <v>562</v>
       </c>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -19774,7 +19784,7 @@
         <v>559</v>
       </c>
       <c r="C8" t="s">
-        <v>580</v>
+        <v>544</v>
       </c>
       <c r="D8" t="s">
         <v>594</v>
@@ -19785,7 +19795,7 @@
         <v>559</v>
       </c>
       <c r="C9" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D9" t="s">
         <v>594</v>
@@ -19796,7 +19806,7 @@
         <v>559</v>
       </c>
       <c r="C10" t="s">
-        <v>545</v>
+        <v>579</v>
       </c>
       <c r="D10" t="s">
         <v>594</v>
@@ -19807,7 +19817,7 @@
         <v>559</v>
       </c>
       <c r="C11" t="s">
-        <v>560</v>
+        <v>545</v>
       </c>
       <c r="D11" t="s">
         <v>594</v>
@@ -19818,7 +19828,7 @@
         <v>559</v>
       </c>
       <c r="C12" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D12" t="s">
         <v>594</v>
@@ -19829,10 +19839,10 @@
         <v>559</v>
       </c>
       <c r="C13" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D13" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="14" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -19840,45 +19850,42 @@
         <v>559</v>
       </c>
       <c r="C14" t="s">
+        <v>563</v>
+      </c>
+      <c r="D14" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>559</v>
+      </c>
+      <c r="C15" t="s">
         <v>586</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="15" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="17" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>564</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>628</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="17" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="19" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>565</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>546</v>
       </c>
-      <c r="D18" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>566</v>
-      </c>
-      <c r="C20" t="s">
-        <v>557</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="D19" t="s">
         <v>594</v>
       </c>
     </row>
@@ -19887,7 +19894,7 @@
         <v>566</v>
       </c>
       <c r="C21" t="s">
-        <v>547</v>
+        <v>557</v>
       </c>
       <c r="D21" t="s">
         <v>594</v>
@@ -19898,21 +19905,20 @@
         <v>566</v>
       </c>
       <c r="C22" t="s">
+        <v>547</v>
+      </c>
+      <c r="D22" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>566</v>
+      </c>
+      <c r="C23" t="s">
         <v>548</v>
       </c>
-      <c r="D22" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>567</v>
-      </c>
-      <c r="C24" t="s">
-        <v>558</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="D23" t="s">
         <v>595</v>
       </c>
     </row>
@@ -19921,19 +19927,21 @@
         <v>567</v>
       </c>
       <c r="C25" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="D25" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="26" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>575</v>
-      </c>
-      <c r="C27" t="s">
-        <v>549</v>
+    <row r="26" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>567</v>
+      </c>
+      <c r="C26" t="s">
+        <v>568</v>
+      </c>
+      <c r="D26" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -19941,25 +19949,23 @@
         <v>575</v>
       </c>
       <c r="C28" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>575</v>
+      </c>
+      <c r="C29" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="29" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>569</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>570</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>571</v>
-      </c>
-      <c r="C32" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -19967,7 +19973,7 @@
         <v>571</v>
       </c>
       <c r="C33" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -19975,91 +19981,77 @@
         <v>571</v>
       </c>
       <c r="C34" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>571</v>
+      </c>
+      <c r="C35" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="35" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="38" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>582</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>583</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="38" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>584</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>587</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>596</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>576</v>
-      </c>
-      <c r="C44" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="C45" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>589</v>
+      </c>
+      <c r="C46" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>591</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="47" spans="2:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="49" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>592</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>593</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>594</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>598</v>
-      </c>
-      <c r="C50" t="s">
-        <v>599</v>
-      </c>
-      <c r="D50" t="s">
-        <v>594</v>
-      </c>
-      <c r="E50" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="51" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
@@ -20067,7 +20059,7 @@
         <v>598</v>
       </c>
       <c r="C51" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D51" t="s">
         <v>594</v>
@@ -20076,25 +20068,33 @@
         <v>601</v>
       </c>
     </row>
-    <row r="52" spans="2:5" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="52" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>598</v>
+      </c>
+      <c r="C52" t="s">
+        <v>600</v>
+      </c>
+      <c r="D52" t="s">
+        <v>594</v>
+      </c>
+      <c r="E52" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>602</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>603</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>594</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:E53" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
-    <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
+  <autoFilter ref="B1:E54" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>
@@ -20104,6 +20104,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -20119,15 +20128,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20354,6 +20354,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -20366,14 +20374,6 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
WIP - PLC AUX - fix missing RX200 issues
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88580305-ED33-4CB7-B259-BB69784F133D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C46CC1-A6C7-4E47-911C-DDA747F70976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2041" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="636">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1782,18 +1782,12 @@
     <t>Umbilical Stop - does it do much? Is it the estop feedback from teleradio?</t>
   </si>
   <si>
-    <t>Interlock in PLC with the Siren?</t>
-  </si>
-  <si>
     <t>Fuel Sender - scale for diagnostics</t>
   </si>
   <si>
     <t>Drum Pressure - scale</t>
   </si>
   <si>
-    <t>Check for stuck signals on power up (directions / req / stop)</t>
-  </si>
-  <si>
     <t>PINCODE</t>
   </si>
   <si>
@@ -1938,7 +1932,28 @@
     <t>check for disconencted valves?</t>
   </si>
   <si>
-    <t>Check direction buttons not active during presiren</t>
+    <t>Check HMI offline during tracking</t>
+  </si>
+  <si>
+    <t>not possible on the remote - cannot see the buttons!</t>
+  </si>
+  <si>
+    <t>HANDSET Check for stuck signals on power up (directions / req / stop)</t>
+  </si>
+  <si>
+    <t>RADIO Check direction buttons not active during presiren</t>
+  </si>
+  <si>
+    <t>Interlock in PLC with the Siren Output?</t>
+  </si>
+  <si>
+    <t>PLC_OUTPUTS</t>
+  </si>
+  <si>
+    <t>IF no coms or estop - ECU is disabled - is this enough?</t>
+  </si>
+  <si>
+    <t>critical signal was not working due to the ECUDISABLE inversion</t>
   </si>
 </sst>
 </file>
@@ -2783,7 +2798,7 @@
         <v>CHASSIS.IN0102</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="L4" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7534,14 +7549,14 @@
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="17" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E67" s="17" t="str">
         <f t="shared" ref="E67:E74" si="20">_xlfn.CONCAT(B67,".",D67)</f>
@@ -7558,7 +7573,7 @@
         <v>AUX.OP0</v>
       </c>
       <c r="K67" s="19" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L67" s="19" t="str">
         <f t="shared" ref="L67" si="22">IF(K67&lt;&gt;"",UPPER(K67),_xlfn.CONCAT("SPARE_",D67))</f>
@@ -7603,14 +7618,14 @@
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C68" s="19"/>
       <c r="D68" s="17" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E68" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7670,14 +7685,14 @@
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="17" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E69" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7737,14 +7752,14 @@
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="17" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="E70" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7761,7 +7776,7 @@
         <v>AUX.OP3</v>
       </c>
       <c r="K70" s="19" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="L70" s="19" t="str">
         <f t="shared" si="33"/>
@@ -7806,14 +7821,14 @@
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="17" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E71" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7830,7 +7845,7 @@
         <v>AUX.OP4</v>
       </c>
       <c r="K71" s="19" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="L71" s="19" t="str">
         <f t="shared" si="33"/>
@@ -7875,14 +7890,14 @@
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C72" s="19"/>
       <c r="D72" s="17" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E72" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7899,7 +7914,7 @@
         <v>AUX.OP5</v>
       </c>
       <c r="K72" s="19" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="L72" s="19" t="str">
         <f t="shared" ref="L72:L75" si="44">IF(K72&lt;&gt;"",UPPER(K72),_xlfn.CONCAT("SPARE_",D72))</f>
@@ -7944,14 +7959,14 @@
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C73" s="19"/>
       <c r="D73" s="17" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="E73" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7968,7 +7983,7 @@
         <v>AUX.OP6</v>
       </c>
       <c r="K73" s="19" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="L73" s="19" t="str">
         <f t="shared" si="44"/>
@@ -8013,14 +8028,14 @@
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C74" s="19"/>
       <c r="D74" s="17" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E74" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8037,7 +8052,7 @@
         <v>AUX.OP7</v>
       </c>
       <c r="K74" s="19" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="L74" s="19" t="str">
         <f t="shared" si="44"/>
@@ -8082,14 +8097,14 @@
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C75" s="19"/>
       <c r="D75" s="17" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E75" s="17" t="str">
         <f t="shared" ref="E75:E78" si="54">_xlfn.CONCAT(B75,".",D75)</f>
@@ -8149,14 +8164,14 @@
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C76" s="19"/>
       <c r="D76" s="17" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E76" s="17" t="str">
         <f t="shared" si="54"/>
@@ -8216,14 +8231,14 @@
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C77" s="19"/>
       <c r="D77" s="17" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E77" s="17" t="str">
         <f t="shared" si="54"/>
@@ -8283,14 +8298,14 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C78" s="19"/>
       <c r="D78" s="17" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E78" s="17" t="str">
         <f t="shared" si="54"/>
@@ -19706,10 +19721,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="B1:E54"/>
+  <dimension ref="B1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19717,21 +19732,21 @@
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="71.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D1" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>576</v>
       </c>
@@ -19739,39 +19754,45 @@
         <v>577</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>576</v>
       </c>
       <c r="C3" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>576</v>
       </c>
       <c r="C4" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+        <v>630</v>
+      </c>
+      <c r="E4" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>576</v>
       </c>
       <c r="C5" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>576</v>
       </c>
       <c r="C6" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+        <v>631</v>
+      </c>
+      <c r="E6" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>559</v>
       </c>
@@ -19779,7 +19800,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>559</v>
       </c>
@@ -19787,32 +19808,32 @@
         <v>544</v>
       </c>
       <c r="D8" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>559</v>
       </c>
       <c r="C9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D9" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>559</v>
       </c>
       <c r="C10" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D10" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>559</v>
       </c>
@@ -19820,10 +19841,10 @@
         <v>545</v>
       </c>
       <c r="D11" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>559</v>
       </c>
@@ -19831,10 +19852,10 @@
         <v>560</v>
       </c>
       <c r="D12" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>559</v>
       </c>
@@ -19842,10 +19863,10 @@
         <v>561</v>
       </c>
       <c r="D13" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>559</v>
       </c>
@@ -19853,18 +19874,18 @@
         <v>563</v>
       </c>
       <c r="D14" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>559</v>
       </c>
       <c r="C15" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D15" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="17" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -19872,10 +19893,18 @@
         <v>564</v>
       </c>
       <c r="C17" t="s">
+        <v>626</v>
+      </c>
+      <c r="D17" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>576</v>
+      </c>
+      <c r="C18" t="s">
         <v>628</v>
-      </c>
-      <c r="D17" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="19" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -19886,7 +19915,7 @@
         <v>546</v>
       </c>
       <c r="D19" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="21" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -19897,7 +19926,7 @@
         <v>557</v>
       </c>
       <c r="D21" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="22" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -19908,7 +19937,7 @@
         <v>547</v>
       </c>
       <c r="D22" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="23" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -19919,7 +19948,7 @@
         <v>548</v>
       </c>
       <c r="D23" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="25" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -19930,7 +19959,7 @@
         <v>558</v>
       </c>
       <c r="D25" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="26" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
@@ -19941,7 +19970,7 @@
         <v>568</v>
       </c>
       <c r="D26" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -19968,7 +19997,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>571</v>
       </c>
@@ -19976,7 +20005,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>571</v>
       </c>
@@ -19984,7 +20013,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>571</v>
       </c>
@@ -19992,105 +20021,116 @@
         <v>574</v>
       </c>
     </row>
-    <row r="38" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>580</v>
+      </c>
+      <c r="C38" t="s">
+        <v>581</v>
+      </c>
+      <c r="D38" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>582</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>583</v>
       </c>
-      <c r="D38" t="s">
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>585</v>
+      </c>
+      <c r="C43" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>584</v>
-      </c>
-      <c r="C41" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>587</v>
-      </c>
-      <c r="C43" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>576</v>
       </c>
       <c r="C45" t="s">
+        <v>586</v>
+      </c>
+      <c r="E45" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>587</v>
+      </c>
+      <c r="C46" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>589</v>
+      </c>
+      <c r="C47" t="s">
         <v>588</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>589</v>
-      </c>
-      <c r="C46" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>591</v>
-      </c>
-      <c r="C47" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="49" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>590</v>
+      </c>
+      <c r="C49" t="s">
+        <v>591</v>
+      </c>
+      <c r="D49" t="s">
         <v>592</v>
-      </c>
-      <c r="C49" t="s">
-        <v>593</v>
-      </c>
-      <c r="D49" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="51" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C51" t="s">
+        <v>597</v>
+      </c>
+      <c r="D51" t="s">
+        <v>592</v>
+      </c>
+      <c r="E51" t="s">
         <v>599</v>
-      </c>
-      <c r="D51" t="s">
-        <v>594</v>
-      </c>
-      <c r="E51" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="52" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>596</v>
+      </c>
+      <c r="C52" t="s">
         <v>598</v>
       </c>
-      <c r="C52" t="s">
-        <v>600</v>
-      </c>
       <c r="D52" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E52" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="54" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C54" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D54" t="s">
-        <v>594</v>
+        <v>592</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>633</v>
+      </c>
+      <c r="C55" t="s">
+        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -20104,15 +20144,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -20128,6 +20159,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20354,14 +20394,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -20374,6 +20406,14 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
WIP - fixed up drum pressure settings and added some snags, ready to try tracking next
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C46CC1-A6C7-4E47-911C-DDA747F70976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6359DCF-13E5-4764-8FD0-1DED57449005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$71</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SNAGS!$B$1:$E$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SNAGS!$A$1:$E$48</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="659">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1830,9 +1830,6 @@
     <t>SKIP</t>
   </si>
   <si>
-    <t>indication that setup mode is on / starting</t>
-  </si>
-  <si>
     <t>very slow interlock on jacks/side - long delay?</t>
   </si>
   <si>
@@ -1954,13 +1951,85 @@
   </si>
   <si>
     <t>critical signal was not working due to the ECUDISABLE inversion</t>
+  </si>
+  <si>
+    <t>Network Page needs more info!</t>
+  </si>
+  <si>
+    <t>AUX_PLC</t>
+  </si>
+  <si>
+    <t>Really a CR0401 - don't see any message to say it is on line like RX200..</t>
+  </si>
+  <si>
+    <t>see if we can get software of conrad to can check if connected</t>
+  </si>
+  <si>
+    <t>RTC</t>
+  </si>
+  <si>
+    <t>USA date format option</t>
+  </si>
+  <si>
+    <t>Settings_2 - can only edit the top row</t>
+  </si>
+  <si>
+    <t>login in as tech - on first settings page</t>
+  </si>
+  <si>
+    <t>review these settings</t>
+  </si>
+  <si>
+    <t>indication that setup mode is on / starting in the footer</t>
+  </si>
+  <si>
+    <t>Symbol on the footer for PreSiren and Active Tracks</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>ESTOP</t>
+  </si>
+  <si>
+    <t>SECUIRTY</t>
+  </si>
+  <si>
+    <t>Hide the Entered PIN code!</t>
+  </si>
+  <si>
+    <t>Settings_3 - can only edit the top row</t>
+  </si>
+  <si>
+    <t>FAN</t>
+  </si>
+  <si>
+    <t>FAN control needs checked</t>
+  </si>
+  <si>
+    <t>FAN control</t>
+  </si>
+  <si>
+    <t>check the pressure sensor scaling!</t>
+  </si>
+  <si>
+    <t>Max pressure setting for the Drum - needs to be a persistant?</t>
+  </si>
+  <si>
+    <t>DRUM</t>
+  </si>
+  <si>
+    <t>Min reset drum pressure sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min Gaps between the settings for drum pressure </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2076,6 +2145,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2112,7 +2195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2192,6 +2275,8 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2798,7 +2883,7 @@
         <v>CHASSIS.IN0102</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="L4" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7549,14 +7634,14 @@
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B67" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="17" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E67" s="17" t="str">
         <f t="shared" ref="E67:E74" si="20">_xlfn.CONCAT(B67,".",D67)</f>
@@ -7573,7 +7658,7 @@
         <v>AUX.OP0</v>
       </c>
       <c r="K67" s="19" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="L67" s="19" t="str">
         <f t="shared" ref="L67" si="22">IF(K67&lt;&gt;"",UPPER(K67),_xlfn.CONCAT("SPARE_",D67))</f>
@@ -7618,14 +7703,14 @@
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B68" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C68" s="19"/>
       <c r="D68" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E68" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7685,14 +7770,14 @@
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B69" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E69" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7752,14 +7837,14 @@
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B70" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E70" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7776,7 +7861,7 @@
         <v>AUX.OP3</v>
       </c>
       <c r="K70" s="19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="L70" s="19" t="str">
         <f t="shared" si="33"/>
@@ -7821,14 +7906,14 @@
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B71" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E71" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7845,7 +7930,7 @@
         <v>AUX.OP4</v>
       </c>
       <c r="K71" s="19" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="L71" s="19" t="str">
         <f t="shared" si="33"/>
@@ -7890,14 +7975,14 @@
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B72" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C72" s="19"/>
       <c r="D72" s="17" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E72" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7914,7 +7999,7 @@
         <v>AUX.OP5</v>
       </c>
       <c r="K72" s="19" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="L72" s="19" t="str">
         <f t="shared" ref="L72:L75" si="44">IF(K72&lt;&gt;"",UPPER(K72),_xlfn.CONCAT("SPARE_",D72))</f>
@@ -7959,14 +8044,14 @@
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B73" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C73" s="19"/>
       <c r="D73" s="17" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E73" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7983,7 +8068,7 @@
         <v>AUX.OP6</v>
       </c>
       <c r="K73" s="19" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="L73" s="19" t="str">
         <f t="shared" si="44"/>
@@ -8028,14 +8113,14 @@
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B74" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C74" s="19"/>
       <c r="D74" s="17" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E74" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8052,7 +8137,7 @@
         <v>AUX.OP7</v>
       </c>
       <c r="K74" s="19" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="L74" s="19" t="str">
         <f t="shared" si="44"/>
@@ -8097,14 +8182,14 @@
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B75" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C75" s="19"/>
       <c r="D75" s="17" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E75" s="17" t="str">
         <f t="shared" ref="E75:E78" si="54">_xlfn.CONCAT(B75,".",D75)</f>
@@ -8164,14 +8249,14 @@
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B76" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C76" s="19"/>
       <c r="D76" s="17" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E76" s="17" t="str">
         <f t="shared" si="54"/>
@@ -8231,14 +8316,14 @@
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B77" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C77" s="19"/>
       <c r="D77" s="17" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E77" s="17" t="str">
         <f t="shared" si="54"/>
@@ -8298,14 +8383,14 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B78" s="17" t="s">
         <v>606</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>607</v>
       </c>
       <c r="C78" s="19"/>
       <c r="D78" s="17" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E78" s="17" t="str">
         <f t="shared" si="54"/>
@@ -19721,10 +19806,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="B1:E55"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19735,18 +19820,24 @@
     <col min="5" max="5" width="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" s="34" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="34" t="s">
+        <v>603</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>604</v>
       </c>
-      <c r="C1" t="s">
-        <v>605</v>
-      </c>
-      <c r="D1" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="34" t="s">
+        <v>602</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>576</v>
       </c>
@@ -19754,53 +19845,71 @@
         <v>577</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>576</v>
       </c>
       <c r="C3" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>576</v>
       </c>
       <c r="C4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E4" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>576</v>
       </c>
       <c r="C5" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>576</v>
       </c>
       <c r="C6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E6" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>559</v>
-      </c>
-      <c r="C7" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>647</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="8" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>559</v>
       </c>
@@ -19811,7 +19920,10 @@
         <v>592</v>
       </c>
     </row>
-    <row r="9" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>559</v>
       </c>
@@ -19822,7 +19934,10 @@
         <v>592</v>
       </c>
     </row>
-    <row r="10" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>559</v>
       </c>
@@ -19833,7 +19948,10 @@
         <v>592</v>
       </c>
     </row>
-    <row r="11" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>559</v>
       </c>
@@ -19844,7 +19962,10 @@
         <v>592</v>
       </c>
     </row>
-    <row r="12" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
         <v>559</v>
       </c>
@@ -19855,7 +19976,10 @@
         <v>592</v>
       </c>
     </row>
-    <row r="13" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>559</v>
       </c>
@@ -19866,7 +19990,10 @@
         <v>592</v>
       </c>
     </row>
-    <row r="14" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>559</v>
       </c>
@@ -19877,7 +20004,10 @@
         <v>593</v>
       </c>
     </row>
-    <row r="15" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>559</v>
       </c>
@@ -19888,254 +20018,489 @@
         <v>592</v>
       </c>
     </row>
-    <row r="17" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>564</v>
       </c>
-      <c r="C17" t="s">
-        <v>626</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C16" t="s">
+        <v>625</v>
+      </c>
+      <c r="D16" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>576</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
       <c r="B18" t="s">
+        <v>565</v>
+      </c>
+      <c r="C18" t="s">
+        <v>546</v>
+      </c>
+      <c r="D18" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>576</v>
       </c>
-      <c r="C18" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>565</v>
-      </c>
       <c r="C19" t="s">
-        <v>546</v>
-      </c>
-      <c r="D19" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>566</v>
+      </c>
+      <c r="C20" t="s">
+        <v>557</v>
+      </c>
+      <c r="D20" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="21" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
       <c r="B21" t="s">
         <v>566</v>
       </c>
       <c r="C21" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
       <c r="D21" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="22" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
       <c r="B22" t="s">
         <v>566</v>
       </c>
       <c r="C22" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D22" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
       <c r="B23" t="s">
-        <v>566</v>
+        <v>576</v>
       </c>
       <c r="C23" t="s">
-        <v>548</v>
-      </c>
-      <c r="D23" t="s">
+        <v>586</v>
+      </c>
+      <c r="E23" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>567</v>
+      </c>
+      <c r="C24" t="s">
+        <v>558</v>
+      </c>
+      <c r="D24" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="25" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
       <c r="B25" t="s">
         <v>567</v>
       </c>
       <c r="C25" t="s">
-        <v>558</v>
+        <v>568</v>
       </c>
       <c r="D25" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="26" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
       <c r="B26" t="s">
-        <v>567</v>
+        <v>575</v>
       </c>
       <c r="C26" t="s">
-        <v>568</v>
-      </c>
-      <c r="D26" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>575</v>
+      </c>
+      <c r="C27" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
       <c r="B28" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="C28" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+        <v>570</v>
+      </c>
+      <c r="D28" t="s">
+        <v>592</v>
+      </c>
+      <c r="E28" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
       <c r="B29" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C29" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>571</v>
+      </c>
+      <c r="C30" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
       <c r="B31" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C31" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>571</v>
-      </c>
-      <c r="C33" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>580</v>
+      </c>
+      <c r="C32" t="s">
+        <v>581</v>
+      </c>
+      <c r="D32" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>582</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>583</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
       <c r="B34" t="s">
-        <v>571</v>
+        <v>585</v>
       </c>
       <c r="C34" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
       <c r="B35" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="C35" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>586</v>
+      </c>
+      <c r="E35" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>587</v>
+      </c>
+      <c r="C36" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>589</v>
+      </c>
+      <c r="C37" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
       <c r="B38" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="C38" t="s">
-        <v>581</v>
+        <v>591</v>
       </c>
       <c r="D38" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>595</v>
+      </c>
+      <c r="C39" t="s">
+        <v>596</v>
+      </c>
+      <c r="D39" t="s">
+        <v>592</v>
+      </c>
+      <c r="E39" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>595</v>
+      </c>
+      <c r="C40" t="s">
+        <v>597</v>
+      </c>
+      <c r="D40" t="s">
+        <v>592</v>
+      </c>
+      <c r="E40" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
       <c r="B41" t="s">
-        <v>582</v>
+        <v>599</v>
       </c>
       <c r="C41" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+      <c r="D41" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>632</v>
+      </c>
+      <c r="C42" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
       <c r="B43" t="s">
-        <v>585</v>
+        <v>599</v>
       </c>
       <c r="C43" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>569</v>
+      </c>
+      <c r="C44" t="s">
+        <v>641</v>
+      </c>
+      <c r="D44" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
       <c r="B45" t="s">
-        <v>576</v>
+        <v>636</v>
       </c>
       <c r="C45" t="s">
-        <v>586</v>
+        <v>637</v>
       </c>
       <c r="E45" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
       <c r="B46" t="s">
-        <v>587</v>
+        <v>639</v>
       </c>
       <c r="C46" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
       <c r="B47" t="s">
-        <v>589</v>
+        <v>648</v>
       </c>
       <c r="C47" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>569</v>
+      </c>
+      <c r="C48" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
       <c r="B49" t="s">
-        <v>590</v>
+        <v>651</v>
       </c>
       <c r="C49" t="s">
-        <v>591</v>
-      </c>
-      <c r="D49" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>569</v>
+      </c>
+      <c r="C50" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>596</v>
+        <v>656</v>
       </c>
       <c r="C51" t="s">
-        <v>597</v>
-      </c>
-      <c r="D51" t="s">
-        <v>592</v>
-      </c>
-      <c r="E51" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>596</v>
+        <v>656</v>
       </c>
       <c r="C52" t="s">
-        <v>598</v>
-      </c>
-      <c r="D52" t="s">
-        <v>592</v>
-      </c>
-      <c r="E52" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>656</v>
+      </c>
+      <c r="C53" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>600</v>
+        <v>656</v>
       </c>
       <c r="C54" t="s">
-        <v>601</v>
-      </c>
-      <c r="D54" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>633</v>
-      </c>
-      <c r="C55" t="s">
-        <v>634</v>
+        <v>658</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:E54" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
-    <filterColumn colId="2">
+  <autoFilter ref="A1:E48" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
+    <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
HMI - IN0102 labels added, Sim Thermostat for the fan control, Pressure sensor changed to 3625 psi (was 2500?), Tracking from handset and extra radio functions working
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6359DCF-13E5-4764-8FD0-1DED57449005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CCFAAB-62A2-4D9A-97F7-0BBA00FFBA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$71</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SNAGS!$A$1:$E$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SNAGS!$A$1:$E$58</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2107" uniqueCount="672">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2007,9 +2007,6 @@
     <t>FAN control needs checked</t>
   </si>
   <si>
-    <t>FAN control</t>
-  </si>
-  <si>
     <t>check the pressure sensor scaling!</t>
   </si>
   <si>
@@ -2019,10 +2016,52 @@
     <t>DRUM</t>
   </si>
   <si>
-    <t>Min reset drum pressure sensor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Min Gaps between the settings for drum pressure </t>
+  </si>
+  <si>
+    <t>header symbol invert - visible when active</t>
+  </si>
+  <si>
+    <t>Flash Header Symbol if it Blipped</t>
+  </si>
+  <si>
+    <t>FUTURE</t>
+  </si>
+  <si>
+    <t>Text for Now - does it really need a tracking Page?</t>
+  </si>
+  <si>
+    <t>FAN control - needs settings?</t>
+  </si>
+  <si>
+    <t>Min reset drum pressure sensor value to be hard coded</t>
+  </si>
+  <si>
+    <t>Button LED's!</t>
+  </si>
+  <si>
+    <t>IN0102 needs Text in the list for HMI!</t>
+  </si>
+  <si>
+    <t>DIAG</t>
+  </si>
+  <si>
+    <t>KEYPAD</t>
+  </si>
+  <si>
+    <t>is all in psi - needs checked! (250bar / 3625psi)</t>
+  </si>
+  <si>
+    <t>Auto Shutdown - slows engine down first?</t>
+  </si>
+  <si>
+    <t>Auto Start - ramps engine at the end????</t>
+  </si>
+  <si>
+    <t>ask mark - material on conveyor - moves very slow!</t>
+  </si>
+  <si>
+    <t>APP</t>
   </si>
 </sst>
 </file>
@@ -2604,8 +2643,8 @@
   <dimension ref="A1:U78"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K70" sqref="K70"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -19806,10 +19845,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19845,7 +19884,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -19854,6 +19893,9 @@
       </c>
       <c r="C3" t="s">
         <v>631</v>
+      </c>
+      <c r="D3" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -19866,11 +19908,8 @@
       <c r="C4" t="s">
         <v>629</v>
       </c>
-      <c r="E4" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -19880,8 +19919,11 @@
       <c r="C5" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -19890,6 +19932,9 @@
       </c>
       <c r="C6" t="s">
         <v>630</v>
+      </c>
+      <c r="D6" t="s">
+        <v>659</v>
       </c>
       <c r="E6" t="s">
         <v>628</v>
@@ -20067,6 +20112,9 @@
       <c r="C19" t="s">
         <v>645</v>
       </c>
+      <c r="E19" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -20110,7 +20158,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -20119,6 +20167,9 @@
       </c>
       <c r="C23" t="s">
         <v>586</v>
+      </c>
+      <c r="D23" t="s">
+        <v>592</v>
       </c>
       <c r="E23" t="s">
         <v>634</v>
@@ -20263,7 +20314,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -20272,6 +20323,9 @@
       </c>
       <c r="C35" t="s">
         <v>586</v>
+      </c>
+      <c r="D35" t="s">
+        <v>592</v>
       </c>
       <c r="E35" t="s">
         <v>634</v>
@@ -20288,7 +20342,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -20297,6 +20351,9 @@
       </c>
       <c r="C37" t="s">
         <v>588</v>
+      </c>
+      <c r="D37" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -20397,7 +20454,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -20406,6 +20463,9 @@
       </c>
       <c r="C45" t="s">
         <v>637</v>
+      </c>
+      <c r="D45" t="s">
+        <v>659</v>
       </c>
       <c r="E45" t="s">
         <v>638</v>
@@ -20433,7 +20493,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -20443,8 +20503,11 @@
       <c r="C48" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
@@ -20454,8 +20517,11 @@
       <c r="C49" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
@@ -20463,43 +20529,101 @@
         <v>569</v>
       </c>
       <c r="C50" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>655</v>
+      </c>
+      <c r="C51" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="33" t="s">
+        <v>655</v>
+      </c>
+      <c r="C52" s="33" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="D52" s="33"/>
+      <c r="E52" s="33" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>655</v>
+      </c>
+      <c r="C53" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>655</v>
+      </c>
+      <c r="C54" t="s">
         <v>656</v>
       </c>
-      <c r="C51" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>656</v>
-      </c>
-      <c r="C52" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>656</v>
-      </c>
-      <c r="C53" t="s">
+    </row>
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>647</v>
+      </c>
+      <c r="C55" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>656</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="D55" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>647</v>
+      </c>
+      <c r="C56" t="s">
         <v>658</v>
       </c>
     </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>666</v>
+      </c>
+      <c r="C57" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>665</v>
+      </c>
+      <c r="C58" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>671</v>
+      </c>
+      <c r="C59" t="s">
+        <v>668</v>
+      </c>
+      <c r="E59" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>671</v>
+      </c>
+      <c r="C60" t="s">
+        <v>669</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E48" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
+  <autoFilter ref="A1:E58" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
@@ -20509,6 +20633,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -20524,15 +20657,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20759,6 +20883,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -20771,14 +20903,6 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
HMI Settings - fixup the settings page issue - table to list
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CCFAAB-62A2-4D9A-97F7-0BBA00FFBA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E6E6FD-0516-451D-9AE8-98820AA3E5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2107" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2118" uniqueCount="680">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2062,6 +2062,30 @@
   </si>
   <si>
     <t>APP</t>
+  </si>
+  <si>
+    <t>Numeric Key Pad - Max text clipping the max value</t>
+  </si>
+  <si>
+    <t>SSETTINGS_1</t>
+  </si>
+  <si>
+    <t>Name in the Dialog box mising for each edit</t>
+  </si>
+  <si>
+    <t>way to backup the factory settings</t>
+  </si>
+  <si>
+    <t>ENGINE</t>
+  </si>
+  <si>
+    <t>Regen Check</t>
+  </si>
+  <si>
+    <t>check the old code?</t>
+  </si>
+  <si>
+    <t>DM1 Clear function</t>
   </si>
 </sst>
 </file>
@@ -19845,10 +19869,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20620,6 +20644,49 @@
       </c>
       <c r="C60" t="s">
         <v>669</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>599</v>
+      </c>
+      <c r="C61" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>673</v>
+      </c>
+      <c r="C62" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>569</v>
+      </c>
+      <c r="C63" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>676</v>
+      </c>
+      <c r="C64" t="s">
+        <v>677</v>
+      </c>
+      <c r="E64" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>676</v>
+      </c>
+      <c r="C65" t="s">
+        <v>679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip - pwm feedback on settings page
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E6E6FD-0516-451D-9AE8-98820AA3E5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70B14BC-9BCD-46B8-B909-3B1C8B0ACD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$71</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SNAGS!$A$1:$E$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SNAGS!$A$1:$E$66</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2118" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="688">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1770,9 +1770,6 @@
     <t>side conveyor graphic not good</t>
   </si>
   <si>
-    <t>feedback of the mA for each function on the main screen</t>
-  </si>
-  <si>
     <t>MACHINE_APP</t>
   </si>
   <si>
@@ -2067,9 +2064,6 @@
     <t>Numeric Key Pad - Max text clipping the max value</t>
   </si>
   <si>
-    <t>SSETTINGS_1</t>
-  </si>
-  <si>
     <t>Name in the Dialog box mising for each edit</t>
   </si>
   <si>
@@ -2079,13 +2073,43 @@
     <t>ENGINE</t>
   </si>
   <si>
-    <t>Regen Check</t>
-  </si>
-  <si>
     <t>check the old code?</t>
   </si>
   <si>
     <t>DM1 Clear function</t>
+  </si>
+  <si>
+    <t>SETTINGS_1</t>
+  </si>
+  <si>
+    <t>Regen Check - Regen Inhibit not being driven?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standstill_RegenRelease - check working with blue dot for </t>
+  </si>
+  <si>
+    <t>feedback of the mA for each function on the main screen / percentage?</t>
+  </si>
+  <si>
+    <t>mA and % if in engineering mode? Or maybe the settings page</t>
+  </si>
+  <si>
+    <t>Knob white/green on the footer - setup mode flash in mimic</t>
+  </si>
+  <si>
+    <t>better lines! Show ecu symbol on the engine can link</t>
+  </si>
+  <si>
+    <t>Access to the min/max Valve mA settings,</t>
+  </si>
+  <si>
+    <t>Access to the min/max Valve mA settings</t>
+  </si>
+  <si>
+    <t>Factory level only</t>
+  </si>
+  <si>
+    <t>Fixed seconds 1200 / 10 / 10 /10 settings</t>
   </si>
 </sst>
 </file>
@@ -2946,7 +2970,7 @@
         <v>CHASSIS.IN0102</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="L4" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7697,14 +7721,14 @@
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B67" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="17" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E67" s="17" t="str">
         <f t="shared" ref="E67:E74" si="20">_xlfn.CONCAT(B67,".",D67)</f>
@@ -7721,7 +7745,7 @@
         <v>AUX.OP0</v>
       </c>
       <c r="K67" s="19" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="L67" s="19" t="str">
         <f t="shared" ref="L67" si="22">IF(K67&lt;&gt;"",UPPER(K67),_xlfn.CONCAT("SPARE_",D67))</f>
@@ -7766,14 +7790,14 @@
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B68" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C68" s="19"/>
       <c r="D68" s="17" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E68" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7833,14 +7857,14 @@
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B69" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E69" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7900,14 +7924,14 @@
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B70" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E70" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7924,7 +7948,7 @@
         <v>AUX.OP3</v>
       </c>
       <c r="K70" s="19" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="L70" s="19" t="str">
         <f t="shared" si="33"/>
@@ -7969,14 +7993,14 @@
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B71" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E71" s="17" t="str">
         <f t="shared" si="20"/>
@@ -7993,7 +8017,7 @@
         <v>AUX.OP4</v>
       </c>
       <c r="K71" s="19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="L71" s="19" t="str">
         <f t="shared" si="33"/>
@@ -8038,14 +8062,14 @@
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B72" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C72" s="19"/>
       <c r="D72" s="17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E72" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8062,7 +8086,7 @@
         <v>AUX.OP5</v>
       </c>
       <c r="K72" s="19" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="L72" s="19" t="str">
         <f t="shared" ref="L72:L75" si="44">IF(K72&lt;&gt;"",UPPER(K72),_xlfn.CONCAT("SPARE_",D72))</f>
@@ -8107,14 +8131,14 @@
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B73" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C73" s="19"/>
       <c r="D73" s="17" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E73" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8131,7 +8155,7 @@
         <v>AUX.OP6</v>
       </c>
       <c r="K73" s="19" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="L73" s="19" t="str">
         <f t="shared" si="44"/>
@@ -8176,14 +8200,14 @@
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B74" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C74" s="19"/>
       <c r="D74" s="17" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E74" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8200,7 +8224,7 @@
         <v>AUX.OP7</v>
       </c>
       <c r="K74" s="19" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="L74" s="19" t="str">
         <f t="shared" si="44"/>
@@ -8245,14 +8269,14 @@
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B75" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C75" s="19"/>
       <c r="D75" s="17" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E75" s="17" t="str">
         <f t="shared" ref="E75:E78" si="54">_xlfn.CONCAT(B75,".",D75)</f>
@@ -8312,14 +8336,14 @@
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B76" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C76" s="19"/>
       <c r="D76" s="17" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E76" s="17" t="str">
         <f t="shared" si="54"/>
@@ -8379,14 +8403,14 @@
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B77" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C77" s="19"/>
       <c r="D77" s="17" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E77" s="17" t="str">
         <f t="shared" si="54"/>
@@ -8446,14 +8470,14 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B78" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="C78" s="19"/>
       <c r="D78" s="17" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E78" s="17" t="str">
         <f t="shared" si="54"/>
@@ -19868,11 +19892,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19885,16 +19908,16 @@
   <sheetData>
     <row r="1" spans="1:5" s="34" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="34" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>603</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>604</v>
-      </c>
       <c r="D1" s="34" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -19902,24 +19925,24 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>575</v>
+      </c>
+      <c r="C2" t="s">
         <v>576</v>
       </c>
-      <c r="C2" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -19927,41 +19950,41 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C4" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D5" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -19969,13 +19992,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C7" s="33" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -19986,10 +20009,10 @@
         <v>544</v>
       </c>
       <c r="D8" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -19997,13 +20020,13 @@
         <v>559</v>
       </c>
       <c r="C9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D9" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -20011,13 +20034,13 @@
         <v>559</v>
       </c>
       <c r="C10" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D10" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -20028,10 +20051,10 @@
         <v>545</v>
       </c>
       <c r="D11" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -20042,10 +20065,10 @@
         <v>560</v>
       </c>
       <c r="D12" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -20056,10 +20079,10 @@
         <v>561</v>
       </c>
       <c r="D13" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -20070,10 +20093,10 @@
         <v>563</v>
       </c>
       <c r="D14" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -20081,13 +20104,13 @@
         <v>559</v>
       </c>
       <c r="C15" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D15" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -20095,10 +20118,10 @@
         <v>564</v>
       </c>
       <c r="C16" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D16" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -20106,13 +20129,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -20123,7 +20146,7 @@
         <v>546</v>
       </c>
       <c r="D18" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -20131,16 +20154,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C19" t="s">
-        <v>645</v>
+        <v>644</v>
+      </c>
+      <c r="D19" t="s">
+        <v>591</v>
       </c>
       <c r="E19" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -20151,10 +20177,10 @@
         <v>557</v>
       </c>
       <c r="D20" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -20165,10 +20191,10 @@
         <v>547</v>
       </c>
       <c r="D21" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -20179,27 +20205,27 @@
         <v>548</v>
       </c>
       <c r="D22" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D23" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E23" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -20210,10 +20236,10 @@
         <v>558</v>
       </c>
       <c r="D24" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -20224,7 +20250,7 @@
         <v>568</v>
       </c>
       <c r="D25" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -20232,7 +20258,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C26" t="s">
         <v>549</v>
@@ -20243,13 +20269,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C27" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -20260,10 +20286,10 @@
         <v>570</v>
       </c>
       <c r="D28" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E28" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -20296,21 +20322,24 @@
         <v>571</v>
       </c>
       <c r="C31" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>680</v>
+      </c>
+      <c r="E31" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>579</v>
+      </c>
+      <c r="C32" t="s">
         <v>580</v>
       </c>
-      <c r="C32" t="s">
-        <v>581</v>
-      </c>
       <c r="D32" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -20318,13 +20347,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="33" t="s">
+        <v>581</v>
+      </c>
+      <c r="C33" s="33" t="s">
         <v>582</v>
       </c>
-      <c r="C33" s="33" t="s">
-        <v>583</v>
-      </c>
       <c r="E33" s="33" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -20332,27 +20361,30 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C34" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>643</v>
+      </c>
+      <c r="E34" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C35" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D35" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E35" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -20360,86 +20392,86 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C36" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C37" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D37" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>589</v>
+      </c>
+      <c r="C38" t="s">
         <v>590</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>591</v>
       </c>
-      <c r="D38" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>594</v>
+      </c>
+      <c r="C39" t="s">
         <v>595</v>
       </c>
-      <c r="C39" t="s">
-        <v>596</v>
-      </c>
       <c r="D39" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E39" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C40" t="s">
+        <v>596</v>
+      </c>
+      <c r="D40" t="s">
+        <v>591</v>
+      </c>
+      <c r="E40" t="s">
         <v>597</v>
       </c>
-      <c r="D40" t="s">
-        <v>592</v>
-      </c>
-      <c r="E40" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>598</v>
+      </c>
+      <c r="C41" t="s">
         <v>599</v>
       </c>
-      <c r="C41" t="s">
-        <v>600</v>
-      </c>
       <c r="D41" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -20447,10 +20479,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>631</v>
+      </c>
+      <c r="C42" t="s">
         <v>632</v>
-      </c>
-      <c r="C42" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -20458,13 +20490,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C43" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>634</v>
+      </c>
+      <c r="E43" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -20472,27 +20507,27 @@
         <v>569</v>
       </c>
       <c r="C44" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D44" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>635</v>
+      </c>
+      <c r="C45" t="s">
         <v>636</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
+        <v>658</v>
+      </c>
+      <c r="E45" t="s">
         <v>637</v>
-      </c>
-      <c r="D45" t="s">
-        <v>659</v>
-      </c>
-      <c r="E45" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -20500,10 +20535,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>638</v>
+      </c>
+      <c r="C46" t="s">
         <v>639</v>
       </c>
-      <c r="C46" t="s">
-        <v>640</v>
+      <c r="D46" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -20511,13 +20549,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>647</v>
+      </c>
+      <c r="C47" t="s">
         <v>648</v>
       </c>
-      <c r="C47" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -20525,190 +20563,277 @@
         <v>569</v>
       </c>
       <c r="C48" t="s">
+        <v>649</v>
+      </c>
+      <c r="D48" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
         <v>650</v>
       </c>
-      <c r="D48" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>49</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>651</v>
       </c>
-      <c r="C49" t="s">
-        <v>652</v>
-      </c>
       <c r="D49" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>569</v>
       </c>
       <c r="C50" t="s">
+        <v>660</v>
+      </c>
+      <c r="D50" t="s">
+        <v>658</v>
+      </c>
+      <c r="E50" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>654</v>
+      </c>
+      <c r="C51" t="s">
+        <v>653</v>
+      </c>
+      <c r="D51" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="33" t="s">
+        <v>654</v>
+      </c>
+      <c r="C52" s="33" t="s">
+        <v>652</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>591</v>
+      </c>
+      <c r="E52" s="33" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>654</v>
+      </c>
+      <c r="C53" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>654</v>
+      </c>
+      <c r="C54" t="s">
         <v>655</v>
       </c>
-      <c r="C51" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="33" t="s">
-        <v>655</v>
-      </c>
-      <c r="C52" s="33" t="s">
-        <v>653</v>
-      </c>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33" t="s">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>646</v>
+      </c>
+      <c r="C55" t="s">
+        <v>656</v>
+      </c>
+      <c r="D55" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>646</v>
+      </c>
+      <c r="C56" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>665</v>
+      </c>
+      <c r="C57" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>664</v>
+      </c>
+      <c r="C58" t="s">
+        <v>663</v>
+      </c>
+      <c r="D58" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>670</v>
+      </c>
+      <c r="C59" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>655</v>
-      </c>
-      <c r="C53" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>655</v>
-      </c>
-      <c r="C54" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>647</v>
-      </c>
-      <c r="C55" t="s">
-        <v>657</v>
-      </c>
-      <c r="D55" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>647</v>
-      </c>
-      <c r="C56" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>666</v>
-      </c>
-      <c r="C57" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>665</v>
-      </c>
-      <c r="C58" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+      <c r="E59" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>670</v>
+      </c>
+      <c r="C60" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>598</v>
+      </c>
+      <c r="C61" t="s">
         <v>671</v>
       </c>
-      <c r="C59" t="s">
-        <v>668</v>
-      </c>
-      <c r="E59" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>671</v>
-      </c>
-      <c r="C60" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>599</v>
-      </c>
-      <c r="C61" t="s">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>677</v>
+      </c>
+      <c r="C62" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>673</v>
-      </c>
-      <c r="C62" t="s">
-        <v>674</v>
+      <c r="D62" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
       <c r="B63" t="s">
         <v>569</v>
       </c>
       <c r="C63" t="s">
+        <v>673</v>
+      </c>
+      <c r="D63" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>674</v>
+      </c>
+      <c r="C64" t="s">
+        <v>678</v>
+      </c>
+      <c r="E64" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>674</v>
+      </c>
+      <c r="C65" t="s">
         <v>676</v>
       </c>
-      <c r="C64" t="s">
-        <v>677</v>
-      </c>
-      <c r="E64" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>676</v>
-      </c>
-      <c r="C65" t="s">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>674</v>
+      </c>
+      <c r="C66" t="s">
         <v>679</v>
       </c>
     </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>569</v>
+      </c>
+      <c r="C67" t="s">
+        <v>685</v>
+      </c>
+      <c r="E67" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>569</v>
+      </c>
+      <c r="C68" t="s">
+        <v>684</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E58" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
-    <filterColumn colId="3">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -20724,6 +20849,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20950,14 +21084,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -20970,6 +21096,14 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
WIP - having issues with SP19 and text lists not working on the CR1076!
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70B14BC-9BCD-46B8-B909-3B1C8B0ACD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6034B0F-BD2E-41FA-85D7-0AE0BD57EA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="5" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$78</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SNAGS!$A$1:$E$66</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="689">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2110,6 +2110,9 @@
   </si>
   <si>
     <t>Fixed seconds 1200 / 10 / 10 /10 settings</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -2685,14 +2688,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4EBF08-015A-4388-B8C8-8A07CE5EF3C7}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U78"/>
+  <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V48" sqref="V48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2710,13 +2713,12 @@
     <col min="12" max="12" width="32.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.85546875" style="4" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="44.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="54" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="54" style="2" customWidth="1"/>
-    <col min="17" max="17" width="70.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="200" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="61.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="57.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="54" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="70.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="200" style="2" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="61.28515625" style="2" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" style="2" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="57.140625" style="2" hidden="1" customWidth="1"/>
     <col min="22" max="25" width="14.140625" style="4" customWidth="1"/>
     <col min="26" max="16384" width="9.140625" style="4"/>
   </cols>
@@ -2782,7 +2784,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>93</v>
       </c>
@@ -2858,7 +2860,7 @@
         <v>CHASSIS.IN0100.Init(Machine_IO.Inputs.ESTOP_OK);</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>93</v>
       </c>
@@ -2934,7 +2936,7 @@
         <v>CHASSIS.IN0101.Init(Machine_IO.Inputs.DRUM_PRESSURE);</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>93</v>
       </c>
@@ -3010,7 +3012,7 @@
         <v>CHASSIS.IN0102.Init(Machine_IO.Inputs.KEYSWITCH_CRANKING);</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>93</v>
       </c>
@@ -3084,7 +3086,7 @@
         <v>CHASSIS.IN0103.Init(Machine_IO.Inputs.SPARE_IN0103);</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>93</v>
       </c>
@@ -3158,7 +3160,7 @@
         <v>CHASSIS.IN0200.Init(Machine_IO.Inputs.SPARE_IN0200);</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>93</v>
       </c>
@@ -3232,7 +3234,7 @@
         <v>CHASSIS.IN0201.Init(Machine_IO.Inputs.SPARE_IN0201);</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>93</v>
       </c>
@@ -3306,7 +3308,7 @@
         <v>CHASSIS.IN0202.Init(Machine_IO.Inputs.SPARE_IN0202);</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>93</v>
       </c>
@@ -3380,7 +3382,7 @@
         <v>CHASSIS.IN0203.Init(Machine_IO.Inputs.SPARE_IN0203);</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>93</v>
       </c>
@@ -3454,7 +3456,7 @@
         <v>CHASSIS.IN0600.Init(Machine_IO.Inputs.SPARE_IN0600);</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>93</v>
       </c>
@@ -3528,7 +3530,7 @@
         <v>CHASSIS.IN0601.Init(Machine_IO.Inputs.SPARE_IN0601);</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>93</v>
       </c>
@@ -3602,7 +3604,7 @@
         <v>CHASSIS.IN0602.Init(Machine_IO.Inputs.SPARE_IN0602);</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>93</v>
       </c>
@@ -3676,7 +3678,7 @@
         <v>CHASSIS.IN0603.Init(Machine_IO.Inputs.SPARE_IN0603);</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>93</v>
       </c>
@@ -3750,7 +3752,7 @@
         <v>CHASSIS.IN0700.Init(Machine_IO.Inputs.SPARE_IN0700);</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>93</v>
       </c>
@@ -3826,7 +3828,7 @@
         <v>CHASSIS.IN0701.Init(Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ);</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>93</v>
       </c>
@@ -3902,7 +3904,7 @@
         <v>CHASSIS.IN0702.Init(Machine_IO.Inputs.RHS_TROMMELDOORSW);</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>93</v>
       </c>
@@ -3978,7 +3980,7 @@
         <v>CHASSIS.IN0703.Init(Machine_IO.Inputs.LHS_TROMMELDOORSW);</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>93</v>
       </c>
@@ -4054,7 +4056,7 @@
         <v>CHASSIS.IN0000.Init(Machine_IO.Inputs.HYDOILTEMP_SW);</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>93</v>
       </c>
@@ -4130,7 +4132,7 @@
         <v>CHASSIS.IN0001.Init(Machine_IO.Inputs.HYDOILLEVEL_SW);</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>93</v>
       </c>
@@ -4206,7 +4208,7 @@
         <v>CHASSIS.IN0002.Init(Machine_IO.Inputs.THERMOSTAT);</v>
       </c>
     </row>
-    <row r="21" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>93</v>
       </c>
@@ -4281,7 +4283,7 @@
         <v>CHASSIS.IN0003.Init(Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ);</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>93</v>
       </c>
@@ -4357,7 +4359,7 @@
         <v>CHASSIS.IN0500.Init(Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ);</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>93</v>
       </c>
@@ -4433,7 +4435,7 @@
         <v>CHASSIS.IN0501.Init(Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ);</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>93</v>
       </c>
@@ -4509,7 +4511,7 @@
         <v>CHASSIS.IN0502.Init(Machine_IO.Inputs.RADIOSIDECONVRAISEREQ);</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>93</v>
       </c>
@@ -4585,7 +4587,7 @@
         <v>CHASSIS.IN0503.Init(Machine_IO.Inputs.RADIOSIDECONVLOWERREQ);</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>93</v>
       </c>
@@ -4659,7 +4661,7 @@
         <v>CHASSIS.IN0400.Init(Machine_IO.Inputs.SPARE_IN0400);</v>
       </c>
     </row>
-    <row r="27" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>93</v>
       </c>
@@ -4735,7 +4737,7 @@
         <v>CHASSIS.IN0401.Init(Machine_IO.Inputs.FUELLEVEL_PERCENT);</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>93</v>
       </c>
@@ -4809,7 +4811,7 @@
         <v>CHASSIS.IN0900.Init(Machine_IO.Inputs.UMBTRACKREQ);</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>93</v>
       </c>
@@ -4883,7 +4885,7 @@
         <v>CHASSIS.IN0901.Init(Machine_IO.Inputs.UMBMACHINESTOP);</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>93</v>
       </c>
@@ -4957,7 +4959,7 @@
         <v>CHASSIS.IN0300.Init(Machine_IO.Inputs.RTF_REQ);</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>93</v>
       </c>
@@ -5031,7 +5033,7 @@
         <v>CHASSIS.IN0301.Init(Machine_IO.Inputs.RTR_REQ);</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>93</v>
       </c>
@@ -5105,7 +5107,7 @@
         <v>CHASSIS.IN0800.Init(Machine_IO.Inputs.LTF_REQ);</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>93</v>
       </c>
@@ -5179,7 +5181,7 @@
         <v>CHASSIS.IN0801.Init(Machine_IO.Inputs.LTR_REQ);</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>93</v>
       </c>
@@ -5257,8 +5259,11 @@
         <f t="shared" ref="U34:U65" si="16">_xlfn.CONCAT(A34,".",D34,".Init(",O34,");")</f>
         <v>CHASSIS.OUT0000.Init(Machine_IO.Outputs.TAILCONVSPD_MA);</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V34" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>93</v>
       </c>
@@ -5337,7 +5342,7 @@
         <v>CHASSIS.OUT0001.Init(Machine_IO.Outputs.RHS_JACKLEGLOWER_OP);</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>93</v>
       </c>
@@ -5415,8 +5420,11 @@
         <f t="shared" si="16"/>
         <v>CHASSIS.OUT0002.Init(Machine_IO.Outputs.SIDECONVSPD_MA);</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V36" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>93</v>
       </c>
@@ -5495,7 +5503,7 @@
         <v>CHASSIS.OUT0003.Init(Machine_IO.Outputs.LHS_JACKLEGRAISE_OP);</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>93</v>
       </c>
@@ -5573,8 +5581,11 @@
         <f t="shared" si="16"/>
         <v>CHASSIS.OUT0004.Init(Machine_IO.Outputs.SIDETRANSFERSPD_MA);</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V38" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>93</v>
       </c>
@@ -5653,7 +5664,7 @@
         <v>CHASSIS.OUT0005.Init(Machine_IO.Outputs.LHS_JACKLEGLOWER_OP);</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>93</v>
       </c>
@@ -5732,7 +5743,7 @@
         <v>CHASSIS.OUT0006.Init(Machine_IO.Outputs.SETUPDUMPVALVE_OP);</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
         <v>93</v>
       </c>
@@ -5810,8 +5821,11 @@
         <f t="shared" si="16"/>
         <v>CHASSIS.OUT0007.Init(Machine_IO.Outputs.COLLECTIONCONVSPD_MA);</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V41" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
         <v>93</v>
       </c>
@@ -5889,8 +5903,11 @@
         <f t="shared" si="16"/>
         <v>CHASSIS.OUT0008.Init(Machine_IO.Outputs.COLLECTIONCONVON_OP);</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V42" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>93</v>
       </c>
@@ -5969,7 +5986,7 @@
         <v>CHASSIS.GROUP0.Init(Machine_IO.Outputs.SUPPLY_GROUP0);</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>93</v>
       </c>
@@ -6047,8 +6064,11 @@
         <f t="shared" si="16"/>
         <v>CHASSIS.OUT0100.Init(Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT);</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V44" s="4" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
         <v>93</v>
       </c>
@@ -6127,7 +6147,7 @@
         <v>CHASSIS.OUT0101.Init(Machine_IO.Outputs.TRACKINGMODE);</v>
       </c>
     </row>
-    <row r="46" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>93</v>
       </c>
@@ -6205,8 +6225,11 @@
         <f t="shared" si="16"/>
         <v>CHASSIS.OUT0102.Init(Machine_IO.Outputs.FEEDERSPD_MA);</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V46" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>93</v>
       </c>
@@ -6285,7 +6308,7 @@
         <v>CHASSIS.OUT0103.Init(Machine_IO.Outputs.CRANKENABLE);</v>
       </c>
     </row>
-    <row r="48" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>93</v>
       </c>
@@ -6364,7 +6387,7 @@
         <v>CHASSIS.OUT0104.Init(Machine_IO.Outputs.DIVERTOILTOTRACK_OP);</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
         <v>93</v>
       </c>
@@ -6443,7 +6466,7 @@
         <v>CHASSIS.OUT0105.Init(Machine_IO.Outputs.RHS_JACKLEGRAISE_OP);</v>
       </c>
     </row>
-    <row r="50" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
         <v>93</v>
       </c>
@@ -6522,7 +6545,7 @@
         <v>CHASSIS.OUT0106.Init(Machine_IO.Outputs.TAILCONVON_OP);</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>93</v>
       </c>
@@ -6600,8 +6623,11 @@
         <f t="shared" si="16"/>
         <v>CHASSIS.OUT0107.Init(Machine_IO.Outputs.SIDECONVON_OP);</v>
       </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V51" s="4" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
         <v>93</v>
       </c>
@@ -6680,7 +6706,7 @@
         <v>CHASSIS.OUT0108.Init(Machine_IO.Outputs.SIDETRANSFERON_OP);</v>
       </c>
     </row>
-    <row r="53" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:22" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>93</v>
       </c>
@@ -6759,7 +6785,7 @@
         <v>CHASSIS.GROUP1.Init(Machine_IO.Outputs.SUPPLY_GROUP1);</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
         <v>93</v>
       </c>
@@ -6838,7 +6864,7 @@
         <v>CHASSIS.OUT0200.Init(Machine_IO.Outputs.LEFTTRACKDIVERT_OP);</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>93</v>
       </c>
@@ -6917,7 +6943,7 @@
         <v>CHASSIS.OUT0201.Init(Machine_IO.Outputs.LTF_OP);</v>
       </c>
     </row>
-    <row r="56" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
         <v>93</v>
       </c>
@@ -6996,7 +7022,7 @@
         <v>CHASSIS.OUT0202.Init(Machine_IO.Outputs.LTR_OP);</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
         <v>93</v>
       </c>
@@ -7075,7 +7101,7 @@
         <v>CHASSIS.OUT0203.Init(Machine_IO.Outputs.RIGHTTRACKDIVERT_OP);</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
         <v>93</v>
       </c>
@@ -7154,7 +7180,7 @@
         <v>CHASSIS.OUT0204.Init(Machine_IO.Outputs.RTF_OP);</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
         <v>93</v>
       </c>
@@ -7233,7 +7259,7 @@
         <v>CHASSIS.OUT0205.Init(Machine_IO.Outputs.RTR_OP);</v>
       </c>
     </row>
-    <row r="60" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>93</v>
       </c>
@@ -7312,7 +7338,7 @@
         <v>CHASSIS.OUT0206.Init(Machine_IO.Outputs.DRUMONOFF_OP);</v>
       </c>
     </row>
-    <row r="61" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
         <v>93</v>
       </c>
@@ -7391,7 +7417,7 @@
         <v>CHASSIS.OUT0207.Init(Machine_IO.Outputs.FEEDERONOFF_OP);</v>
       </c>
     </row>
-    <row r="62" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
         <v>93</v>
       </c>
@@ -7470,7 +7496,7 @@
         <v>CHASSIS.OUT0208.Init(Machine_IO.Outputs.ECUENABLE);</v>
       </c>
     </row>
-    <row r="63" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:22" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
         <v>93</v>
       </c>
@@ -7549,7 +7575,7 @@
         <v>CHASSIS.GROUP2.Init(Machine_IO.Outputs.SUPPLY_GROUP2);</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" s="17" t="s">
         <v>93</v>
       </c>
@@ -8536,7 +8562,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP71" xr:uid="{1E4EBF08-015A-4388-B8C8-8A07CE5EF3C7}"/>
+  <autoFilter ref="A1:AP78" xr:uid="{1E4EBF08-015A-4388-B8C8-8A07CE5EF3C7}">
+    <filterColumn colId="5">
+      <filters blank="1">
+        <filter val="OUT"/>
+        <filter val="OUTA"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.23622047244094488" right="0.23622047244094488" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="71" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -19894,8 +19927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20834,6 +20867,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -20849,15 +20891,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21084,6 +21117,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -21096,14 +21137,6 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixes for the network page (plc offline) stop auto mode if plc offlien. setup hyd mode icons fix
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6034B0F-BD2E-41FA-85D7-0AE0BD57EA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CA26CF-CC5C-4137-A6B4-453CF39415CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView minimized="1" xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15345" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
-    <sheet name="Settings" sheetId="32" r:id="rId2"/>
-    <sheet name="IfmPinRef" sheetId="21" r:id="rId3"/>
-    <sheet name="ALARMS" sheetId="24" r:id="rId4"/>
-    <sheet name="ALARMS_IO" sheetId="31" r:id="rId5"/>
-    <sheet name="SNAGS" sheetId="33" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="34" r:id="rId2"/>
+    <sheet name="Settings" sheetId="32" r:id="rId3"/>
+    <sheet name="IfmPinRef" sheetId="21" r:id="rId4"/>
+    <sheet name="ALARMS" sheetId="24" r:id="rId5"/>
+    <sheet name="ALARMS_IO" sheetId="31" r:id="rId6"/>
+    <sheet name="SNAGS" sheetId="33" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$78</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SNAGS!$A$1:$E$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">SNAGS!$A$1:$E$68</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2293" uniqueCount="826">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2052,9 +2053,6 @@
     <t>Auto Shutdown - slows engine down first?</t>
   </si>
   <si>
-    <t>Auto Start - ramps engine at the end????</t>
-  </si>
-  <si>
     <t>ask mark - material on conveyor - moves very slow!</t>
   </si>
   <si>
@@ -2113,6 +2111,420 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>STAT_INACTIVE</t>
+  </si>
+  <si>
+    <t>STAT_DONE</t>
+  </si>
+  <si>
+    <t>STAT_BUSY</t>
+  </si>
+  <si>
+    <t>STAT_PREPARING</t>
+  </si>
+  <si>
+    <t>STAT_READY</t>
+  </si>
+  <si>
+    <t>STAT_RESET</t>
+  </si>
+  <si>
+    <t>STAT_ABORTED</t>
+  </si>
+  <si>
+    <t>RESERVED_07</t>
+  </si>
+  <si>
+    <t>RESERVED_08</t>
+  </si>
+  <si>
+    <t>RESERVED_09</t>
+  </si>
+  <si>
+    <t>ERR_OPEN_CIRCUIT</t>
+  </si>
+  <si>
+    <t>ERR_SHORT_CIRCUIT</t>
+  </si>
+  <si>
+    <t>ERR_OVERLOAD_CURRENT</t>
+  </si>
+  <si>
+    <t>ERR_LOW_CURRENT</t>
+  </si>
+  <si>
+    <t>ERR_UNDERVOLTAGE_VBBX</t>
+  </si>
+  <si>
+    <t>ERR_OVERVOLTAGE_VBBX</t>
+  </si>
+  <si>
+    <t>ERR_STUCK_AT_HIGH</t>
+  </si>
+  <si>
+    <t>ERR_STUCK_AT_LOW</t>
+  </si>
+  <si>
+    <t>ERR_HIGH_TEMPERATURE</t>
+  </si>
+  <si>
+    <t>ERR_LOW_TEMPERATURE</t>
+  </si>
+  <si>
+    <t>ERR_INVALID_VALUE</t>
+  </si>
+  <si>
+    <t>ERR_INVALID_CHANNEL</t>
+  </si>
+  <si>
+    <t>ERR_INVALID_MODE</t>
+  </si>
+  <si>
+    <t>ERR_INVALID_FREQUENCY</t>
+  </si>
+  <si>
+    <t>ERR_INVALID_DITHER</t>
+  </si>
+  <si>
+    <t>ERR_INVALID_FILTER</t>
+  </si>
+  <si>
+    <t>ERR_UNREACHABLE_CURRENT</t>
+  </si>
+  <si>
+    <t>ERR_SLOW_SIGNAL</t>
+  </si>
+  <si>
+    <t>ERR_CHANGEOVER_TIME</t>
+  </si>
+  <si>
+    <t>ERR_INSTANCE</t>
+  </si>
+  <si>
+    <t>ERR_INSTANCE_LIMIT</t>
+  </si>
+  <si>
+    <t>ERR_INVALID_COLOUR</t>
+  </si>
+  <si>
+    <t>ERR_NO_IDENTITY</t>
+  </si>
+  <si>
+    <t>ERR_ACCESS</t>
+  </si>
+  <si>
+    <t>ERR_UNDEFINED</t>
+  </si>
+  <si>
+    <t>ERR_FUNC_KEY_MISSED</t>
+  </si>
+  <si>
+    <t>ERR_BUFFER_OVERFLOW</t>
+  </si>
+  <si>
+    <t>ERR_BAUDRATE_ALREADY_SET</t>
+  </si>
+  <si>
+    <t>ERR_INACTIVE_INTERFACE</t>
+  </si>
+  <si>
+    <t>ERR_TIMEOUT</t>
+  </si>
+  <si>
+    <t>ERR_OUT_OF_MEMORY</t>
+  </si>
+  <si>
+    <t>ERR_BUS_OFF</t>
+  </si>
+  <si>
+    <t>ERR_BAD_CRC</t>
+  </si>
+  <si>
+    <t>ERR_EXCEEDED_RANGE</t>
+  </si>
+  <si>
+    <t>ERR_INTERNAL_COMMUNICATION</t>
+  </si>
+  <si>
+    <t>ERR_NOT_SUPPORTED</t>
+  </si>
+  <si>
+    <t>ERR_TIMING</t>
+  </si>
+  <si>
+    <t>ERR_INTERNAL</t>
+  </si>
+  <si>
+    <t>ERR_FILE_SYSTEM</t>
+  </si>
+  <si>
+    <t>ERR_INVALID_IP_CFG</t>
+  </si>
+  <si>
+    <t>ERR_FAILED_ERR_RESET</t>
+  </si>
+  <si>
+    <t>ERR_DEVICE_NOT_AVAILABLE</t>
+  </si>
+  <si>
+    <t>ERR_NO_OBJECT</t>
+  </si>
+  <si>
+    <t>ERR_UNREACHABLE_VOLTAGE</t>
+  </si>
+  <si>
+    <t>ERR_AT_GROUP_OUTPUT</t>
+  </si>
+  <si>
+    <t>ERR_CONTROL_DITHER</t>
+  </si>
+  <si>
+    <t>ERR_UNDERVOLTAGE_VBBX_WARNING</t>
+  </si>
+  <si>
+    <t>ERR_OVERVOLTAGE_VBBX_WARNING</t>
+  </si>
+  <si>
+    <t>ERR_LOW_TEMPERATURE_WARNING</t>
+  </si>
+  <si>
+    <t>ERR_HIGH_TEMPERATURE_WARNING</t>
+  </si>
+  <si>
+    <t>ERR_RANGE_OVERRUN</t>
+  </si>
+  <si>
+    <t>ERR_RANGE_UNDERRUN</t>
+  </si>
+  <si>
+    <t>DIAG_INVALID_VALUE</t>
+  </si>
+  <si>
+    <t>DIAG_INTERNAL</t>
+  </si>
+  <si>
+    <t>DIAG_OPEN_CIRCUIT</t>
+  </si>
+  <si>
+    <t>DIAG_SHORT_CIRCUIT</t>
+  </si>
+  <si>
+    <t>DIAG_UNDERVOLTAGE_VBBX</t>
+  </si>
+  <si>
+    <t>DIAG_OVERVOLTAGE_VBBX</t>
+  </si>
+  <si>
+    <t>DIAG_OVERLOAD_CURRENT</t>
+  </si>
+  <si>
+    <t>DIAG_STUCK_AT</t>
+  </si>
+  <si>
+    <t>DIAG_STUCK_AT_HIGH</t>
+  </si>
+  <si>
+    <t>DIAG_STUCK_AT_LOW</t>
+  </si>
+  <si>
+    <t>DIAG_INVALID_COLOUR</t>
+  </si>
+  <si>
+    <t>DIAG_OVERVOLTAGE</t>
+  </si>
+  <si>
+    <t>DIAG_UNDERVOLTAGE</t>
+  </si>
+  <si>
+    <t>DIAG_NO_CALIB</t>
+  </si>
+  <si>
+    <t>DIAG_ACCESS</t>
+  </si>
+  <si>
+    <t>DIAG_CHANGEOVER_TIME</t>
+  </si>
+  <si>
+    <t>ERR_OVERVOLTAGE</t>
+  </si>
+  <si>
+    <t>ERR_UNDERVOLTAGE</t>
+  </si>
+  <si>
+    <t>ERR_STUCK_AT</t>
+  </si>
+  <si>
+    <t>DIAG_CONTROL_DITHER</t>
+  </si>
+  <si>
+    <t>DIAG_SLOW_SIGNAL</t>
+  </si>
+  <si>
+    <t>DIAG_DIAG_PRO_MODE</t>
+  </si>
+  <si>
+    <t>DIAG_WINDOW</t>
+  </si>
+  <si>
+    <t>ERR_SDO_IDX_NOT_EXIST</t>
+  </si>
+  <si>
+    <t>ERR_SDO_SUBIDX_NOT_EXIST</t>
+  </si>
+  <si>
+    <t>ERR_SDO_UNSUPPORTED_ACCESS</t>
+  </si>
+  <si>
+    <t>ERR_SDO_DATA_TYPE</t>
+  </si>
+  <si>
+    <t>DIAG_LOW_TEMPERATURE</t>
+  </si>
+  <si>
+    <t>DIAG_HIGH_TEMPERATURE</t>
+  </si>
+  <si>
+    <t>DIAG_INVALID_DITHER</t>
+  </si>
+  <si>
+    <t>DIAG_INVALID_FREQUENCY</t>
+  </si>
+  <si>
+    <t>DIAG_RANGE_OVERRUN</t>
+  </si>
+  <si>
+    <t>DIAG_RANGE_UNDERRUN</t>
+  </si>
+  <si>
+    <t>DIAG_INVALID_FILTER</t>
+  </si>
+  <si>
+    <t>ERR_COMPARE_MISMATCH</t>
+  </si>
+  <si>
+    <t>DIAG_INVALID_IP_CFG</t>
+  </si>
+  <si>
+    <t>DIAG_LOW_CURRENT</t>
+  </si>
+  <si>
+    <t>DIAG_AT_GROUP_OUTPUT</t>
+  </si>
+  <si>
+    <t>ERR_SDO_UNKNOWN</t>
+  </si>
+  <si>
+    <t>ERR_BAUDRATE_INVALID_OR_ALREADY_SET</t>
+  </si>
+  <si>
+    <t>DIAG_COMPARE_MISMATCH</t>
+  </si>
+  <si>
+    <t>DIAG_COMPARE_MISMATCH_VSYS</t>
+  </si>
+  <si>
+    <t>DIAG_GROUP_OVERLOAD_CURRENT</t>
+  </si>
+  <si>
+    <t>ERR_GROUP_OVERLOAD_CURRENT</t>
+  </si>
+  <si>
+    <t>STAT_PAUSED</t>
+  </si>
+  <si>
+    <t>STAT_ABORT</t>
+  </si>
+  <si>
+    <t>STAT_EVNT_OPEN_PLUG_STORAGE</t>
+  </si>
+  <si>
+    <t>STAT_EVNT_OPEN_UNPLUG_STORAGE</t>
+  </si>
+  <si>
+    <t>STAT_EVNT_OPEN_DONE</t>
+  </si>
+  <si>
+    <t>STAT_EVNT_REGI_PLUG_STORAGE</t>
+  </si>
+  <si>
+    <t>STAT_EVNT_REGI_UNPLUG_STORAGE</t>
+  </si>
+  <si>
+    <t>STAT_EVNT_REGI_DONE</t>
+  </si>
+  <si>
+    <t>STAT_EVNT_UNREGI</t>
+  </si>
+  <si>
+    <t>STAT_EVNT_UNREGI_DONE</t>
+  </si>
+  <si>
+    <t>STAT_EVNT_CLOSE</t>
+  </si>
+  <si>
+    <t>STAT_EVNT_CLOSE_DONE</t>
+  </si>
+  <si>
+    <t>ERR_INSTANCE_RESTRICTION</t>
+  </si>
+  <si>
+    <t>ERR_NO_FILE</t>
+  </si>
+  <si>
+    <t>ERR_EVNT_OPEN</t>
+  </si>
+  <si>
+    <t>ERR_EVNT_REGI</t>
+  </si>
+  <si>
+    <t>ERR_EVNT_UNREGI</t>
+  </si>
+  <si>
+    <t>ERR_EVNT_CLOSE</t>
+  </si>
+  <si>
+    <t>ERR_GET_STORAGE_LIST</t>
+  </si>
+  <si>
+    <t>ERR_UNPLUG_STORAGE</t>
+  </si>
+  <si>
+    <t>DIAG_INVALID_CHANNEL</t>
+  </si>
+  <si>
+    <t>DIAG_INVALID_MODE</t>
+  </si>
+  <si>
+    <t>ERR_H_BRIDGE_TEST</t>
+  </si>
+  <si>
+    <t>ERR_GROUP_SW_TEST</t>
+  </si>
+  <si>
+    <t>ERR_TX_ERROR</t>
+  </si>
+  <si>
+    <t>ERR_RX_ERROR</t>
+  </si>
+  <si>
+    <t>DIAG_PHASE_MISSING_B</t>
+  </si>
+  <si>
+    <t>DIAG_PHASE_TOO_MANY_B</t>
+  </si>
+  <si>
+    <t>Auto Start - ramps engine at the end?</t>
+  </si>
+  <si>
+    <t>NETWORK</t>
+  </si>
+  <si>
+    <t>HMI program reset if the coms goes down</t>
+  </si>
+  <si>
+    <t>via critical shutdown signal</t>
   </si>
 </sst>
 </file>
@@ -2693,9 +3105,9 @@
   </sheetPr>
   <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V48" sqref="V48"/>
+      <selection pane="bottomLeft" activeCell="V45" sqref="V45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -5260,7 +5672,7 @@
         <v>CHASSIS.OUT0000.Init(Machine_IO.Outputs.TAILCONVSPD_MA);</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="35" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5421,7 +5833,7 @@
         <v>CHASSIS.OUT0002.Init(Machine_IO.Outputs.SIDECONVSPD_MA);</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="37" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5582,7 +5994,7 @@
         <v>CHASSIS.OUT0004.Init(Machine_IO.Outputs.SIDETRANSFERSPD_MA);</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="39" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5822,7 +6234,7 @@
         <v>CHASSIS.OUT0007.Init(Machine_IO.Outputs.COLLECTIONCONVSPD_MA);</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="42" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5904,7 +6316,7 @@
         <v>CHASSIS.OUT0008.Init(Machine_IO.Outputs.COLLECTIONCONVON_OP);</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="43" spans="1:22" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -6065,7 +6477,7 @@
         <v>CHASSIS.OUT0100.Init(Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT);</v>
       </c>
       <c r="V44" s="4" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6226,7 +6638,7 @@
         <v>CHASSIS.OUT0102.Init(Machine_IO.Outputs.FEEDERSPD_MA);</v>
       </c>
       <c r="V46" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="47" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6624,7 +7036,7 @@
         <v>CHASSIS.OUT0107.Init(Machine_IO.Outputs.SIDECONVON_OP);</v>
       </c>
       <c r="V51" s="4" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
@@ -8577,6 +8989,1634 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C40DF00-F28E-4B7C-BC19-351897567202}">
+  <dimension ref="A2:C135"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>688</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("IF CODE = ",A2," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B2,"';&lt;cr&gt;END_IF;")</f>
+        <v>IF CODE = 0 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_INACTIVE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>689</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C66" si="0">_xlfn.CONCAT("IF CODE = ",A3," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B3,"';&lt;cr&gt;END_IF;")</f>
+        <v>IF CODE = 1 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_DONE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>690</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 2 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_BUSY';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>691</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 3 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_PREPARING';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>692</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 4 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_READY';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>693</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 5 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_RESET';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>694</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 6 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_ABORTED';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>695</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 7 THEN&lt;cr&gt;&lt;t&gt;TEXT:='RESERVED_07';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>696</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 8 THEN&lt;cr&gt;&lt;t&gt;TEXT:='RESERVED_08';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>697</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 9 THEN&lt;cr&gt;&lt;t&gt;TEXT:='RESERVED_09';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>698</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 10 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_OPEN_CIRCUIT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>699</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 11 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_SHORT_CIRCUIT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>700</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 12 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_OVERLOAD_CURRENT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>701</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 13 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_LOW_CURRENT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>702</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 14 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_UNDERVOLTAGE_VBBX';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>703</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 15 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_OVERVOLTAGE_VBBX';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>704</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 16 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_STUCK_AT_HIGH';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>705</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 17 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_STUCK_AT_LOW';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>706</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 18 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_HIGH_TEMPERATURE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>707</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 19 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_LOW_TEMPERATURE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>708</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 20 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INVALID_VALUE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>709</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 21 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INVALID_CHANNEL';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>710</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 22 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INVALID_MODE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>711</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 23 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INVALID_FREQUENCY';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>712</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 24 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INVALID_DITHER';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>713</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 25 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INVALID_FILTER';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>714</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 26 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_UNREACHABLE_CURRENT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>715</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 27 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_SLOW_SIGNAL';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>716</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 28 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_CHANGEOVER_TIME';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>717</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 29 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INSTANCE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>718</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 30 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INSTANCE_LIMIT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>719</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 31 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INVALID_COLOUR';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>720</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 32 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_NO_IDENTITY';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>721</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 33 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_ACCESS';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>722</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 34 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_UNDEFINED';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>723</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 35 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_FUNC_KEY_MISSED';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>724</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 36 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_BUFFER_OVERFLOW';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>725</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 37 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_BAUDRATE_ALREADY_SET';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>726</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 38 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INACTIVE_INTERFACE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>727</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 39 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_TIMEOUT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>728</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 40 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_OUT_OF_MEMORY';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>729</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 41 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_BUS_OFF';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>730</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 42 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_BAD_CRC';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>731</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 43 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_EXCEEDED_RANGE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>732</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 44 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INTERNAL_COMMUNICATION';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>733</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 45 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_NOT_SUPPORTED';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>734</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 46 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_TIMING';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>735</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 47 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INTERNAL';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>736</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 48 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_FILE_SYSTEM';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>737</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 49 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INVALID_IP_CFG';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>738</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 50 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_FAILED_ERR_RESET';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>739</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 51 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_DEVICE_NOT_AVAILABLE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>740</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 52 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_NO_OBJECT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>741</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 53 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_UNREACHABLE_VOLTAGE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>742</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 54 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_AT_GROUP_OUTPUT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>743</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 55 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_CONTROL_DITHER';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>744</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 56 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_UNDERVOLTAGE_VBBX_WARNING';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>745</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 57 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_OVERVOLTAGE_VBBX_WARNING';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>746</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 58 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_LOW_TEMPERATURE_WARNING';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>747</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 59 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_HIGH_TEMPERATURE_WARNING';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>748</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 60 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_RANGE_OVERRUN';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>749</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 61 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_RANGE_UNDERRUN';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>750</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 62 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_INVALID_VALUE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>751</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 63 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_INTERNAL';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>752</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="0"/>
+        <v>IF CODE = 64 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_OPEN_CIRCUIT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>753</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" ref="C67:C130" si="1">_xlfn.CONCAT("IF CODE = ",A67," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B67,"';&lt;cr&gt;END_IF;")</f>
+        <v>IF CODE = 65 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_SHORT_CIRCUIT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>754</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 66 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_UNDERVOLTAGE_VBBX';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>755</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 67 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_OVERVOLTAGE_VBBX';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>756</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 68 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_OVERLOAD_CURRENT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>757</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 69 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_STUCK_AT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>758</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 70 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_STUCK_AT_HIGH';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>759</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 71 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_STUCK_AT_LOW';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>760</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 72 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_INVALID_COLOUR';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>761</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 73 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_OVERVOLTAGE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>762</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 74 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_UNDERVOLTAGE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>763</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 75 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_NO_CALIB';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>764</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 76 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_ACCESS';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>765</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 77 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_CHANGEOVER_TIME';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>766</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 78 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_OVERVOLTAGE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>767</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 79 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_UNDERVOLTAGE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>768</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 80 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_STUCK_AT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>769</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 81 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_CONTROL_DITHER';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>770</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 82 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_SLOW_SIGNAL';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>771</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 83 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_DIAG_PRO_MODE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>772</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 84 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_WINDOW';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>773</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 85 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_SDO_IDX_NOT_EXIST';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>774</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 86 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_SDO_SUBIDX_NOT_EXIST';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>775</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 87 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_SDO_UNSUPPORTED_ACCESS';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>776</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 88 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_SDO_DATA_TYPE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>777</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 89 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_LOW_TEMPERATURE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>778</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 90 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_HIGH_TEMPERATURE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>779</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 91 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_INVALID_DITHER';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>780</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 92 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_INVALID_FREQUENCY';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>781</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 93 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_RANGE_OVERRUN';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>782</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 94 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_RANGE_UNDERRUN';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>783</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 95 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_INVALID_FILTER';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>784</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 96 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_COMPARE_MISMATCH';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>785</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 97 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_INVALID_IP_CFG';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>786</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 98 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_LOW_CURRENT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>787</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 99 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_AT_GROUP_OUTPUT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>788</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 100 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_SDO_UNKNOWN';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>789</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 101 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_BAUDRATE_INVALID_OR_ALREADY_SET';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>790</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 102 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_COMPARE_MISMATCH';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>791</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 103 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_COMPARE_MISMATCH_VSYS';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>792</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 104 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_GROUP_OVERLOAD_CURRENT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>793</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 105 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_GROUP_OVERLOAD_CURRENT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>794</v>
+      </c>
+      <c r="C108" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 106 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_PAUSED';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>795</v>
+      </c>
+      <c r="C109" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 107 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_ABORT';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>796</v>
+      </c>
+      <c r="C110" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 108 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_EVNT_OPEN_PLUG_STORAGE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>797</v>
+      </c>
+      <c r="C111" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 109 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_EVNT_OPEN_UNPLUG_STORAGE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>798</v>
+      </c>
+      <c r="C112" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 110 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_EVNT_OPEN_DONE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>799</v>
+      </c>
+      <c r="C113" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 111 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_EVNT_REGI_PLUG_STORAGE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>800</v>
+      </c>
+      <c r="C114" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 112 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_EVNT_REGI_UNPLUG_STORAGE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>801</v>
+      </c>
+      <c r="C115" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 113 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_EVNT_REGI_DONE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>802</v>
+      </c>
+      <c r="C116" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 114 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_EVNT_UNREGI';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
+        <v>803</v>
+      </c>
+      <c r="C117" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 115 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_EVNT_UNREGI_DONE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>804</v>
+      </c>
+      <c r="C118" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 116 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_EVNT_CLOSE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>117</v>
+      </c>
+      <c r="B119" t="s">
+        <v>805</v>
+      </c>
+      <c r="C119" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 117 THEN&lt;cr&gt;&lt;t&gt;TEXT:='STAT_EVNT_CLOSE_DONE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>806</v>
+      </c>
+      <c r="C120" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 118 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_INSTANCE_RESTRICTION';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121" t="s">
+        <v>807</v>
+      </c>
+      <c r="C121" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 119 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_NO_FILE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>808</v>
+      </c>
+      <c r="C122" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 120 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_EVNT_OPEN';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>809</v>
+      </c>
+      <c r="C123" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 121 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_EVNT_REGI';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>810</v>
+      </c>
+      <c r="C124" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 122 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_EVNT_UNREGI';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125" t="s">
+        <v>811</v>
+      </c>
+      <c r="C125" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 123 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_EVNT_CLOSE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126" t="s">
+        <v>812</v>
+      </c>
+      <c r="C126" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 124 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_GET_STORAGE_LIST';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>813</v>
+      </c>
+      <c r="C127" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 125 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_UNPLUG_STORAGE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128" t="s">
+        <v>814</v>
+      </c>
+      <c r="C128" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 126 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_INVALID_CHANNEL';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129" t="s">
+        <v>815</v>
+      </c>
+      <c r="C129" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 127 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_INVALID_MODE';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>128</v>
+      </c>
+      <c r="B130" t="s">
+        <v>816</v>
+      </c>
+      <c r="C130" t="str">
+        <f t="shared" si="1"/>
+        <v>IF CODE = 128 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_H_BRIDGE_TEST';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>129</v>
+      </c>
+      <c r="B131" t="s">
+        <v>817</v>
+      </c>
+      <c r="C131" t="str">
+        <f t="shared" ref="C131:C135" si="2">_xlfn.CONCAT("IF CODE = ",A131," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B131,"';&lt;cr&gt;END_IF;")</f>
+        <v>IF CODE = 129 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_GROUP_SW_TEST';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>130</v>
+      </c>
+      <c r="B132" t="s">
+        <v>818</v>
+      </c>
+      <c r="C132" t="str">
+        <f t="shared" si="2"/>
+        <v>IF CODE = 130 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_TX_ERROR';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>131</v>
+      </c>
+      <c r="B133" t="s">
+        <v>819</v>
+      </c>
+      <c r="C133" t="str">
+        <f t="shared" si="2"/>
+        <v>IF CODE = 131 THEN&lt;cr&gt;&lt;t&gt;TEXT:='ERR_RX_ERROR';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>132</v>
+      </c>
+      <c r="B134" t="s">
+        <v>820</v>
+      </c>
+      <c r="C134" t="str">
+        <f t="shared" si="2"/>
+        <v>IF CODE = 132 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_PHASE_MISSING_B';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>133</v>
+      </c>
+      <c r="B135" t="s">
+        <v>821</v>
+      </c>
+      <c r="C135" t="str">
+        <f t="shared" si="2"/>
+        <v>IF CODE = 133 THEN&lt;cr&gt;&lt;t&gt;TEXT:='DIAG_PHASE_TOO_MANY_B';&lt;cr&gt;END_IF;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C712512B-3394-456F-A3A8-618A03016890}">
   <dimension ref="B2:D31"/>
   <sheetViews>
@@ -8788,7 +10828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E538D0C9-5DB1-4DD2-BFB3-B509B6A8D4D3}">
   <dimension ref="A1:Q196"/>
   <sheetViews>
@@ -15023,7 +17063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D6A96C-314C-4D0F-A31C-2D0C36E8E519}">
   <dimension ref="A1:I59"/>
   <sheetViews>
@@ -16984,7 +19024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B17012-44D7-48B2-87FC-FA2A9133EF8D}">
   <dimension ref="A1:L65"/>
   <sheetViews>
@@ -19923,12 +21963,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
-  <dimension ref="A1:E68"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19953,7 +21994,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -19963,8 +22004,11 @@
       <c r="C2" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -19978,7 +22022,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -19988,8 +22032,11 @@
       <c r="C4" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -20003,7 +22050,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -20031,7 +22078,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -20045,7 +22092,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -20059,7 +22106,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -20073,7 +22120,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -20087,7 +22134,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -20101,7 +22148,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -20115,7 +22162,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -20129,7 +22176,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -20143,7 +22190,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -20168,7 +22215,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -20182,7 +22229,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -20199,7 +22246,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -20213,7 +22260,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -20227,7 +22274,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -20241,7 +22288,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -20258,7 +22305,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -20272,7 +22319,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -20308,7 +22355,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -20347,7 +22394,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -20355,13 +22402,16 @@
         <v>571</v>
       </c>
       <c r="C31" t="s">
+        <v>679</v>
+      </c>
+      <c r="D31" t="s">
+        <v>591</v>
+      </c>
+      <c r="E31" t="s">
         <v>680</v>
       </c>
-      <c r="E31" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -20400,10 +22450,10 @@
         <v>643</v>
       </c>
       <c r="E34" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -20431,7 +22481,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -20445,7 +22495,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -20459,7 +22509,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -20476,7 +22526,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -20493,7 +22543,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -20529,10 +22579,10 @@
         <v>634</v>
       </c>
       <c r="E43" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -20546,7 +22596,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -20563,7 +22613,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -20577,7 +22627,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -20587,8 +22637,11 @@
       <c r="C47" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -20602,7 +22655,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -20616,7 +22669,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -20630,10 +22683,10 @@
         <v>658</v>
       </c>
       <c r="E50" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -20647,7 +22700,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -20664,7 +22717,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -20674,8 +22727,11 @@
       <c r="C53" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -20685,8 +22741,11 @@
       <c r="C54" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -20700,7 +22759,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -20709,6 +22768,9 @@
       </c>
       <c r="C56" t="s">
         <v>657</v>
+      </c>
+      <c r="D56" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -20722,7 +22784,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -20741,13 +22803,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C59" t="s">
         <v>667</v>
       </c>
       <c r="E59" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -20755,13 +22817,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C60" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -20769,24 +22831,27 @@
         <v>598</v>
       </c>
       <c r="C61" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>670</v>
+      </c>
+      <c r="D61" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C62" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D62" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -20794,7 +22859,7 @@
         <v>569</v>
       </c>
       <c r="C63" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D63" t="s">
         <v>658</v>
@@ -20805,13 +22870,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>673</v>
+      </c>
+      <c r="C64" t="s">
+        <v>677</v>
+      </c>
+      <c r="E64" t="s">
         <v>674</v>
-      </c>
-      <c r="C64" t="s">
-        <v>678</v>
-      </c>
-      <c r="E64" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -20819,10 +22884,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C65" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -20830,13 +22895,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C66" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -20844,13 +22909,16 @@
         <v>569</v>
       </c>
       <c r="C67" t="s">
+        <v>684</v>
+      </c>
+      <c r="D67" t="s">
+        <v>658</v>
+      </c>
+      <c r="E67" t="s">
         <v>685</v>
       </c>
-      <c r="E67" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -20858,10 +22926,35 @@
         <v>569</v>
       </c>
       <c r="C68" t="s">
-        <v>684</v>
+        <v>683</v>
+      </c>
+      <c r="D68" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>823</v>
+      </c>
+      <c r="C69" t="s">
+        <v>824</v>
+      </c>
+      <c r="D69" t="s">
+        <v>591</v>
+      </c>
+      <c r="E69" t="s">
+        <v>825</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E68" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
+    <filterColumn colId="3">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
More small snags for UDP timeouts
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CA26CF-CC5C-4137-A6B4-453CF39415CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439F7255-F711-4FFF-9C43-164BBE7BCDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15345" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$78</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">SNAGS!$A$1:$E$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">SNAGS!$A$1:$E$70</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2293" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="827">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2525,6 +2525,9 @@
   </si>
   <si>
     <t>via critical shutdown signal</t>
+  </si>
+  <si>
+    <t>Check Tracks request is on to allow outputs to work</t>
   </si>
 </sst>
 </file>
@@ -3107,7 +3110,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V45" sqref="V45"/>
+      <selection pane="bottomLeft" activeCell="W54" sqref="W54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -21966,10 +21969,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22067,7 +22070,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -22076,6 +22079,9 @@
       </c>
       <c r="C7" s="33" t="s">
         <v>562</v>
+      </c>
+      <c r="D7" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22204,7 +22210,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -22213,6 +22219,9 @@
       </c>
       <c r="C17" s="33" t="s">
         <v>626</v>
+      </c>
+      <c r="D17" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22333,7 +22342,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -22342,6 +22351,9 @@
       </c>
       <c r="C26" t="s">
         <v>549</v>
+      </c>
+      <c r="D26" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -22439,7 +22451,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -22448,6 +22460,9 @@
       </c>
       <c r="C34" t="s">
         <v>643</v>
+      </c>
+      <c r="D34" t="s">
+        <v>591</v>
       </c>
       <c r="E34" t="s">
         <v>681</v>
@@ -22470,7 +22485,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -22479,6 +22494,9 @@
       </c>
       <c r="C36" t="s">
         <v>593</v>
+      </c>
+      <c r="D36" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22932,7 +22950,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>69</v>
       </c>
@@ -22949,8 +22967,16 @@
         <v>825</v>
       </c>
     </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>575</v>
+      </c>
+      <c r="C70" t="s">
+        <v>826</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E68" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
+  <autoFilter ref="A1:E70" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
@@ -22960,15 +22986,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -22984,6 +23001,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23210,14 +23236,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -23230,6 +23248,14 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
PLC - Move the Keyswitch Crank signal as it is already used on the radial! EXCEL - updated the IO! - renamed the side conveyor functions used for the radial functions on the other machine
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439F7255-F711-4FFF-9C43-164BBE7BCDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F13699-A317-4824-A6C8-7AB1EAC3EEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="830">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2528,6 +2528,15 @@
   </si>
   <si>
     <t>Check Tracks request is on to allow outputs to work</t>
+  </si>
+  <si>
+    <t>Radial_RightLimitSwitch</t>
+  </si>
+  <si>
+    <t>Radial_LeftLimitSwitch</t>
+  </si>
+  <si>
+    <t>MachineMode</t>
   </si>
 </sst>
 </file>
@@ -3103,14 +3112,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4EBF08-015A-4388-B8C8-8A07CE5EF3C7}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W54" sqref="W54"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3199,7 +3208,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>93</v>
       </c>
@@ -3275,7 +3284,7 @@
         <v>CHASSIS.IN0100.Init(Machine_IO.Inputs.ESTOP_OK);</v>
       </c>
     </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>93</v>
       </c>
@@ -3351,7 +3360,7 @@
         <v>CHASSIS.IN0101.Init(Machine_IO.Inputs.DRUM_PRESSURE);</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>93</v>
       </c>
@@ -3387,36 +3396,36 @@
         <v>CHASSIS.IN0102</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>600</v>
+        <v>827</v>
       </c>
       <c r="L4" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>KEYSWITCH_CRANKING</v>
+        <v>RADIAL_RIGHTLIMITSWITCH</v>
       </c>
       <c r="M4" s="19"/>
       <c r="N4" s="20" t="str">
         <f t="shared" si="8"/>
-        <v>KEYSWITCH_CRANKING:IpCom; // CHASSIS IN0102</v>
+        <v>RADIAL_RIGHTLIMITSWITCH:IpCom; // CHASSIS IN0102</v>
       </c>
       <c r="O4" s="20" t="str">
         <f t="shared" si="9"/>
-        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING</v>
+        <v>Machine_IO.Inputs.RADIAL_RIGHTLIMITSWITCH</v>
       </c>
       <c r="P4" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING.Dig</v>
+        <v>Machine_IO.Inputs.RADIAL_RIGHTLIMITSWITCH.Dig</v>
       </c>
       <c r="Q4" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING(); // CR0709.IN0102</v>
+        <v>Machine_IO.Inputs.RADIAL_RIGHTLIMITSWITCH(); // CR0709.IN0102</v>
       </c>
       <c r="R4" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING.Init('CHASSIS','KEYSWITCH_CRANKING','IN0102','a65',NVL_IO_CHASSIS.All_Inputs.IN0102,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.RADIAL_RIGHTLIMITSWITCH.Init('CHASSIS','RADIAL_RIGHTLIMITSWITCH','IN0102','a65',NVL_IO_CHASSIS.All_Inputs.IN0102,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="S4" s="20" t="str">
         <f t="shared" si="3"/>
-        <v>KEYSWITCH_CRANKING: Mimic_Input_FB; // CHASSIS:IN0102</v>
+        <v>Radial_RightLimitSwitch: Mimic_Input_FB; // CHASSIS:IN0102</v>
       </c>
       <c r="T4" s="20" t="str">
         <f t="shared" si="4"/>
@@ -3424,10 +3433,10 @@
       </c>
       <c r="U4" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>CHASSIS.IN0102.Init(Machine_IO.Inputs.KEYSWITCH_CRANKING);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>CHASSIS.IN0102.Init(Machine_IO.Inputs.RADIAL_RIGHTLIMITSWITCH);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>93</v>
       </c>
@@ -3462,35 +3471,37 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0103</v>
       </c>
-      <c r="K5" s="19"/>
+      <c r="K5" s="19" t="s">
+        <v>828</v>
+      </c>
       <c r="L5" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>SPARE_IN0103</v>
+        <v>RADIAL_LEFTLIMITSWITCH</v>
       </c>
       <c r="M5" s="19"/>
       <c r="N5" s="20" t="str">
         <f t="shared" si="8"/>
-        <v>SPARE_IN0103:IpCom; // CHASSIS IN0103</v>
+        <v>RADIAL_LEFTLIMITSWITCH:IpCom; // CHASSIS IN0103</v>
       </c>
       <c r="O5" s="20" t="str">
         <f t="shared" si="9"/>
-        <v>Machine_IO.Inputs.SPARE_IN0103</v>
+        <v>Machine_IO.Inputs.RADIAL_LEFTLIMITSWITCH</v>
       </c>
       <c r="P5" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.SPARE_IN0103.Dig</v>
+        <v>Machine_IO.Inputs.RADIAL_LEFTLIMITSWITCH.Dig</v>
       </c>
       <c r="Q5" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>Machine_IO.Inputs.SPARE_IN0103(); // CR0709.IN0103</v>
+        <v>Machine_IO.Inputs.RADIAL_LEFTLIMITSWITCH(); // CR0709.IN0103</v>
       </c>
       <c r="R5" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>Machine_IO.Inputs.SPARE_IN0103.Init('CHASSIS','SPARE_IN0103','IN0103','a66',NVL_IO_CHASSIS.All_Inputs.IN0103,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.RADIAL_LEFTLIMITSWITCH.Init('CHASSIS','RADIAL_LEFTLIMITSWITCH','IN0103','a66',NVL_IO_CHASSIS.All_Inputs.IN0103,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="S5" s="20" t="str">
         <f t="shared" si="3"/>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0103</v>
+        <v>Radial_LeftLimitSwitch: Mimic_Input_FB; // CHASSIS:IN0103</v>
       </c>
       <c r="T5" s="20" t="str">
         <f t="shared" si="4"/>
@@ -3498,10 +3509,10 @@
       </c>
       <c r="U5" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>CHASSIS.IN0103.Init(Machine_IO.Inputs.SPARE_IN0103);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+        <v>CHASSIS.IN0103.Init(Machine_IO.Inputs.RADIAL_LEFTLIMITSWITCH);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>93</v>
       </c>
@@ -3536,35 +3547,37 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0200</v>
       </c>
-      <c r="K6" s="19"/>
+      <c r="K6" s="19" t="s">
+        <v>829</v>
+      </c>
       <c r="L6" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>SPARE_IN0200</v>
+        <v>MACHINEMODE</v>
       </c>
       <c r="M6" s="19"/>
       <c r="N6" s="20" t="str">
         <f t="shared" si="8"/>
-        <v>SPARE_IN0200:IpCom; // CHASSIS IN0200</v>
+        <v>MACHINEMODE:IpCom; // CHASSIS IN0200</v>
       </c>
       <c r="O6" s="20" t="str">
         <f t="shared" si="9"/>
-        <v>Machine_IO.Inputs.SPARE_IN0200</v>
+        <v>Machine_IO.Inputs.MACHINEMODE</v>
       </c>
       <c r="P6" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.SPARE_IN0200.Dig</v>
+        <v>Machine_IO.Inputs.MACHINEMODE.Dig</v>
       </c>
       <c r="Q6" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>Machine_IO.Inputs.SPARE_IN0200(); // CR0709.IN0200</v>
+        <v>Machine_IO.Inputs.MACHINEMODE(); // CR0709.IN0200</v>
       </c>
       <c r="R6" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>Machine_IO.Inputs.SPARE_IN0200.Init('CHASSIS','SPARE_IN0200','IN0200','a67',NVL_IO_CHASSIS.All_Inputs.IN0200,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.MACHINEMODE.Init('CHASSIS','MACHINEMODE','IN0200','a67',NVL_IO_CHASSIS.All_Inputs.IN0200,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="S6" s="20" t="str">
         <f t="shared" si="3"/>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0200</v>
+        <v>MachineMode: Mimic_Input_FB; // CHASSIS:IN0200</v>
       </c>
       <c r="T6" s="20" t="str">
         <f t="shared" si="4"/>
@@ -3572,10 +3585,10 @@
       </c>
       <c r="U6" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>CHASSIS.IN0200.Init(Machine_IO.Inputs.SPARE_IN0200);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>CHASSIS.IN0200.Init(Machine_IO.Inputs.MACHINEMODE);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>93</v>
       </c>
@@ -3610,35 +3623,37 @@
         <f t="shared" si="1"/>
         <v>CHASSIS.IN0201</v>
       </c>
-      <c r="K7" s="19"/>
+      <c r="K7" s="31" t="s">
+        <v>600</v>
+      </c>
       <c r="L7" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>SPARE_IN0201</v>
+        <v>KEYSWITCH_CRANKING</v>
       </c>
       <c r="M7" s="19"/>
       <c r="N7" s="20" t="str">
         <f t="shared" si="8"/>
-        <v>SPARE_IN0201:IpCom; // CHASSIS IN0201</v>
+        <v>KEYSWITCH_CRANKING:IpCom; // CHASSIS IN0201</v>
       </c>
       <c r="O7" s="20" t="str">
         <f t="shared" si="9"/>
-        <v>Machine_IO.Inputs.SPARE_IN0201</v>
+        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING</v>
       </c>
       <c r="P7" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.SPARE_IN0201.Dig</v>
+        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING.Dig</v>
       </c>
       <c r="Q7" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>Machine_IO.Inputs.SPARE_IN0201(); // CR0709.IN0201</v>
+        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING(); // CR0709.IN0201</v>
       </c>
       <c r="R7" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>Machine_IO.Inputs.SPARE_IN0201.Init('CHASSIS','SPARE_IN0201','IN0201','a68',NVL_IO_CHASSIS.All_Inputs.IN0201,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.KEYSWITCH_CRANKING.Init('CHASSIS','KEYSWITCH_CRANKING','IN0201','a68',NVL_IO_CHASSIS.All_Inputs.IN0201,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="S7" s="20" t="str">
         <f t="shared" si="3"/>
-        <v>: Mimic_Input_FB; // CHASSIS:IN0201</v>
+        <v>KEYSWITCH_CRANKING: Mimic_Input_FB; // CHASSIS:IN0201</v>
       </c>
       <c r="T7" s="20" t="str">
         <f t="shared" si="4"/>
@@ -3646,10 +3661,10 @@
       </c>
       <c r="U7" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>CHASSIS.IN0201.Init(Machine_IO.Inputs.SPARE_IN0201);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+        <v>CHASSIS.IN0201.Init(Machine_IO.Inputs.KEYSWITCH_CRANKING);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>93</v>
       </c>
@@ -3723,7 +3738,7 @@
         <v>CHASSIS.IN0202.Init(Machine_IO.Inputs.SPARE_IN0202);</v>
       </c>
     </row>
-    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>93</v>
       </c>
@@ -3797,7 +3812,7 @@
         <v>CHASSIS.IN0203.Init(Machine_IO.Inputs.SPARE_IN0203);</v>
       </c>
     </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>93</v>
       </c>
@@ -3871,7 +3886,7 @@
         <v>CHASSIS.IN0600.Init(Machine_IO.Inputs.SPARE_IN0600);</v>
       </c>
     </row>
-    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>93</v>
       </c>
@@ -3945,7 +3960,7 @@
         <v>CHASSIS.IN0601.Init(Machine_IO.Inputs.SPARE_IN0601);</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>93</v>
       </c>
@@ -4019,7 +4034,7 @@
         <v>CHASSIS.IN0602.Init(Machine_IO.Inputs.SPARE_IN0602);</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>93</v>
       </c>
@@ -4093,7 +4108,7 @@
         <v>CHASSIS.IN0603.Init(Machine_IO.Inputs.SPARE_IN0603);</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>93</v>
       </c>
@@ -4167,7 +4182,7 @@
         <v>CHASSIS.IN0700.Init(Machine_IO.Inputs.SPARE_IN0700);</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>93</v>
       </c>
@@ -4243,7 +4258,7 @@
         <v>CHASSIS.IN0701.Init(Machine_IO.Inputs.RADIORHS_JACKLEGRAISE_REQ);</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>93</v>
       </c>
@@ -4319,7 +4334,7 @@
         <v>CHASSIS.IN0702.Init(Machine_IO.Inputs.RHS_TROMMELDOORSW);</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>93</v>
       </c>
@@ -4395,7 +4410,7 @@
         <v>CHASSIS.IN0703.Init(Machine_IO.Inputs.LHS_TROMMELDOORSW);</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>93</v>
       </c>
@@ -4471,7 +4486,7 @@
         <v>CHASSIS.IN0000.Init(Machine_IO.Inputs.HYDOILTEMP_SW);</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>93</v>
       </c>
@@ -4547,7 +4562,7 @@
         <v>CHASSIS.IN0001.Init(Machine_IO.Inputs.HYDOILLEVEL_SW);</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>93</v>
       </c>
@@ -4623,7 +4638,7 @@
         <v>CHASSIS.IN0002.Init(Machine_IO.Inputs.THERMOSTAT);</v>
       </c>
     </row>
-    <row r="21" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>93</v>
       </c>
@@ -4698,7 +4713,7 @@
         <v>CHASSIS.IN0003.Init(Machine_IO.Inputs.RADIORHS_JACKLEGLOWER_REQ);</v>
       </c>
     </row>
-    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>93</v>
       </c>
@@ -4774,7 +4789,7 @@
         <v>CHASSIS.IN0500.Init(Machine_IO.Inputs.RADIOLHS_JACKLEGRAISE_REQ);</v>
       </c>
     </row>
-    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>93</v>
       </c>
@@ -4850,7 +4865,7 @@
         <v>CHASSIS.IN0501.Init(Machine_IO.Inputs.RADIOLHS_JACKLEGLOWER_REQ);</v>
       </c>
     </row>
-    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>93</v>
       </c>
@@ -4926,7 +4941,7 @@
         <v>CHASSIS.IN0502.Init(Machine_IO.Inputs.RADIOSIDECONVRAISEREQ);</v>
       </c>
     </row>
-    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>93</v>
       </c>
@@ -5002,7 +5017,7 @@
         <v>CHASSIS.IN0503.Init(Machine_IO.Inputs.RADIOSIDECONVLOWERREQ);</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>93</v>
       </c>
@@ -5076,7 +5091,7 @@
         <v>CHASSIS.IN0400.Init(Machine_IO.Inputs.SPARE_IN0400);</v>
       </c>
     </row>
-    <row r="27" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>93</v>
       </c>
@@ -5152,7 +5167,7 @@
         <v>CHASSIS.IN0401.Init(Machine_IO.Inputs.FUELLEVEL_PERCENT);</v>
       </c>
     </row>
-    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>93</v>
       </c>
@@ -5226,7 +5241,7 @@
         <v>CHASSIS.IN0900.Init(Machine_IO.Inputs.UMBTRACKREQ);</v>
       </c>
     </row>
-    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>93</v>
       </c>
@@ -5300,7 +5315,7 @@
         <v>CHASSIS.IN0901.Init(Machine_IO.Inputs.UMBMACHINESTOP);</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>93</v>
       </c>
@@ -5374,7 +5389,7 @@
         <v>CHASSIS.IN0300.Init(Machine_IO.Inputs.RTF_REQ);</v>
       </c>
     </row>
-    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>93</v>
       </c>
@@ -5448,7 +5463,7 @@
         <v>CHASSIS.IN0301.Init(Machine_IO.Inputs.RTR_REQ);</v>
       </c>
     </row>
-    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>93</v>
       </c>
@@ -5522,7 +5537,7 @@
         <v>CHASSIS.IN0800.Init(Machine_IO.Inputs.LTF_REQ);</v>
       </c>
     </row>
-    <row r="33" spans="1:22" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>93</v>
       </c>
@@ -6322,7 +6337,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="43" spans="1:22" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>93</v>
       </c>
@@ -7121,7 +7136,7 @@
         <v>CHASSIS.OUT0108.Init(Machine_IO.Outputs.SIDETRANSFERON_OP);</v>
       </c>
     </row>
-    <row r="53" spans="1:22" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>93</v>
       </c>
@@ -7911,7 +7926,7 @@
         <v>CHASSIS.OUT0208.Init(Machine_IO.Outputs.ECUENABLE);</v>
       </c>
     </row>
-    <row r="63" spans="1:22" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
         <v>93</v>
       </c>
@@ -8977,14 +8992,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP78" xr:uid="{1E4EBF08-015A-4388-B8C8-8A07CE5EF3C7}">
-    <filterColumn colId="5">
-      <filters blank="1">
-        <filter val="OUT"/>
-        <filter val="OUTA"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AP78" xr:uid="{1E4EBF08-015A-4388-B8C8-8A07CE5EF3C7}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.23622047244094488" right="0.23622047244094488" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="71" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -21971,7 +21979,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
@@ -22986,6 +22994,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -23001,15 +23018,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23236,6 +23244,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -23248,14 +23264,6 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
radial code in - ready for site test tomorrow
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F13699-A317-4824-A6C8-7AB1EAC3EEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35475C7-3A8E-471F-B366-75B19A31533F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" tabRatio="857" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$78</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">SNAGS!$A$1:$E$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">SNAGS!$A$1:$E$71</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="832">
   <si>
     <t>PLC Name</t>
   </si>
@@ -1153,12 +1153,6 @@
     <t>RadioLHS_JackLegLower_Req</t>
   </si>
   <si>
-    <t>RadioSideConvRaiseReq</t>
-  </si>
-  <si>
-    <t>RadioSideConvLowerReq</t>
-  </si>
-  <si>
     <t>FuelLevel_Percent</t>
   </si>
   <si>
@@ -1915,12 +1909,6 @@
     <t>FAN_REVERSE</t>
   </si>
   <si>
-    <t>SIDE_CONV_RAISE</t>
-  </si>
-  <si>
-    <t>SIDE_CONV_LOWER</t>
-  </si>
-  <si>
     <t>CR0403 8 outputs</t>
   </si>
   <si>
@@ -2537,6 +2525,24 @@
   </si>
   <si>
     <t>MachineMode</t>
+  </si>
+  <si>
+    <t>SideConvRaise_RadialMoveLeft</t>
+  </si>
+  <si>
+    <t>SideConvLower_RadialMoveRight</t>
+  </si>
+  <si>
+    <t>Show door status on the main page</t>
+  </si>
+  <si>
+    <t>SIDE_CONV_RAISE_RADIAL_LEFT</t>
+  </si>
+  <si>
+    <t>SIDE_CONV_LOWER_RADIAL_RIGHT</t>
+  </si>
+  <si>
+    <t>MAIN_MIMIC</t>
   </si>
 </sst>
 </file>
@@ -3117,9 +3123,9 @@
   </sheetPr>
   <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3396,7 +3402,7 @@
         <v>CHASSIS.IN0102</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="L4" s="19" t="str">
         <f t="shared" si="7"/>
@@ -3472,7 +3478,7 @@
         <v>CHASSIS.IN0103</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="L5" s="19" t="str">
         <f t="shared" si="7"/>
@@ -3548,7 +3554,7 @@
         <v>CHASSIS.IN0200</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="L6" s="19" t="str">
         <f t="shared" si="7"/>
@@ -3624,7 +3630,7 @@
         <v>CHASSIS.IN0201</v>
       </c>
       <c r="K7" s="31" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L7" s="19" t="str">
         <f t="shared" si="7"/>
@@ -4901,36 +4907,36 @@
         <v>CHASSIS.IN0502</v>
       </c>
       <c r="K24" s="32" t="s">
-        <v>368</v>
+        <v>826</v>
       </c>
       <c r="L24" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>RADIOSIDECONVRAISEREQ</v>
+        <v>SIDECONVRAISE_RADIALMOVELEFT</v>
       </c>
       <c r="M24" s="19"/>
       <c r="N24" s="20" t="str">
         <f t="shared" si="8"/>
-        <v>RADIOSIDECONVRAISEREQ:IpCom; // CHASSIS IN0502</v>
+        <v>SIDECONVRAISE_RADIALMOVELEFT:IpCom; // CHASSIS IN0502</v>
       </c>
       <c r="O24" s="20" t="str">
         <f t="shared" si="9"/>
-        <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ</v>
+        <v>Machine_IO.Inputs.SIDECONVRAISE_RADIALMOVELEFT</v>
       </c>
       <c r="P24" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ.Dig</v>
+        <v>Machine_IO.Inputs.SIDECONVRAISE_RADIALMOVELEFT.Dig</v>
       </c>
       <c r="Q24" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ(); // CR0709.IN0502</v>
+        <v>Machine_IO.Inputs.SIDECONVRAISE_RADIALMOVELEFT(); // CR0709.IN0502</v>
       </c>
       <c r="R24" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>Machine_IO.Inputs.RADIOSIDECONVRAISEREQ.Init('CHASSIS','RADIOSIDECONVRAISEREQ','IN0502','a42',NVL_IO_CHASSIS.All_Inputs.IN0502,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SIDECONVRAISE_RADIALMOVELEFT.Init('CHASSIS','SIDECONVRAISE_RADIALMOVELEFT','IN0502','a42',NVL_IO_CHASSIS.All_Inputs.IN0502,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="S24" s="20" t="str">
         <f t="shared" si="3"/>
-        <v>RadioSideConvRaiseReq: Mimic_Input_FB; // CHASSIS:IN0502</v>
+        <v>SideConvRaise_RadialMoveLeft: Mimic_Input_FB; // CHASSIS:IN0502</v>
       </c>
       <c r="T24" s="20" t="str">
         <f t="shared" si="4"/>
@@ -4938,7 +4944,7 @@
       </c>
       <c r="U24" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>CHASSIS.IN0502.Init(Machine_IO.Inputs.RADIOSIDECONVRAISEREQ);</v>
+        <v>CHASSIS.IN0502.Init(Machine_IO.Inputs.SIDECONVRAISE_RADIALMOVELEFT);</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
@@ -4977,36 +4983,36 @@
         <v>CHASSIS.IN0503</v>
       </c>
       <c r="K25" s="32" t="s">
-        <v>369</v>
+        <v>827</v>
       </c>
       <c r="L25" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>RADIOSIDECONVLOWERREQ</v>
+        <v>SIDECONVLOWER_RADIALMOVERIGHT</v>
       </c>
       <c r="M25" s="19"/>
       <c r="N25" s="20" t="str">
         <f t="shared" si="8"/>
-        <v>RADIOSIDECONVLOWERREQ:IpCom; // CHASSIS IN0503</v>
+        <v>SIDECONVLOWER_RADIALMOVERIGHT:IpCom; // CHASSIS IN0503</v>
       </c>
       <c r="O25" s="20" t="str">
         <f t="shared" si="9"/>
-        <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ</v>
+        <v>Machine_IO.Inputs.SIDECONVLOWER_RADIALMOVERIGHT</v>
       </c>
       <c r="P25" s="20" t="str">
         <f t="shared" si="10"/>
-        <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ.Dig</v>
+        <v>Machine_IO.Inputs.SIDECONVLOWER_RADIALMOVERIGHT.Dig</v>
       </c>
       <c r="Q25" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ(); // CR0709.IN0503</v>
+        <v>Machine_IO.Inputs.SIDECONVLOWER_RADIALMOVERIGHT(); // CR0709.IN0503</v>
       </c>
       <c r="R25" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>Machine_IO.Inputs.RADIOSIDECONVLOWERREQ.Init('CHASSIS','RADIOSIDECONVLOWERREQ','IN0503','a43',NVL_IO_CHASSIS.All_Inputs.IN0503,Machine_IO.Node_CHASSIS);</v>
+        <v>Machine_IO.Inputs.SIDECONVLOWER_RADIALMOVERIGHT.Init('CHASSIS','SIDECONVLOWER_RADIALMOVERIGHT','IN0503','a43',NVL_IO_CHASSIS.All_Inputs.IN0503,Machine_IO.Node_CHASSIS);</v>
       </c>
       <c r="S25" s="20" t="str">
         <f t="shared" si="3"/>
-        <v>RadioSideConvLowerReq: Mimic_Input_FB; // CHASSIS:IN0503</v>
+        <v>SideConvLower_RadialMoveRight: Mimic_Input_FB; // CHASSIS:IN0503</v>
       </c>
       <c r="T25" s="20" t="str">
         <f t="shared" si="4"/>
@@ -5014,7 +5020,7 @@
       </c>
       <c r="U25" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>CHASSIS.IN0503.Init(Machine_IO.Inputs.RADIOSIDECONVLOWERREQ);</v>
+        <v>CHASSIS.IN0503.Init(Machine_IO.Inputs.SIDECONVLOWER_RADIALMOVERIGHT);</v>
       </c>
     </row>
     <row r="26" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5127,7 +5133,7 @@
         <v>CHASSIS.IN0401</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L27" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5201,7 +5207,7 @@
         <v>CHASSIS.IN0900</v>
       </c>
       <c r="K28" s="31" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L28" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5275,7 +5281,7 @@
         <v>CHASSIS.IN0901</v>
       </c>
       <c r="K29" s="31" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L29" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5349,7 +5355,7 @@
         <v>CHASSIS.IN0300</v>
       </c>
       <c r="K30" s="31" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L30" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5423,7 +5429,7 @@
         <v>CHASSIS.IN0301</v>
       </c>
       <c r="K31" s="31" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="L31" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5497,7 +5503,7 @@
         <v>CHASSIS.IN0800</v>
       </c>
       <c r="K32" s="31" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="L32" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5571,7 +5577,7 @@
         <v>CHASSIS.IN0801</v>
       </c>
       <c r="K33" s="31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L33" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5640,14 +5646,14 @@
         <v>PWM 2.5A</v>
       </c>
       <c r="I34" s="30" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="J34" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0000</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="L34" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5690,7 +5696,7 @@
         <v>CHASSIS.OUT0000.Init(Machine_IO.Outputs.TAILCONVSPD_MA);</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="35" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5729,7 +5735,7 @@
         <v>CHASSIS.OUT0001</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="L35" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5801,14 +5807,14 @@
         <v>PWM 2.5A</v>
       </c>
       <c r="I36" s="30" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="J36" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0002</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L36" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5851,7 +5857,7 @@
         <v>CHASSIS.OUT0002.Init(Machine_IO.Outputs.SIDECONVSPD_MA);</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="37" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5890,7 +5896,7 @@
         <v>CHASSIS.OUT0003</v>
       </c>
       <c r="K37" s="19" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L37" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5962,14 +5968,14 @@
         <v>PWM 2.5A</v>
       </c>
       <c r="I38" s="30" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="J38" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0004</v>
       </c>
       <c r="K38" s="19" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L38" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6012,7 +6018,7 @@
         <v>CHASSIS.OUT0004.Init(Machine_IO.Outputs.SIDETRANSFERSPD_MA);</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="39" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6051,7 +6057,7 @@
         <v>CHASSIS.OUT0005</v>
       </c>
       <c r="K39" s="19" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L39" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6130,7 +6136,7 @@
         <v>CHASSIS.OUT0006</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L40" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6202,14 +6208,14 @@
         <v>PWM 4A</v>
       </c>
       <c r="I41" s="30" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="J41" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0007</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L41" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6252,7 +6258,7 @@
         <v>CHASSIS.OUT0007.Init(Machine_IO.Outputs.COLLECTIONCONVSPD_MA);</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="42" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6291,7 +6297,7 @@
         <v>CHASSIS.OUT0008</v>
       </c>
       <c r="K42" s="19" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L42" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6334,7 +6340,7 @@
         <v>CHASSIS.OUT0008.Init(Machine_IO.Outputs.COLLECTIONCONVON_OP);</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="43" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6373,7 +6379,7 @@
         <v>CHASSIS.GROUP0</v>
       </c>
       <c r="K43" s="19" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="L43" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6445,14 +6451,14 @@
         <v>PWM 2.5A</v>
       </c>
       <c r="I44" s="30" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="J44" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0100</v>
       </c>
       <c r="K44" s="19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L44" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6495,7 +6501,7 @@
         <v>CHASSIS.OUT0100.Init(Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT);</v>
       </c>
       <c r="V44" s="4" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6534,7 +6540,7 @@
         <v>CHASSIS.OUT0101</v>
       </c>
       <c r="K45" s="31" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L45" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6606,14 +6612,14 @@
         <v>PWM 2.5A</v>
       </c>
       <c r="I46" s="30" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="J46" s="21" t="str">
         <f t="shared" si="1"/>
         <v>CHASSIS.OUT0102</v>
       </c>
       <c r="K46" s="19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="L46" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6656,7 +6662,7 @@
         <v>CHASSIS.OUT0102.Init(Machine_IO.Outputs.FEEDERSPD_MA);</v>
       </c>
       <c r="V46" s="2" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="47" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6695,7 +6701,7 @@
         <v>CHASSIS.OUT0103</v>
       </c>
       <c r="K47" s="31" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L47" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6774,7 +6780,7 @@
         <v>CHASSIS.OUT0104</v>
       </c>
       <c r="K48" s="19" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="L48" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6853,7 +6859,7 @@
         <v>CHASSIS.OUT0105</v>
       </c>
       <c r="K49" s="19" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L49" s="19" t="str">
         <f t="shared" si="7"/>
@@ -6932,7 +6938,7 @@
         <v>CHASSIS.OUT0106</v>
       </c>
       <c r="K50" s="19" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L50" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7011,7 +7017,7 @@
         <v>CHASSIS.OUT0107</v>
       </c>
       <c r="K51" s="19" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="L51" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7054,7 +7060,7 @@
         <v>CHASSIS.OUT0107.Init(Machine_IO.Outputs.SIDECONVON_OP);</v>
       </c>
       <c r="V51" s="4" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
@@ -7093,7 +7099,7 @@
         <v>CHASSIS.OUT0108</v>
       </c>
       <c r="K52" s="19" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L52" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7172,7 +7178,7 @@
         <v>CHASSIS.GROUP1</v>
       </c>
       <c r="K53" s="19" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="L53" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7251,7 +7257,7 @@
         <v>CHASSIS.OUT0200</v>
       </c>
       <c r="K54" s="31" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="L54" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7330,7 +7336,7 @@
         <v>CHASSIS.OUT0201</v>
       </c>
       <c r="K55" s="31" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="L55" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7409,7 +7415,7 @@
         <v>CHASSIS.OUT0202</v>
       </c>
       <c r="K56" s="31" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L56" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7488,7 +7494,7 @@
         <v>CHASSIS.OUT0203</v>
       </c>
       <c r="K57" s="31" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L57" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7567,7 +7573,7 @@
         <v>CHASSIS.OUT0204</v>
       </c>
       <c r="K58" s="31" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L58" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7646,7 +7652,7 @@
         <v>CHASSIS.OUT0205</v>
       </c>
       <c r="K59" s="31" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L59" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7725,7 +7731,7 @@
         <v>CHASSIS.OUT0206</v>
       </c>
       <c r="K60" s="19" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L60" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7804,7 +7810,7 @@
         <v>CHASSIS.OUT0207</v>
       </c>
       <c r="K61" s="19" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L61" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7883,7 +7889,7 @@
         <v>CHASSIS.OUT0208</v>
       </c>
       <c r="K62" s="31" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="L62" s="19" t="str">
         <f t="shared" si="7"/>
@@ -7962,7 +7968,7 @@
         <v>CHASSIS.GROUP2</v>
       </c>
       <c r="K63" s="19" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="L63" s="19" t="str">
         <f t="shared" si="7"/>
@@ -8177,14 +8183,14 @@
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="17" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="E67" s="17" t="str">
         <f t="shared" ref="E67:E74" si="20">_xlfn.CONCAT(B67,".",D67)</f>
@@ -8201,7 +8207,7 @@
         <v>AUX.OP0</v>
       </c>
       <c r="K67" s="19" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L67" s="19" t="str">
         <f t="shared" ref="L67" si="22">IF(K67&lt;&gt;"",UPPER(K67),_xlfn.CONCAT("SPARE_",D67))</f>
@@ -8246,14 +8252,14 @@
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C68" s="19"/>
       <c r="D68" s="17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E68" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8313,14 +8319,14 @@
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="17" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E69" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8380,14 +8386,14 @@
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="17" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E70" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8404,7 +8410,7 @@
         <v>AUX.OP3</v>
       </c>
       <c r="K70" s="19" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="L70" s="19" t="str">
         <f t="shared" si="33"/>
@@ -8449,14 +8455,14 @@
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="17" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E71" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8473,7 +8479,7 @@
         <v>AUX.OP4</v>
       </c>
       <c r="K71" s="19" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="L71" s="19" t="str">
         <f t="shared" si="33"/>
@@ -8518,14 +8524,14 @@
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C72" s="19"/>
       <c r="D72" s="17" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E72" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8542,7 +8548,7 @@
         <v>AUX.OP5</v>
       </c>
       <c r="K72" s="19" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="L72" s="19" t="str">
         <f t="shared" ref="L72:L75" si="44">IF(K72&lt;&gt;"",UPPER(K72),_xlfn.CONCAT("SPARE_",D72))</f>
@@ -8587,14 +8593,14 @@
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C73" s="19"/>
       <c r="D73" s="17" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E73" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8611,39 +8617,39 @@
         <v>AUX.OP6</v>
       </c>
       <c r="K73" s="19" t="s">
-        <v>622</v>
+        <v>829</v>
       </c>
       <c r="L73" s="19" t="str">
         <f t="shared" si="44"/>
-        <v>SIDE_CONV_RAISE</v>
+        <v>SIDE_CONV_RAISE_RADIAL_LEFT</v>
       </c>
       <c r="M73" s="19" t="str">
         <f t="shared" si="45"/>
-        <v>SIDE_CONV_RAISE:BOOL;</v>
+        <v>SIDE_CONV_RAISE_RADIAL_LEFT:BOOL;</v>
       </c>
       <c r="N73" s="20" t="str">
         <f t="shared" si="46"/>
-        <v>SIDE_CONV_RAISE:OpCom; // AUX.OP6</v>
+        <v>SIDE_CONV_RAISE_RADIAL_LEFT:OpCom; // AUX.OP6</v>
       </c>
       <c r="O73" s="20" t="str">
         <f t="shared" si="47"/>
-        <v>Machine_IO.Outputs.SIDE_CONV_RAISE</v>
+        <v>Machine_IO.Outputs.SIDE_CONV_RAISE_RADIAL_LEFT</v>
       </c>
       <c r="P73" s="20" t="str">
         <f t="shared" si="48"/>
-        <v>Machine_IO.Outputs.SIDE_CONV_RAISE.Dig</v>
+        <v>Machine_IO.Outputs.SIDE_CONV_RAISE_RADIAL_LEFT.Dig</v>
       </c>
       <c r="Q73" s="20" t="str">
         <f t="shared" si="49"/>
-        <v>Machine_IO.Outputs.SIDE_CONV_RAISE(); // CR0403.OP6</v>
+        <v>Machine_IO.Outputs.SIDE_CONV_RAISE_RADIAL_LEFT(); // CR0403.OP6</v>
       </c>
       <c r="R73" s="20" t="str">
         <f t="shared" si="50"/>
-        <v>Machine_IO.Outputs.SIDE_CONV_RAISE.Init('AUX','SIDE_CONV_RAISE','OP6','',NVL_Outputs_States_AUX.All.OP6,NVL_IO_CHASSIS.All_Outputs_Diag.OP6,Machine_IO.Node_AUX);</v>
+        <v>Machine_IO.Outputs.SIDE_CONV_RAISE_RADIAL_LEFT.Init('AUX','SIDE_CONV_RAISE_RADIAL_LEFT','OP6','',NVL_Outputs_States_AUX.All.OP6,NVL_IO_CHASSIS.All_Outputs_Diag.OP6,Machine_IO.Node_AUX);</v>
       </c>
       <c r="S73" s="20" t="str">
         <f t="shared" si="51"/>
-        <v>SIDE_CONV_RAISE: Mimic_Output_FB; // AUX:OP6</v>
+        <v>SIDE_CONV_RAISE_RADIAL_LEFT: Mimic_Output_FB; // AUX:OP6</v>
       </c>
       <c r="T73" s="20" t="str">
         <f t="shared" si="52"/>
@@ -8651,19 +8657,19 @@
       </c>
       <c r="U73" s="20" t="str">
         <f t="shared" si="53"/>
-        <v>AUX.OP6.Init(Machine_IO.Outputs.SIDE_CONV_RAISE);</v>
+        <v>AUX.OP6.Init(Machine_IO.Outputs.SIDE_CONV_RAISE_RADIAL_LEFT);</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C74" s="19"/>
       <c r="D74" s="17" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="E74" s="17" t="str">
         <f t="shared" si="20"/>
@@ -8680,39 +8686,39 @@
         <v>AUX.OP7</v>
       </c>
       <c r="K74" s="19" t="s">
-        <v>623</v>
+        <v>830</v>
       </c>
       <c r="L74" s="19" t="str">
         <f t="shared" si="44"/>
-        <v>SIDE_CONV_LOWER</v>
+        <v>SIDE_CONV_LOWER_RADIAL_RIGHT</v>
       </c>
       <c r="M74" s="19" t="str">
         <f t="shared" si="45"/>
-        <v>SIDE_CONV_LOWER:BOOL;</v>
+        <v>SIDE_CONV_LOWER_RADIAL_RIGHT:BOOL;</v>
       </c>
       <c r="N74" s="20" t="str">
         <f t="shared" si="46"/>
-        <v>SIDE_CONV_LOWER:OpCom; // AUX.OP7</v>
+        <v>SIDE_CONV_LOWER_RADIAL_RIGHT:OpCom; // AUX.OP7</v>
       </c>
       <c r="O74" s="20" t="str">
         <f t="shared" si="47"/>
-        <v>Machine_IO.Outputs.SIDE_CONV_LOWER</v>
+        <v>Machine_IO.Outputs.SIDE_CONV_LOWER_RADIAL_RIGHT</v>
       </c>
       <c r="P74" s="20" t="str">
         <f t="shared" si="48"/>
-        <v>Machine_IO.Outputs.SIDE_CONV_LOWER.Dig</v>
+        <v>Machine_IO.Outputs.SIDE_CONV_LOWER_RADIAL_RIGHT.Dig</v>
       </c>
       <c r="Q74" s="20" t="str">
         <f t="shared" si="49"/>
-        <v>Machine_IO.Outputs.SIDE_CONV_LOWER(); // CR0403.OP7</v>
+        <v>Machine_IO.Outputs.SIDE_CONV_LOWER_RADIAL_RIGHT(); // CR0403.OP7</v>
       </c>
       <c r="R74" s="20" t="str">
         <f t="shared" si="50"/>
-        <v>Machine_IO.Outputs.SIDE_CONV_LOWER.Init('AUX','SIDE_CONV_LOWER','OP7','',NVL_Outputs_States_AUX.All.OP7,NVL_IO_CHASSIS.All_Outputs_Diag.OP7,Machine_IO.Node_AUX);</v>
+        <v>Machine_IO.Outputs.SIDE_CONV_LOWER_RADIAL_RIGHT.Init('AUX','SIDE_CONV_LOWER_RADIAL_RIGHT','OP7','',NVL_Outputs_States_AUX.All.OP7,NVL_IO_CHASSIS.All_Outputs_Diag.OP7,Machine_IO.Node_AUX);</v>
       </c>
       <c r="S74" s="20" t="str">
         <f t="shared" si="51"/>
-        <v>SIDE_CONV_LOWER: Mimic_Output_FB; // AUX:OP7</v>
+        <v>SIDE_CONV_LOWER_RADIAL_RIGHT: Mimic_Output_FB; // AUX:OP7</v>
       </c>
       <c r="T74" s="20" t="str">
         <f t="shared" si="52"/>
@@ -8720,19 +8726,19 @@
       </c>
       <c r="U74" s="20" t="str">
         <f t="shared" si="53"/>
-        <v>AUX.OP7.Init(Machine_IO.Outputs.SIDE_CONV_LOWER);</v>
+        <v>AUX.OP7.Init(Machine_IO.Outputs.SIDE_CONV_LOWER_RADIAL_RIGHT);</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C75" s="19"/>
       <c r="D75" s="17" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E75" s="17" t="str">
         <f t="shared" ref="E75:E78" si="54">_xlfn.CONCAT(B75,".",D75)</f>
@@ -8792,14 +8798,14 @@
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C76" s="19"/>
       <c r="D76" s="17" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E76" s="17" t="str">
         <f t="shared" si="54"/>
@@ -8859,14 +8865,14 @@
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C77" s="19"/>
       <c r="D77" s="17" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="E77" s="17" t="str">
         <f t="shared" si="54"/>
@@ -8926,14 +8932,14 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C78" s="19"/>
       <c r="D78" s="17" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E78" s="17" t="str">
         <f t="shared" si="54"/>
@@ -9019,7 +9025,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT("IF CODE = ",A2," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B2,"';&lt;cr&gt;END_IF;")</f>
@@ -9031,7 +9037,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C66" si="0">_xlfn.CONCAT("IF CODE = ",A3," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B3,"';&lt;cr&gt;END_IF;")</f>
@@ -9043,7 +9049,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -9055,7 +9061,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -9067,7 +9073,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -9079,7 +9085,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -9091,7 +9097,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -9103,7 +9109,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -9115,7 +9121,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -9127,7 +9133,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -9139,7 +9145,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -9151,7 +9157,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -9163,7 +9169,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -9175,7 +9181,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -9187,7 +9193,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -9199,7 +9205,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -9211,7 +9217,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -9223,7 +9229,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -9235,7 +9241,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -9247,7 +9253,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -9259,7 +9265,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -9271,7 +9277,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -9283,7 +9289,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -9295,7 +9301,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -9307,7 +9313,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -9319,7 +9325,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -9331,7 +9337,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -9343,7 +9349,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -9355,7 +9361,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -9367,7 +9373,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -9379,7 +9385,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -9391,7 +9397,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -9403,7 +9409,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -9415,7 +9421,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -9427,7 +9433,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
@@ -9439,7 +9445,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
@@ -9451,7 +9457,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
@@ -9463,7 +9469,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
@@ -9475,7 +9481,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
@@ -9487,7 +9493,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
@@ -9499,7 +9505,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
@@ -9511,7 +9517,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
@@ -9523,7 +9529,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
@@ -9535,7 +9541,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
@@ -9547,7 +9553,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
@@ -9559,7 +9565,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
@@ -9571,7 +9577,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
@@ -9583,7 +9589,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
@@ -9595,7 +9601,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
@@ -9607,7 +9613,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
@@ -9619,7 +9625,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
@@ -9631,7 +9637,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
@@ -9643,7 +9649,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
@@ -9655,7 +9661,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
@@ -9667,7 +9673,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
@@ -9679,7 +9685,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
@@ -9691,7 +9697,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
@@ -9703,7 +9709,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
@@ -9715,7 +9721,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
@@ -9727,7 +9733,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
@@ -9739,7 +9745,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
@@ -9751,7 +9757,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
@@ -9763,7 +9769,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
@@ -9775,7 +9781,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
@@ -9787,7 +9793,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="0"/>
@@ -9799,7 +9805,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C130" si="1">_xlfn.CONCAT("IF CODE = ",A67," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B67,"';&lt;cr&gt;END_IF;")</f>
@@ -9811,7 +9817,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
@@ -9823,7 +9829,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
@@ -9835,7 +9841,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
@@ -9847,7 +9853,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
@@ -9859,7 +9865,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
@@ -9871,7 +9877,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
@@ -9883,7 +9889,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
@@ -9895,7 +9901,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
@@ -9907,7 +9913,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
@@ -9919,7 +9925,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
@@ -9931,7 +9937,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
@@ -9943,7 +9949,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
@@ -9955,7 +9961,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
@@ -9967,7 +9973,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
@@ -9979,7 +9985,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
@@ -9991,7 +9997,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
@@ -10003,7 +10009,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
@@ -10015,7 +10021,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
@@ -10027,7 +10033,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
@@ -10039,7 +10045,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
@@ -10051,7 +10057,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="1"/>
@@ -10063,7 +10069,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="1"/>
@@ -10075,7 +10081,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="1"/>
@@ -10087,7 +10093,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="1"/>
@@ -10099,7 +10105,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="1"/>
@@ -10111,7 +10117,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="1"/>
@@ -10123,7 +10129,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="1"/>
@@ -10135,7 +10141,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="1"/>
@@ -10147,7 +10153,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="1"/>
@@ -10159,7 +10165,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="1"/>
@@ -10171,7 +10177,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="1"/>
@@ -10183,7 +10189,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="1"/>
@@ -10195,7 +10201,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="1"/>
@@ -10207,7 +10213,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="1"/>
@@ -10219,7 +10225,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="1"/>
@@ -10231,7 +10237,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="1"/>
@@ -10243,7 +10249,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="1"/>
@@ -10255,7 +10261,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="1"/>
@@ -10267,7 +10273,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="1"/>
@@ -10279,7 +10285,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
@@ -10291,7 +10297,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="1"/>
@@ -10303,7 +10309,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="1"/>
@@ -10315,7 +10321,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="1"/>
@@ -10327,7 +10333,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="1"/>
@@ -10339,7 +10345,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="1"/>
@@ -10351,7 +10357,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C113" t="str">
         <f t="shared" si="1"/>
@@ -10363,7 +10369,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="1"/>
@@ -10375,7 +10381,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="1"/>
@@ -10387,7 +10393,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="1"/>
@@ -10399,7 +10405,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="1"/>
@@ -10411,7 +10417,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="1"/>
@@ -10423,7 +10429,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="1"/>
@@ -10435,7 +10441,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="C120" t="str">
         <f t="shared" si="1"/>
@@ -10447,7 +10453,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="1"/>
@@ -10459,7 +10465,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="1"/>
@@ -10471,7 +10477,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="1"/>
@@ -10483,7 +10489,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="1"/>
@@ -10495,7 +10501,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C125" t="str">
         <f t="shared" si="1"/>
@@ -10507,7 +10513,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C126" t="str">
         <f t="shared" si="1"/>
@@ -10519,7 +10525,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="C127" t="str">
         <f t="shared" si="1"/>
@@ -10531,7 +10537,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C128" t="str">
         <f t="shared" si="1"/>
@@ -10543,7 +10549,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C129" t="str">
         <f t="shared" si="1"/>
@@ -10555,7 +10561,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C130" t="str">
         <f t="shared" si="1"/>
@@ -10567,7 +10573,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="C131" t="str">
         <f t="shared" ref="C131:C135" si="2">_xlfn.CONCAT("IF CODE = ",A131," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B131,"';&lt;cr&gt;END_IF;")</f>
@@ -10579,7 +10585,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="C132" t="str">
         <f t="shared" si="2"/>
@@ -10591,7 +10597,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="C133" t="str">
         <f t="shared" si="2"/>
@@ -10603,7 +10609,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C134" t="str">
         <f t="shared" si="2"/>
@@ -10615,7 +10621,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="C135" t="str">
         <f t="shared" si="2"/>
@@ -10642,7 +10648,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -10650,7 +10656,7 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D3">
         <v>1500</v>
@@ -10658,7 +10664,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -10666,7 +10672,7 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D6">
         <v>1500</v>
@@ -10674,7 +10680,7 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -10682,7 +10688,7 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D9">
         <v>1500</v>
@@ -10690,7 +10696,7 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -10698,7 +10704,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D12">
         <v>1500</v>
@@ -10706,7 +10712,7 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -10714,7 +10720,7 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D15">
         <v>1500</v>
@@ -10722,7 +10728,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -10730,7 +10736,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D18">
         <v>1500</v>
@@ -10738,7 +10744,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -10749,7 +10755,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -10757,12 +10763,12 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D24">
         <v>250</v>
@@ -10770,7 +10776,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -10781,7 +10787,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -10792,7 +10798,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -10803,7 +10809,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -10814,7 +10820,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -10825,7 +10831,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -19096,7 +19102,7 @@
         <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D2" s="26">
         <f t="shared" ref="D2:D28" si="0">IFERROR(FIND("IN",C2,1),"")</f>
@@ -19141,7 +19147,7 @@
         <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D3" s="26">
         <f t="shared" si="0"/>
@@ -19186,7 +19192,7 @@
         <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D4" s="26">
         <f t="shared" si="0"/>
@@ -19201,7 +19207,7 @@
         <v/>
       </c>
       <c r="G4" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="3"/>
@@ -19231,7 +19237,7 @@
         <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D5" s="26">
         <f t="shared" si="0"/>
@@ -19246,7 +19252,7 @@
         <v/>
       </c>
       <c r="G5" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="3"/>
@@ -19276,7 +19282,7 @@
         <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D6" s="26">
         <f t="shared" si="0"/>
@@ -19291,7 +19297,7 @@
         <v/>
       </c>
       <c r="G6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="3"/>
@@ -19321,7 +19327,7 @@
         <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D7" s="26">
         <f t="shared" si="0"/>
@@ -19336,7 +19342,7 @@
         <v/>
       </c>
       <c r="G7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="3"/>
@@ -19366,7 +19372,7 @@
         <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D8" s="26">
         <f t="shared" si="0"/>
@@ -19381,7 +19387,7 @@
         <v/>
       </c>
       <c r="G8" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="3"/>
@@ -19411,7 +19417,7 @@
         <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D9" s="26">
         <f t="shared" si="0"/>
@@ -19426,7 +19432,7 @@
         <v/>
       </c>
       <c r="G9" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="3"/>
@@ -19456,7 +19462,7 @@
         <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D10" s="26">
         <f t="shared" si="0"/>
@@ -19471,7 +19477,7 @@
         <v/>
       </c>
       <c r="G10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="3"/>
@@ -19501,7 +19507,7 @@
         <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D11" s="26">
         <f t="shared" si="0"/>
@@ -19516,7 +19522,7 @@
         <v/>
       </c>
       <c r="G11" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="3"/>
@@ -19546,7 +19552,7 @@
         <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D12" s="26">
         <f t="shared" si="0"/>
@@ -19561,7 +19567,7 @@
         <v/>
       </c>
       <c r="G12" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="3"/>
@@ -19591,7 +19597,7 @@
         <v>93</v>
       </c>
       <c r="C13" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D13" s="26">
         <f t="shared" si="0"/>
@@ -19606,7 +19612,7 @@
         <v/>
       </c>
       <c r="G13" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="3"/>
@@ -19636,7 +19642,7 @@
         <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D14" s="26">
         <f t="shared" si="0"/>
@@ -19651,7 +19657,7 @@
         <v/>
       </c>
       <c r="G14" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="3"/>
@@ -19681,7 +19687,7 @@
         <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D15" s="26">
         <f t="shared" si="0"/>
@@ -19696,7 +19702,7 @@
         <v/>
       </c>
       <c r="G15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="3"/>
@@ -19726,7 +19732,7 @@
         <v>93</v>
       </c>
       <c r="C16" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D16" s="26">
         <f t="shared" si="0"/>
@@ -19741,7 +19747,7 @@
         <v/>
       </c>
       <c r="G16" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="3"/>
@@ -19771,7 +19777,7 @@
         <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D17" s="26">
         <f t="shared" si="0"/>
@@ -19786,7 +19792,7 @@
         <v/>
       </c>
       <c r="G17" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="3"/>
@@ -19816,7 +19822,7 @@
         <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D18" s="26">
         <f t="shared" si="0"/>
@@ -19831,7 +19837,7 @@
         <v/>
       </c>
       <c r="G18" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="3"/>
@@ -19861,7 +19867,7 @@
         <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D19" s="26">
         <f t="shared" si="0"/>
@@ -19876,7 +19882,7 @@
         <v/>
       </c>
       <c r="G19" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="3"/>
@@ -19906,7 +19912,7 @@
         <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D20" s="26">
         <f t="shared" si="0"/>
@@ -19921,7 +19927,7 @@
         <v/>
       </c>
       <c r="G20" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="3"/>
@@ -19951,7 +19957,7 @@
         <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D21" s="26">
         <f t="shared" si="0"/>
@@ -19966,7 +19972,7 @@
         <v/>
       </c>
       <c r="G21" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="3"/>
@@ -19996,7 +20002,7 @@
         <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D22" s="26">
         <f t="shared" si="0"/>
@@ -20011,7 +20017,7 @@
         <v/>
       </c>
       <c r="G22" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="3"/>
@@ -20041,7 +20047,7 @@
         <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D23" s="26">
         <f t="shared" si="0"/>
@@ -20056,7 +20062,7 @@
         <v/>
       </c>
       <c r="G23" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="3"/>
@@ -20086,7 +20092,7 @@
         <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D24" s="26">
         <f t="shared" si="0"/>
@@ -20101,7 +20107,7 @@
         <v/>
       </c>
       <c r="G24" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="3"/>
@@ -20131,7 +20137,7 @@
         <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D25" s="26">
         <f t="shared" si="0"/>
@@ -20146,7 +20152,7 @@
         <v/>
       </c>
       <c r="G25" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="3"/>
@@ -20176,7 +20182,7 @@
         <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D26" s="26">
         <f t="shared" si="0"/>
@@ -20191,7 +20197,7 @@
         <v/>
       </c>
       <c r="G26" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" ref="H26:H33" si="7">_xlfn.CONCAT(G26," {",B26,".",C26,"}")</f>
@@ -20221,7 +20227,7 @@
         <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D27" s="26">
         <f t="shared" si="0"/>
@@ -20236,7 +20242,7 @@
         <v/>
       </c>
       <c r="G27" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="7"/>
@@ -20266,7 +20272,7 @@
         <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D28" s="26">
         <f t="shared" si="0"/>
@@ -20281,7 +20287,7 @@
         <v/>
       </c>
       <c r="G28" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="7"/>
@@ -20311,7 +20317,7 @@
         <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D29" s="26">
         <f t="shared" ref="D29:D48" si="11">IFERROR(FIND("IN",C29,1),"")</f>
@@ -20326,7 +20332,7 @@
         <v/>
       </c>
       <c r="G29" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="7"/>
@@ -20356,7 +20362,7 @@
         <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D30" s="26">
         <f t="shared" si="11"/>
@@ -20371,7 +20377,7 @@
         <v/>
       </c>
       <c r="G30" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="7"/>
@@ -20401,7 +20407,7 @@
         <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D31" s="26">
         <f t="shared" si="11"/>
@@ -20416,7 +20422,7 @@
         <v/>
       </c>
       <c r="G31" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="7"/>
@@ -20446,7 +20452,7 @@
         <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D32" s="26">
         <f t="shared" si="11"/>
@@ -20461,7 +20467,7 @@
         <v/>
       </c>
       <c r="G32" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="7"/>
@@ -20491,7 +20497,7 @@
         <v>93</v>
       </c>
       <c r="C33" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D33" s="26">
         <f t="shared" si="11"/>
@@ -20506,7 +20512,7 @@
         <v/>
       </c>
       <c r="G33" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="7"/>
@@ -20536,7 +20542,7 @@
         <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D34" s="26" t="str">
         <f t="shared" si="11"/>
@@ -20551,7 +20557,7 @@
         <v/>
       </c>
       <c r="G34" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" ref="H34" si="14">_xlfn.CONCAT(G34," {",B34,".",C34,"}")</f>
@@ -20581,7 +20587,7 @@
         <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D35" s="26" t="str">
         <f t="shared" si="11"/>
@@ -20596,7 +20602,7 @@
         <v/>
       </c>
       <c r="G35" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" ref="H35:H65" si="18">_xlfn.CONCAT(G35," {",B35,".",C35,"}")</f>
@@ -20626,7 +20632,7 @@
         <v>93</v>
       </c>
       <c r="C36" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D36" s="26" t="str">
         <f t="shared" si="11"/>
@@ -20641,7 +20647,7 @@
         <v/>
       </c>
       <c r="G36" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="18"/>
@@ -20671,7 +20677,7 @@
         <v>93</v>
       </c>
       <c r="C37" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D37" s="26" t="str">
         <f t="shared" si="11"/>
@@ -20686,7 +20692,7 @@
         <v/>
       </c>
       <c r="G37" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="18"/>
@@ -20716,7 +20722,7 @@
         <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D38" s="26" t="str">
         <f t="shared" si="11"/>
@@ -20731,7 +20737,7 @@
         <v/>
       </c>
       <c r="G38" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="18"/>
@@ -20761,7 +20767,7 @@
         <v>93</v>
       </c>
       <c r="C39" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D39" s="26" t="str">
         <f t="shared" si="11"/>
@@ -20776,7 +20782,7 @@
         <v/>
       </c>
       <c r="G39" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="18"/>
@@ -20806,7 +20812,7 @@
         <v>93</v>
       </c>
       <c r="C40" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D40" s="26" t="str">
         <f t="shared" si="11"/>
@@ -20821,7 +20827,7 @@
         <v/>
       </c>
       <c r="G40" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="18"/>
@@ -20851,7 +20857,7 @@
         <v>93</v>
       </c>
       <c r="C41" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D41" s="26" t="str">
         <f t="shared" si="11"/>
@@ -20866,7 +20872,7 @@
         <v/>
       </c>
       <c r="G41" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="18"/>
@@ -20896,7 +20902,7 @@
         <v>93</v>
       </c>
       <c r="C42" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D42" s="26" t="str">
         <f t="shared" si="11"/>
@@ -20911,7 +20917,7 @@
         <v/>
       </c>
       <c r="G42" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="18"/>
@@ -20941,7 +20947,7 @@
         <v>93</v>
       </c>
       <c r="C43" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D43" s="26" t="str">
         <f t="shared" si="11"/>
@@ -20956,7 +20962,7 @@
         <v>9</v>
       </c>
       <c r="G43" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="18"/>
@@ -20986,7 +20992,7 @@
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D44" s="26" t="str">
         <f t="shared" si="11"/>
@@ -21001,7 +21007,7 @@
         <v/>
       </c>
       <c r="G44" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="18"/>
@@ -21031,7 +21037,7 @@
         <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D45" s="26" t="str">
         <f t="shared" si="11"/>
@@ -21046,7 +21052,7 @@
         <v/>
       </c>
       <c r="G45" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="18"/>
@@ -21076,7 +21082,7 @@
         <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D46" s="26" t="str">
         <f t="shared" si="11"/>
@@ -21091,7 +21097,7 @@
         <v/>
       </c>
       <c r="G46" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="18"/>
@@ -21121,7 +21127,7 @@
         <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D47" s="26" t="str">
         <f t="shared" si="11"/>
@@ -21136,7 +21142,7 @@
         <v/>
       </c>
       <c r="G47" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="18"/>
@@ -21166,7 +21172,7 @@
         <v>93</v>
       </c>
       <c r="C48" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D48" s="26" t="str">
         <f t="shared" si="11"/>
@@ -21181,7 +21187,7 @@
         <v/>
       </c>
       <c r="G48" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="18"/>
@@ -21211,7 +21217,7 @@
         <v>93</v>
       </c>
       <c r="C49" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D49" s="26" t="str">
         <f t="shared" ref="D49:D65" si="22">IFERROR(FIND("IN",C49,1),"")</f>
@@ -21226,7 +21232,7 @@
         <v/>
       </c>
       <c r="G49" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="18"/>
@@ -21256,7 +21262,7 @@
         <v>93</v>
       </c>
       <c r="C50" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D50" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21271,7 +21277,7 @@
         <v/>
       </c>
       <c r="G50" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="18"/>
@@ -21301,7 +21307,7 @@
         <v>93</v>
       </c>
       <c r="C51" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D51" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21316,7 +21322,7 @@
         <v/>
       </c>
       <c r="G51" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="18"/>
@@ -21346,7 +21352,7 @@
         <v>93</v>
       </c>
       <c r="C52" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D52" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21361,7 +21367,7 @@
         <v/>
       </c>
       <c r="G52" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="18"/>
@@ -21391,7 +21397,7 @@
         <v>93</v>
       </c>
       <c r="C53" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D53" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21406,7 +21412,7 @@
         <v>9</v>
       </c>
       <c r="G53" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="18"/>
@@ -21436,7 +21442,7 @@
         <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D54" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21451,7 +21457,7 @@
         <v/>
       </c>
       <c r="G54" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="18"/>
@@ -21481,7 +21487,7 @@
         <v>93</v>
       </c>
       <c r="C55" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D55" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21496,7 +21502,7 @@
         <v/>
       </c>
       <c r="G55" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="18"/>
@@ -21526,7 +21532,7 @@
         <v>93</v>
       </c>
       <c r="C56" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D56" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21541,7 +21547,7 @@
         <v/>
       </c>
       <c r="G56" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="18"/>
@@ -21571,7 +21577,7 @@
         <v>93</v>
       </c>
       <c r="C57" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D57" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21586,7 +21592,7 @@
         <v/>
       </c>
       <c r="G57" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="18"/>
@@ -21616,7 +21622,7 @@
         <v>93</v>
       </c>
       <c r="C58" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D58" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21631,7 +21637,7 @@
         <v/>
       </c>
       <c r="G58" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="18"/>
@@ -21661,7 +21667,7 @@
         <v>93</v>
       </c>
       <c r="C59" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D59" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21676,7 +21682,7 @@
         <v/>
       </c>
       <c r="G59" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="18"/>
@@ -21706,7 +21712,7 @@
         <v>93</v>
       </c>
       <c r="C60" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D60" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21721,7 +21727,7 @@
         <v/>
       </c>
       <c r="G60" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="18"/>
@@ -21751,7 +21757,7 @@
         <v>93</v>
       </c>
       <c r="C61" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D61" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21766,7 +21772,7 @@
         <v/>
       </c>
       <c r="G61" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="18"/>
@@ -21796,7 +21802,7 @@
         <v>93</v>
       </c>
       <c r="C62" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D62" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21811,7 +21817,7 @@
         <v/>
       </c>
       <c r="G62" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="18"/>
@@ -21841,7 +21847,7 @@
         <v>93</v>
       </c>
       <c r="C63" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D63" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21856,7 +21862,7 @@
         <v>9</v>
       </c>
       <c r="G63" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="18"/>
@@ -21886,7 +21892,7 @@
         <v>93</v>
       </c>
       <c r="C64" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D64" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21901,7 +21907,7 @@
         <v/>
       </c>
       <c r="G64" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="18"/>
@@ -21931,7 +21937,7 @@
         <v>93</v>
       </c>
       <c r="C65" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D65" s="26" t="str">
         <f t="shared" si="22"/>
@@ -21946,7 +21952,7 @@
         <v/>
       </c>
       <c r="G65" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="18"/>
@@ -21977,10 +21983,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21993,16 +21999,16 @@
   <sheetData>
     <row r="1" spans="1:5" s="34" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="34" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22010,13 +22016,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22024,13 +22030,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C3" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="D3" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22038,13 +22044,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C4" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="D4" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22052,13 +22058,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C5" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D5" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22066,16 +22072,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C6" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="D6" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="E6" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
     </row>
     <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22083,13 +22089,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D7" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22097,13 +22103,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C8" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D8" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22111,13 +22117,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C9" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D9" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22125,13 +22131,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C10" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D10" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22139,13 +22145,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C11" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D11" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22153,13 +22159,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C12" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D12" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22167,13 +22173,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>557</v>
+      </c>
+      <c r="C13" t="s">
         <v>559</v>
       </c>
-      <c r="C13" t="s">
-        <v>561</v>
-      </c>
       <c r="D13" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22181,13 +22187,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C14" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D14" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22195,13 +22201,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C15" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D15" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22209,13 +22215,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C16" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D16" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22223,13 +22229,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="D17" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22237,13 +22243,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C18" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D18" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22251,16 +22257,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C19" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D19" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E19" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22268,13 +22274,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C20" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D20" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22282,13 +22288,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C21" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D21" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22296,13 +22302,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C22" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D22" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22310,16 +22316,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C23" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D23" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E23" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22327,13 +22333,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C24" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D24" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22341,13 +22347,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C25" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D25" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22355,24 +22361,27 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C26" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D26" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C27" t="s">
-        <v>550</v>
+        <v>548</v>
+      </c>
+      <c r="D27" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22380,16 +22389,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C28" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D28" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E28" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -22397,10 +22406,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C29" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -22408,10 +22417,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>569</v>
+      </c>
+      <c r="C30" t="s">
         <v>571</v>
-      </c>
-      <c r="C30" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22419,16 +22428,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C31" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D31" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E31" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22436,13 +22445,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D32" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -22450,13 +22459,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22464,16 +22473,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C34" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D34" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E34" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22481,16 +22490,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C35" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D35" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E35" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22498,13 +22507,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C36" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D36" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22512,13 +22521,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C37" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D37" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22526,13 +22535,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>587</v>
+      </c>
+      <c r="C38" t="s">
+        <v>588</v>
+      </c>
+      <c r="D38" t="s">
         <v>589</v>
-      </c>
-      <c r="C38" t="s">
-        <v>590</v>
-      </c>
-      <c r="D38" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22540,16 +22549,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C39" t="s">
+        <v>593</v>
+      </c>
+      <c r="D39" t="s">
+        <v>589</v>
+      </c>
+      <c r="E39" t="s">
         <v>595</v>
-      </c>
-      <c r="D39" t="s">
-        <v>591</v>
-      </c>
-      <c r="E39" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22557,16 +22566,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>592</v>
+      </c>
+      <c r="C40" t="s">
         <v>594</v>
       </c>
-      <c r="C40" t="s">
-        <v>596</v>
-      </c>
       <c r="D40" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E40" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22574,13 +22583,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C41" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D41" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -22588,10 +22597,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="C42" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -22599,13 +22608,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C43" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="E43" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
     </row>
     <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22613,13 +22622,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C44" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D44" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22627,16 +22636,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C45" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D45" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="E45" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22644,13 +22653,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C46" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D46" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22658,13 +22667,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C47" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D47" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22672,13 +22681,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C48" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="D48" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22686,13 +22695,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C49" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D49" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22700,16 +22709,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C50" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D50" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="E50" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
     </row>
     <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22717,13 +22726,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C51" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="D51" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22731,16 +22740,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="33" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="D52" s="33" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E52" s="33" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
     </row>
     <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22748,13 +22757,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>650</v>
+      </c>
+      <c r="C53" t="s">
+        <v>657</v>
+      </c>
+      <c r="D53" t="s">
         <v>654</v>
-      </c>
-      <c r="C53" t="s">
-        <v>661</v>
-      </c>
-      <c r="D53" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22762,13 +22771,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>650</v>
+      </c>
+      <c r="C54" t="s">
+        <v>651</v>
+      </c>
+      <c r="D54" t="s">
         <v>654</v>
-      </c>
-      <c r="C54" t="s">
-        <v>655</v>
-      </c>
-      <c r="D54" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22776,13 +22785,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C55" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="D55" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22790,13 +22799,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C56" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="D56" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -22804,10 +22813,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C57" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
     </row>
     <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22815,38 +22824,44 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C58" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D58" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C59" t="s">
-        <v>667</v>
+        <v>663</v>
+      </c>
+      <c r="D59" t="s">
+        <v>589</v>
       </c>
       <c r="E59" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C60" t="s">
-        <v>822</v>
+        <v>818</v>
+      </c>
+      <c r="D60" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22854,13 +22869,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C61" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D61" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22868,13 +22883,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="C62" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D62" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22882,13 +22897,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C63" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="D63" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -22896,13 +22911,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>669</v>
+      </c>
+      <c r="C64" t="s">
         <v>673</v>
       </c>
-      <c r="C64" t="s">
-        <v>677</v>
-      </c>
       <c r="E64" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -22910,10 +22925,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="C65" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -22921,10 +22936,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="C66" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22932,16 +22947,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C67" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="D67" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="E67" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22949,13 +22964,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C68" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D68" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22963,28 +22978,45 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C69" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D69" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E69" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>70</v>
+      </c>
       <c r="B70" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C70" t="s">
-        <v>826</v>
+        <v>822</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>831</v>
+      </c>
+      <c r="C71" t="s">
+        <v>828</v>
+      </c>
+      <c r="D71" t="s">
+        <v>589</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E70" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
+  <autoFilter ref="A1:E71" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
@@ -22994,15 +23026,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
@@ -23018,6 +23041,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23244,14 +23276,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
@@ -23264,6 +23288,14 @@
     <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
excel sngas from the last commit
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35475C7-3A8E-471F-B366-75B19A31533F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B792A7B-A0BB-4669-97F5-95C74FF482CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="837">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2543,6 +2543,21 @@
   </si>
   <si>
     <t>MAIN_MIMIC</t>
+  </si>
+  <si>
+    <t>Starting tracks stops suto mode?</t>
+  </si>
+  <si>
+    <t>RADIAL_MODE</t>
+  </si>
+  <si>
+    <t>Starting tracks stops auto radial mode?</t>
+  </si>
+  <si>
+    <t>Cannot stop unless amchine shut down?</t>
+  </si>
+  <si>
+    <t>Reset the radial timeout if mode changed?</t>
   </si>
 </sst>
 </file>
@@ -21983,10 +21998,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23015,6 +23030,38 @@
         <v>589</v>
       </c>
     </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>573</v>
+      </c>
+      <c r="C72" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>833</v>
+      </c>
+      <c r="C73" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>573</v>
+      </c>
+      <c r="C74" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>833</v>
+      </c>
+      <c r="C75" t="s">
+        <v>836</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E71" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
     <filterColumn colId="3">
@@ -23026,33 +23073,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
-    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
-      <UserInfo>
-        <DisplayName>Noel Loughran</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9F7729ADF49144A01A6175DD599202" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f00ebe7287476f312414df31db46304">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c96d9849-7071-4555-8535-ee11c374d0f7" xmlns:ns3="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f2e969a0d0c60cbdf6bd0d859a86451" ns2:_="" ns3:_="">
     <xsd:import namespace="c96d9849-7071-4555-8535-ee11c374d0f7"/>
@@ -23275,32 +23295,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
+    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
+      <UserInfo>
+        <DisplayName>Noel Loughran</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6596B7D1-B3E6-40CB-B05E-2E959D1A2B6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23317,4 +23339,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
connected to standard machine onsite - no changes tracking/manaul/auto checked. small change to the tracking enable - does not reset it radio tracking stopped/started - no need to press again.
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B792A7B-A0BB-4669-97F5-95C74FF482CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E99C87B-7FE0-46BB-BB37-7751FA5D2CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="839">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2558,6 +2558,12 @@
   </si>
   <si>
     <t>Reset the radial timeout if mode changed?</t>
+  </si>
+  <si>
+    <t>MANUAL MODE</t>
+  </si>
+  <si>
+    <t>standard 3/2 need to be swapped on the main mimic</t>
   </si>
 </sst>
 </file>
@@ -21998,10 +22004,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23062,6 +23068,14 @@
         <v>836</v>
       </c>
     </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>837</v>
+      </c>
+      <c r="C76" t="s">
+        <v>838</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E71" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
     <filterColumn colId="3">
@@ -23073,6 +23087,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9F7729ADF49144A01A6175DD599202" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f00ebe7287476f312414df31db46304">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c96d9849-7071-4555-8535-ee11c374d0f7" xmlns:ns3="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f2e969a0d0c60cbdf6bd0d859a86451" ns2:_="" ns3:_="">
     <xsd:import namespace="c96d9849-7071-4555-8535-ee11c374d0f7"/>
@@ -23295,15 +23318,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -23323,6 +23337,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6596B7D1-B3E6-40CB-B05E-2E959D1A2B6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23337,14 +23359,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
HMI/PLC - some radiial testing done - see the snags
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E99C87B-7FE0-46BB-BB37-7751FA5D2CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB481680-CB3F-4477-A512-07F31B1CE39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2339" uniqueCount="855">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2545,9 +2545,6 @@
     <t>MAIN_MIMIC</t>
   </si>
   <si>
-    <t>Starting tracks stops suto mode?</t>
-  </si>
-  <si>
     <t>RADIAL_MODE</t>
   </si>
   <si>
@@ -2564,6 +2561,57 @@
   </si>
   <si>
     <t>standard 3/2 need to be swapped on the main mimic</t>
+  </si>
+  <si>
+    <t>radial 2 + 3 disappear as not present!</t>
+  </si>
+  <si>
+    <t>Radial 1 = tail</t>
+  </si>
+  <si>
+    <t>Radial 2 = stockpile</t>
+  </si>
+  <si>
+    <t>Radial 4 = under collection + stockpile swivel  feed conveyor</t>
+  </si>
+  <si>
+    <t>Radial 6 = feeder</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>Radial 5 drum</t>
+  </si>
+  <si>
+    <t>Radial 3 - not present</t>
+  </si>
+  <si>
+    <t>simailar to side conveyor interlocked with tail!</t>
+  </si>
+  <si>
+    <t>SHUTDOWNS</t>
+  </si>
+  <si>
+    <t>check all the system shutodwns!</t>
+  </si>
+  <si>
+    <t>check fan control + settings</t>
+  </si>
+  <si>
+    <t>fuel sender scaling / alarms+ resets!</t>
+  </si>
+  <si>
+    <t>feed alarms into fault logger and show active on a single page</t>
+  </si>
+  <si>
+    <t>Starting tracks stops auto mode?</t>
+  </si>
+  <si>
+    <t>is this allowed from the remote? Digger operator wants to move machine with getting out?</t>
+  </si>
+  <si>
+    <t>radio mode stops when tracking started? Tracks has priority - would be better if we had the normal buttons through radio!</t>
   </si>
 </sst>
 </file>
@@ -22004,10 +22052,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23041,15 +23089,21 @@
         <v>573</v>
       </c>
       <c r="C72" t="s">
-        <v>832</v>
+        <v>852</v>
+      </c>
+      <c r="E72" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
+        <v>832</v>
+      </c>
+      <c r="C73" t="s">
         <v>833</v>
       </c>
-      <c r="C73" t="s">
-        <v>834</v>
+      <c r="E73" t="s">
+        <v>854</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -23057,23 +23111,99 @@
         <v>573</v>
       </c>
       <c r="C74" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C75" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
+        <v>836</v>
+      </c>
+      <c r="C76" t="s">
         <v>837</v>
       </c>
-      <c r="C76" t="s">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>836</v>
+      </c>
+      <c r="C77" t="s">
         <v>838</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>847</v>
+      </c>
+      <c r="C78" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>839</v>
+      </c>
+      <c r="D86" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>840</v>
+      </c>
+      <c r="E87" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="88" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="89" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>841</v>
+      </c>
+      <c r="D89" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="90" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>844</v>
+      </c>
+      <c r="D90" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="91" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>842</v>
+      </c>
+      <c r="D91" t="s">
+        <v>843</v>
       </c>
     </row>
   </sheetData>
@@ -23087,15 +23217,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9F7729ADF49144A01A6175DD599202" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f00ebe7287476f312414df31db46304">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c96d9849-7071-4555-8535-ee11c374d0f7" xmlns:ns3="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f2e969a0d0c60cbdf6bd0d859a86451" ns2:_="" ns3:_="">
     <xsd:import namespace="c96d9849-7071-4555-8535-ee11c374d0f7"/>
@@ -23318,6 +23439,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -23337,14 +23467,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6596B7D1-B3E6-40CB-B05E-2E959D1A2B6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23359,6 +23481,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
WIP adding the radial mimic
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB481680-CB3F-4477-A512-07F31B1CE39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910BD9DB-1594-47D8-B294-3703C55767DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$1:$AP$78</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">SNAGS!$A$1:$E$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">SNAGS!$A$1:$E$91</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2339" uniqueCount="855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="856">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2590,15 +2590,9 @@
     <t>simailar to side conveyor interlocked with tail!</t>
   </si>
   <si>
-    <t>SHUTDOWNS</t>
-  </si>
-  <si>
     <t>check all the system shutodwns!</t>
   </si>
   <si>
-    <t>check fan control + settings</t>
-  </si>
-  <si>
     <t>fuel sender scaling / alarms+ resets!</t>
   </si>
   <si>
@@ -2608,10 +2602,19 @@
     <t>Starting tracks stops auto mode?</t>
   </si>
   <si>
-    <t>is this allowed from the remote? Digger operator wants to move machine with getting out?</t>
-  </si>
-  <si>
     <t>radio mode stops when tracking started? Tracks has priority - would be better if we had the normal buttons through radio!</t>
+  </si>
+  <si>
+    <t>ALARMS</t>
+  </si>
+  <si>
+    <t>is this allowed from the remote? Digger operator wants to move machine with getting out? Will this work on the radial?</t>
+  </si>
+  <si>
+    <t>Timeout on the tracks enable</t>
+  </si>
+  <si>
+    <t>tracks started but not used?</t>
   </si>
 </sst>
 </file>
@@ -22055,7 +22058,7 @@
   <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22063,7 +22066,7 @@
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="71.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="62" customWidth="1"/>
+    <col min="5" max="5" width="136.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="34" customFormat="1" ht="21" x14ac:dyDescent="0.35">
@@ -23089,7 +23092,7 @@
         <v>573</v>
       </c>
       <c r="C72" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="E72" t="s">
         <v>853</v>
@@ -23097,13 +23100,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>832</v>
+        <v>573</v>
       </c>
       <c r="C73" t="s">
-        <v>833</v>
-      </c>
-      <c r="E73" t="s">
-        <v>854</v>
+        <v>834</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -23111,57 +23111,72 @@
         <v>573</v>
       </c>
       <c r="C74" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>832</v>
-      </c>
-      <c r="C75" t="s">
-        <v>835</v>
+        <v>854</v>
+      </c>
+      <c r="E74" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>836</v>
+        <v>852</v>
       </c>
       <c r="C76" t="s">
-        <v>837</v>
+        <v>847</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>836</v>
+        <v>852</v>
       </c>
       <c r="C77" t="s">
-        <v>838</v>
+        <v>849</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>847</v>
-      </c>
       <c r="C78" t="s">
         <v>848</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>849</v>
-      </c>
-    </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>832</v>
+      </c>
       <c r="C80" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
+        <v>833</v>
+      </c>
+      <c r="E80" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>832</v>
+      </c>
       <c r="C81" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>836</v>
+      </c>
+      <c r="C83" t="s">
+        <v>837</v>
+      </c>
+      <c r="D83" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>836</v>
+      </c>
+      <c r="C84" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
         <v>839</v>
       </c>
@@ -23169,7 +23184,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
         <v>840</v>
       </c>
@@ -23177,12 +23192,12 @@
         <v>846</v>
       </c>
     </row>
-    <row r="88" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="89" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
         <v>841</v>
       </c>
@@ -23190,7 +23205,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="90" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
         <v>844</v>
       </c>
@@ -23198,7 +23213,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="91" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
         <v>842</v>
       </c>
@@ -23207,7 +23222,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E71" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
+  <autoFilter ref="A1:E91" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
WIP - needs to finish up the radial arrows - should be easy now lib fixed.
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910BD9DB-1594-47D8-B294-3703C55767DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223DAC8C-C9AA-479A-91A8-5D99A090916D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="ALARMS" sheetId="24" r:id="rId5"/>
     <sheet name="ALARMS_IO" sheetId="31" r:id="rId6"/>
     <sheet name="SNAGS" sheetId="33" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="35" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2369" uniqueCount="864">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2615,6 +2616,30 @@
   </si>
   <si>
     <t>tracks started but not used?</t>
+  </si>
+  <si>
+    <t>Radial drum</t>
+  </si>
+  <si>
+    <t>Radial under collection + stockpile swivel  feed conveyor</t>
+  </si>
+  <si>
+    <t>Radial stockpile</t>
+  </si>
+  <si>
+    <t>Radial tail</t>
+  </si>
+  <si>
+    <t>Radial feeder</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -2787,7 +2812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2869,6 +2894,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -22055,10 +22083,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23221,6 +23249,106 @@
         <v>843</v>
       </c>
     </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>839</v>
+      </c>
+      <c r="D94" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>840</v>
+      </c>
+      <c r="E95" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>841</v>
+      </c>
+      <c r="D97" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>844</v>
+      </c>
+      <c r="D98" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>842</v>
+      </c>
+      <c r="D99" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>859</v>
+      </c>
+      <c r="D103" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>2</v>
+      </c>
+      <c r="C104" t="s">
+        <v>858</v>
+      </c>
+      <c r="E104" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>857</v>
+      </c>
+      <c r="D105" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>4</v>
+      </c>
+      <c r="C106" t="s">
+        <v>856</v>
+      </c>
+      <c r="D106" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>860</v>
+      </c>
+      <c r="D107" t="s">
+        <v>843</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E91" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
     <filterColumn colId="3">
@@ -23231,7 +23359,148 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692637BC-36A2-49E1-8104-C2CAB79C8E2F}">
+  <dimension ref="B3:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="6" width="9.140625" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>861</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>862</v>
+      </c>
+      <c r="C4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f>DEGREES(ATAN($C$3/$C$4))</f>
+        <v>18.43494882292201</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f>RADIANS(C5)</f>
+        <v>0.32175055439664219</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="26" t="s">
+        <v>863</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>861</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="35">
+        <v>0</v>
+      </c>
+      <c r="E10" s="26">
+        <f>$C$4*C10</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="26">
+        <f>$C$3*C10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="35">
+        <v>0.25</v>
+      </c>
+      <c r="E11" s="26">
+        <f t="shared" ref="E11:E14" si="0">$C$4*C11</f>
+        <v>37.5</v>
+      </c>
+      <c r="F11" s="26">
+        <f t="shared" ref="F11:F14" si="1">$C$3*C11</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="26">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F12" s="26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="E13" s="26">
+        <f t="shared" si="0"/>
+        <v>112.5</v>
+      </c>
+      <c r="F13" s="26">
+        <f t="shared" si="1"/>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="35">
+        <v>1</v>
+      </c>
+      <c r="E14" s="26">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="F14" s="26">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9F7729ADF49144A01A6175DD599202" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f00ebe7287476f312414df31db46304">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c96d9849-7071-4555-8535-ee11c374d0f7" xmlns:ns3="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f2e969a0d0c60cbdf6bd0d859a86451" ns2:_="" ns3:_="">
     <xsd:import namespace="c96d9849-7071-4555-8535-ee11c374d0f7"/>
@@ -23454,15 +23723,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -23482,6 +23742,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6596B7D1-B3E6-40CB-B05E-2E959D1A2B6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23496,14 +23764,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Onsite testing with Mark - see snags - mainly J1939 stuff , some settings and a little mimics
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223DAC8C-C9AA-479A-91A8-5D99A090916D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B621FDAD-C458-4BB3-9F54-57AA519779D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2369" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2390" uniqueCount="874">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2060,9 +2060,6 @@
     <t>ENGINE</t>
   </si>
   <si>
-    <t>check the old code?</t>
-  </si>
-  <si>
     <t>DM1 Clear function</t>
   </si>
   <si>
@@ -2552,9 +2549,6 @@
     <t>Starting tracks stops auto radial mode?</t>
   </si>
   <si>
-    <t>Cannot stop unless amchine shut down?</t>
-  </si>
-  <si>
     <t>Reset the radial timeout if mode changed?</t>
   </si>
   <si>
@@ -2594,9 +2588,6 @@
     <t>check all the system shutodwns!</t>
   </si>
   <si>
-    <t>fuel sender scaling / alarms+ resets!</t>
-  </si>
-  <si>
     <t>feed alarms into fault logger and show active on a single page</t>
   </si>
   <si>
@@ -2640,6 +2631,45 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Radial mode - swap buttons 2+3</t>
+  </si>
+  <si>
+    <t>collection has to be started first?</t>
+  </si>
+  <si>
+    <t>fix up the naming on the milla amp settings on the radial</t>
+  </si>
+  <si>
+    <t>Alarms Page to cover all the shutdowns</t>
+  </si>
+  <si>
+    <t>FAN Settings on Screen - add the counters to the screen</t>
+  </si>
+  <si>
+    <t>engine load not on screen</t>
+  </si>
+  <si>
+    <t>CAT - dbs file and feedback for the regen</t>
+  </si>
+  <si>
+    <t>Engine Ramp Up Speed 0 add setting</t>
+  </si>
+  <si>
+    <t>reverse the image from the CAD guys?</t>
+  </si>
+  <si>
+    <t>check the old code? - Feedback is just off the button!</t>
+  </si>
+  <si>
+    <t>check with the new libs + dbc file</t>
+  </si>
+  <si>
+    <t>Cannot stop unless machine shut down?</t>
+  </si>
+  <si>
+    <t>ENGINE_SCREEN</t>
   </si>
 </sst>
 </file>
@@ -3502,7 +3532,7 @@
         <v>CHASSIS.IN0102</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="L4" s="19" t="str">
         <f t="shared" si="7"/>
@@ -3578,7 +3608,7 @@
         <v>CHASSIS.IN0103</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="L5" s="19" t="str">
         <f t="shared" si="7"/>
@@ -3654,7 +3684,7 @@
         <v>CHASSIS.IN0200</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="L6" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5007,7 +5037,7 @@
         <v>CHASSIS.IN0502</v>
       </c>
       <c r="K24" s="32" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="L24" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5083,7 +5113,7 @@
         <v>CHASSIS.IN0503</v>
       </c>
       <c r="K25" s="32" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="L25" s="19" t="str">
         <f t="shared" si="7"/>
@@ -5796,7 +5826,7 @@
         <v>CHASSIS.OUT0000.Init(Machine_IO.Outputs.TAILCONVSPD_MA);</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="35" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5957,7 +5987,7 @@
         <v>CHASSIS.OUT0002.Init(Machine_IO.Outputs.SIDECONVSPD_MA);</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="37" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6118,7 +6148,7 @@
         <v>CHASSIS.OUT0004.Init(Machine_IO.Outputs.SIDETRANSFERSPD_MA);</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="39" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6358,7 +6388,7 @@
         <v>CHASSIS.OUT0007.Init(Machine_IO.Outputs.COLLECTIONCONVSPD_MA);</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="42" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6440,7 +6470,7 @@
         <v>CHASSIS.OUT0008.Init(Machine_IO.Outputs.COLLECTIONCONVON_OP);</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="43" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6601,7 +6631,7 @@
         <v>CHASSIS.OUT0100.Init(Machine_IO.Outputs.DRUMSPD_MA_RAMP_LIMIT);</v>
       </c>
       <c r="V44" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6762,7 +6792,7 @@
         <v>CHASSIS.OUT0102.Init(Machine_IO.Outputs.FEEDERSPD_MA);</v>
       </c>
       <c r="V46" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="47" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7160,7 +7190,7 @@
         <v>CHASSIS.OUT0107.Init(Machine_IO.Outputs.SIDECONVON_OP);</v>
       </c>
       <c r="V51" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
@@ -8717,7 +8747,7 @@
         <v>AUX.OP6</v>
       </c>
       <c r="K73" s="19" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="L73" s="19" t="str">
         <f t="shared" si="44"/>
@@ -8786,7 +8816,7 @@
         <v>AUX.OP7</v>
       </c>
       <c r="K74" s="19" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="L74" s="19" t="str">
         <f t="shared" si="44"/>
@@ -9125,7 +9155,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT("IF CODE = ",A2," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B2,"';&lt;cr&gt;END_IF;")</f>
@@ -9137,7 +9167,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C66" si="0">_xlfn.CONCAT("IF CODE = ",A3," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B3,"';&lt;cr&gt;END_IF;")</f>
@@ -9149,7 +9179,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -9161,7 +9191,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -9173,7 +9203,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -9185,7 +9215,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -9197,7 +9227,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -9209,7 +9239,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -9221,7 +9251,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -9233,7 +9263,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -9245,7 +9275,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -9257,7 +9287,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -9269,7 +9299,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -9281,7 +9311,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -9293,7 +9323,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -9305,7 +9335,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -9317,7 +9347,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -9329,7 +9359,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -9341,7 +9371,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -9353,7 +9383,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -9365,7 +9395,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -9377,7 +9407,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -9389,7 +9419,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -9401,7 +9431,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -9413,7 +9443,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -9425,7 +9455,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -9437,7 +9467,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -9449,7 +9479,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -9461,7 +9491,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -9473,7 +9503,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -9485,7 +9515,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -9497,7 +9527,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -9509,7 +9539,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -9521,7 +9551,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -9533,7 +9563,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
@@ -9545,7 +9575,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
@@ -9557,7 +9587,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
@@ -9569,7 +9599,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
@@ -9581,7 +9611,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
@@ -9593,7 +9623,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
@@ -9605,7 +9635,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
@@ -9617,7 +9647,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
@@ -9629,7 +9659,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
@@ -9641,7 +9671,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
@@ -9653,7 +9683,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
@@ -9665,7 +9695,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
@@ -9677,7 +9707,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
@@ -9689,7 +9719,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
@@ -9701,7 +9731,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
@@ -9713,7 +9743,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
@@ -9725,7 +9755,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
@@ -9737,7 +9767,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
@@ -9749,7 +9779,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
@@ -9761,7 +9791,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
@@ -9773,7 +9803,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
@@ -9785,7 +9815,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
@@ -9797,7 +9827,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
@@ -9809,7 +9839,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
@@ -9821,7 +9851,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
@@ -9833,7 +9863,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
@@ -9845,7 +9875,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
@@ -9857,7 +9887,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
@@ -9869,7 +9899,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
@@ -9881,7 +9911,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
@@ -9893,7 +9923,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="0"/>
@@ -9905,7 +9935,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C130" si="1">_xlfn.CONCAT("IF CODE = ",A67," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B67,"';&lt;cr&gt;END_IF;")</f>
@@ -9917,7 +9947,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
@@ -9929,7 +9959,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
@@ -9941,7 +9971,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
@@ -9953,7 +9983,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
@@ -9965,7 +9995,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
@@ -9977,7 +10007,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
@@ -9989,7 +10019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
@@ -10001,7 +10031,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
@@ -10013,7 +10043,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
@@ -10025,7 +10055,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
@@ -10037,7 +10067,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
@@ -10049,7 +10079,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
@@ -10061,7 +10091,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
@@ -10073,7 +10103,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
@@ -10085,7 +10115,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
@@ -10097,7 +10127,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
@@ -10109,7 +10139,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
@@ -10121,7 +10151,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
@@ -10133,7 +10163,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
@@ -10145,7 +10175,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
@@ -10157,7 +10187,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="1"/>
@@ -10169,7 +10199,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="1"/>
@@ -10181,7 +10211,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="1"/>
@@ -10193,7 +10223,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="1"/>
@@ -10205,7 +10235,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="1"/>
@@ -10217,7 +10247,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="1"/>
@@ -10229,7 +10259,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="1"/>
@@ -10241,7 +10271,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="1"/>
@@ -10253,7 +10283,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="1"/>
@@ -10265,7 +10295,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="1"/>
@@ -10277,7 +10307,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="1"/>
@@ -10289,7 +10319,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="1"/>
@@ -10301,7 +10331,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="1"/>
@@ -10313,7 +10343,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="1"/>
@@ -10325,7 +10355,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="1"/>
@@ -10337,7 +10367,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="1"/>
@@ -10349,7 +10379,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="1"/>
@@ -10361,7 +10391,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="1"/>
@@ -10373,7 +10403,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="1"/>
@@ -10385,7 +10415,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
@@ -10397,7 +10427,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="1"/>
@@ -10409,7 +10439,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="1"/>
@@ -10421,7 +10451,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="1"/>
@@ -10433,7 +10463,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="1"/>
@@ -10445,7 +10475,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="1"/>
@@ -10457,7 +10487,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C113" t="str">
         <f t="shared" si="1"/>
@@ -10469,7 +10499,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="1"/>
@@ -10481,7 +10511,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="1"/>
@@ -10493,7 +10523,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="1"/>
@@ -10505,7 +10535,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="1"/>
@@ -10517,7 +10547,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="1"/>
@@ -10529,7 +10559,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="1"/>
@@ -10541,7 +10571,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C120" t="str">
         <f t="shared" si="1"/>
@@ -10553,7 +10583,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="1"/>
@@ -10565,7 +10595,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="1"/>
@@ -10577,7 +10607,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="1"/>
@@ -10589,7 +10619,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="1"/>
@@ -10601,7 +10631,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C125" t="str">
         <f t="shared" si="1"/>
@@ -10613,7 +10643,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C126" t="str">
         <f t="shared" si="1"/>
@@ -10625,7 +10655,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C127" t="str">
         <f t="shared" si="1"/>
@@ -10637,7 +10667,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C128" t="str">
         <f t="shared" si="1"/>
@@ -10649,7 +10679,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C129" t="str">
         <f t="shared" si="1"/>
@@ -10661,7 +10691,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C130" t="str">
         <f t="shared" si="1"/>
@@ -10673,7 +10703,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C131" t="str">
         <f t="shared" ref="C131:C135" si="2">_xlfn.CONCAT("IF CODE = ",A131," THEN&lt;cr&gt;&lt;t&gt;TEXT:='",B131,"';&lt;cr&gt;END_IF;")</f>
@@ -10685,7 +10715,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C132" t="str">
         <f t="shared" si="2"/>
@@ -10697,7 +10727,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C133" t="str">
         <f t="shared" si="2"/>
@@ -10709,7 +10739,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C134" t="str">
         <f t="shared" si="2"/>
@@ -10721,7 +10751,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C135" t="str">
         <f t="shared" si="2"/>
@@ -22083,10 +22113,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A526D88A-D53C-48FF-978F-7E496FB8AA8D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22501,7 +22531,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -22510,6 +22540,9 @@
       </c>
       <c r="C29" t="s">
         <v>570</v>
+      </c>
+      <c r="D29" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -22522,6 +22555,9 @@
       <c r="C30" t="s">
         <v>571</v>
       </c>
+      <c r="E30" t="s">
+        <v>869</v>
+      </c>
     </row>
     <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -22531,13 +22567,13 @@
         <v>569</v>
       </c>
       <c r="C31" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D31" t="s">
         <v>589</v>
       </c>
       <c r="E31" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22554,7 +22590,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="33" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -22563,6 +22599,9 @@
       </c>
       <c r="C33" s="33" t="s">
         <v>580</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>589</v>
       </c>
       <c r="E33" s="33" t="s">
         <v>638</v>
@@ -22582,7 +22621,7 @@
         <v>589</v>
       </c>
       <c r="E34" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22692,7 +22731,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -22701,6 +22740,9 @@
       </c>
       <c r="C42" t="s">
         <v>628</v>
+      </c>
+      <c r="D42" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -22714,7 +22756,7 @@
         <v>630</v>
       </c>
       <c r="E43" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22818,7 +22860,7 @@
         <v>654</v>
       </c>
       <c r="E50" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -22958,7 +23000,7 @@
         <v>665</v>
       </c>
       <c r="C60" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D60" t="s">
         <v>589</v>
@@ -22983,7 +23025,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C62" t="s">
         <v>667</v>
@@ -23011,13 +23053,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>669</v>
+        <v>873</v>
       </c>
       <c r="C64" t="s">
-        <v>673</v>
-      </c>
-      <c r="E64" t="s">
-        <v>670</v>
+        <v>672</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>870</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -23028,7 +23070,10 @@
         <v>669</v>
       </c>
       <c r="C65" t="s">
-        <v>671</v>
+        <v>670</v>
+      </c>
+      <c r="E65" t="s">
+        <v>871</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -23039,7 +23084,7 @@
         <v>669</v>
       </c>
       <c r="C66" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -23050,13 +23095,13 @@
         <v>567</v>
       </c>
       <c r="C67" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D67" t="s">
         <v>654</v>
       </c>
       <c r="E67" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -23067,7 +23112,7 @@
         <v>567</v>
       </c>
       <c r="C68" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D68" t="s">
         <v>654</v>
@@ -23078,19 +23123,19 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
+        <v>818</v>
+      </c>
+      <c r="C69" t="s">
         <v>819</v>
-      </c>
-      <c r="C69" t="s">
-        <v>820</v>
       </c>
       <c r="D69" t="s">
         <v>589</v>
       </c>
       <c r="E69" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>70</v>
       </c>
@@ -23098,7 +23143,10 @@
         <v>573</v>
       </c>
       <c r="C70" t="s">
-        <v>822</v>
+        <v>821</v>
+      </c>
+      <c r="D70" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -23106,10 +23154,10 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C71" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D71" t="s">
         <v>589</v>
@@ -23120,10 +23168,10 @@
         <v>573</v>
       </c>
       <c r="C72" t="s">
+        <v>847</v>
+      </c>
+      <c r="E72" t="s">
         <v>850</v>
-      </c>
-      <c r="E72" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -23131,7 +23179,7 @@
         <v>573</v>
       </c>
       <c r="C73" t="s">
-        <v>834</v>
+        <v>872</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -23139,214 +23187,271 @@
         <v>573</v>
       </c>
       <c r="C74" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="E74" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="C76" t="s">
-        <v>847</v>
+        <v>845</v>
+      </c>
+      <c r="D76" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="C77" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
+        <v>831</v>
+      </c>
+      <c r="C80" t="s">
         <v>832</v>
       </c>
-      <c r="C80" t="s">
-        <v>833</v>
-      </c>
       <c r="E80" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C81" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="83" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C83" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D83" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+    <row r="84" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>861</v>
+      </c>
+      <c r="D84" t="s">
+        <v>589</v>
+      </c>
+      <c r="E84" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>567</v>
+      </c>
+      <c r="C87" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>849</v>
+      </c>
+      <c r="C89" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>567</v>
+      </c>
+      <c r="C90" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>567</v>
+      </c>
+      <c r="C91" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>873</v>
+      </c>
+      <c r="C92" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>873</v>
+      </c>
+      <c r="C93" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>834</v>
+      </c>
+      <c r="C108" t="s">
         <v>836</v>
       </c>
-      <c r="C84" t="s">
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>837</v>
+      </c>
+      <c r="D110" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="86" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C86" t="s">
+      <c r="E111" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
         <v>839</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D113" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>842</v>
+      </c>
+      <c r="D114" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>840</v>
+      </c>
+      <c r="D115" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>837</v>
+      </c>
+      <c r="D118" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>838</v>
+      </c>
+      <c r="E119" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C87" t="s">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>839</v>
+      </c>
+      <c r="D121" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>842</v>
+      </c>
+      <c r="D122" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
         <v>840</v>
       </c>
-      <c r="E87" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C88" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
+      <c r="D123" t="s">
         <v>841</v>
       </c>
-      <c r="D89" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C90" t="s">
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127" t="s">
+        <v>856</v>
+      </c>
+      <c r="D127" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>2</v>
+      </c>
+      <c r="C128" t="s">
+        <v>855</v>
+      </c>
+      <c r="E128" t="s">
         <v>844</v>
       </c>
-      <c r="D90" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
-        <v>842</v>
-      </c>
-      <c r="D91" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C94" t="s">
-        <v>839</v>
-      </c>
-      <c r="D94" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C95" t="s">
-        <v>840</v>
-      </c>
-      <c r="E95" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C96" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C97" t="s">
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>3</v>
+      </c>
+      <c r="C129" t="s">
+        <v>854</v>
+      </c>
+      <c r="D129" t="s">
         <v>841</v>
       </c>
-      <c r="D97" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C98" t="s">
-        <v>844</v>
-      </c>
-      <c r="D98" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C99" t="s">
-        <v>842</v>
-      </c>
-      <c r="D99" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B103">
-        <v>1</v>
-      </c>
-      <c r="C103" t="s">
-        <v>859</v>
-      </c>
-      <c r="D103" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B104">
-        <v>2</v>
-      </c>
-      <c r="C104" t="s">
-        <v>858</v>
-      </c>
-      <c r="E104" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B105">
-        <v>3</v>
-      </c>
-      <c r="C105" t="s">
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>4</v>
+      </c>
+      <c r="C130" t="s">
+        <v>853</v>
+      </c>
+      <c r="D130" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>5</v>
+      </c>
+      <c r="C131" t="s">
         <v>857</v>
       </c>
-      <c r="D105" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B106">
-        <v>4</v>
-      </c>
-      <c r="C106" t="s">
-        <v>856</v>
-      </c>
-      <c r="D106" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B107">
-        <v>5</v>
-      </c>
-      <c r="C107" t="s">
-        <v>860</v>
-      </c>
-      <c r="D107" t="s">
-        <v>843</v>
+      <c r="D131" t="s">
+        <v>841</v>
       </c>
     </row>
   </sheetData>
@@ -23374,7 +23479,7 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -23382,7 +23487,7 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="C4">
         <v>150</v>
@@ -23402,13 +23507,13 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" s="26" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -23492,15 +23597,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9F7729ADF49144A01A6175DD599202" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f00ebe7287476f312414df31db46304">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c96d9849-7071-4555-8535-ee11c374d0f7" xmlns:ns3="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f2e969a0d0c60cbdf6bd0d859a86451" ns2:_="" ns3:_="">
     <xsd:import namespace="c96d9849-7071-4555-8535-ee11c374d0f7"/>
@@ -23723,6 +23819,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -23742,14 +23847,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6596B7D1-B3E6-40CB-B05E-2E959D1A2B6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23764,6 +23861,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
EXCEL - updateing the J1939 list for C3.6 PGN's we need to support
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B621FDAD-C458-4BB3-9F54-57AA519779D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7A860E-81A6-4EBD-AAB6-A95F4BE82496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="6" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="857" activeTab="7" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">SNAGS!$A$1:$E$91</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2390" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2528" uniqueCount="975">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2624,15 +2625,6 @@
     <t>Radial feeder</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Radial mode - swap buttons 2+3</t>
   </si>
   <si>
@@ -2670,13 +2662,325 @@
   </si>
   <si>
     <t>ENGINE_SCREEN</t>
+  </si>
+  <si>
+    <t>TSC1</t>
+  </si>
+  <si>
+    <t>CM2</t>
+  </si>
+  <si>
+    <t>CM1</t>
+  </si>
+  <si>
+    <t>F004</t>
+  </si>
+  <si>
+    <t>FEEE</t>
+  </si>
+  <si>
+    <t>FEEF</t>
+  </si>
+  <si>
+    <t>FECA</t>
+  </si>
+  <si>
+    <t>FEE5</t>
+  </si>
+  <si>
+    <t>FD7C</t>
+  </si>
+  <si>
+    <t>ENGINE TEMPERATURE 1</t>
+  </si>
+  <si>
+    <t>PGN HEX</t>
+  </si>
+  <si>
+    <t>PGN Dec</t>
+  </si>
+  <si>
+    <t>ENGINE FLUID LEVEL PRESSURE 1</t>
+  </si>
+  <si>
+    <t>Active Diagnostic Trouble Codes</t>
+  </si>
+  <si>
+    <t>ENGINE HOURS</t>
+  </si>
+  <si>
+    <t>DM2</t>
+  </si>
+  <si>
+    <t>FECB</t>
+  </si>
+  <si>
+    <t>DPFC1</t>
+  </si>
+  <si>
+    <t>DIESEL PARTICULATE FILTER CONTROL 1</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>Engine Ignition Control Maintenance Hours Reset</t>
+  </si>
+  <si>
+    <t>DE00</t>
+  </si>
+  <si>
+    <t>RX</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>EEC1</t>
+  </si>
+  <si>
+    <t>ELECTRONIC ENGINE CONTROLLER 1</t>
+  </si>
+  <si>
+    <t>ELECTRONIC ENGINE CONTROLLER 3</t>
+  </si>
+  <si>
+    <t>EEC3</t>
+  </si>
+  <si>
+    <t>FEDF</t>
+  </si>
+  <si>
+    <t>ET1</t>
+  </si>
+  <si>
+    <t>FLUID</t>
+  </si>
+  <si>
+    <t>HOURS</t>
+  </si>
+  <si>
+    <t>LFC</t>
+  </si>
+  <si>
+    <t>FEE9</t>
+  </si>
+  <si>
+    <t>FUEL ECONOMY</t>
+  </si>
+  <si>
+    <t>FUEL CONSUMPTION</t>
+  </si>
+  <si>
+    <t>LIQUID</t>
+  </si>
+  <si>
+    <t>FEF2</t>
+  </si>
+  <si>
+    <t>On Req</t>
+  </si>
+  <si>
+    <t>AMBIENT CONDITIONS</t>
+  </si>
+  <si>
+    <t>FEF5</t>
+  </si>
+  <si>
+    <t>INTAKE/EXHAUST CONDITIONS 1</t>
+  </si>
+  <si>
+    <t>FEF6</t>
+  </si>
+  <si>
+    <t>ENGINE FLUID LEVEL/PRESSURE 1</t>
+  </si>
+  <si>
+    <t>AFTERTREATMENT 1 INTAKE GAS 2</t>
+  </si>
+  <si>
+    <t>FDB4</t>
+  </si>
+  <si>
+    <t>ENGINE FLUID LEVEL/PRESSURE 2</t>
+  </si>
+  <si>
+    <t>FEDB</t>
+  </si>
+  <si>
+    <t>AFTERTREATMENT 1 DIESEL EXHAUST FLUID TANK 1 INFORMATION</t>
+  </si>
+  <si>
+    <t>FE56</t>
+  </si>
+  <si>
+    <t>Engine Charge Air Cooler 1 Outlet Temperature</t>
+  </si>
+  <si>
+    <t>Aftertreatment 1 SCR System State</t>
+  </si>
+  <si>
+    <t>F023</t>
+  </si>
+  <si>
+    <t>FE6A</t>
+  </si>
+  <si>
+    <t>AFTERTREATMENT 1 SCR EXHAUST GAS TEMPERATURE 1</t>
+  </si>
+  <si>
+    <t>FD3E</t>
+  </si>
+  <si>
+    <t>VEHICLE ELECTRICAL POWER 1</t>
+  </si>
+  <si>
+    <t>FEF7</t>
+  </si>
+  <si>
+    <t>VEP1</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>AMB</t>
+  </si>
+  <si>
+    <t>EFLP1</t>
+  </si>
+  <si>
+    <t>E000</t>
+  </si>
+  <si>
+    <t>Cab Message 1 (Aftertreatment Regeneration Inhibit Switch)</t>
+  </si>
+  <si>
+    <t>Throttle Speed Command Message 1</t>
+  </si>
+  <si>
+    <t>CAB Message 2</t>
+  </si>
+  <si>
+    <t>AT1IG2</t>
+  </si>
+  <si>
+    <t>https://www.isobus.net/isobus/pGNAndSPN/index?PGNAndSPN_page=3</t>
+  </si>
+  <si>
+    <t>EFL/P2</t>
+  </si>
+  <si>
+    <t>AT1T1I1</t>
+  </si>
+  <si>
+    <t>EFS</t>
+  </si>
+  <si>
+    <t>ENGINE FUEL/LUBE SYSTEMS</t>
+  </si>
+  <si>
+    <t>A1SCRDSI1</t>
+  </si>
+  <si>
+    <t>ET3</t>
+  </si>
+  <si>
+    <t>A1SCREGT1</t>
+  </si>
+  <si>
+    <t>SAE NAME</t>
+  </si>
+  <si>
+    <t>PGN Group</t>
+  </si>
+  <si>
+    <t>ELECTRONIC ENGINE CONTROLLER 5</t>
+  </si>
+  <si>
+    <t>EEC5</t>
+  </si>
+  <si>
+    <t>FDD5</t>
+  </si>
+  <si>
+    <t>FD20</t>
+  </si>
+  <si>
+    <t>AFTERTREATMENT 1 DIESEL OXIDATION CATALYST</t>
+  </si>
+  <si>
+    <t>A1DOC</t>
+  </si>
+  <si>
+    <t>TURBOCHARGER WASTEGATE</t>
+  </si>
+  <si>
+    <t>TCW</t>
+  </si>
+  <si>
+    <t>FC31</t>
+  </si>
+  <si>
+    <t>OPERATOR INDICATORS</t>
+  </si>
+  <si>
+    <t>FEFF</t>
+  </si>
+  <si>
+    <t>OI</t>
+  </si>
+  <si>
+    <t>ELECTRONIC ENGINE CONTROLLER 2</t>
+  </si>
+  <si>
+    <t>EEC2</t>
+  </si>
+  <si>
+    <t>F003</t>
+  </si>
+  <si>
+    <t>DIRECT LAMP CONTROL COMMAND 1</t>
+  </si>
+  <si>
+    <t>DLCC1</t>
+  </si>
+  <si>
+    <t>FD07</t>
+  </si>
+  <si>
+    <t>Direct Lamp Control Data 1</t>
+  </si>
+  <si>
+    <t>DLCD1#</t>
+  </si>
+  <si>
+    <t>FD05</t>
+  </si>
+  <si>
+    <t>SOFTWARE IDENTIFICATION</t>
+  </si>
+  <si>
+    <t>FEDA</t>
+  </si>
+  <si>
+    <t>SOFT</t>
+  </si>
+  <si>
+    <t>COMPONENT IDENTIFICATION</t>
+  </si>
+  <si>
+    <t>FEEB</t>
+  </si>
+  <si>
+    <t>CI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2806,6 +3110,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2839,10 +3151,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2924,11 +3237,23 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -22115,7 +22440,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -22556,7 +22881,7 @@
         <v>571</v>
       </c>
       <c r="E30" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
     </row>
     <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -23053,13 +23378,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="C64" t="s">
         <v>672</v>
       </c>
       <c r="E64" s="33" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -23073,7 +23398,7 @@
         <v>670</v>
       </c>
       <c r="E65" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -23179,7 +23504,7 @@
         <v>573</v>
       </c>
       <c r="C73" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -23244,13 +23569,13 @@
     </row>
     <row r="84" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="D84" t="s">
         <v>589</v>
       </c>
       <c r="E84" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
@@ -23258,7 +23583,7 @@
         <v>567</v>
       </c>
       <c r="C87" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
@@ -23266,7 +23591,7 @@
         <v>849</v>
       </c>
       <c r="C89" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
@@ -23274,7 +23599,7 @@
         <v>567</v>
       </c>
       <c r="C90" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
@@ -23282,23 +23607,23 @@
         <v>567</v>
       </c>
       <c r="C91" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="C92" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="C93" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
@@ -23466,137 +23791,689 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692637BC-36A2-49E1-8104-C2CAB79C8E2F}">
-  <dimension ref="B3:F20"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="6" width="9.140625" style="26"/>
+    <col min="1" max="1" width="64.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="35"/>
+    <col min="4" max="5" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>858</v>
-      </c>
-      <c r="C3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>859</v>
-      </c>
-      <c r="C4">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <f>DEGREES(ATAN($C$3/$C$4))</f>
-        <v>18.43494882292201</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <f>RADIANS(C5)</f>
-        <v>0.32175055439664219</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="26" t="s">
-        <v>860</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>858</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="35">
+    <row r="1" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>947</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>946</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>881</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>882</v>
+      </c>
+      <c r="E1" s="40"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>896</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>895</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>874</v>
+      </c>
+      <c r="D2" s="26">
+        <f>HEX2DEC(C2)</f>
+        <v>61444</v>
+      </c>
+      <c r="F2" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>960</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>961</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>962</v>
+      </c>
+      <c r="D3" s="26">
+        <f>HEX2DEC(C3)</f>
+        <v>61443</v>
+      </c>
+      <c r="F3" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>897</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>898</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>899</v>
+      </c>
+      <c r="D4" s="26">
+        <f>HEX2DEC(C4)</f>
+        <v>65247</v>
+      </c>
+      <c r="F4" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>948</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>949</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>950</v>
+      </c>
+      <c r="D5" s="26">
+        <f>HEX2DEC(C5)</f>
+        <v>64981</v>
+      </c>
+      <c r="F5" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>880</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>900</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>875</v>
+      </c>
+      <c r="D6" s="26">
+        <f t="shared" ref="D6:D7" si="0">HEX2DEC(C6)</f>
+        <v>65262</v>
+      </c>
+      <c r="F6" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>883</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>901</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>876</v>
+      </c>
+      <c r="D7" s="26">
+        <f t="shared" si="0"/>
+        <v>65263</v>
+      </c>
+      <c r="F7" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>885</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>902</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>878</v>
+      </c>
+      <c r="D8" s="26">
+        <f>HEX2DEC(C8)</f>
+        <v>65253</v>
+      </c>
+      <c r="F8" t="s">
+        <v>894</v>
+      </c>
+      <c r="G8" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
+        <v>884</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>564</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>877</v>
+      </c>
+      <c r="D9" s="26">
+        <f>HEX2DEC(C9)</f>
+        <v>65226</v>
+      </c>
+      <c r="F9" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
+        <v>884</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>886</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>887</v>
+      </c>
+      <c r="D10" s="26">
+        <f>HEX2DEC(C10)</f>
+        <v>65227</v>
+      </c>
+      <c r="F10" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>917</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>939</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>918</v>
+      </c>
+      <c r="D11" s="26">
+        <f>HEX2DEC(C11)</f>
+        <v>65243</v>
+      </c>
+      <c r="F11" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>905</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>907</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>908</v>
+      </c>
+      <c r="D12" s="26">
+        <f>HEX2DEC(C12)</f>
+        <v>65266</v>
+      </c>
+      <c r="F12" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>906</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>903</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>904</v>
+      </c>
+      <c r="D13" s="26">
+        <f>HEX2DEC(C13)</f>
+        <v>65257</v>
+      </c>
+      <c r="F13" t="s">
+        <v>894</v>
+      </c>
+      <c r="G13" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>910</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>931</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>911</v>
+      </c>
+      <c r="D14" s="26">
+        <f>HEX2DEC(C14)</f>
+        <v>65269</v>
+      </c>
+      <c r="F14" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>912</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>930</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>913</v>
+      </c>
+      <c r="D15" s="26">
+        <f>HEX2DEC(C15)</f>
+        <v>65270</v>
+      </c>
+      <c r="F15" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>914</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>932</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>876</v>
+      </c>
+      <c r="D16" s="26">
+        <f>HEX2DEC(C16)</f>
+        <v>65263</v>
+      </c>
+      <c r="F16" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>927</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>929</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>928</v>
+      </c>
+      <c r="D17" s="26">
+        <f>HEX2DEC(C17)</f>
+        <v>65271</v>
+      </c>
+      <c r="F17" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>942</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>941</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>924</v>
+      </c>
+      <c r="D18" s="26">
+        <f>HEX2DEC(C18)</f>
+        <v>65130</v>
+      </c>
+      <c r="F18" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>935</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>871</v>
+      </c>
+      <c r="C20" s="35">
         <v>0</v>
       </c>
-      <c r="E10" s="26">
-        <f>$C$4*C10</f>
+      <c r="D20" s="26">
+        <f>HEX2DEC(C20)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="26">
-        <f>$C$3*C10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="35">
-        <v>0.25</v>
-      </c>
-      <c r="E11" s="26">
-        <f t="shared" ref="E11:E14" si="0">$C$4*C11</f>
-        <v>37.5</v>
-      </c>
-      <c r="F11" s="26">
-        <f t="shared" ref="F11:F14" si="1">$C$3*C11</f>
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="E12" s="26">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="F12" s="26">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="35">
-        <v>0.75</v>
-      </c>
-      <c r="E13" s="26">
-        <f t="shared" si="0"/>
-        <v>112.5</v>
-      </c>
-      <c r="F13" s="26">
-        <f t="shared" si="1"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="35">
-        <v>1</v>
-      </c>
-      <c r="E14" s="26">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="F14" s="26">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>100</v>
-      </c>
+      <c r="F20" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>934</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>873</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>933</v>
+      </c>
+      <c r="D21" s="26">
+        <f>HEX2DEC(C21)</f>
+        <v>57344</v>
+      </c>
+      <c r="F21" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>936</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>872</v>
+      </c>
+      <c r="C22" s="35">
+        <v>8500</v>
+      </c>
+      <c r="D22" s="26">
+        <f>HEX2DEC(C22)</f>
+        <v>34048</v>
+      </c>
+      <c r="F22" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>891</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>890</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>892</v>
+      </c>
+      <c r="D23" s="26">
+        <f>HEX2DEC(C23)</f>
+        <v>56832</v>
+      </c>
+      <c r="F23" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>889</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>888</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>879</v>
+      </c>
+      <c r="D25" s="26">
+        <f>HEX2DEC(C25)</f>
+        <v>64892</v>
+      </c>
+      <c r="F25" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>915</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>937</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>916</v>
+      </c>
+      <c r="D26" s="26">
+        <f>HEX2DEC(C26)</f>
+        <v>64948</v>
+      </c>
+      <c r="F26" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>919</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>940</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>920</v>
+      </c>
+      <c r="D27" s="26">
+        <f>HEX2DEC(C27)</f>
+        <v>65110</v>
+      </c>
+      <c r="F27" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>922</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>943</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>923</v>
+      </c>
+      <c r="D28" s="26">
+        <f t="shared" ref="D28:D39" si="1">HEX2DEC(C28)</f>
+        <v>61475</v>
+      </c>
+      <c r="F28" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>921</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>944</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>920</v>
+      </c>
+      <c r="D29" s="26">
+        <f t="shared" si="1"/>
+        <v>65110</v>
+      </c>
+      <c r="F29" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>925</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>945</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>926</v>
+      </c>
+      <c r="D30" s="26">
+        <f t="shared" si="1"/>
+        <v>64830</v>
+      </c>
+      <c r="F30" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>952</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>953</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>951</v>
+      </c>
+      <c r="D31" s="26">
+        <f t="shared" si="1"/>
+        <v>64800</v>
+      </c>
+      <c r="F31" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>954</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>955</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>956</v>
+      </c>
+      <c r="D32" s="26">
+        <f t="shared" si="1"/>
+        <v>64561</v>
+      </c>
+      <c r="F32" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>957</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>959</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>958</v>
+      </c>
+      <c r="D34" s="26">
+        <f t="shared" si="1"/>
+        <v>65279</v>
+      </c>
+      <c r="F34" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>963</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>964</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>965</v>
+      </c>
+      <c r="D35" s="26">
+        <f t="shared" si="1"/>
+        <v>64775</v>
+      </c>
+      <c r="F35" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>966</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>967</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>968</v>
+      </c>
+      <c r="D36" s="26">
+        <f t="shared" si="1"/>
+        <v>64773</v>
+      </c>
+      <c r="F36" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>969</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>971</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>970</v>
+      </c>
+      <c r="D38" s="26">
+        <f t="shared" si="1"/>
+        <v>65242</v>
+      </c>
+      <c r="F38" t="s">
+        <v>894</v>
+      </c>
+      <c r="G38" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>972</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>974</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>973</v>
+      </c>
+      <c r="D39" s="26">
+        <f t="shared" si="1"/>
+        <v>65259</v>
+      </c>
+      <c r="F39" t="s">
+        <v>894</v>
+      </c>
+      <c r="G39" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="37" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="36"/>
+      <c r="B50" s="36"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="36"/>
+      <c r="B51" s="36"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A41" r:id="rId1" xr:uid="{B80028AB-436B-4C7D-979E-21DB1B952145}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9F7729ADF49144A01A6175DD599202" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f00ebe7287476f312414df31db46304">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c96d9849-7071-4555-8535-ee11c374d0f7" xmlns:ns3="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f2e969a0d0c60cbdf6bd0d859a86451" ns2:_="" ns3:_="">
     <xsd:import namespace="c96d9849-7071-4555-8535-ee11c374d0f7"/>
@@ -23819,15 +24696,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -23847,6 +24715,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6596B7D1-B3E6-40CB-B05E-2E959D1A2B6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23861,14 +24737,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
EXCEL - file for the last commit
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7A860E-81A6-4EBD-AAB6-A95F4BE82496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B73E109-712A-415D-89B3-A65687DE5400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="857" activeTab="7" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="7" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">SNAGS!$A$1:$E$91</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2528" uniqueCount="975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2524" uniqueCount="973">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2793,9 +2792,6 @@
     <t>FEF6</t>
   </si>
   <si>
-    <t>ENGINE FLUID LEVEL/PRESSURE 1</t>
-  </si>
-  <si>
     <t>AFTERTREATMENT 1 INTAKE GAS 2</t>
   </si>
   <si>
@@ -2847,9 +2843,6 @@
     <t>AMB</t>
   </si>
   <si>
-    <t>EFLP1</t>
-  </si>
-  <si>
     <t>E000</t>
   </si>
   <si>
@@ -2868,9 +2861,6 @@
     <t>https://www.isobus.net/isobus/pGNAndSPN/index?PGNAndSPN_page=3</t>
   </si>
   <si>
-    <t>EFL/P2</t>
-  </si>
-  <si>
     <t>AT1T1I1</t>
   </si>
   <si>
@@ -2974,13 +2964,16 @@
   </si>
   <si>
     <t>CI</t>
+  </si>
+  <si>
+    <t>EFL_P2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3118,13 +3111,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -3155,7 +3161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3249,6 +3255,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -23791,9 +23810,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692637BC-36A2-49E1-8104-C2CAB79C8E2F}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23805,10 +23826,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="C1" s="39" t="s">
         <v>881</v>
@@ -23838,13 +23859,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="D3" s="26">
         <f>HEX2DEC(C3)</f>
@@ -23874,13 +23895,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="D5" s="26">
         <f>HEX2DEC(C5)</f>
@@ -23937,7 +23958,7 @@
         <v>878</v>
       </c>
       <c r="D8" s="26">
-        <f>HEX2DEC(C8)</f>
+        <f t="shared" ref="D8:D17" si="1">HEX2DEC(C8)</f>
         <v>65253</v>
       </c>
       <c r="F8" t="s">
@@ -23958,7 +23979,7 @@
         <v>877</v>
       </c>
       <c r="D9" s="26">
-        <f>HEX2DEC(C9)</f>
+        <f t="shared" si="1"/>
         <v>65226</v>
       </c>
       <c r="F9" t="s">
@@ -23976,7 +23997,7 @@
         <v>887</v>
       </c>
       <c r="D10" s="26">
-        <f>HEX2DEC(C10)</f>
+        <f t="shared" si="1"/>
         <v>65227</v>
       </c>
       <c r="F10" t="s">
@@ -23985,16 +24006,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>916</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>972</v>
+      </c>
+      <c r="C11" s="35" t="s">
         <v>917</v>
       </c>
-      <c r="B11" s="35" t="s">
-        <v>939</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>918</v>
-      </c>
       <c r="D11" s="26">
-        <f>HEX2DEC(C11)</f>
+        <f t="shared" si="1"/>
         <v>65243</v>
       </c>
       <c r="F11" t="s">
@@ -24012,7 +24033,7 @@
         <v>908</v>
       </c>
       <c r="D12" s="26">
-        <f>HEX2DEC(C12)</f>
+        <f t="shared" si="1"/>
         <v>65266</v>
       </c>
       <c r="F12" t="s">
@@ -24030,7 +24051,7 @@
         <v>904</v>
       </c>
       <c r="D13" s="26">
-        <f>HEX2DEC(C13)</f>
+        <f t="shared" si="1"/>
         <v>65257</v>
       </c>
       <c r="F13" t="s">
@@ -24045,13 +24066,13 @@
         <v>910</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>911</v>
       </c>
       <c r="D14" s="26">
-        <f>HEX2DEC(C14)</f>
+        <f t="shared" si="1"/>
         <v>65269</v>
       </c>
       <c r="F14" t="s">
@@ -24063,13 +24084,13 @@
         <v>912</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>913</v>
       </c>
       <c r="D15" s="26">
-        <f>HEX2DEC(C15)</f>
+        <f t="shared" si="1"/>
         <v>65270</v>
       </c>
       <c r="F15" t="s">
@@ -24078,17 +24099,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>914</v>
+        <v>926</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>876</v>
+        <v>927</v>
       </c>
       <c r="D16" s="26">
-        <f>HEX2DEC(C16)</f>
-        <v>65263</v>
+        <f t="shared" si="1"/>
+        <v>65271</v>
       </c>
       <c r="F16" t="s">
         <v>894</v>
@@ -24096,125 +24117,129 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>927</v>
+        <v>939</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>929</v>
+        <v>938</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>928</v>
+        <v>923</v>
       </c>
       <c r="D17" s="26">
-        <f>HEX2DEC(C17)</f>
-        <v>65271</v>
+        <f t="shared" si="1"/>
+        <v>65130</v>
       </c>
       <c r="F17" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>942</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>941</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>924</v>
-      </c>
-      <c r="D18" s="26">
-        <f>HEX2DEC(C18)</f>
-        <v>65130</v>
-      </c>
-      <c r="F18" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="43" t="s">
+        <v>933</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>871</v>
+      </c>
+      <c r="C19" s="44">
+        <v>0</v>
+      </c>
+      <c r="D19" s="45">
+        <f>HEX2DEC(C19)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="45"/>
+      <c r="F19" s="43" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="43" t="s">
+        <v>932</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>873</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>931</v>
+      </c>
+      <c r="D20" s="45">
+        <f>HEX2DEC(C20)</f>
+        <v>57344</v>
+      </c>
+      <c r="E20" s="45"/>
+      <c r="F20" s="43" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="43" t="s">
+        <v>934</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>872</v>
+      </c>
+      <c r="C21" s="44">
+        <v>8500</v>
+      </c>
+      <c r="D21" s="45">
+        <f>HEX2DEC(C21)</f>
+        <v>34048</v>
+      </c>
+      <c r="E21" s="45"/>
+      <c r="F21" s="43" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>891</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>890</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>892</v>
+      </c>
+      <c r="D22" s="45">
+        <f>HEX2DEC(C22)</f>
+        <v>56832</v>
+      </c>
+      <c r="E22" s="45"/>
+      <c r="F22" s="43" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>889</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>888</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>879</v>
+      </c>
+      <c r="D24" s="26">
+        <f>HEX2DEC(C24)</f>
+        <v>64892</v>
+      </c>
+      <c r="F24" t="s">
         <v>894</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>935</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>871</v>
-      </c>
-      <c r="C20" s="35">
-        <v>0</v>
-      </c>
-      <c r="D20" s="26">
-        <f>HEX2DEC(C20)</f>
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>934</v>
-      </c>
-      <c r="B21" s="35" t="s">
-        <v>873</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>933</v>
-      </c>
-      <c r="D21" s="26">
-        <f>HEX2DEC(C21)</f>
-        <v>57344</v>
-      </c>
-      <c r="F21" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>936</v>
-      </c>
-      <c r="B22" s="35" t="s">
-        <v>872</v>
-      </c>
-      <c r="C22" s="35">
-        <v>8500</v>
-      </c>
-      <c r="D22" s="26">
-        <f>HEX2DEC(C22)</f>
-        <v>34048</v>
-      </c>
-      <c r="F22" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>891</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>890</v>
-      </c>
-      <c r="C23" s="35" t="s">
-        <v>892</v>
-      </c>
-      <c r="D23" s="26">
-        <f>HEX2DEC(C23)</f>
-        <v>56832</v>
-      </c>
-      <c r="F23" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>889</v>
+        <v>914</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>888</v>
+        <v>935</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>879</v>
+        <v>915</v>
       </c>
       <c r="D25" s="26">
         <f>HEX2DEC(C25)</f>
-        <v>64892</v>
+        <v>64948</v>
       </c>
       <c r="F25" t="s">
         <v>894</v>
@@ -24222,17 +24247,17 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="B26" s="35" t="s">
         <v>937</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
       <c r="D26" s="26">
         <f>HEX2DEC(C26)</f>
-        <v>64948</v>
+        <v>65110</v>
       </c>
       <c r="F26" t="s">
         <v>894</v>
@@ -24240,17 +24265,17 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="B27" s="35" t="s">
         <v>940</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D27" s="26">
-        <f>HEX2DEC(C27)</f>
-        <v>65110</v>
+        <f t="shared" ref="D27:D38" si="2">HEX2DEC(C27)</f>
+        <v>61475</v>
       </c>
       <c r="F27" t="s">
         <v>894</v>
@@ -24258,17 +24283,17 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="D28" s="26">
-        <f t="shared" ref="D28:D39" si="1">HEX2DEC(C28)</f>
-        <v>61475</v>
+        <f t="shared" si="2"/>
+        <v>65110</v>
       </c>
       <c r="F28" t="s">
         <v>894</v>
@@ -24276,17 +24301,17 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>920</v>
+        <v>925</v>
       </c>
       <c r="D29" s="26">
-        <f t="shared" si="1"/>
-        <v>65110</v>
+        <f t="shared" si="2"/>
+        <v>64830</v>
       </c>
       <c r="F29" t="s">
         <v>894</v>
@@ -24294,71 +24319,72 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>925</v>
+        <v>949</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>945</v>
+        <v>950</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>926</v>
+        <v>948</v>
       </c>
       <c r="D30" s="26">
-        <f t="shared" si="1"/>
-        <v>64830</v>
+        <f t="shared" si="2"/>
+        <v>64800</v>
       </c>
       <c r="F30" t="s">
         <v>894</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="33" t="s">
+        <v>951</v>
+      </c>
+      <c r="B31" s="41" t="s">
         <v>952</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="C31" s="41" t="s">
         <v>953</v>
       </c>
-      <c r="C31" s="35" t="s">
-        <v>951</v>
-      </c>
-      <c r="D31" s="26">
-        <f t="shared" si="1"/>
-        <v>64800</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="D31" s="42">
+        <f t="shared" si="2"/>
+        <v>64561</v>
+      </c>
+      <c r="E31" s="42"/>
+      <c r="F31" s="33" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>954</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B33" s="35" t="s">
+        <v>956</v>
+      </c>
+      <c r="C33" s="35" t="s">
         <v>955</v>
       </c>
-      <c r="C32" s="35" t="s">
-        <v>956</v>
-      </c>
-      <c r="D32" s="26">
-        <f t="shared" si="1"/>
-        <v>64561</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="D33" s="26">
+        <f t="shared" si="2"/>
+        <v>65279</v>
+      </c>
+      <c r="F33" t="s">
         <v>894</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>957</v>
+        <v>960</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>958</v>
+        <v>962</v>
       </c>
       <c r="D34" s="26">
-        <f t="shared" si="1"/>
-        <v>65279</v>
+        <f t="shared" si="2"/>
+        <v>64775</v>
       </c>
       <c r="F34" t="s">
         <v>894</v>
@@ -24375,29 +24401,32 @@
         <v>965</v>
       </c>
       <c r="D35" s="26">
-        <f t="shared" si="1"/>
-        <v>64775</v>
+        <f t="shared" si="2"/>
+        <v>64773</v>
       </c>
       <c r="F35" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>966</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B37" s="35" t="s">
+        <v>968</v>
+      </c>
+      <c r="C37" s="35" t="s">
         <v>967</v>
       </c>
-      <c r="C36" s="35" t="s">
-        <v>968</v>
-      </c>
-      <c r="D36" s="26">
-        <f t="shared" si="1"/>
-        <v>64773</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="D37" s="26">
+        <f t="shared" si="2"/>
+        <v>65242</v>
+      </c>
+      <c r="F37" t="s">
         <v>894</v>
+      </c>
+      <c r="G37" t="s">
+        <v>909</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -24411,8 +24440,8 @@
         <v>970</v>
       </c>
       <c r="D38" s="26">
-        <f t="shared" si="1"/>
-        <v>65242</v>
+        <f t="shared" si="2"/>
+        <v>65259</v>
       </c>
       <c r="F38" t="s">
         <v>894</v>
@@ -24421,43 +24450,22 @@
         <v>909</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>972</v>
-      </c>
-      <c r="B39" s="35" t="s">
-        <v>974</v>
-      </c>
-      <c r="C39" s="35" t="s">
-        <v>973</v>
-      </c>
-      <c r="D39" s="26">
-        <f t="shared" si="1"/>
-        <v>65259</v>
-      </c>
-      <c r="F39" t="s">
-        <v>894</v>
-      </c>
-      <c r="G39" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="37" t="s">
-        <v>938</v>
-      </c>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="37" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="36"/>
+      <c r="B49" s="36"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="36"/>
       <c r="B50" s="36"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="36"/>
-      <c r="B51" s="36"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A41" r:id="rId1" xr:uid="{B80028AB-436B-4C7D-979E-21DB1B952145}"/>
+    <hyperlink ref="A40" r:id="rId1" xr:uid="{B80028AB-436B-4C7D-979E-21DB1B952145}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -24465,12 +24473,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
+    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
+      <UserInfo>
+        <DisplayName>Noel Loughran</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24697,27 +24714,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
-    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
-      <UserInfo>
-        <DisplayName>Noel Loughran</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -24742,18 +24759,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
EXCEL from last commit
</commit_message>
<xml_diff>
--- a/T620X_IO.xlsx
+++ b/T620X_IO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_plc\MTech\MTech_T620X_Trommel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLC_DEV\MTech\Mtech_T620X_Trommel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B73E109-712A-415D-89B3-A65687DE5400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0FBAE4-DA39-47A2-9099-4879E8FF8915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" tabRatio="857" activeTab="7" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="857" activeTab="8" xr2:uid="{2FCBBB71-3591-49CF-88C3-9E3184A7626E}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="11" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="ALARMS_IO" sheetId="31" r:id="rId6"/>
     <sheet name="SNAGS" sheetId="33" r:id="rId7"/>
     <sheet name="Sheet2" sheetId="35" r:id="rId8"/>
+    <sheet name="Sheet3" sheetId="36" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ALARMS_IO!$A$1:$K$48</definedName>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2524" uniqueCount="973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2617" uniqueCount="1008">
   <si>
     <t>PLC Name</t>
   </si>
@@ -2967,6 +2968,111 @@
   </si>
   <si>
     <t>EFL_P2</t>
+  </si>
+  <si>
+    <t>EngRqedSpeedCtrlConditions</t>
+  </si>
+  <si>
+    <t>EngOverrideCtrlMode</t>
+  </si>
+  <si>
+    <t>OverrideCtrlModePriority</t>
+  </si>
+  <si>
+    <t>EngRqedSpeed_SpeedLimit</t>
+  </si>
+  <si>
+    <t>EngRqedTorque_TorqueLimit</t>
+  </si>
+  <si>
+    <t>TransmissionRate</t>
+  </si>
+  <si>
+    <t>ControlPurpose</t>
+  </si>
+  <si>
+    <t>EngineRequestedTorqueHiRes</t>
+  </si>
+  <si>
+    <t>MessageCounter</t>
+  </si>
+  <si>
+    <t>MessageChecksum</t>
+  </si>
+  <si>
+    <t>USINT</t>
+  </si>
+  <si>
+    <t>REAL</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>EngTorqueMode</t>
+  </si>
+  <si>
+    <t>ActlEngPrcntTrqueHighResolution</t>
+  </si>
+  <si>
+    <t>DriversDemandEngPercentTorque</t>
+  </si>
+  <si>
+    <t>ActualEngPercentTorque</t>
+  </si>
+  <si>
+    <t>EngSpeed</t>
+  </si>
+  <si>
+    <t>SrcAddrssOfCtrllngDvcFrEngCntrl</t>
+  </si>
+  <si>
+    <t>EngStarterMode</t>
+  </si>
+  <si>
+    <t>EngDemandPercentTorque</t>
+  </si>
+  <si>
+    <t>ProtectLampStatus</t>
+  </si>
+  <si>
+    <t>AmberWarningLampStatus</t>
+  </si>
+  <si>
+    <t>RedStopLampState</t>
+  </si>
+  <si>
+    <t>MalfunctionIndicatorLampStatus</t>
+  </si>
+  <si>
+    <t>FlashProtectLamp</t>
+  </si>
+  <si>
+    <t>FlashAmberWarningLamp</t>
+  </si>
+  <si>
+    <t>FlashRedStopLamp</t>
+  </si>
+  <si>
+    <t>FlashMalfuncIndicatorLamp</t>
+  </si>
+  <si>
+    <t>DTC1</t>
+  </si>
+  <si>
+    <t>DTC2</t>
+  </si>
+  <si>
+    <t>DTC3</t>
+  </si>
+  <si>
+    <t>DTC4</t>
+  </si>
+  <si>
+    <t>DTC5</t>
+  </si>
+  <si>
+    <t>UDINT</t>
   </si>
 </sst>
 </file>
@@ -23812,7 +23918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692637BC-36A2-49E1-8104-C2CAB79C8E2F}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -24472,22 +24578,413 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67835F87-8E16-4012-B1FC-4AA8A57E1B78}">
+  <dimension ref="B3:H38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>871</v>
+      </c>
+      <c r="C3" t="s">
+        <v>974</v>
+      </c>
+      <c r="E3" t="s">
+        <v>983</v>
+      </c>
+      <c r="H3" t="str">
+        <f>_xlfn.CONCAT(B3,C3,":",E3,";")</f>
+        <v>TSC1EngOverrideCtrlMode:USINT;</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>871</v>
+      </c>
+      <c r="C4" t="s">
+        <v>973</v>
+      </c>
+      <c r="E4" t="s">
+        <v>983</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H12" si="0">_xlfn.CONCAT(B4,C4,":",E4,";")</f>
+        <v>TSC1EngRqedSpeedCtrlConditions:USINT;</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>871</v>
+      </c>
+      <c r="C5" t="s">
+        <v>975</v>
+      </c>
+      <c r="E5" t="s">
+        <v>983</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>TSC1OverrideCtrlModePriority:USINT;</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>871</v>
+      </c>
+      <c r="C6" t="s">
+        <v>976</v>
+      </c>
+      <c r="E6" t="s">
+        <v>984</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>TSC1EngRqedSpeed_SpeedLimit:REAL;</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>871</v>
+      </c>
+      <c r="C7" t="s">
+        <v>977</v>
+      </c>
+      <c r="E7" t="s">
+        <v>985</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>TSC1EngRqedTorque_TorqueLimit:INT;</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>871</v>
+      </c>
+      <c r="C8" t="s">
+        <v>978</v>
+      </c>
+      <c r="E8" t="s">
+        <v>983</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>TSC1TransmissionRate:USINT;</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>871</v>
+      </c>
+      <c r="C9" t="s">
+        <v>979</v>
+      </c>
+      <c r="E9" t="s">
+        <v>983</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>TSC1ControlPurpose:USINT;</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>871</v>
+      </c>
+      <c r="C10" t="s">
+        <v>980</v>
+      </c>
+      <c r="E10" t="s">
+        <v>984</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>TSC1EngineRequestedTorqueHiRes:REAL;</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>871</v>
+      </c>
+      <c r="C11" t="s">
+        <v>981</v>
+      </c>
+      <c r="E11" t="s">
+        <v>983</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>TSC1MessageCounter:USINT;</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>871</v>
+      </c>
+      <c r="C12" t="s">
+        <v>982</v>
+      </c>
+      <c r="E12" t="s">
+        <v>983</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>TSC1MessageChecksum:USINT;</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>895</v>
+      </c>
+      <c r="C15" t="s">
+        <v>986</v>
+      </c>
+      <c r="E15" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>895</v>
+      </c>
+      <c r="C16" t="s">
+        <v>987</v>
+      </c>
+      <c r="E16" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>895</v>
+      </c>
+      <c r="C17" t="s">
+        <v>988</v>
+      </c>
+      <c r="E17" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>895</v>
+      </c>
+      <c r="C18" t="s">
+        <v>989</v>
+      </c>
+      <c r="E18" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>895</v>
+      </c>
+      <c r="C19" t="s">
+        <v>990</v>
+      </c>
+      <c r="E19" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>895</v>
+      </c>
+      <c r="C20" t="s">
+        <v>991</v>
+      </c>
+      <c r="E20" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>895</v>
+      </c>
+      <c r="C21" t="s">
+        <v>992</v>
+      </c>
+      <c r="E21" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>895</v>
+      </c>
+      <c r="C22" t="s">
+        <v>993</v>
+      </c>
+      <c r="E22" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>564</v>
+      </c>
+      <c r="C26" t="s">
+        <v>994</v>
+      </c>
+      <c r="E26" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>564</v>
+      </c>
+      <c r="C27" t="s">
+        <v>995</v>
+      </c>
+      <c r="E27" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>564</v>
+      </c>
+      <c r="C28" t="s">
+        <v>996</v>
+      </c>
+      <c r="E28" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>564</v>
+      </c>
+      <c r="C29" t="s">
+        <v>997</v>
+      </c>
+      <c r="E29" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>564</v>
+      </c>
+      <c r="C30" t="s">
+        <v>998</v>
+      </c>
+      <c r="E30" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>564</v>
+      </c>
+      <c r="C31" t="s">
+        <v>999</v>
+      </c>
+      <c r="E31" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>564</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E32" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>564</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E33" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>564</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>564</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>564</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>564</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>564</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
-    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
-      <UserInfo>
-        <DisplayName>Noel Loughran</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24714,27 +25211,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c96d9849-7071-4555-8535-ee11c374d0f7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef" xsi:nil="true"/>
+    <SharedWithUsers xmlns="3f324c86-ae15-4ed4-b4a2-09335a7d28ef">
+      <UserInfo>
+        <DisplayName>Noel Loughran</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -24759,9 +25256,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3E59E7C-5896-4162-AB70-9CA3CEB6A0FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DE4EA8D-9182-4C6A-B31C-49373749A7AE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="3f324c86-ae15-4ed4-b4a2-09335a7d28ef"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="c96d9849-7071-4555-8535-ee11c374d0f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>